<commit_message>
Update TimJA Per Subkomponen
versi lama per MAK akun
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -348,6 +348,42 @@
   </si>
   <si>
     <t>'626402.175.522119.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AB.001077</t>
+  </si>
+  <si>
+    <t>2024-01-19</t>
+  </si>
+  <si>
+    <t>'00026T</t>
+  </si>
+  <si>
+    <t>'241751303000213</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.348,B.349/BPPSDM.1/KP.440/I/2024 Tgl.16-1-2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AA.001066</t>
+  </si>
+  <si>
+    <t>'00027T</t>
+  </si>
+  <si>
+    <t>'241751303000212</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.956.101.AA.000256</t>
+  </si>
+  <si>
+    <t>2024-01-18</t>
+  </si>
+  <si>
+    <t>'00029T</t>
+  </si>
+  <si>
+    <t>'241751303000204</t>
+  </si>
+  <si>
+    <t>Penggantian Uang Persediaan KKP Untuk keperluan Belanja Barang (BPP 001 SET BRSDMKP)</t>
   </si>
 </sst>
 </file>
@@ -689,7 +725,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -2641,6 +2677,120 @@
       </c>
       <c r="L53">
         <v>266514</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54">
+        <v>626402</v>
+      </c>
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+      <c r="E54" t="s">
+        <v>112</v>
+      </c>
+      <c r="F54" t="s">
+        <v>113</v>
+      </c>
+      <c r="G54" t="s">
+        <v>114</v>
+      </c>
+      <c r="H54" t="s">
+        <v>115</v>
+      </c>
+      <c r="I54" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>39160000</v>
+      </c>
+      <c r="L54">
+        <v>39160000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55">
+        <v>626402</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" t="s">
+        <v>111</v>
+      </c>
+      <c r="E55" t="s">
+        <v>116</v>
+      </c>
+      <c r="F55" t="s">
+        <v>117</v>
+      </c>
+      <c r="G55" t="s">
+        <v>114</v>
+      </c>
+      <c r="H55" t="s">
+        <v>118</v>
+      </c>
+      <c r="I55" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>33460000</v>
+      </c>
+      <c r="L55">
+        <v>33460000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>626402</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s">
+        <v>119</v>
+      </c>
+      <c r="E56" t="s">
+        <v>120</v>
+      </c>
+      <c r="F56" t="s">
+        <v>121</v>
+      </c>
+      <c r="G56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H56" t="s">
+        <v>115</v>
+      </c>
+      <c r="I56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>5618285</v>
+      </c>
+      <c r="L56">
+        <v>5618285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
realisasi 1 feb 2024 eror div dan ref
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="231">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -206,6 +206,45 @@
     <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:0006/AGA.04.02/020700/2024 Tgl.3 Januari 2024 Pembayaran Rekening Listrik Bulan Januari 2024 Untuk pemakaian Listrik Bulan Desember 2023 Gd. Arsip Depok</t>
   </si>
   <si>
+    <t>2024-02-01</t>
+  </si>
+  <si>
+    <t>'00011T</t>
+  </si>
+  <si>
+    <t>'241751504000088</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran gaji induk pegawai Sekretariat BRSDM bulan Februari 2024 untuk 73 pegawai/194 Jiwa )</t>
+  </si>
+  <si>
+    <t>'00012T</t>
+  </si>
+  <si>
+    <t>'241751504000072</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran gaji pegawai Pusat pendidikan bulan Februari 2024 untuk 42 pegawai/115 Jiwa)</t>
+  </si>
+  <si>
+    <t>'00013T</t>
+  </si>
+  <si>
+    <t>'241751504000073</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran gaji pegawai Pusat Pelatihan bulan Februari 2024 untuk 37 pegawai/105 Jiwa)</t>
+  </si>
+  <si>
+    <t>'00014T</t>
+  </si>
+  <si>
+    <t>'241751508000060</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran gaji pegawai Sekretariat BRSDM bulan Februari 2024 untuk 2 pegawai/5 Jiwa)</t>
+  </si>
+  <si>
     <t>2024-01-15</t>
   </si>
   <si>
@@ -384,6 +423,291 @@
   </si>
   <si>
     <t>Penggantian Uang Persediaan KKP Untuk keperluan Belanja Barang (BPP 001 SET BRSDMKP)</t>
+  </si>
+  <si>
+    <t>2024-01-25</t>
+  </si>
+  <si>
+    <t>'00031T</t>
+  </si>
+  <si>
+    <t>'241751303000450</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai (pembayaran uang makan pegawai Pusdik bulan Nopember 2023 untuk 1 orang)</t>
+  </si>
+  <si>
+    <t>'00032T</t>
+  </si>
+  <si>
+    <t>'241751303000451</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran uang makan pegawai Pusdik bulan Desember 2023 untuk 1 pegawai)</t>
+  </si>
+  <si>
+    <t>'00033T</t>
+  </si>
+  <si>
+    <t>'241751303000448</t>
+  </si>
+  <si>
+    <t>Penggantian uang persediaan KKP untuk keperluan belanja barang (BPP 001 Set BRSDM)</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000432</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000433</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0B.000890</t>
+  </si>
+  <si>
+    <t>2024-01-29</t>
+  </si>
+  <si>
+    <t>'00034T</t>
+  </si>
+  <si>
+    <t>'241751303000457</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang sesuai dengan Surat Tugas No.31,33/BPPSDM.5/KP.440/I/2024.Tanggal 09 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0A.000959</t>
+  </si>
+  <si>
+    <t>'00035T</t>
+  </si>
+  <si>
+    <t>'241751303000449</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran kekurangan gaji pegawai Sekretariat BRSDM an. Ari Setyawan bulan Desember 2023)</t>
+  </si>
+  <si>
+    <t>'00036T</t>
+  </si>
+  <si>
+    <t>'241751303000458</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang sesuai dengan surat tugas,ST.B 14/BRSDM.5/KP.440/I/2024.Tanggal 4 Januari 2024.</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0D.000169</t>
+  </si>
+  <si>
+    <t>'00037T</t>
+  </si>
+  <si>
+    <t>'241751504000129</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Berupa Honor PPNPN Bulan Januari Tahun 2024 untuk 31 Pegawai.Sesuai SK No:1/KPA/BPPSDM/I/2024 tgl.2-1 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000463</t>
+  </si>
+  <si>
+    <t>'00038T</t>
+  </si>
+  <si>
+    <t>'241751504000131</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Berupa Honor PPNPN Bulan Januari Tahun 2024 untuk 2 Pegawai.Sesuai SK No:1/KPA/BPPSDM/I/2024 tgl.2-1 2024</t>
+  </si>
+  <si>
+    <t>'00039T</t>
+  </si>
+  <si>
+    <t>'241751504000142</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang-Honor PPNPN Bulan Januari Tahun 2024 untuk 11 Pegawai.Sesuai dengan SK.No KEP.14/KPA/BPPSDM/I/2024.Tanggal 2 Januari 2024.</t>
+  </si>
+  <si>
+    <t>'00040T</t>
+  </si>
+  <si>
+    <t>'241751504000141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang-Honor PPNPN Bulan Januari Tahun 2024 untuk 3 Pegawai.Sesuai dengan SK.No KEP.14/KPA/BPPSDM/I/2024.Tanggal 2 Januari 2024. </t>
+  </si>
+  <si>
+    <t>2024-01-31</t>
+  </si>
+  <si>
+    <t>'00042T</t>
+  </si>
+  <si>
+    <t>'241751303000730</t>
+  </si>
+  <si>
+    <t>Penggantian uang persediaan KKP untuk keperluan belanja barang (BPP PuslatluhKP)</t>
+  </si>
+  <si>
+    <t>'626402.175.522119.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.DB.000542</t>
+  </si>
+  <si>
+    <t>'00043T</t>
+  </si>
+  <si>
+    <t>'241751303000696</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.327/BPPSDM.1/KP.440/I/2024 Tgl.16 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.974.101.0C.001044</t>
+  </si>
+  <si>
+    <t>'00044T</t>
+  </si>
+  <si>
+    <t>'241751303000695</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.827/BPPSDM.1/TU.350/I/2024 Tgl.26 Januari 2024 (PERDIN LN)</t>
+  </si>
+  <si>
+    <t>'626402.175.524211.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.106.0A.000366</t>
+  </si>
+  <si>
+    <t>2024-02-02</t>
+  </si>
+  <si>
+    <t>'00045T</t>
+  </si>
+  <si>
+    <t>'241751303000882</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Perdin Jkt-Serang (PP) tgl 11-12 Januari 2024 an.Sutrisno dan Adityo Bayu sesuai ST No B.88/BPSDM.4/KP.440/I/2024 Tgl 10/1/2024, keg. Koordinasi pelaksanaan dan lounching SFV-UPT</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.306.0A.000387</t>
+  </si>
+  <si>
+    <t>'00046T</t>
+  </si>
+  <si>
+    <t>'241751303000860</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Perdin Jkt-Serang(PP) tgl 11-12 Jan 2023 an. Luh Dewi, dkk sesuai ST No B.84/BRSDM.4/KP.440/I/2024 Tgl 10/1/2023, keg. Melakukan kunjungan ke SFV UPT Politeknik Ahli Usaha Perikanan Kampus Serang</t>
+  </si>
+  <si>
+    <t>'00047T</t>
+  </si>
+  <si>
+    <t>'241751301001178</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:009-01/BTA/I/2024 Tgl.16-1-2024</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000428</t>
+  </si>
+  <si>
+    <t>'00048T</t>
+  </si>
+  <si>
+    <t>'241751301001171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Kuitansi Nomor:123 Tgl.10-1-2024 </t>
+  </si>
+  <si>
+    <t>'00049T</t>
+  </si>
+  <si>
+    <t>'241751303000840</t>
+  </si>
+  <si>
+    <t>Penggantian Uang Persediaan untuk Keperluan Belanja Barang (BPP 002 Pusat Pendidikan KP)</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.306.0A.000380</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.301.0B.000996</t>
+  </si>
+  <si>
+    <t>'626402.175.521219.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.306.0A.000382</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2376ABW.A000000001.00000.1.0151.2.000000.000000.001.051.0A.001378</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2376AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0A.000208</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.301.0A.001152</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.301.0C.001165</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.4345EBC.A000000001.00000.1.0151.2.000000.000000.996.301.0A.001337</t>
+  </si>
+  <si>
+    <t>'626402.175.524119.03212DL.2376AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.001381</t>
+  </si>
+  <si>
+    <t>'00050T</t>
+  </si>
+  <si>
+    <t>'241751303000861</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.65/BPPSDM.5/KP.440/I/2024 Tgl.15 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524119.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0C.000977</t>
+  </si>
+  <si>
+    <t>'00053T</t>
+  </si>
+  <si>
+    <t>'241751303000862</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.171/BPPSDM.5/KP.440/I/2024 Tgl.29 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.000102</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.000103</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.001431</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.001432</t>
+  </si>
+  <si>
+    <t>'00054T</t>
+  </si>
+  <si>
+    <t>'241751303000863</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.000113</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.000114</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.001433</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.001434</t>
   </si>
 </sst>
 </file>
@@ -725,7 +1049,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -2170,7 +2494,7 @@
         <v>66</v>
       </c>
       <c r="H40" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="I40" t="s">
         <v>19</v>
@@ -2179,10 +2503,10 @@
         <v>1</v>
       </c>
       <c r="K40">
-        <v>86718779</v>
+        <v>260757140</v>
       </c>
       <c r="L40">
-        <v>86718779</v>
+        <v>260757140</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2196,19 +2520,19 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E41" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F41" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G41" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H41" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="I41" t="s">
         <v>19</v>
@@ -2217,10 +2541,10 @@
         <v>1</v>
       </c>
       <c r="K41">
-        <v>14428000</v>
+        <v>3790</v>
       </c>
       <c r="L41">
-        <v>14428000</v>
+        <v>3790</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2237,16 +2561,16 @@
         <v>63</v>
       </c>
       <c r="E42" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F42" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G42" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H42" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="I42" t="s">
         <v>19</v>
@@ -2255,10 +2579,10 @@
         <v>1</v>
       </c>
       <c r="K42">
-        <v>5074000</v>
+        <v>15669430</v>
       </c>
       <c r="L42">
-        <v>5074000</v>
+        <v>15669430</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2272,19 +2596,19 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E43" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F43" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G43" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="H43" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="I43" t="s">
         <v>19</v>
@@ -2293,10 +2617,10 @@
         <v>1</v>
       </c>
       <c r="K43">
-        <v>14000000</v>
+        <v>5644768</v>
       </c>
       <c r="L43">
-        <v>14000000</v>
+        <v>5644768</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2310,19 +2634,19 @@
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F44" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G44" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H44" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="I44" t="s">
         <v>19</v>
@@ -2331,10 +2655,10 @@
         <v>1</v>
       </c>
       <c r="K44">
-        <v>12741699</v>
+        <v>8750000</v>
       </c>
       <c r="L44">
-        <v>12741699</v>
+        <v>8750000</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2348,19 +2672,19 @@
         <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="F45" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="G45" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="H45" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="I45" t="s">
         <v>19</v>
@@ -2369,10 +2693,10 @@
         <v>1</v>
       </c>
       <c r="K45">
-        <v>4377162</v>
+        <v>26177000</v>
       </c>
       <c r="L45">
-        <v>4377162</v>
+        <v>26177000</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2386,19 +2710,19 @@
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E46" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="F46" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="G46" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="H46" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="I46" t="s">
         <v>19</v>
@@ -2407,10 +2731,10 @@
         <v>1</v>
       </c>
       <c r="K46">
-        <v>49500000</v>
+        <v>509699</v>
       </c>
       <c r="L46">
-        <v>49500000</v>
+        <v>509699</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2424,19 +2748,19 @@
         <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="F47" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="G47" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="H47" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="I47" t="s">
         <v>19</v>
@@ -2445,10 +2769,10 @@
         <v>1</v>
       </c>
       <c r="K47">
-        <v>29700000</v>
+        <v>14049480</v>
       </c>
       <c r="L47">
-        <v>29700000</v>
+        <v>14049480</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -2462,19 +2786,19 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E48" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="F48" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="G48" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="H48" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="I48" t="s">
         <v>19</v>
@@ -2483,10 +2807,10 @@
         <v>1</v>
       </c>
       <c r="K48">
-        <v>8250000</v>
+        <v>7030000</v>
       </c>
       <c r="L48">
-        <v>8250000</v>
+        <v>7030000</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2500,19 +2824,19 @@
         <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E49" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="F49" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="G49" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="H49" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="I49" t="s">
         <v>19</v>
@@ -2521,10 +2845,10 @@
         <v>1</v>
       </c>
       <c r="K49">
-        <v>37452000</v>
+        <v>151639300</v>
       </c>
       <c r="L49">
-        <v>37452000</v>
+        <v>151639300</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2538,19 +2862,19 @@
         <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E50" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="F50" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="G50" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="H50" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="I50" t="s">
         <v>19</v>
@@ -2559,10 +2883,10 @@
         <v>1</v>
       </c>
       <c r="K50">
-        <v>20581340</v>
+        <v>2287</v>
       </c>
       <c r="L50">
-        <v>20581340</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2576,19 +2900,19 @@
         <v>13</v>
       </c>
       <c r="D51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51" t="s">
         <v>68</v>
       </c>
-      <c r="E51" t="s">
-        <v>106</v>
-      </c>
-      <c r="F51" t="s">
-        <v>107</v>
-      </c>
       <c r="G51" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="H51" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="I51" t="s">
         <v>19</v>
@@ -2597,10 +2921,10 @@
         <v>1</v>
       </c>
       <c r="K51">
-        <v>24726460</v>
+        <v>10272060</v>
       </c>
       <c r="L51">
-        <v>24726460</v>
+        <v>10272060</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -2614,19 +2938,19 @@
         <v>13</v>
       </c>
       <c r="D52" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" t="s">
         <v>68</v>
       </c>
-      <c r="E52" t="s">
-        <v>106</v>
-      </c>
-      <c r="F52" t="s">
-        <v>107</v>
-      </c>
       <c r="G52" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="H52" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="I52" t="s">
         <v>19</v>
@@ -2635,10 +2959,10 @@
         <v>1</v>
       </c>
       <c r="K52">
-        <v>429372</v>
+        <v>3188432</v>
       </c>
       <c r="L52">
-        <v>429372</v>
+        <v>3188432</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -2652,19 +2976,19 @@
         <v>13</v>
       </c>
       <c r="D53" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F53" t="s">
         <v>68</v>
       </c>
-      <c r="E53" t="s">
-        <v>106</v>
-      </c>
-      <c r="F53" t="s">
-        <v>107</v>
-      </c>
       <c r="G53" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="H53" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="I53" t="s">
         <v>19</v>
@@ -2673,10 +2997,10 @@
         <v>1</v>
       </c>
       <c r="K53">
-        <v>266514</v>
+        <v>2520000</v>
       </c>
       <c r="L53">
-        <v>266514</v>
+        <v>2520000</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -2690,19 +3014,19 @@
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="E54" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="F54" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="G54" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="H54" t="s">
-        <v>115</v>
+        <v>51</v>
       </c>
       <c r="I54" t="s">
         <v>19</v>
@@ -2711,10 +3035,10 @@
         <v>1</v>
       </c>
       <c r="K54">
-        <v>39160000</v>
+        <v>11960000</v>
       </c>
       <c r="L54">
-        <v>39160000</v>
+        <v>11960000</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -2728,19 +3052,19 @@
         <v>13</v>
       </c>
       <c r="D55" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="E55" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="F55" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="G55" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="H55" t="s">
-        <v>118</v>
+        <v>52</v>
       </c>
       <c r="I55" t="s">
         <v>19</v>
@@ -2749,10 +3073,10 @@
         <v>1</v>
       </c>
       <c r="K55">
-        <v>33460000</v>
+        <v>156201</v>
       </c>
       <c r="L55">
-        <v>33460000</v>
+        <v>156201</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -2766,31 +3090,2919 @@
         <v>13</v>
       </c>
       <c r="D56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" t="s">
+        <v>67</v>
+      </c>
+      <c r="F56" t="s">
+        <v>68</v>
+      </c>
+      <c r="G56" t="s">
+        <v>69</v>
+      </c>
+      <c r="H56" t="s">
+        <v>53</v>
+      </c>
+      <c r="I56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>8328300</v>
+      </c>
+      <c r="L56">
+        <v>8328300</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <v>626402</v>
+      </c>
+      <c r="C57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" t="s">
+        <v>67</v>
+      </c>
+      <c r="F57" t="s">
+        <v>68</v>
+      </c>
+      <c r="G57" t="s">
+        <v>69</v>
+      </c>
+      <c r="H57" t="s">
+        <v>54</v>
+      </c>
+      <c r="I57" t="s">
+        <v>19</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>4620000</v>
+      </c>
+      <c r="L57">
+        <v>4620000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>626402</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" t="s">
+        <v>71</v>
+      </c>
+      <c r="G58" t="s">
+        <v>72</v>
+      </c>
+      <c r="H58" t="s">
+        <v>34</v>
+      </c>
+      <c r="I58" t="s">
+        <v>19</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>146434000</v>
+      </c>
+      <c r="L58">
+        <v>146434000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59">
+        <v>626402</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" t="s">
+        <v>63</v>
+      </c>
+      <c r="E59" t="s">
+        <v>70</v>
+      </c>
+      <c r="F59" t="s">
+        <v>71</v>
+      </c>
+      <c r="G59" t="s">
+        <v>72</v>
+      </c>
+      <c r="H59" t="s">
+        <v>35</v>
+      </c>
+      <c r="I59" t="s">
+        <v>19</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1662</v>
+      </c>
+      <c r="L59">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60">
+        <v>626402</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" t="s">
+        <v>70</v>
+      </c>
+      <c r="F60" t="s">
+        <v>71</v>
+      </c>
+      <c r="G60" t="s">
+        <v>72</v>
+      </c>
+      <c r="H60" t="s">
+        <v>36</v>
+      </c>
+      <c r="I60" t="s">
+        <v>19</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>10770030</v>
+      </c>
+      <c r="L60">
+        <v>10770030</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61">
+        <v>626402</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" t="s">
+        <v>70</v>
+      </c>
+      <c r="F61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G61" t="s">
+        <v>72</v>
+      </c>
+      <c r="H61" t="s">
+        <v>37</v>
+      </c>
+      <c r="I61" t="s">
+        <v>19</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>3213758</v>
+      </c>
+      <c r="L61">
+        <v>3213758</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62">
+        <v>626402</v>
+      </c>
+      <c r="C62" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" t="s">
+        <v>71</v>
+      </c>
+      <c r="G62" t="s">
+        <v>72</v>
+      </c>
+      <c r="H62" t="s">
+        <v>38</v>
+      </c>
+      <c r="I62" t="s">
+        <v>19</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>3250000</v>
+      </c>
+      <c r="L62">
+        <v>3250000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63">
+        <v>626402</v>
+      </c>
+      <c r="C63" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" t="s">
+        <v>70</v>
+      </c>
+      <c r="F63" t="s">
+        <v>71</v>
+      </c>
+      <c r="G63" t="s">
+        <v>72</v>
+      </c>
+      <c r="H63" t="s">
+        <v>39</v>
+      </c>
+      <c r="I63" t="s">
+        <v>19</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>15660000</v>
+      </c>
+      <c r="L63">
+        <v>15660000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64">
+        <v>626402</v>
+      </c>
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" t="s">
+        <v>63</v>
+      </c>
+      <c r="E64" t="s">
+        <v>70</v>
+      </c>
+      <c r="F64" t="s">
+        <v>71</v>
+      </c>
+      <c r="G64" t="s">
+        <v>72</v>
+      </c>
+      <c r="H64" t="s">
+        <v>40</v>
+      </c>
+      <c r="I64" t="s">
+        <v>19</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>461168</v>
+      </c>
+      <c r="L64">
+        <v>461168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65">
+        <v>626402</v>
+      </c>
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" t="s">
+        <v>70</v>
+      </c>
+      <c r="F65" t="s">
+        <v>71</v>
+      </c>
+      <c r="G65" t="s">
+        <v>72</v>
+      </c>
+      <c r="H65" t="s">
+        <v>41</v>
+      </c>
+      <c r="I65" t="s">
+        <v>19</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>7604100</v>
+      </c>
+      <c r="L65">
+        <v>7604100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66">
+        <v>626402</v>
+      </c>
+      <c r="C66" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" t="s">
+        <v>70</v>
+      </c>
+      <c r="F66" t="s">
+        <v>71</v>
+      </c>
+      <c r="G66" t="s">
+        <v>72</v>
+      </c>
+      <c r="H66" t="s">
+        <v>42</v>
+      </c>
+      <c r="I66" t="s">
+        <v>19</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66">
+        <v>3150000</v>
+      </c>
+      <c r="L66">
+        <v>3150000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <v>626402</v>
+      </c>
+      <c r="C67" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" t="s">
+        <v>73</v>
+      </c>
+      <c r="F67" t="s">
+        <v>74</v>
+      </c>
+      <c r="G67" t="s">
+        <v>75</v>
+      </c>
+      <c r="H67" t="s">
+        <v>18</v>
+      </c>
+      <c r="I67" t="s">
+        <v>19</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67">
+        <v>7605200</v>
+      </c>
+      <c r="L67">
+        <v>7605200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68">
+        <v>626402</v>
+      </c>
+      <c r="C68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E68" t="s">
+        <v>73</v>
+      </c>
+      <c r="F68" t="s">
+        <v>74</v>
+      </c>
+      <c r="G68" t="s">
+        <v>75</v>
+      </c>
+      <c r="H68" t="s">
+        <v>20</v>
+      </c>
+      <c r="I68" t="s">
+        <v>19</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68">
+        <v>102</v>
+      </c>
+      <c r="L68">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69">
+        <v>626402</v>
+      </c>
+      <c r="C69" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" t="s">
+        <v>63</v>
+      </c>
+      <c r="E69" t="s">
+        <v>73</v>
+      </c>
+      <c r="F69" t="s">
+        <v>74</v>
+      </c>
+      <c r="G69" t="s">
+        <v>75</v>
+      </c>
+      <c r="H69" t="s">
+        <v>21</v>
+      </c>
+      <c r="I69" t="s">
+        <v>19</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>341060</v>
+      </c>
+      <c r="L69">
+        <v>341060</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70">
+        <v>626402</v>
+      </c>
+      <c r="C70" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" t="s">
+        <v>63</v>
+      </c>
+      <c r="E70" t="s">
+        <v>73</v>
+      </c>
+      <c r="F70" t="s">
+        <v>74</v>
+      </c>
+      <c r="G70" t="s">
+        <v>75</v>
+      </c>
+      <c r="H70" t="s">
+        <v>22</v>
+      </c>
+      <c r="I70" t="s">
+        <v>19</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>136424</v>
+      </c>
+      <c r="L70">
+        <v>136424</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71">
+        <v>626402</v>
+      </c>
+      <c r="C71" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" t="s">
+        <v>73</v>
+      </c>
+      <c r="F71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G71" t="s">
+        <v>75</v>
+      </c>
+      <c r="H71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I71" t="s">
+        <v>19</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>2180000</v>
+      </c>
+      <c r="L71">
+        <v>2180000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72">
+        <v>69</v>
+      </c>
+      <c r="B72">
+        <v>626402</v>
+      </c>
+      <c r="C72" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" t="s">
+        <v>63</v>
+      </c>
+      <c r="E72" t="s">
+        <v>73</v>
+      </c>
+      <c r="F72" t="s">
+        <v>74</v>
+      </c>
+      <c r="G72" t="s">
+        <v>75</v>
+      </c>
+      <c r="H72" t="s">
+        <v>24</v>
+      </c>
+      <c r="I72" t="s">
+        <v>19</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>33270</v>
+      </c>
+      <c r="L72">
+        <v>33270</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73">
+        <v>70</v>
+      </c>
+      <c r="B73">
+        <v>626402</v>
+      </c>
+      <c r="C73" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" t="s">
+        <v>63</v>
+      </c>
+      <c r="E73" t="s">
+        <v>73</v>
+      </c>
+      <c r="F73" t="s">
+        <v>74</v>
+      </c>
+      <c r="G73" t="s">
+        <v>75</v>
+      </c>
+      <c r="H73" t="s">
+        <v>25</v>
+      </c>
+      <c r="I73" t="s">
+        <v>19</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>362100</v>
+      </c>
+      <c r="L73">
+        <v>362100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74">
+        <v>71</v>
+      </c>
+      <c r="B74">
+        <v>626402</v>
+      </c>
+      <c r="C74" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" t="s">
+        <v>76</v>
+      </c>
+      <c r="E74" t="s">
+        <v>77</v>
+      </c>
+      <c r="F74" t="s">
+        <v>78</v>
+      </c>
+      <c r="G74" t="s">
+        <v>79</v>
+      </c>
+      <c r="H74" t="s">
+        <v>80</v>
+      </c>
+      <c r="I74" t="s">
+        <v>19</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>86718779</v>
+      </c>
+      <c r="L74">
+        <v>86718779</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75">
+        <v>626402</v>
+      </c>
+      <c r="C75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" t="s">
+        <v>81</v>
+      </c>
+      <c r="E75" t="s">
+        <v>82</v>
+      </c>
+      <c r="F75" t="s">
+        <v>83</v>
+      </c>
+      <c r="G75" t="s">
+        <v>84</v>
+      </c>
+      <c r="H75" t="s">
+        <v>85</v>
+      </c>
+      <c r="I75" t="s">
+        <v>19</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>14428000</v>
+      </c>
+      <c r="L75">
+        <v>14428000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76">
+        <v>626402</v>
+      </c>
+      <c r="C76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" t="s">
+        <v>76</v>
+      </c>
+      <c r="E76" t="s">
+        <v>86</v>
+      </c>
+      <c r="F76" t="s">
+        <v>87</v>
+      </c>
+      <c r="G76" t="s">
+        <v>88</v>
+      </c>
+      <c r="H76" t="s">
+        <v>89</v>
+      </c>
+      <c r="I76" t="s">
+        <v>19</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>5074000</v>
+      </c>
+      <c r="L76">
+        <v>5074000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77">
+        <v>626402</v>
+      </c>
+      <c r="C77" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" t="s">
+        <v>81</v>
+      </c>
+      <c r="E77" t="s">
+        <v>90</v>
+      </c>
+      <c r="F77" t="s">
+        <v>91</v>
+      </c>
+      <c r="G77" t="s">
+        <v>92</v>
+      </c>
+      <c r="H77" t="s">
+        <v>93</v>
+      </c>
+      <c r="I77" t="s">
+        <v>19</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>14000000</v>
+      </c>
+      <c r="L77">
+        <v>14000000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78">
+        <v>626402</v>
+      </c>
+      <c r="C78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" t="s">
+        <v>81</v>
+      </c>
+      <c r="E78" t="s">
+        <v>94</v>
+      </c>
+      <c r="F78" t="s">
+        <v>95</v>
+      </c>
+      <c r="G78" t="s">
+        <v>96</v>
+      </c>
+      <c r="H78" t="s">
+        <v>97</v>
+      </c>
+      <c r="I78" t="s">
+        <v>19</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78">
+        <v>12741699</v>
+      </c>
+      <c r="L78">
+        <v>12741699</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79">
+        <v>626402</v>
+      </c>
+      <c r="C79" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" t="s">
+        <v>81</v>
+      </c>
+      <c r="E79" t="s">
+        <v>98</v>
+      </c>
+      <c r="F79" t="s">
+        <v>99</v>
+      </c>
+      <c r="G79" t="s">
+        <v>100</v>
+      </c>
+      <c r="H79" t="s">
+        <v>101</v>
+      </c>
+      <c r="I79" t="s">
+        <v>19</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>4377162</v>
+      </c>
+      <c r="L79">
+        <v>4377162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80">
+        <v>626402</v>
+      </c>
+      <c r="C80" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80" t="s">
+        <v>81</v>
+      </c>
+      <c r="E80" t="s">
+        <v>102</v>
+      </c>
+      <c r="F80" t="s">
+        <v>103</v>
+      </c>
+      <c r="G80" t="s">
+        <v>104</v>
+      </c>
+      <c r="H80" t="s">
+        <v>93</v>
+      </c>
+      <c r="I80" t="s">
+        <v>19</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>49500000</v>
+      </c>
+      <c r="L80">
+        <v>49500000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81">
+        <v>626402</v>
+      </c>
+      <c r="C81" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" t="s">
+        <v>105</v>
+      </c>
+      <c r="E81" t="s">
+        <v>106</v>
+      </c>
+      <c r="F81" t="s">
+        <v>107</v>
+      </c>
+      <c r="G81" t="s">
+        <v>108</v>
+      </c>
+      <c r="H81" t="s">
+        <v>109</v>
+      </c>
+      <c r="I81" t="s">
+        <v>19</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>29700000</v>
+      </c>
+      <c r="L81">
+        <v>29700000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82">
+        <v>79</v>
+      </c>
+      <c r="B82">
+        <v>626402</v>
+      </c>
+      <c r="C82" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" t="s">
+        <v>105</v>
+      </c>
+      <c r="E82" t="s">
+        <v>106</v>
+      </c>
+      <c r="F82" t="s">
+        <v>107</v>
+      </c>
+      <c r="G82" t="s">
+        <v>108</v>
+      </c>
+      <c r="H82" t="s">
+        <v>110</v>
+      </c>
+      <c r="I82" t="s">
+        <v>19</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>8250000</v>
+      </c>
+      <c r="L82">
+        <v>8250000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83">
+        <v>80</v>
+      </c>
+      <c r="B83">
+        <v>626402</v>
+      </c>
+      <c r="C83" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" t="s">
+        <v>105</v>
+      </c>
+      <c r="E83" t="s">
+        <v>111</v>
+      </c>
+      <c r="F83" t="s">
+        <v>112</v>
+      </c>
+      <c r="G83" t="s">
+        <v>113</v>
+      </c>
+      <c r="H83" t="s">
+        <v>114</v>
+      </c>
+      <c r="I83" t="s">
+        <v>19</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>37452000</v>
+      </c>
+      <c r="L83">
+        <v>37452000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84">
+        <v>81</v>
+      </c>
+      <c r="B84">
+        <v>626402</v>
+      </c>
+      <c r="C84" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" t="s">
+        <v>105</v>
+      </c>
+      <c r="E84" t="s">
+        <v>115</v>
+      </c>
+      <c r="F84" t="s">
+        <v>116</v>
+      </c>
+      <c r="G84" t="s">
+        <v>117</v>
+      </c>
+      <c r="H84" t="s">
+        <v>118</v>
+      </c>
+      <c r="I84" t="s">
+        <v>19</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84">
+        <v>20581340</v>
+      </c>
+      <c r="L84">
+        <v>20581340</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85">
+        <v>82</v>
+      </c>
+      <c r="B85">
+        <v>626402</v>
+      </c>
+      <c r="C85" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" t="s">
+        <v>81</v>
+      </c>
+      <c r="E85" t="s">
         <v>119</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F85" t="s">
         <v>120</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G85" t="s">
         <v>121</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H85" t="s">
+        <v>89</v>
+      </c>
+      <c r="I85" t="s">
+        <v>19</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85">
+        <v>24726460</v>
+      </c>
+      <c r="L85">
+        <v>24726460</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86">
+        <v>83</v>
+      </c>
+      <c r="B86">
+        <v>626402</v>
+      </c>
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" t="s">
+        <v>81</v>
+      </c>
+      <c r="E86" t="s">
+        <v>119</v>
+      </c>
+      <c r="F86" t="s">
+        <v>120</v>
+      </c>
+      <c r="G86" t="s">
+        <v>121</v>
+      </c>
+      <c r="H86" t="s">
         <v>122</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I86" t="s">
+        <v>19</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
+      </c>
+      <c r="K86">
+        <v>429372</v>
+      </c>
+      <c r="L86">
+        <v>429372</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87">
+        <v>84</v>
+      </c>
+      <c r="B87">
+        <v>626402</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F87" t="s">
+        <v>120</v>
+      </c>
+      <c r="G87" t="s">
+        <v>121</v>
+      </c>
+      <c r="H87" t="s">
+        <v>123</v>
+      </c>
+      <c r="I87" t="s">
+        <v>19</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="K87">
+        <v>266514</v>
+      </c>
+      <c r="L87">
+        <v>266514</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88">
+        <v>85</v>
+      </c>
+      <c r="B88">
+        <v>626402</v>
+      </c>
+      <c r="C88" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" t="s">
+        <v>124</v>
+      </c>
+      <c r="E88" t="s">
+        <v>125</v>
+      </c>
+      <c r="F88" t="s">
+        <v>126</v>
+      </c>
+      <c r="G88" t="s">
+        <v>127</v>
+      </c>
+      <c r="H88" t="s">
+        <v>128</v>
+      </c>
+      <c r="I88" t="s">
+        <v>19</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88">
+        <v>39160000</v>
+      </c>
+      <c r="L88">
+        <v>39160000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89">
+        <v>86</v>
+      </c>
+      <c r="B89">
+        <v>626402</v>
+      </c>
+      <c r="C89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" t="s">
+        <v>124</v>
+      </c>
+      <c r="E89" t="s">
+        <v>129</v>
+      </c>
+      <c r="F89" t="s">
+        <v>130</v>
+      </c>
+      <c r="G89" t="s">
+        <v>127</v>
+      </c>
+      <c r="H89" t="s">
+        <v>131</v>
+      </c>
+      <c r="I89" t="s">
+        <v>19</v>
+      </c>
+      <c r="J89">
+        <v>1</v>
+      </c>
+      <c r="K89">
+        <v>33460000</v>
+      </c>
+      <c r="L89">
+        <v>33460000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90">
+        <v>87</v>
+      </c>
+      <c r="B90">
+        <v>626402</v>
+      </c>
+      <c r="C90" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" t="s">
+        <v>132</v>
+      </c>
+      <c r="E90" t="s">
+        <v>133</v>
+      </c>
+      <c r="F90" t="s">
+        <v>134</v>
+      </c>
+      <c r="G90" t="s">
+        <v>135</v>
+      </c>
+      <c r="H90" t="s">
+        <v>128</v>
+      </c>
+      <c r="I90" t="s">
+        <v>19</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90">
+        <v>5618285</v>
+      </c>
+      <c r="L90">
+        <v>5618285</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91">
+        <v>88</v>
+      </c>
+      <c r="B91">
+        <v>626402</v>
+      </c>
+      <c r="C91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" t="s">
+        <v>136</v>
+      </c>
+      <c r="E91" t="s">
+        <v>137</v>
+      </c>
+      <c r="F91" t="s">
+        <v>138</v>
+      </c>
+      <c r="G91" t="s">
+        <v>139</v>
+      </c>
+      <c r="H91" t="s">
+        <v>85</v>
+      </c>
+      <c r="I91" t="s">
+        <v>19</v>
+      </c>
+      <c r="J91">
+        <v>1</v>
+      </c>
+      <c r="K91">
+        <v>595000</v>
+      </c>
+      <c r="L91">
+        <v>595000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92">
+        <v>89</v>
+      </c>
+      <c r="B92">
+        <v>626402</v>
+      </c>
+      <c r="C92" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" t="s">
+        <v>136</v>
+      </c>
+      <c r="E92" t="s">
+        <v>140</v>
+      </c>
+      <c r="F92" t="s">
+        <v>141</v>
+      </c>
+      <c r="G92" t="s">
+        <v>142</v>
+      </c>
+      <c r="H92" t="s">
+        <v>85</v>
+      </c>
+      <c r="I92" t="s">
+        <v>19</v>
+      </c>
+      <c r="J92">
+        <v>1</v>
+      </c>
+      <c r="K92">
+        <v>385000</v>
+      </c>
+      <c r="L92">
+        <v>385000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93">
+        <v>90</v>
+      </c>
+      <c r="B93">
+        <v>626402</v>
+      </c>
+      <c r="C93" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" t="s">
+        <v>136</v>
+      </c>
+      <c r="E93" t="s">
+        <v>143</v>
+      </c>
+      <c r="F93" t="s">
+        <v>144</v>
+      </c>
+      <c r="G93" t="s">
+        <v>145</v>
+      </c>
+      <c r="H93" t="s">
+        <v>146</v>
+      </c>
+      <c r="I93" t="s">
+        <v>19</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="K93">
+        <v>10888600</v>
+      </c>
+      <c r="L93">
+        <v>10888600</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94">
+        <v>91</v>
+      </c>
+      <c r="B94">
+        <v>626402</v>
+      </c>
+      <c r="C94" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" t="s">
+        <v>136</v>
+      </c>
+      <c r="E94" t="s">
+        <v>143</v>
+      </c>
+      <c r="F94" t="s">
+        <v>144</v>
+      </c>
+      <c r="G94" t="s">
+        <v>145</v>
+      </c>
+      <c r="H94" t="s">
+        <v>147</v>
+      </c>
+      <c r="I94" t="s">
+        <v>19</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+      <c r="K94">
+        <v>2737000</v>
+      </c>
+      <c r="L94">
+        <v>2737000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95">
+        <v>92</v>
+      </c>
+      <c r="B95">
+        <v>626402</v>
+      </c>
+      <c r="C95" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" t="s">
+        <v>136</v>
+      </c>
+      <c r="E95" t="s">
+        <v>143</v>
+      </c>
+      <c r="F95" t="s">
+        <v>144</v>
+      </c>
+      <c r="G95" t="s">
+        <v>145</v>
+      </c>
+      <c r="H95" t="s">
+        <v>148</v>
+      </c>
+      <c r="I95" t="s">
+        <v>19</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+      <c r="K95">
+        <v>1436000</v>
+      </c>
+      <c r="L95">
+        <v>1436000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96">
+        <v>93</v>
+      </c>
+      <c r="B96">
+        <v>626402</v>
+      </c>
+      <c r="C96" t="s">
+        <v>13</v>
+      </c>
+      <c r="D96" t="s">
+        <v>136</v>
+      </c>
+      <c r="E96" t="s">
+        <v>143</v>
+      </c>
+      <c r="F96" t="s">
+        <v>144</v>
+      </c>
+      <c r="G96" t="s">
+        <v>145</v>
+      </c>
+      <c r="H96" t="s">
+        <v>128</v>
+      </c>
+      <c r="I96" t="s">
+        <v>19</v>
+      </c>
+      <c r="J96">
+        <v>1</v>
+      </c>
+      <c r="K96">
+        <v>2258800</v>
+      </c>
+      <c r="L96">
+        <v>2258800</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97">
+        <v>94</v>
+      </c>
+      <c r="B97">
+        <v>626402</v>
+      </c>
+      <c r="C97" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" t="s">
+        <v>149</v>
+      </c>
+      <c r="E97" t="s">
+        <v>150</v>
+      </c>
+      <c r="F97" t="s">
+        <v>151</v>
+      </c>
+      <c r="G97" t="s">
+        <v>152</v>
+      </c>
+      <c r="H97" t="s">
+        <v>153</v>
+      </c>
+      <c r="I97" t="s">
+        <v>19</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+      <c r="K97">
+        <v>17281700</v>
+      </c>
+      <c r="L97">
+        <v>17281700</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98">
+        <v>95</v>
+      </c>
+      <c r="B98">
+        <v>626402</v>
+      </c>
+      <c r="C98" t="s">
+        <v>13</v>
+      </c>
+      <c r="D98" t="s">
+        <v>136</v>
+      </c>
+      <c r="E98" t="s">
+        <v>154</v>
+      </c>
+      <c r="F98" t="s">
+        <v>155</v>
+      </c>
+      <c r="G98" t="s">
+        <v>156</v>
+      </c>
+      <c r="H98" t="s">
+        <v>18</v>
+      </c>
+      <c r="I98" t="s">
+        <v>19</v>
+      </c>
+      <c r="J98">
+        <v>1</v>
+      </c>
+      <c r="K98">
+        <v>121600</v>
+      </c>
+      <c r="L98">
+        <v>121600</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99">
+        <v>96</v>
+      </c>
+      <c r="B99">
+        <v>626402</v>
+      </c>
+      <c r="C99" t="s">
+        <v>13</v>
+      </c>
+      <c r="D99" t="s">
+        <v>136</v>
+      </c>
+      <c r="E99" t="s">
+        <v>154</v>
+      </c>
+      <c r="F99" t="s">
+        <v>155</v>
+      </c>
+      <c r="G99" t="s">
+        <v>156</v>
+      </c>
+      <c r="H99" t="s">
+        <v>20</v>
+      </c>
+      <c r="I99" t="s">
+        <v>19</v>
+      </c>
+      <c r="J99">
+        <v>1</v>
+      </c>
+      <c r="K99">
+        <v>164</v>
+      </c>
+      <c r="L99">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100">
+        <v>97</v>
+      </c>
+      <c r="B100">
+        <v>626402</v>
+      </c>
+      <c r="C100" t="s">
+        <v>13</v>
+      </c>
+      <c r="D100" t="s">
+        <v>136</v>
+      </c>
+      <c r="E100" t="s">
+        <v>154</v>
+      </c>
+      <c r="F100" t="s">
+        <v>155</v>
+      </c>
+      <c r="G100" t="s">
+        <v>156</v>
+      </c>
+      <c r="H100" t="s">
+        <v>21</v>
+      </c>
+      <c r="I100" t="s">
+        <v>19</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+      <c r="K100">
+        <v>12160</v>
+      </c>
+      <c r="L100">
+        <v>12160</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101">
+        <v>98</v>
+      </c>
+      <c r="B101">
+        <v>626402</v>
+      </c>
+      <c r="C101" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" t="s">
+        <v>136</v>
+      </c>
+      <c r="E101" t="s">
+        <v>154</v>
+      </c>
+      <c r="F101" t="s">
+        <v>155</v>
+      </c>
+      <c r="G101" t="s">
+        <v>156</v>
+      </c>
+      <c r="H101" t="s">
+        <v>22</v>
+      </c>
+      <c r="I101" t="s">
+        <v>19</v>
+      </c>
+      <c r="J101">
+        <v>1</v>
+      </c>
+      <c r="K101">
+        <v>2432</v>
+      </c>
+      <c r="L101">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="A102">
+        <v>99</v>
+      </c>
+      <c r="B102">
+        <v>626402</v>
+      </c>
+      <c r="C102" t="s">
+        <v>13</v>
+      </c>
+      <c r="D102" t="s">
+        <v>149</v>
+      </c>
+      <c r="E102" t="s">
+        <v>157</v>
+      </c>
+      <c r="F102" t="s">
+        <v>158</v>
+      </c>
+      <c r="G102" t="s">
+        <v>159</v>
+      </c>
+      <c r="H102" t="s">
+        <v>160</v>
+      </c>
+      <c r="I102" t="s">
+        <v>19</v>
+      </c>
+      <c r="J102">
+        <v>1</v>
+      </c>
+      <c r="K102">
+        <v>4266500</v>
+      </c>
+      <c r="L102">
+        <v>4266500</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
+      <c r="A103">
+        <v>100</v>
+      </c>
+      <c r="B103">
+        <v>626402</v>
+      </c>
+      <c r="C103" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103" t="s">
+        <v>63</v>
+      </c>
+      <c r="E103" t="s">
+        <v>161</v>
+      </c>
+      <c r="F103" t="s">
+        <v>162</v>
+      </c>
+      <c r="G103" t="s">
+        <v>163</v>
+      </c>
+      <c r="H103" t="s">
+        <v>164</v>
+      </c>
+      <c r="I103" t="s">
+        <v>19</v>
+      </c>
+      <c r="J103">
+        <v>1</v>
+      </c>
+      <c r="K103">
+        <v>158224000</v>
+      </c>
+      <c r="L103">
+        <v>158224000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
+      <c r="A104">
+        <v>101</v>
+      </c>
+      <c r="B104">
+        <v>626402</v>
+      </c>
+      <c r="C104" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104" t="s">
+        <v>63</v>
+      </c>
+      <c r="E104" t="s">
+        <v>165</v>
+      </c>
+      <c r="F104" t="s">
+        <v>166</v>
+      </c>
+      <c r="G104" t="s">
+        <v>167</v>
+      </c>
+      <c r="H104" t="s">
+        <v>164</v>
+      </c>
+      <c r="I104" t="s">
+        <v>19</v>
+      </c>
+      <c r="J104">
+        <v>1</v>
+      </c>
+      <c r="K104">
+        <v>10208000</v>
+      </c>
+      <c r="L104">
+        <v>10208000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="A105">
+        <v>102</v>
+      </c>
+      <c r="B105">
+        <v>626402</v>
+      </c>
+      <c r="C105" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105" t="s">
+        <v>63</v>
+      </c>
+      <c r="E105" t="s">
+        <v>168</v>
+      </c>
+      <c r="F105" t="s">
+        <v>169</v>
+      </c>
+      <c r="G105" t="s">
+        <v>170</v>
+      </c>
+      <c r="H105" t="s">
+        <v>164</v>
+      </c>
+      <c r="I105" t="s">
+        <v>19</v>
+      </c>
+      <c r="J105">
+        <v>1</v>
+      </c>
+      <c r="K105">
+        <v>56144000</v>
+      </c>
+      <c r="L105">
+        <v>56144000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="A106">
+        <v>103</v>
+      </c>
+      <c r="B106">
+        <v>626402</v>
+      </c>
+      <c r="C106" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" t="s">
+        <v>63</v>
+      </c>
+      <c r="E106" t="s">
+        <v>171</v>
+      </c>
+      <c r="F106" t="s">
+        <v>172</v>
+      </c>
+      <c r="G106" t="s">
+        <v>173</v>
+      </c>
+      <c r="H106" t="s">
+        <v>164</v>
+      </c>
+      <c r="I106" t="s">
+        <v>19</v>
+      </c>
+      <c r="J106">
+        <v>1</v>
+      </c>
+      <c r="K106">
+        <v>15312000</v>
+      </c>
+      <c r="L106">
+        <v>15312000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="A107">
+        <v>104</v>
+      </c>
+      <c r="B107">
+        <v>626402</v>
+      </c>
+      <c r="C107" t="s">
+        <v>13</v>
+      </c>
+      <c r="D107" t="s">
+        <v>174</v>
+      </c>
+      <c r="E107" t="s">
+        <v>175</v>
+      </c>
+      <c r="F107" t="s">
+        <v>176</v>
+      </c>
+      <c r="G107" t="s">
+        <v>177</v>
+      </c>
+      <c r="H107" t="s">
+        <v>178</v>
+      </c>
+      <c r="I107" t="s">
+        <v>19</v>
+      </c>
+      <c r="J107">
+        <v>1</v>
+      </c>
+      <c r="K107">
+        <v>2412514</v>
+      </c>
+      <c r="L107">
+        <v>2412514</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="A108">
+        <v>105</v>
+      </c>
+      <c r="B108">
+        <v>626402</v>
+      </c>
+      <c r="C108" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108" t="s">
+        <v>63</v>
+      </c>
+      <c r="E108" t="s">
+        <v>179</v>
+      </c>
+      <c r="F108" t="s">
+        <v>180</v>
+      </c>
+      <c r="G108" t="s">
+        <v>181</v>
+      </c>
+      <c r="H108" t="s">
+        <v>182</v>
+      </c>
+      <c r="I108" t="s">
+        <v>19</v>
+      </c>
+      <c r="J108">
+        <v>1</v>
+      </c>
+      <c r="K108">
+        <v>19247944</v>
+      </c>
+      <c r="L108">
+        <v>19247944</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109">
+        <v>106</v>
+      </c>
+      <c r="B109">
+        <v>626402</v>
+      </c>
+      <c r="C109" t="s">
+        <v>13</v>
+      </c>
+      <c r="D109" t="s">
+        <v>63</v>
+      </c>
+      <c r="E109" t="s">
+        <v>183</v>
+      </c>
+      <c r="F109" t="s">
+        <v>184</v>
+      </c>
+      <c r="G109" t="s">
+        <v>185</v>
+      </c>
+      <c r="H109" t="s">
+        <v>186</v>
+      </c>
+      <c r="I109" t="s">
+        <v>19</v>
+      </c>
+      <c r="J109">
+        <v>1</v>
+      </c>
+      <c r="K109">
+        <v>484491206</v>
+      </c>
+      <c r="L109">
+        <v>484491206</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
+      <c r="A110">
+        <v>107</v>
+      </c>
+      <c r="B110">
+        <v>626402</v>
+      </c>
+      <c r="C110" t="s">
+        <v>13</v>
+      </c>
+      <c r="D110" t="s">
+        <v>187</v>
+      </c>
+      <c r="E110" t="s">
+        <v>188</v>
+      </c>
+      <c r="F110" t="s">
+        <v>189</v>
+      </c>
+      <c r="G110" t="s">
+        <v>190</v>
+      </c>
+      <c r="H110" t="s">
+        <v>191</v>
+      </c>
+      <c r="I110" t="s">
+        <v>19</v>
+      </c>
+      <c r="J110">
+        <v>1</v>
+      </c>
+      <c r="K110">
+        <v>3808600</v>
+      </c>
+      <c r="L110">
+        <v>3808600</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
+      <c r="A111">
+        <v>108</v>
+      </c>
+      <c r="B111">
+        <v>626402</v>
+      </c>
+      <c r="C111" t="s">
+        <v>13</v>
+      </c>
+      <c r="D111" t="s">
+        <v>187</v>
+      </c>
+      <c r="E111" t="s">
+        <v>192</v>
+      </c>
+      <c r="F111" t="s">
+        <v>193</v>
+      </c>
+      <c r="G111" t="s">
+        <v>194</v>
+      </c>
+      <c r="H111" t="s">
+        <v>191</v>
+      </c>
+      <c r="I111" t="s">
+        <v>19</v>
+      </c>
+      <c r="J111">
+        <v>1</v>
+      </c>
+      <c r="K111">
+        <v>4090700</v>
+      </c>
+      <c r="L111">
+        <v>4090700</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
+      <c r="A112">
+        <v>109</v>
+      </c>
+      <c r="B112">
+        <v>626402</v>
+      </c>
+      <c r="C112" t="s">
+        <v>13</v>
+      </c>
+      <c r="D112" t="s">
+        <v>187</v>
+      </c>
+      <c r="E112" t="s">
+        <v>195</v>
+      </c>
+      <c r="F112" t="s">
+        <v>196</v>
+      </c>
+      <c r="G112" t="s">
+        <v>197</v>
+      </c>
+      <c r="H112" t="s">
+        <v>198</v>
+      </c>
+      <c r="I112" t="s">
+        <v>19</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+      <c r="K112">
+        <v>46320300</v>
+      </c>
+      <c r="L112">
+        <v>46320300</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="A113">
+        <v>110</v>
+      </c>
+      <c r="B113">
+        <v>626402</v>
+      </c>
+      <c r="C113" t="s">
+        <v>13</v>
+      </c>
+      <c r="D113" t="s">
+        <v>187</v>
+      </c>
+      <c r="E113" t="s">
+        <v>199</v>
+      </c>
+      <c r="F113" t="s">
+        <v>200</v>
+      </c>
+      <c r="G113" t="s">
+        <v>201</v>
+      </c>
+      <c r="H113" t="s">
+        <v>198</v>
+      </c>
+      <c r="I113" t="s">
+        <v>19</v>
+      </c>
+      <c r="J113">
+        <v>1</v>
+      </c>
+      <c r="K113">
+        <v>18326100</v>
+      </c>
+      <c r="L113">
+        <v>18326100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="A114">
+        <v>111</v>
+      </c>
+      <c r="B114">
+        <v>626402</v>
+      </c>
+      <c r="C114" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114" t="s">
+        <v>63</v>
+      </c>
+      <c r="E114" t="s">
+        <v>202</v>
+      </c>
+      <c r="F114" t="s">
+        <v>203</v>
+      </c>
+      <c r="G114" t="s">
+        <v>204</v>
+      </c>
+      <c r="H114" t="s">
+        <v>205</v>
+      </c>
+      <c r="I114" t="s">
+        <v>19</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+      <c r="K114">
+        <v>2740500</v>
+      </c>
+      <c r="L114">
+        <v>2740500</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="A115">
+        <v>112</v>
+      </c>
+      <c r="B115">
+        <v>626402</v>
+      </c>
+      <c r="C115" t="s">
+        <v>13</v>
+      </c>
+      <c r="D115" t="s">
+        <v>63</v>
+      </c>
+      <c r="E115" t="s">
+        <v>202</v>
+      </c>
+      <c r="F115" t="s">
+        <v>203</v>
+      </c>
+      <c r="G115" t="s">
+        <v>204</v>
+      </c>
+      <c r="H115" t="s">
+        <v>206</v>
+      </c>
+      <c r="I115" t="s">
+        <v>19</v>
+      </c>
+      <c r="J115">
+        <v>1</v>
+      </c>
+      <c r="K115">
+        <v>1500000</v>
+      </c>
+      <c r="L115">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="A116">
+        <v>113</v>
+      </c>
+      <c r="B116">
+        <v>626402</v>
+      </c>
+      <c r="C116" t="s">
+        <v>13</v>
+      </c>
+      <c r="D116" t="s">
+        <v>63</v>
+      </c>
+      <c r="E116" t="s">
+        <v>202</v>
+      </c>
+      <c r="F116" t="s">
+        <v>203</v>
+      </c>
+      <c r="G116" t="s">
+        <v>204</v>
+      </c>
+      <c r="H116" t="s">
+        <v>207</v>
+      </c>
+      <c r="I116" t="s">
+        <v>19</v>
+      </c>
+      <c r="J116">
+        <v>1</v>
+      </c>
+      <c r="K116">
+        <v>1615470</v>
+      </c>
+      <c r="L116">
+        <v>1615470</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="A117">
+        <v>114</v>
+      </c>
+      <c r="B117">
+        <v>626402</v>
+      </c>
+      <c r="C117" t="s">
+        <v>13</v>
+      </c>
+      <c r="D117" t="s">
+        <v>63</v>
+      </c>
+      <c r="E117" t="s">
+        <v>202</v>
+      </c>
+      <c r="F117" t="s">
+        <v>203</v>
+      </c>
+      <c r="G117" t="s">
+        <v>204</v>
+      </c>
+      <c r="H117" t="s">
+        <v>208</v>
+      </c>
+      <c r="I117" t="s">
+        <v>19</v>
+      </c>
+      <c r="J117">
+        <v>1</v>
+      </c>
+      <c r="K117">
+        <v>16523260</v>
+      </c>
+      <c r="L117">
+        <v>16523260</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118">
         <v>115</v>
       </c>
-      <c r="I56" t="s">
-        <v>19</v>
-      </c>
-      <c r="J56">
-        <v>1</v>
-      </c>
-      <c r="K56">
-        <v>5618285</v>
-      </c>
-      <c r="L56">
-        <v>5618285</v>
+      <c r="B118">
+        <v>626402</v>
+      </c>
+      <c r="C118" t="s">
+        <v>13</v>
+      </c>
+      <c r="D118" t="s">
+        <v>63</v>
+      </c>
+      <c r="E118" t="s">
+        <v>202</v>
+      </c>
+      <c r="F118" t="s">
+        <v>203</v>
+      </c>
+      <c r="G118" t="s">
+        <v>204</v>
+      </c>
+      <c r="H118" t="s">
+        <v>209</v>
+      </c>
+      <c r="I118" t="s">
+        <v>19</v>
+      </c>
+      <c r="J118">
+        <v>1</v>
+      </c>
+      <c r="K118">
+        <v>818500</v>
+      </c>
+      <c r="L118">
+        <v>818500</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119">
+        <v>116</v>
+      </c>
+      <c r="B119">
+        <v>626402</v>
+      </c>
+      <c r="C119" t="s">
+        <v>13</v>
+      </c>
+      <c r="D119" t="s">
+        <v>63</v>
+      </c>
+      <c r="E119" t="s">
+        <v>202</v>
+      </c>
+      <c r="F119" t="s">
+        <v>203</v>
+      </c>
+      <c r="G119" t="s">
+        <v>204</v>
+      </c>
+      <c r="H119" t="s">
+        <v>191</v>
+      </c>
+      <c r="I119" t="s">
+        <v>19</v>
+      </c>
+      <c r="J119">
+        <v>1</v>
+      </c>
+      <c r="K119">
+        <v>7000500</v>
+      </c>
+      <c r="L119">
+        <v>7000500</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120">
+        <v>117</v>
+      </c>
+      <c r="B120">
+        <v>626402</v>
+      </c>
+      <c r="C120" t="s">
+        <v>13</v>
+      </c>
+      <c r="D120" t="s">
+        <v>63</v>
+      </c>
+      <c r="E120" t="s">
+        <v>202</v>
+      </c>
+      <c r="F120" t="s">
+        <v>203</v>
+      </c>
+      <c r="G120" t="s">
+        <v>204</v>
+      </c>
+      <c r="H120" t="s">
+        <v>210</v>
+      </c>
+      <c r="I120" t="s">
+        <v>19</v>
+      </c>
+      <c r="J120">
+        <v>1</v>
+      </c>
+      <c r="K120">
+        <v>6756655</v>
+      </c>
+      <c r="L120">
+        <v>6756655</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121">
+        <v>118</v>
+      </c>
+      <c r="B121">
+        <v>626402</v>
+      </c>
+      <c r="C121" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" t="s">
+        <v>63</v>
+      </c>
+      <c r="E121" t="s">
+        <v>202</v>
+      </c>
+      <c r="F121" t="s">
+        <v>203</v>
+      </c>
+      <c r="G121" t="s">
+        <v>204</v>
+      </c>
+      <c r="H121" t="s">
+        <v>211</v>
+      </c>
+      <c r="I121" t="s">
+        <v>19</v>
+      </c>
+      <c r="J121">
+        <v>1</v>
+      </c>
+      <c r="K121">
+        <v>5285500</v>
+      </c>
+      <c r="L121">
+        <v>5285500</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122">
+        <v>119</v>
+      </c>
+      <c r="B122">
+        <v>626402</v>
+      </c>
+      <c r="C122" t="s">
+        <v>13</v>
+      </c>
+      <c r="D122" t="s">
+        <v>63</v>
+      </c>
+      <c r="E122" t="s">
+        <v>202</v>
+      </c>
+      <c r="F122" t="s">
+        <v>203</v>
+      </c>
+      <c r="G122" t="s">
+        <v>204</v>
+      </c>
+      <c r="H122" t="s">
+        <v>212</v>
+      </c>
+      <c r="I122" t="s">
+        <v>19</v>
+      </c>
+      <c r="J122">
+        <v>1</v>
+      </c>
+      <c r="K122">
+        <v>14478054</v>
+      </c>
+      <c r="L122">
+        <v>14478054</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123">
+        <v>120</v>
+      </c>
+      <c r="B123">
+        <v>626402</v>
+      </c>
+      <c r="C123" t="s">
+        <v>13</v>
+      </c>
+      <c r="D123" t="s">
+        <v>63</v>
+      </c>
+      <c r="E123" t="s">
+        <v>202</v>
+      </c>
+      <c r="F123" t="s">
+        <v>203</v>
+      </c>
+      <c r="G123" t="s">
+        <v>204</v>
+      </c>
+      <c r="H123" t="s">
+        <v>213</v>
+      </c>
+      <c r="I123" t="s">
+        <v>19</v>
+      </c>
+      <c r="J123">
+        <v>1</v>
+      </c>
+      <c r="K123">
+        <v>43014384</v>
+      </c>
+      <c r="L123">
+        <v>43014384</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124">
+        <v>121</v>
+      </c>
+      <c r="B124">
+        <v>626402</v>
+      </c>
+      <c r="C124" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124" t="s">
+        <v>187</v>
+      </c>
+      <c r="E124" t="s">
+        <v>214</v>
+      </c>
+      <c r="F124" t="s">
+        <v>215</v>
+      </c>
+      <c r="G124" t="s">
+        <v>216</v>
+      </c>
+      <c r="H124" t="s">
+        <v>217</v>
+      </c>
+      <c r="I124" t="s">
+        <v>19</v>
+      </c>
+      <c r="J124">
+        <v>1</v>
+      </c>
+      <c r="K124">
+        <v>10892300</v>
+      </c>
+      <c r="L124">
+        <v>10892300</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125">
+        <v>122</v>
+      </c>
+      <c r="B125">
+        <v>626402</v>
+      </c>
+      <c r="C125" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" t="s">
+        <v>187</v>
+      </c>
+      <c r="E125" t="s">
+        <v>218</v>
+      </c>
+      <c r="F125" t="s">
+        <v>219</v>
+      </c>
+      <c r="G125" t="s">
+        <v>220</v>
+      </c>
+      <c r="H125" t="s">
+        <v>221</v>
+      </c>
+      <c r="I125" t="s">
+        <v>19</v>
+      </c>
+      <c r="J125">
+        <v>1</v>
+      </c>
+      <c r="K125">
+        <v>1800000</v>
+      </c>
+      <c r="L125">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126">
+        <v>123</v>
+      </c>
+      <c r="B126">
+        <v>626402</v>
+      </c>
+      <c r="C126" t="s">
+        <v>13</v>
+      </c>
+      <c r="D126" t="s">
+        <v>187</v>
+      </c>
+      <c r="E126" t="s">
+        <v>218</v>
+      </c>
+      <c r="F126" t="s">
+        <v>219</v>
+      </c>
+      <c r="G126" t="s">
+        <v>220</v>
+      </c>
+      <c r="H126" t="s">
+        <v>222</v>
+      </c>
+      <c r="I126" t="s">
+        <v>19</v>
+      </c>
+      <c r="J126">
+        <v>1</v>
+      </c>
+      <c r="K126">
+        <v>4800000</v>
+      </c>
+      <c r="L126">
+        <v>4800000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="A127">
+        <v>124</v>
+      </c>
+      <c r="B127">
+        <v>626402</v>
+      </c>
+      <c r="C127" t="s">
+        <v>13</v>
+      </c>
+      <c r="D127" t="s">
+        <v>187</v>
+      </c>
+      <c r="E127" t="s">
+        <v>218</v>
+      </c>
+      <c r="F127" t="s">
+        <v>219</v>
+      </c>
+      <c r="G127" t="s">
+        <v>220</v>
+      </c>
+      <c r="H127" t="s">
+        <v>223</v>
+      </c>
+      <c r="I127" t="s">
+        <v>19</v>
+      </c>
+      <c r="J127">
+        <v>1</v>
+      </c>
+      <c r="K127">
+        <v>4070000</v>
+      </c>
+      <c r="L127">
+        <v>4070000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="A128">
+        <v>125</v>
+      </c>
+      <c r="B128">
+        <v>626402</v>
+      </c>
+      <c r="C128" t="s">
+        <v>13</v>
+      </c>
+      <c r="D128" t="s">
+        <v>187</v>
+      </c>
+      <c r="E128" t="s">
+        <v>218</v>
+      </c>
+      <c r="F128" t="s">
+        <v>219</v>
+      </c>
+      <c r="G128" t="s">
+        <v>220</v>
+      </c>
+      <c r="H128" t="s">
+        <v>224</v>
+      </c>
+      <c r="I128" t="s">
+        <v>19</v>
+      </c>
+      <c r="J128">
+        <v>1</v>
+      </c>
+      <c r="K128">
+        <v>450000</v>
+      </c>
+      <c r="L128">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129">
+        <v>126</v>
+      </c>
+      <c r="B129">
+        <v>626402</v>
+      </c>
+      <c r="C129" t="s">
+        <v>13</v>
+      </c>
+      <c r="D129" t="s">
+        <v>187</v>
+      </c>
+      <c r="E129" t="s">
+        <v>225</v>
+      </c>
+      <c r="F129" t="s">
+        <v>226</v>
+      </c>
+      <c r="G129" t="s">
+        <v>220</v>
+      </c>
+      <c r="H129" t="s">
+        <v>227</v>
+      </c>
+      <c r="I129" t="s">
+        <v>19</v>
+      </c>
+      <c r="J129">
+        <v>1</v>
+      </c>
+      <c r="K129">
+        <v>1200000</v>
+      </c>
+      <c r="L129">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130">
+        <v>127</v>
+      </c>
+      <c r="B130">
+        <v>626402</v>
+      </c>
+      <c r="C130" t="s">
+        <v>13</v>
+      </c>
+      <c r="D130" t="s">
+        <v>187</v>
+      </c>
+      <c r="E130" t="s">
+        <v>225</v>
+      </c>
+      <c r="F130" t="s">
+        <v>226</v>
+      </c>
+      <c r="G130" t="s">
+        <v>220</v>
+      </c>
+      <c r="H130" t="s">
+        <v>228</v>
+      </c>
+      <c r="I130" t="s">
+        <v>19</v>
+      </c>
+      <c r="J130">
+        <v>1</v>
+      </c>
+      <c r="K130">
+        <v>3600000</v>
+      </c>
+      <c r="L130">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131">
+        <v>128</v>
+      </c>
+      <c r="B131">
+        <v>626402</v>
+      </c>
+      <c r="C131" t="s">
+        <v>13</v>
+      </c>
+      <c r="D131" t="s">
+        <v>187</v>
+      </c>
+      <c r="E131" t="s">
+        <v>225</v>
+      </c>
+      <c r="F131" t="s">
+        <v>226</v>
+      </c>
+      <c r="G131" t="s">
+        <v>220</v>
+      </c>
+      <c r="H131" t="s">
+        <v>229</v>
+      </c>
+      <c r="I131" t="s">
+        <v>19</v>
+      </c>
+      <c r="J131">
+        <v>1</v>
+      </c>
+      <c r="K131">
+        <v>2960000</v>
+      </c>
+      <c r="L131">
+        <v>2960000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="A132">
+        <v>129</v>
+      </c>
+      <c r="B132">
+        <v>626402</v>
+      </c>
+      <c r="C132" t="s">
+        <v>13</v>
+      </c>
+      <c r="D132" t="s">
+        <v>187</v>
+      </c>
+      <c r="E132" t="s">
+        <v>225</v>
+      </c>
+      <c r="F132" t="s">
+        <v>226</v>
+      </c>
+      <c r="G132" t="s">
+        <v>220</v>
+      </c>
+      <c r="H132" t="s">
+        <v>230</v>
+      </c>
+      <c r="I132" t="s">
+        <v>19</v>
+      </c>
+      <c r="J132">
+        <v>1</v>
+      </c>
+      <c r="K132">
+        <v>300000</v>
+      </c>
+      <c r="L132">
+        <v>300000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 2 februari 2024
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="295">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -671,6 +671,27 @@
     <t>'626402.175.524119.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0C.000977</t>
   </si>
   <si>
+    <t>'00051T</t>
+  </si>
+  <si>
+    <t>'241751303000909</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran kekurangan gaji pegawai Pusdik bulan Januari 2024 an. Gelora wijayanto untuk 1 pegawai)</t>
+  </si>
+  <si>
+    <t>'00052T</t>
+  </si>
+  <si>
+    <t>'241751303000908</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Honor Susulan PPNPN Pusdik KP bulan Januari 2024 sebanyak 7 pegawai an. M. Arif Mustaqim dkk sesuai SK Nomor :KEP.13/KPA/BPPSDM/I/2024 tgl 02 Januari 2024.</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.GA.000563</t>
+  </si>
+  <si>
     <t>'00053T</t>
   </si>
   <si>
@@ -708,6 +729,177 @@
   </si>
   <si>
     <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.001434</t>
+  </si>
+  <si>
+    <t>'00055T</t>
+  </si>
+  <si>
+    <t>'241751303000907</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Honor Susulan PPNPN Pusdik KP bulan Januari 2024 sebanyak 3 pegawai an. Joko Pitoyo,dkk sesuai SK Nomor KEP.13/KPA/BPPSDM/I/2024 tgl 02 Januari 2024.</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.GA.000564</t>
+  </si>
+  <si>
+    <t>'00056T</t>
+  </si>
+  <si>
+    <t>'241751303000910</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran gaji susulan pegawai PPPK Sekretariat BRSDM bulan Januari-Februari 2024 untuk 2 pegawai/5 Jiwa)</t>
+  </si>
+  <si>
+    <t>'626402.175.511611.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.AA.001359</t>
+  </si>
+  <si>
+    <t>'626402.175.511619.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.AA.001360</t>
+  </si>
+  <si>
+    <t>'626402.175.511621.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.AA.001361</t>
+  </si>
+  <si>
+    <t>'626402.175.511622.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.AA.001362</t>
+  </si>
+  <si>
+    <t>'626402.175.511624.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.AA.001363</t>
+  </si>
+  <si>
+    <t>'626402.175.511625.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.AA.001364</t>
+  </si>
+  <si>
+    <t>'00057T</t>
+  </si>
+  <si>
+    <t>'241751303000912</t>
+  </si>
+  <si>
+    <t>Penggantian uang persediaan untuk keperluan belanja barang (BPP001 Set.BRSDM)</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000423</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000426</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000427</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000465</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000466</t>
+  </si>
+  <si>
+    <t>'626402.175.521114.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AB.000441</t>
+  </si>
+  <si>
+    <t>'626402.175.521119.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000430</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AA.001057</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AA.001060</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AA.001061</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.106.0A.000361</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.106.0B.000368</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000496</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AB.001076</t>
+  </si>
+  <si>
+    <t>'626402.175.522191.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.101.0A.000343</t>
+  </si>
+  <si>
+    <t>'626402.175.523121.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AC.000446</t>
+  </si>
+  <si>
+    <t>'626402.175.523121.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AC.000449</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.956.101.AC.000266</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.101.0A.000344</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AB.001081</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.974.101.0A.001033</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.101.0A.000346</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.101.0A.000347</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.106.0A.000364</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.958.106.0A.000365</t>
+  </si>
+  <si>
+    <t>2024-02-05</t>
+  </si>
+  <si>
+    <t>'00058T</t>
+  </si>
+  <si>
+    <t>'241751303000971</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.330/BPPSDM.1/KP.440/I/2024 Tanggal 15 Januari 2024 a.n Untung Januar, dkk</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AC.001091</t>
+  </si>
+  <si>
+    <t>'00059T</t>
+  </si>
+  <si>
+    <t>'241751303000972</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.37,B.45,B.107,B.374,B.700/BPPSDM.1/KP.440/I/2024 Tanggal 9,16,17 Januari 2024 a.n I Nyoman Radiarta, dkk</t>
+  </si>
+  <si>
+    <t>'00060T</t>
+  </si>
+  <si>
+    <t>'241751303000973</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.89/BPPSDM.1/KP.440/I/2024 Tanggal 3 Januari 2024 a.n Tri Yuwono, dkk</t>
+  </si>
+  <si>
+    <t>'626402.175.524113.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.101.0B.001515</t>
+  </si>
+  <si>
+    <t>'626402.175.524113.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.101.0B.001516</t>
+  </si>
+  <si>
+    <t>'00061T</t>
+  </si>
+  <si>
+    <t>'241751303000970</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.829/BPPSDM.1/KP.440/I/2024 Tanggal 26 Januari 2024 a.n Rizky Hendriansyah, dkk</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1241,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L132"/>
+  <dimension ref="A1:L179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -5712,7 +5904,7 @@
         <v>13</v>
       </c>
       <c r="D125" t="s">
-        <v>187</v>
+        <v>63</v>
       </c>
       <c r="E125" t="s">
         <v>218</v>
@@ -5724,7 +5916,7 @@
         <v>220</v>
       </c>
       <c r="H125" t="s">
-        <v>221</v>
+        <v>46</v>
       </c>
       <c r="I125" t="s">
         <v>19</v>
@@ -5733,10 +5925,10 @@
         <v>1</v>
       </c>
       <c r="K125">
-        <v>1800000</v>
+        <v>205000</v>
       </c>
       <c r="L125">
-        <v>1800000</v>
+        <v>205000</v>
       </c>
     </row>
     <row r="126" spans="1:12">
@@ -5750,7 +5942,7 @@
         <v>13</v>
       </c>
       <c r="D126" t="s">
-        <v>187</v>
+        <v>63</v>
       </c>
       <c r="E126" t="s">
         <v>218</v>
@@ -5762,7 +5954,7 @@
         <v>220</v>
       </c>
       <c r="H126" t="s">
-        <v>222</v>
+        <v>52</v>
       </c>
       <c r="I126" t="s">
         <v>19</v>
@@ -5771,10 +5963,10 @@
         <v>1</v>
       </c>
       <c r="K126">
-        <v>4800000</v>
+        <v>9750</v>
       </c>
       <c r="L126">
-        <v>4800000</v>
+        <v>9750</v>
       </c>
     </row>
     <row r="127" spans="1:12">
@@ -5788,19 +5980,19 @@
         <v>13</v>
       </c>
       <c r="D127" t="s">
-        <v>187</v>
+        <v>63</v>
       </c>
       <c r="E127" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F127" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G127" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H127" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I127" t="s">
         <v>19</v>
@@ -5809,10 +6001,10 @@
         <v>1</v>
       </c>
       <c r="K127">
-        <v>4070000</v>
+        <v>35728000</v>
       </c>
       <c r="L127">
-        <v>4070000</v>
+        <v>35728000</v>
       </c>
     </row>
     <row r="128" spans="1:12">
@@ -5829,16 +6021,16 @@
         <v>187</v>
       </c>
       <c r="E128" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="F128" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="G128" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="H128" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="I128" t="s">
         <v>19</v>
@@ -5847,10 +6039,10 @@
         <v>1</v>
       </c>
       <c r="K128">
-        <v>450000</v>
+        <v>1800000</v>
       </c>
       <c r="L128">
-        <v>450000</v>
+        <v>1800000</v>
       </c>
     </row>
     <row r="129" spans="1:12">
@@ -5873,10 +6065,10 @@
         <v>226</v>
       </c>
       <c r="G129" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="H129" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I129" t="s">
         <v>19</v>
@@ -5885,10 +6077,10 @@
         <v>1</v>
       </c>
       <c r="K129">
-        <v>1200000</v>
+        <v>4800000</v>
       </c>
       <c r="L129">
-        <v>1200000</v>
+        <v>4800000</v>
       </c>
     </row>
     <row r="130" spans="1:12">
@@ -5911,10 +6103,10 @@
         <v>226</v>
       </c>
       <c r="G130" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="H130" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="I130" t="s">
         <v>19</v>
@@ -5923,10 +6115,10 @@
         <v>1</v>
       </c>
       <c r="K130">
-        <v>3600000</v>
+        <v>4070000</v>
       </c>
       <c r="L130">
-        <v>3600000</v>
+        <v>4070000</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -5949,10 +6141,10 @@
         <v>226</v>
       </c>
       <c r="G131" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="H131" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="I131" t="s">
         <v>19</v>
@@ -5961,10 +6153,10 @@
         <v>1</v>
       </c>
       <c r="K131">
-        <v>2960000</v>
+        <v>450000</v>
       </c>
       <c r="L131">
-        <v>2960000</v>
+        <v>450000</v>
       </c>
     </row>
     <row r="132" spans="1:12">
@@ -5981,16 +6173,16 @@
         <v>187</v>
       </c>
       <c r="E132" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="F132" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="G132" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="H132" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="I132" t="s">
         <v>19</v>
@@ -5999,10 +6191,1796 @@
         <v>1</v>
       </c>
       <c r="K132">
+        <v>1200000</v>
+      </c>
+      <c r="L132">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133">
+        <v>130</v>
+      </c>
+      <c r="B133">
+        <v>626402</v>
+      </c>
+      <c r="C133" t="s">
+        <v>13</v>
+      </c>
+      <c r="D133" t="s">
+        <v>187</v>
+      </c>
+      <c r="E133" t="s">
+        <v>232</v>
+      </c>
+      <c r="F133" t="s">
+        <v>233</v>
+      </c>
+      <c r="G133" t="s">
+        <v>227</v>
+      </c>
+      <c r="H133" t="s">
+        <v>235</v>
+      </c>
+      <c r="I133" t="s">
+        <v>19</v>
+      </c>
+      <c r="J133">
+        <v>1</v>
+      </c>
+      <c r="K133">
+        <v>3600000</v>
+      </c>
+      <c r="L133">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134">
+        <v>131</v>
+      </c>
+      <c r="B134">
+        <v>626402</v>
+      </c>
+      <c r="C134" t="s">
+        <v>13</v>
+      </c>
+      <c r="D134" t="s">
+        <v>187</v>
+      </c>
+      <c r="E134" t="s">
+        <v>232</v>
+      </c>
+      <c r="F134" t="s">
+        <v>233</v>
+      </c>
+      <c r="G134" t="s">
+        <v>227</v>
+      </c>
+      <c r="H134" t="s">
+        <v>236</v>
+      </c>
+      <c r="I134" t="s">
+        <v>19</v>
+      </c>
+      <c r="J134">
+        <v>1</v>
+      </c>
+      <c r="K134">
+        <v>2960000</v>
+      </c>
+      <c r="L134">
+        <v>2960000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="A135">
+        <v>132</v>
+      </c>
+      <c r="B135">
+        <v>626402</v>
+      </c>
+      <c r="C135" t="s">
+        <v>13</v>
+      </c>
+      <c r="D135" t="s">
+        <v>187</v>
+      </c>
+      <c r="E135" t="s">
+        <v>232</v>
+      </c>
+      <c r="F135" t="s">
+        <v>233</v>
+      </c>
+      <c r="G135" t="s">
+        <v>227</v>
+      </c>
+      <c r="H135" t="s">
+        <v>237</v>
+      </c>
+      <c r="I135" t="s">
+        <v>19</v>
+      </c>
+      <c r="J135">
+        <v>1</v>
+      </c>
+      <c r="K135">
         <v>300000</v>
       </c>
-      <c r="L132">
+      <c r="L135">
         <v>300000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136">
+        <v>133</v>
+      </c>
+      <c r="B136">
+        <v>626402</v>
+      </c>
+      <c r="C136" t="s">
+        <v>13</v>
+      </c>
+      <c r="D136" t="s">
+        <v>63</v>
+      </c>
+      <c r="E136" t="s">
+        <v>238</v>
+      </c>
+      <c r="F136" t="s">
+        <v>239</v>
+      </c>
+      <c r="G136" t="s">
+        <v>240</v>
+      </c>
+      <c r="H136" t="s">
+        <v>224</v>
+      </c>
+      <c r="I136" t="s">
+        <v>19</v>
+      </c>
+      <c r="J136">
+        <v>1</v>
+      </c>
+      <c r="K136">
+        <v>10208000</v>
+      </c>
+      <c r="L136">
+        <v>10208000</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="A137">
+        <v>134</v>
+      </c>
+      <c r="B137">
+        <v>626402</v>
+      </c>
+      <c r="C137" t="s">
+        <v>13</v>
+      </c>
+      <c r="D137" t="s">
+        <v>63</v>
+      </c>
+      <c r="E137" t="s">
+        <v>238</v>
+      </c>
+      <c r="F137" t="s">
+        <v>239</v>
+      </c>
+      <c r="G137" t="s">
+        <v>240</v>
+      </c>
+      <c r="H137" t="s">
+        <v>241</v>
+      </c>
+      <c r="I137" t="s">
+        <v>19</v>
+      </c>
+      <c r="J137">
+        <v>1</v>
+      </c>
+      <c r="K137">
+        <v>5615000</v>
+      </c>
+      <c r="L137">
+        <v>5615000</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
+      <c r="A138">
+        <v>135</v>
+      </c>
+      <c r="B138">
+        <v>626402</v>
+      </c>
+      <c r="C138" t="s">
+        <v>13</v>
+      </c>
+      <c r="D138" t="s">
+        <v>63</v>
+      </c>
+      <c r="E138" t="s">
+        <v>242</v>
+      </c>
+      <c r="F138" t="s">
+        <v>243</v>
+      </c>
+      <c r="G138" t="s">
+        <v>244</v>
+      </c>
+      <c r="H138" t="s">
+        <v>245</v>
+      </c>
+      <c r="I138" t="s">
+        <v>19</v>
+      </c>
+      <c r="J138">
+        <v>1</v>
+      </c>
+      <c r="K138">
+        <v>11866000</v>
+      </c>
+      <c r="L138">
+        <v>11866000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="A139">
+        <v>136</v>
+      </c>
+      <c r="B139">
+        <v>626402</v>
+      </c>
+      <c r="C139" t="s">
+        <v>13</v>
+      </c>
+      <c r="D139" t="s">
+        <v>63</v>
+      </c>
+      <c r="E139" t="s">
+        <v>242</v>
+      </c>
+      <c r="F139" t="s">
+        <v>243</v>
+      </c>
+      <c r="G139" t="s">
+        <v>244</v>
+      </c>
+      <c r="H139" t="s">
+        <v>246</v>
+      </c>
+      <c r="I139" t="s">
+        <v>19</v>
+      </c>
+      <c r="J139">
+        <v>1</v>
+      </c>
+      <c r="K139">
+        <v>150</v>
+      </c>
+      <c r="L139">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
+      <c r="A140">
+        <v>137</v>
+      </c>
+      <c r="B140">
+        <v>626402</v>
+      </c>
+      <c r="C140" t="s">
+        <v>13</v>
+      </c>
+      <c r="D140" t="s">
+        <v>63</v>
+      </c>
+      <c r="E140" t="s">
+        <v>242</v>
+      </c>
+      <c r="F140" t="s">
+        <v>243</v>
+      </c>
+      <c r="G140" t="s">
+        <v>244</v>
+      </c>
+      <c r="H140" t="s">
+        <v>247</v>
+      </c>
+      <c r="I140" t="s">
+        <v>19</v>
+      </c>
+      <c r="J140">
+        <v>1</v>
+      </c>
+      <c r="K140">
+        <v>593300</v>
+      </c>
+      <c r="L140">
+        <v>593300</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
+      <c r="A141">
+        <v>138</v>
+      </c>
+      <c r="B141">
+        <v>626402</v>
+      </c>
+      <c r="C141" t="s">
+        <v>13</v>
+      </c>
+      <c r="D141" t="s">
+        <v>63</v>
+      </c>
+      <c r="E141" t="s">
+        <v>242</v>
+      </c>
+      <c r="F141" t="s">
+        <v>243</v>
+      </c>
+      <c r="G141" t="s">
+        <v>244</v>
+      </c>
+      <c r="H141" t="s">
+        <v>248</v>
+      </c>
+      <c r="I141" t="s">
+        <v>19</v>
+      </c>
+      <c r="J141">
+        <v>1</v>
+      </c>
+      <c r="K141">
+        <v>237320</v>
+      </c>
+      <c r="L141">
+        <v>237320</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
+      <c r="A142">
+        <v>139</v>
+      </c>
+      <c r="B142">
+        <v>626402</v>
+      </c>
+      <c r="C142" t="s">
+        <v>13</v>
+      </c>
+      <c r="D142" t="s">
+        <v>63</v>
+      </c>
+      <c r="E142" t="s">
+        <v>242</v>
+      </c>
+      <c r="F142" t="s">
+        <v>243</v>
+      </c>
+      <c r="G142" t="s">
+        <v>244</v>
+      </c>
+      <c r="H142" t="s">
+        <v>249</v>
+      </c>
+      <c r="I142" t="s">
+        <v>19</v>
+      </c>
+      <c r="J142">
+        <v>1</v>
+      </c>
+      <c r="K142">
+        <v>2160000</v>
+      </c>
+      <c r="L142">
+        <v>2160000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
+      <c r="A143">
+        <v>140</v>
+      </c>
+      <c r="B143">
+        <v>626402</v>
+      </c>
+      <c r="C143" t="s">
+        <v>13</v>
+      </c>
+      <c r="D143" t="s">
+        <v>63</v>
+      </c>
+      <c r="E143" t="s">
+        <v>242</v>
+      </c>
+      <c r="F143" t="s">
+        <v>243</v>
+      </c>
+      <c r="G143" t="s">
+        <v>244</v>
+      </c>
+      <c r="H143" t="s">
+        <v>250</v>
+      </c>
+      <c r="I143" t="s">
+        <v>19</v>
+      </c>
+      <c r="J143">
+        <v>1</v>
+      </c>
+      <c r="K143">
+        <v>724200</v>
+      </c>
+      <c r="L143">
+        <v>724200</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
+      <c r="A144">
+        <v>141</v>
+      </c>
+      <c r="B144">
+        <v>626402</v>
+      </c>
+      <c r="C144" t="s">
+        <v>13</v>
+      </c>
+      <c r="D144" t="s">
+        <v>63</v>
+      </c>
+      <c r="E144" t="s">
+        <v>251</v>
+      </c>
+      <c r="F144" t="s">
+        <v>252</v>
+      </c>
+      <c r="G144" t="s">
+        <v>253</v>
+      </c>
+      <c r="H144" t="s">
+        <v>254</v>
+      </c>
+      <c r="I144" t="s">
+        <v>19</v>
+      </c>
+      <c r="J144">
+        <v>1</v>
+      </c>
+      <c r="K144">
+        <v>28290250</v>
+      </c>
+      <c r="L144">
+        <v>28290250</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12">
+      <c r="A145">
+        <v>142</v>
+      </c>
+      <c r="B145">
+        <v>626402</v>
+      </c>
+      <c r="C145" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145" t="s">
+        <v>63</v>
+      </c>
+      <c r="E145" t="s">
+        <v>251</v>
+      </c>
+      <c r="F145" t="s">
+        <v>252</v>
+      </c>
+      <c r="G145" t="s">
+        <v>253</v>
+      </c>
+      <c r="H145" t="s">
+        <v>255</v>
+      </c>
+      <c r="I145" t="s">
+        <v>19</v>
+      </c>
+      <c r="J145">
+        <v>1</v>
+      </c>
+      <c r="K145">
+        <v>490000</v>
+      </c>
+      <c r="L145">
+        <v>490000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12">
+      <c r="A146">
+        <v>143</v>
+      </c>
+      <c r="B146">
+        <v>626402</v>
+      </c>
+      <c r="C146" t="s">
+        <v>13</v>
+      </c>
+      <c r="D146" t="s">
+        <v>63</v>
+      </c>
+      <c r="E146" t="s">
+        <v>251</v>
+      </c>
+      <c r="F146" t="s">
+        <v>252</v>
+      </c>
+      <c r="G146" t="s">
+        <v>253</v>
+      </c>
+      <c r="H146" t="s">
+        <v>256</v>
+      </c>
+      <c r="I146" t="s">
+        <v>19</v>
+      </c>
+      <c r="J146">
+        <v>1</v>
+      </c>
+      <c r="K146">
+        <v>8486722</v>
+      </c>
+      <c r="L146">
+        <v>8486722</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
+      <c r="A147">
+        <v>144</v>
+      </c>
+      <c r="B147">
+        <v>626402</v>
+      </c>
+      <c r="C147" t="s">
+        <v>13</v>
+      </c>
+      <c r="D147" t="s">
+        <v>63</v>
+      </c>
+      <c r="E147" t="s">
+        <v>251</v>
+      </c>
+      <c r="F147" t="s">
+        <v>252</v>
+      </c>
+      <c r="G147" t="s">
+        <v>253</v>
+      </c>
+      <c r="H147" t="s">
+        <v>198</v>
+      </c>
+      <c r="I147" t="s">
+        <v>19</v>
+      </c>
+      <c r="J147">
+        <v>1</v>
+      </c>
+      <c r="K147">
+        <v>1630000</v>
+      </c>
+      <c r="L147">
+        <v>1630000</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
+      <c r="A148">
+        <v>145</v>
+      </c>
+      <c r="B148">
+        <v>626402</v>
+      </c>
+      <c r="C148" t="s">
+        <v>13</v>
+      </c>
+      <c r="D148" t="s">
+        <v>63</v>
+      </c>
+      <c r="E148" t="s">
+        <v>251</v>
+      </c>
+      <c r="F148" t="s">
+        <v>252</v>
+      </c>
+      <c r="G148" t="s">
+        <v>253</v>
+      </c>
+      <c r="H148" t="s">
+        <v>257</v>
+      </c>
+      <c r="I148" t="s">
+        <v>19</v>
+      </c>
+      <c r="J148">
+        <v>1</v>
+      </c>
+      <c r="K148">
+        <v>1130026</v>
+      </c>
+      <c r="L148">
+        <v>1130026</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
+      <c r="A149">
+        <v>146</v>
+      </c>
+      <c r="B149">
+        <v>626402</v>
+      </c>
+      <c r="C149" t="s">
+        <v>13</v>
+      </c>
+      <c r="D149" t="s">
+        <v>63</v>
+      </c>
+      <c r="E149" t="s">
+        <v>251</v>
+      </c>
+      <c r="F149" t="s">
+        <v>252</v>
+      </c>
+      <c r="G149" t="s">
+        <v>253</v>
+      </c>
+      <c r="H149" t="s">
+        <v>258</v>
+      </c>
+      <c r="I149" t="s">
+        <v>19</v>
+      </c>
+      <c r="J149">
+        <v>1</v>
+      </c>
+      <c r="K149">
+        <v>121284</v>
+      </c>
+      <c r="L149">
+        <v>121284</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
+      <c r="A150">
+        <v>147</v>
+      </c>
+      <c r="B150">
+        <v>626402</v>
+      </c>
+      <c r="C150" t="s">
+        <v>13</v>
+      </c>
+      <c r="D150" t="s">
+        <v>63</v>
+      </c>
+      <c r="E150" t="s">
+        <v>251</v>
+      </c>
+      <c r="F150" t="s">
+        <v>252</v>
+      </c>
+      <c r="G150" t="s">
+        <v>253</v>
+      </c>
+      <c r="H150" t="s">
+        <v>259</v>
+      </c>
+      <c r="I150" t="s">
+        <v>19</v>
+      </c>
+      <c r="J150">
+        <v>1</v>
+      </c>
+      <c r="K150">
+        <v>744936</v>
+      </c>
+      <c r="L150">
+        <v>744936</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
+      <c r="A151">
+        <v>148</v>
+      </c>
+      <c r="B151">
+        <v>626402</v>
+      </c>
+      <c r="C151" t="s">
+        <v>13</v>
+      </c>
+      <c r="D151" t="s">
+        <v>63</v>
+      </c>
+      <c r="E151" t="s">
+        <v>251</v>
+      </c>
+      <c r="F151" t="s">
+        <v>252</v>
+      </c>
+      <c r="G151" t="s">
+        <v>253</v>
+      </c>
+      <c r="H151" t="s">
+        <v>260</v>
+      </c>
+      <c r="I151" t="s">
+        <v>19</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+      <c r="K151">
+        <v>594000</v>
+      </c>
+      <c r="L151">
+        <v>594000</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12">
+      <c r="A152">
+        <v>149</v>
+      </c>
+      <c r="B152">
+        <v>626402</v>
+      </c>
+      <c r="C152" t="s">
+        <v>13</v>
+      </c>
+      <c r="D152" t="s">
+        <v>63</v>
+      </c>
+      <c r="E152" t="s">
+        <v>251</v>
+      </c>
+      <c r="F152" t="s">
+        <v>252</v>
+      </c>
+      <c r="G152" t="s">
+        <v>253</v>
+      </c>
+      <c r="H152" t="s">
+        <v>261</v>
+      </c>
+      <c r="I152" t="s">
+        <v>19</v>
+      </c>
+      <c r="J152">
+        <v>1</v>
+      </c>
+      <c r="K152">
+        <v>24000</v>
+      </c>
+      <c r="L152">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
+      <c r="A153">
+        <v>150</v>
+      </c>
+      <c r="B153">
+        <v>626402</v>
+      </c>
+      <c r="C153" t="s">
+        <v>13</v>
+      </c>
+      <c r="D153" t="s">
+        <v>63</v>
+      </c>
+      <c r="E153" t="s">
+        <v>251</v>
+      </c>
+      <c r="F153" t="s">
+        <v>252</v>
+      </c>
+      <c r="G153" t="s">
+        <v>253</v>
+      </c>
+      <c r="H153" t="s">
+        <v>262</v>
+      </c>
+      <c r="I153" t="s">
+        <v>19</v>
+      </c>
+      <c r="J153">
+        <v>1</v>
+      </c>
+      <c r="K153">
+        <v>402280</v>
+      </c>
+      <c r="L153">
+        <v>402280</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
+      <c r="A154">
+        <v>151</v>
+      </c>
+      <c r="B154">
+        <v>626402</v>
+      </c>
+      <c r="C154" t="s">
+        <v>13</v>
+      </c>
+      <c r="D154" t="s">
+        <v>63</v>
+      </c>
+      <c r="E154" t="s">
+        <v>251</v>
+      </c>
+      <c r="F154" t="s">
+        <v>252</v>
+      </c>
+      <c r="G154" t="s">
+        <v>253</v>
+      </c>
+      <c r="H154" t="s">
+        <v>263</v>
+      </c>
+      <c r="I154" t="s">
+        <v>19</v>
+      </c>
+      <c r="J154">
+        <v>1</v>
+      </c>
+      <c r="K154">
+        <v>215400</v>
+      </c>
+      <c r="L154">
+        <v>215400</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12">
+      <c r="A155">
+        <v>152</v>
+      </c>
+      <c r="B155">
+        <v>626402</v>
+      </c>
+      <c r="C155" t="s">
+        <v>13</v>
+      </c>
+      <c r="D155" t="s">
+        <v>63</v>
+      </c>
+      <c r="E155" t="s">
+        <v>251</v>
+      </c>
+      <c r="F155" t="s">
+        <v>252</v>
+      </c>
+      <c r="G155" t="s">
+        <v>253</v>
+      </c>
+      <c r="H155" t="s">
+        <v>264</v>
+      </c>
+      <c r="I155" t="s">
+        <v>19</v>
+      </c>
+      <c r="J155">
+        <v>1</v>
+      </c>
+      <c r="K155">
+        <v>977500</v>
+      </c>
+      <c r="L155">
+        <v>977500</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
+      <c r="A156">
+        <v>153</v>
+      </c>
+      <c r="B156">
+        <v>626402</v>
+      </c>
+      <c r="C156" t="s">
+        <v>13</v>
+      </c>
+      <c r="D156" t="s">
+        <v>63</v>
+      </c>
+      <c r="E156" t="s">
+        <v>251</v>
+      </c>
+      <c r="F156" t="s">
+        <v>252</v>
+      </c>
+      <c r="G156" t="s">
+        <v>253</v>
+      </c>
+      <c r="H156" t="s">
+        <v>265</v>
+      </c>
+      <c r="I156" t="s">
+        <v>19</v>
+      </c>
+      <c r="J156">
+        <v>1</v>
+      </c>
+      <c r="K156">
+        <v>930800</v>
+      </c>
+      <c r="L156">
+        <v>930800</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
+      <c r="A157">
+        <v>154</v>
+      </c>
+      <c r="B157">
+        <v>626402</v>
+      </c>
+      <c r="C157" t="s">
+        <v>13</v>
+      </c>
+      <c r="D157" t="s">
+        <v>63</v>
+      </c>
+      <c r="E157" t="s">
+        <v>251</v>
+      </c>
+      <c r="F157" t="s">
+        <v>252</v>
+      </c>
+      <c r="G157" t="s">
+        <v>253</v>
+      </c>
+      <c r="H157" t="s">
+        <v>266</v>
+      </c>
+      <c r="I157" t="s">
+        <v>19</v>
+      </c>
+      <c r="J157">
+        <v>1</v>
+      </c>
+      <c r="K157">
+        <v>1713000</v>
+      </c>
+      <c r="L157">
+        <v>1713000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12">
+      <c r="A158">
+        <v>155</v>
+      </c>
+      <c r="B158">
+        <v>626402</v>
+      </c>
+      <c r="C158" t="s">
+        <v>13</v>
+      </c>
+      <c r="D158" t="s">
+        <v>63</v>
+      </c>
+      <c r="E158" t="s">
+        <v>251</v>
+      </c>
+      <c r="F158" t="s">
+        <v>252</v>
+      </c>
+      <c r="G158" t="s">
+        <v>253</v>
+      </c>
+      <c r="H158" t="s">
+        <v>267</v>
+      </c>
+      <c r="I158" t="s">
+        <v>19</v>
+      </c>
+      <c r="J158">
+        <v>1</v>
+      </c>
+      <c r="K158">
+        <v>1400000</v>
+      </c>
+      <c r="L158">
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
+      <c r="A159">
+        <v>156</v>
+      </c>
+      <c r="B159">
+        <v>626402</v>
+      </c>
+      <c r="C159" t="s">
+        <v>13</v>
+      </c>
+      <c r="D159" t="s">
+        <v>63</v>
+      </c>
+      <c r="E159" t="s">
+        <v>251</v>
+      </c>
+      <c r="F159" t="s">
+        <v>252</v>
+      </c>
+      <c r="G159" t="s">
+        <v>253</v>
+      </c>
+      <c r="H159" t="s">
+        <v>122</v>
+      </c>
+      <c r="I159" t="s">
+        <v>19</v>
+      </c>
+      <c r="J159">
+        <v>1</v>
+      </c>
+      <c r="K159">
+        <v>571650</v>
+      </c>
+      <c r="L159">
+        <v>571650</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12">
+      <c r="A160">
+        <v>157</v>
+      </c>
+      <c r="B160">
+        <v>626402</v>
+      </c>
+      <c r="C160" t="s">
+        <v>13</v>
+      </c>
+      <c r="D160" t="s">
+        <v>63</v>
+      </c>
+      <c r="E160" t="s">
+        <v>251</v>
+      </c>
+      <c r="F160" t="s">
+        <v>252</v>
+      </c>
+      <c r="G160" t="s">
+        <v>253</v>
+      </c>
+      <c r="H160" t="s">
+        <v>268</v>
+      </c>
+      <c r="I160" t="s">
+        <v>19</v>
+      </c>
+      <c r="J160">
+        <v>1</v>
+      </c>
+      <c r="K160">
+        <v>624736</v>
+      </c>
+      <c r="L160">
+        <v>624736</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12">
+      <c r="A161">
+        <v>158</v>
+      </c>
+      <c r="B161">
+        <v>626402</v>
+      </c>
+      <c r="C161" t="s">
+        <v>13</v>
+      </c>
+      <c r="D161" t="s">
+        <v>63</v>
+      </c>
+      <c r="E161" t="s">
+        <v>251</v>
+      </c>
+      <c r="F161" t="s">
+        <v>252</v>
+      </c>
+      <c r="G161" t="s">
+        <v>253</v>
+      </c>
+      <c r="H161" t="s">
+        <v>269</v>
+      </c>
+      <c r="I161" t="s">
+        <v>19</v>
+      </c>
+      <c r="J161">
+        <v>1</v>
+      </c>
+      <c r="K161">
+        <v>288800</v>
+      </c>
+      <c r="L161">
+        <v>288800</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12">
+      <c r="A162">
+        <v>159</v>
+      </c>
+      <c r="B162">
+        <v>626402</v>
+      </c>
+      <c r="C162" t="s">
+        <v>13</v>
+      </c>
+      <c r="D162" t="s">
+        <v>63</v>
+      </c>
+      <c r="E162" t="s">
+        <v>251</v>
+      </c>
+      <c r="F162" t="s">
+        <v>252</v>
+      </c>
+      <c r="G162" t="s">
+        <v>253</v>
+      </c>
+      <c r="H162" t="s">
+        <v>270</v>
+      </c>
+      <c r="I162" t="s">
+        <v>19</v>
+      </c>
+      <c r="J162">
+        <v>1</v>
+      </c>
+      <c r="K162">
+        <v>2200000</v>
+      </c>
+      <c r="L162">
+        <v>2200000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12">
+      <c r="A163">
+        <v>160</v>
+      </c>
+      <c r="B163">
+        <v>626402</v>
+      </c>
+      <c r="C163" t="s">
+        <v>13</v>
+      </c>
+      <c r="D163" t="s">
+        <v>63</v>
+      </c>
+      <c r="E163" t="s">
+        <v>251</v>
+      </c>
+      <c r="F163" t="s">
+        <v>252</v>
+      </c>
+      <c r="G163" t="s">
+        <v>253</v>
+      </c>
+      <c r="H163" t="s">
+        <v>131</v>
+      </c>
+      <c r="I163" t="s">
+        <v>19</v>
+      </c>
+      <c r="J163">
+        <v>1</v>
+      </c>
+      <c r="K163">
+        <v>2432400</v>
+      </c>
+      <c r="L163">
+        <v>2432400</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12">
+      <c r="A164">
+        <v>161</v>
+      </c>
+      <c r="B164">
+        <v>626402</v>
+      </c>
+      <c r="C164" t="s">
+        <v>13</v>
+      </c>
+      <c r="D164" t="s">
+        <v>63</v>
+      </c>
+      <c r="E164" t="s">
+        <v>251</v>
+      </c>
+      <c r="F164" t="s">
+        <v>252</v>
+      </c>
+      <c r="G164" t="s">
+        <v>253</v>
+      </c>
+      <c r="H164" t="s">
+        <v>271</v>
+      </c>
+      <c r="I164" t="s">
+        <v>19</v>
+      </c>
+      <c r="J164">
+        <v>1</v>
+      </c>
+      <c r="K164">
+        <v>1676236</v>
+      </c>
+      <c r="L164">
+        <v>1676236</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12">
+      <c r="A165">
+        <v>162</v>
+      </c>
+      <c r="B165">
+        <v>626402</v>
+      </c>
+      <c r="C165" t="s">
+        <v>13</v>
+      </c>
+      <c r="D165" t="s">
+        <v>63</v>
+      </c>
+      <c r="E165" t="s">
+        <v>251</v>
+      </c>
+      <c r="F165" t="s">
+        <v>252</v>
+      </c>
+      <c r="G165" t="s">
+        <v>253</v>
+      </c>
+      <c r="H165" t="s">
+        <v>272</v>
+      </c>
+      <c r="I165" t="s">
+        <v>19</v>
+      </c>
+      <c r="J165">
+        <v>1</v>
+      </c>
+      <c r="K165">
+        <v>12905381</v>
+      </c>
+      <c r="L165">
+        <v>12905381</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12">
+      <c r="A166">
+        <v>163</v>
+      </c>
+      <c r="B166">
+        <v>626402</v>
+      </c>
+      <c r="C166" t="s">
+        <v>13</v>
+      </c>
+      <c r="D166" t="s">
+        <v>63</v>
+      </c>
+      <c r="E166" t="s">
+        <v>251</v>
+      </c>
+      <c r="F166" t="s">
+        <v>252</v>
+      </c>
+      <c r="G166" t="s">
+        <v>253</v>
+      </c>
+      <c r="H166" t="s">
+        <v>148</v>
+      </c>
+      <c r="I166" t="s">
+        <v>19</v>
+      </c>
+      <c r="J166">
+        <v>1</v>
+      </c>
+      <c r="K166">
+        <v>1600500</v>
+      </c>
+      <c r="L166">
+        <v>1600500</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12">
+      <c r="A167">
+        <v>164</v>
+      </c>
+      <c r="B167">
+        <v>626402</v>
+      </c>
+      <c r="C167" t="s">
+        <v>13</v>
+      </c>
+      <c r="D167" t="s">
+        <v>63</v>
+      </c>
+      <c r="E167" t="s">
+        <v>251</v>
+      </c>
+      <c r="F167" t="s">
+        <v>252</v>
+      </c>
+      <c r="G167" t="s">
+        <v>253</v>
+      </c>
+      <c r="H167" t="s">
+        <v>128</v>
+      </c>
+      <c r="I167" t="s">
+        <v>19</v>
+      </c>
+      <c r="J167">
+        <v>1</v>
+      </c>
+      <c r="K167">
+        <v>5495500</v>
+      </c>
+      <c r="L167">
+        <v>5495500</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12">
+      <c r="A168">
+        <v>165</v>
+      </c>
+      <c r="B168">
+        <v>626402</v>
+      </c>
+      <c r="C168" t="s">
+        <v>13</v>
+      </c>
+      <c r="D168" t="s">
+        <v>63</v>
+      </c>
+      <c r="E168" t="s">
+        <v>251</v>
+      </c>
+      <c r="F168" t="s">
+        <v>252</v>
+      </c>
+      <c r="G168" t="s">
+        <v>253</v>
+      </c>
+      <c r="H168" t="s">
+        <v>273</v>
+      </c>
+      <c r="I168" t="s">
+        <v>19</v>
+      </c>
+      <c r="J168">
+        <v>1</v>
+      </c>
+      <c r="K168">
+        <v>600000</v>
+      </c>
+      <c r="L168">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12">
+      <c r="A169">
+        <v>166</v>
+      </c>
+      <c r="B169">
+        <v>626402</v>
+      </c>
+      <c r="C169" t="s">
+        <v>13</v>
+      </c>
+      <c r="D169" t="s">
+        <v>63</v>
+      </c>
+      <c r="E169" t="s">
+        <v>251</v>
+      </c>
+      <c r="F169" t="s">
+        <v>252</v>
+      </c>
+      <c r="G169" t="s">
+        <v>253</v>
+      </c>
+      <c r="H169" t="s">
+        <v>274</v>
+      </c>
+      <c r="I169" t="s">
+        <v>19</v>
+      </c>
+      <c r="J169">
+        <v>1</v>
+      </c>
+      <c r="K169">
+        <v>2090000</v>
+      </c>
+      <c r="L169">
+        <v>2090000</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12">
+      <c r="A170">
+        <v>167</v>
+      </c>
+      <c r="B170">
+        <v>626402</v>
+      </c>
+      <c r="C170" t="s">
+        <v>13</v>
+      </c>
+      <c r="D170" t="s">
+        <v>63</v>
+      </c>
+      <c r="E170" t="s">
+        <v>251</v>
+      </c>
+      <c r="F170" t="s">
+        <v>252</v>
+      </c>
+      <c r="G170" t="s">
+        <v>253</v>
+      </c>
+      <c r="H170" t="s">
+        <v>182</v>
+      </c>
+      <c r="I170" t="s">
+        <v>19</v>
+      </c>
+      <c r="J170">
+        <v>1</v>
+      </c>
+      <c r="K170">
+        <v>9495062</v>
+      </c>
+      <c r="L170">
+        <v>9495062</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12">
+      <c r="A171">
+        <v>168</v>
+      </c>
+      <c r="B171">
+        <v>626402</v>
+      </c>
+      <c r="C171" t="s">
+        <v>13</v>
+      </c>
+      <c r="D171" t="s">
+        <v>63</v>
+      </c>
+      <c r="E171" t="s">
+        <v>251</v>
+      </c>
+      <c r="F171" t="s">
+        <v>252</v>
+      </c>
+      <c r="G171" t="s">
+        <v>253</v>
+      </c>
+      <c r="H171" t="s">
+        <v>275</v>
+      </c>
+      <c r="I171" t="s">
+        <v>19</v>
+      </c>
+      <c r="J171">
+        <v>1</v>
+      </c>
+      <c r="K171">
+        <v>320000</v>
+      </c>
+      <c r="L171">
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12">
+      <c r="A172">
+        <v>169</v>
+      </c>
+      <c r="B172">
+        <v>626402</v>
+      </c>
+      <c r="C172" t="s">
+        <v>13</v>
+      </c>
+      <c r="D172" t="s">
+        <v>63</v>
+      </c>
+      <c r="E172" t="s">
+        <v>251</v>
+      </c>
+      <c r="F172" t="s">
+        <v>252</v>
+      </c>
+      <c r="G172" t="s">
+        <v>253</v>
+      </c>
+      <c r="H172" t="s">
+        <v>276</v>
+      </c>
+      <c r="I172" t="s">
+        <v>19</v>
+      </c>
+      <c r="J172">
+        <v>1</v>
+      </c>
+      <c r="K172">
+        <v>260000</v>
+      </c>
+      <c r="L172">
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12">
+      <c r="A173">
+        <v>170</v>
+      </c>
+      <c r="B173">
+        <v>626402</v>
+      </c>
+      <c r="C173" t="s">
+        <v>13</v>
+      </c>
+      <c r="D173" t="s">
+        <v>63</v>
+      </c>
+      <c r="E173" t="s">
+        <v>251</v>
+      </c>
+      <c r="F173" t="s">
+        <v>252</v>
+      </c>
+      <c r="G173" t="s">
+        <v>253</v>
+      </c>
+      <c r="H173" t="s">
+        <v>277</v>
+      </c>
+      <c r="I173" t="s">
+        <v>19</v>
+      </c>
+      <c r="J173">
+        <v>1</v>
+      </c>
+      <c r="K173">
+        <v>390000</v>
+      </c>
+      <c r="L173">
+        <v>390000</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12">
+      <c r="A174">
+        <v>171</v>
+      </c>
+      <c r="B174">
+        <v>626402</v>
+      </c>
+      <c r="C174" t="s">
+        <v>13</v>
+      </c>
+      <c r="D174" t="s">
+        <v>63</v>
+      </c>
+      <c r="E174" t="s">
+        <v>251</v>
+      </c>
+      <c r="F174" t="s">
+        <v>252</v>
+      </c>
+      <c r="G174" t="s">
+        <v>253</v>
+      </c>
+      <c r="H174" t="s">
+        <v>278</v>
+      </c>
+      <c r="I174" t="s">
+        <v>19</v>
+      </c>
+      <c r="J174">
+        <v>1</v>
+      </c>
+      <c r="K174">
+        <v>450000</v>
+      </c>
+      <c r="L174">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12">
+      <c r="A175">
+        <v>172</v>
+      </c>
+      <c r="B175">
+        <v>626402</v>
+      </c>
+      <c r="C175" t="s">
+        <v>13</v>
+      </c>
+      <c r="D175" t="s">
+        <v>279</v>
+      </c>
+      <c r="E175" t="s">
+        <v>280</v>
+      </c>
+      <c r="F175" t="s">
+        <v>281</v>
+      </c>
+      <c r="G175" t="s">
+        <v>282</v>
+      </c>
+      <c r="H175" t="s">
+        <v>283</v>
+      </c>
+      <c r="I175" t="s">
+        <v>19</v>
+      </c>
+      <c r="J175">
+        <v>1</v>
+      </c>
+      <c r="K175">
+        <v>7440500</v>
+      </c>
+      <c r="L175">
+        <v>7440500</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12">
+      <c r="A176">
+        <v>173</v>
+      </c>
+      <c r="B176">
+        <v>626402</v>
+      </c>
+      <c r="C176" t="s">
+        <v>13</v>
+      </c>
+      <c r="D176" t="s">
+        <v>279</v>
+      </c>
+      <c r="E176" t="s">
+        <v>284</v>
+      </c>
+      <c r="F176" t="s">
+        <v>285</v>
+      </c>
+      <c r="G176" t="s">
+        <v>286</v>
+      </c>
+      <c r="H176" t="s">
+        <v>274</v>
+      </c>
+      <c r="I176" t="s">
+        <v>19</v>
+      </c>
+      <c r="J176">
+        <v>1</v>
+      </c>
+      <c r="K176">
+        <v>12092580</v>
+      </c>
+      <c r="L176">
+        <v>12092580</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12">
+      <c r="A177">
+        <v>174</v>
+      </c>
+      <c r="B177">
+        <v>626402</v>
+      </c>
+      <c r="C177" t="s">
+        <v>13</v>
+      </c>
+      <c r="D177" t="s">
+        <v>279</v>
+      </c>
+      <c r="E177" t="s">
+        <v>287</v>
+      </c>
+      <c r="F177" t="s">
+        <v>288</v>
+      </c>
+      <c r="G177" t="s">
+        <v>289</v>
+      </c>
+      <c r="H177" t="s">
+        <v>290</v>
+      </c>
+      <c r="I177" t="s">
+        <v>19</v>
+      </c>
+      <c r="J177">
+        <v>1</v>
+      </c>
+      <c r="K177">
+        <v>1560000</v>
+      </c>
+      <c r="L177">
+        <v>1560000</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12">
+      <c r="A178">
+        <v>175</v>
+      </c>
+      <c r="B178">
+        <v>626402</v>
+      </c>
+      <c r="C178" t="s">
+        <v>13</v>
+      </c>
+      <c r="D178" t="s">
+        <v>279</v>
+      </c>
+      <c r="E178" t="s">
+        <v>287</v>
+      </c>
+      <c r="F178" t="s">
+        <v>288</v>
+      </c>
+      <c r="G178" t="s">
+        <v>289</v>
+      </c>
+      <c r="H178" t="s">
+        <v>291</v>
+      </c>
+      <c r="I178" t="s">
+        <v>19</v>
+      </c>
+      <c r="J178">
+        <v>1</v>
+      </c>
+      <c r="K178">
+        <v>2040000</v>
+      </c>
+      <c r="L178">
+        <v>2040000</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12">
+      <c r="A179">
+        <v>176</v>
+      </c>
+      <c r="B179">
+        <v>626402</v>
+      </c>
+      <c r="C179" t="s">
+        <v>13</v>
+      </c>
+      <c r="D179" t="s">
+        <v>279</v>
+      </c>
+      <c r="E179" t="s">
+        <v>292</v>
+      </c>
+      <c r="F179" t="s">
+        <v>293</v>
+      </c>
+      <c r="G179" t="s">
+        <v>294</v>
+      </c>
+      <c r="H179" t="s">
+        <v>274</v>
+      </c>
+      <c r="I179" t="s">
+        <v>19</v>
+      </c>
+      <c r="J179">
+        <v>1</v>
+      </c>
+      <c r="K179">
+        <v>1410000</v>
+      </c>
+      <c r="L179">
+        <v>1410000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Realisasi 13 Feb (3,56%)
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="376">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -900,6 +900,249 @@
   </si>
   <si>
     <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.829/BPPSDM.1/KP.440/I/2024 Tanggal 26 Januari 2024 a.n Rizky Hendriansyah, dkk</t>
+  </si>
+  <si>
+    <t>2024-02-06</t>
+  </si>
+  <si>
+    <t>'00063T</t>
+  </si>
+  <si>
+    <t>'241751303001087</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barangberupa biaya perjadin sesuai STNo.B.309,B.356,B.729/BPPSDM.1/KP.440/I/2024 Tanggal 15,16 dan 19 Januari 2024 a.n Achmad Irfansyah, dkk</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.957.101.0A.000311</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.957.101.0B.000322</t>
+  </si>
+  <si>
+    <t>'626402.175.524113.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.957.101.0B.000323</t>
+  </si>
+  <si>
+    <t>'626402.175.524113.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.957.101.0B.000324</t>
+  </si>
+  <si>
+    <t>'00064T</t>
+  </si>
+  <si>
+    <t>'241751303001088</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.206,B.261,B.278,B.704/BRSDM.1/KP.440/I/2023 Tgl.9,11,12,17 Januari 2024 Perjadin an.Andriawan Doni Purnama,DKK.</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.962.101.0A.000602</t>
+  </si>
+  <si>
+    <t>'00065T</t>
+  </si>
+  <si>
+    <t>'241751303001091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.49,B.258/BRSDM.1/KP.440/I/2024 Tgl.9,11 Januari 2024 Perjadin an.Rudi Alek Wahyudin, DKK. </t>
+  </si>
+  <si>
+    <t>'00066T</t>
+  </si>
+  <si>
+    <t>'241751303001092</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.235, B.698, B.728/BPPSDM.1/KP.440/I/2024 Tanggal 10, 17 dan 19 Januari 2024 a.n Niken Financia</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0D.000941</t>
+  </si>
+  <si>
+    <t>'00067T</t>
+  </si>
+  <si>
+    <t>'241751303001093</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.342/BRSDM.1/KP.440/I/2024 Tgl.16 Januari 2024 Perjadin an.Wawan Nurliansyah,DKK.</t>
+  </si>
+  <si>
+    <t>'00068T</t>
+  </si>
+  <si>
+    <t>'241751303001094</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.158, B.297 /BPPSDM.1/KP.440/I/2024 Tanggal 8 dan 15 Januari 2024 a.n Nurkholis Abellian, dkk</t>
+  </si>
+  <si>
+    <t>'00069T</t>
+  </si>
+  <si>
+    <t>'241751303001095</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.263, B.728/BPPSDM.1/KP.440/I/2024 Tanggal 10 dan 19 Januari 2024 a.n Setyawati, dkk</t>
+  </si>
+  <si>
+    <t>'00070T</t>
+  </si>
+  <si>
+    <t>'241751303001086</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.311/BPPSDM.1/KP.440/I/2024 Tanggal 15 Januari 2024 a.n Rudi Alek Wahyudin, dkk</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0D.000943</t>
+  </si>
+  <si>
+    <t>'00071T</t>
+  </si>
+  <si>
+    <t>'241751301001456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Kuitansi Nomor:042/NNI/I/24 Tgl.29 Januari 2024 </t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000425</t>
+  </si>
+  <si>
+    <t>'00072T</t>
+  </si>
+  <si>
+    <t>'241751301001452</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:011/PO-Sales/Kompas.com/I/2024 tgl.29 Januari 2024</t>
+  </si>
+  <si>
+    <t>2024-02-07</t>
+  </si>
+  <si>
+    <t>'00073T</t>
+  </si>
+  <si>
+    <t>'241751301001568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang-Sesuai SPK No:1230/SPK/PPBJ/BPPSDM.5/XII/2023 Tgl.29-12-2023,BAST No:BAST.1231/PPBJ.PL/BPPSDM.5/I/2024.Tgl.31-1-2024,BAP No:1231/PPBJ.PL/BPPSDM.5/II/2024 Tgl.01-02-2024.Pembayaran Bulan Januari 2024  </t>
+  </si>
+  <si>
+    <t>'626402.175.522191.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.DA.000539</t>
+  </si>
+  <si>
+    <t>'00074T</t>
+  </si>
+  <si>
+    <t>'241751302001394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang-Sesuai SPK No:1220/SPK/PPBJ/BPPSDM.5/XII/2023 Tgl.29-12-2023,BAST No:BAST.1221/PPBJ.PL/BPPSDM.5/I/2024.Tgl.31-1-2024,BAP No:1221/PPBJ.PL/BPPSDM.5/II/2024 Tgl.01-02-2024.Pembayaran Bulan Januari 2024 </t>
+  </si>
+  <si>
+    <t>'626402.175.522191.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.DA.000540</t>
+  </si>
+  <si>
+    <t>'00075T</t>
+  </si>
+  <si>
+    <t>'241751302001395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang-Sesuai SPK No:1210/SPK/PPBJ/BPPSDM.5/XII/2023 Tgl.29-12-2023,BAST No:BAST.1211/PPBJ.PL/BPPSDM.5/I/2024.Tgl.31-1-2024,BAP No:1211/PPBJ.PL/BPPSDM.5/II/2024 Tgl.01-02-2024.Pembayaran Bulan Januari 2024 </t>
+  </si>
+  <si>
+    <t>2024-02-12</t>
+  </si>
+  <si>
+    <t>'00076T</t>
+  </si>
+  <si>
+    <t>'241751302001665</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:021/KW-AH/I/2024 Tanggal 30 Januari 2024</t>
+  </si>
+  <si>
+    <t>'00077T</t>
+  </si>
+  <si>
+    <t>'241751303001168</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.271/BPPSDM.1/KP.440/I/2024 Tgl. 12 Januari 2024 Perjadin an.Ollyvia Maria Christy, DKK.</t>
+  </si>
+  <si>
+    <t>'00078T</t>
+  </si>
+  <si>
+    <t>'241751303001420</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0F.001423</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0B.001473</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0D.001478</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0D.001479</t>
+  </si>
+  <si>
+    <t>'00083T</t>
+  </si>
+  <si>
+    <t>'241751303001234</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No. B.135,B.277,B.332,B.688,B.712/BPPSDM.1/KP.440/I/2024 Tanggal 4,12,16,17, dan 18 Januari 2024 a.n Hari Purwanto, dkk</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.960.101.0A.000788</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.960.102.0A.000805</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.103.0A.000860</t>
+  </si>
+  <si>
+    <t>'00085T</t>
+  </si>
+  <si>
+    <t>'241751303001528</t>
+  </si>
+  <si>
+    <t>Pembayaran tunjangan kinerja susulan Pusluh bulan Januari tahun 2024 untuk 33 Pegawai/Anggota Polri/Prajurit TNI.</t>
+  </si>
+  <si>
+    <t>'626402.175.512411.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.DA.000410</t>
+  </si>
+  <si>
+    <t>'00086T</t>
+  </si>
+  <si>
+    <t>'241751303001563</t>
+  </si>
+  <si>
+    <t>Pembayaran tunjangan kinerja susulan Pegawai Sekretariat BRSDM bulan Januari tahun 2024 untuk 74 Pegawai/Anggota Polri/Prajurit TNI.</t>
+  </si>
+  <si>
+    <t>'626402.175.512411.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.AA.000399</t>
+  </si>
+  <si>
+    <t>'00087T</t>
+  </si>
+  <si>
+    <t>'241751303001562</t>
+  </si>
+  <si>
+    <t>Pembayaran tunjangan kinerja susulan bulan Januari tahun 2024 untuk 40 Pegawai/Anggota Polri/Prajurit TNI (Pusdik KP)</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1484,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L179"/>
+  <dimension ref="A1:L209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -7981,6 +8224,1146 @@
       </c>
       <c r="L179">
         <v>1410000</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12">
+      <c r="A180">
+        <v>177</v>
+      </c>
+      <c r="B180">
+        <v>626402</v>
+      </c>
+      <c r="C180" t="s">
+        <v>13</v>
+      </c>
+      <c r="D180" t="s">
+        <v>295</v>
+      </c>
+      <c r="E180" t="s">
+        <v>296</v>
+      </c>
+      <c r="F180" t="s">
+        <v>297</v>
+      </c>
+      <c r="G180" t="s">
+        <v>298</v>
+      </c>
+      <c r="H180" t="s">
+        <v>299</v>
+      </c>
+      <c r="I180" t="s">
+        <v>19</v>
+      </c>
+      <c r="J180">
+        <v>1</v>
+      </c>
+      <c r="K180">
+        <v>2316500</v>
+      </c>
+      <c r="L180">
+        <v>2316500</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12">
+      <c r="A181">
+        <v>178</v>
+      </c>
+      <c r="B181">
+        <v>626402</v>
+      </c>
+      <c r="C181" t="s">
+        <v>13</v>
+      </c>
+      <c r="D181" t="s">
+        <v>295</v>
+      </c>
+      <c r="E181" t="s">
+        <v>296</v>
+      </c>
+      <c r="F181" t="s">
+        <v>297</v>
+      </c>
+      <c r="G181" t="s">
+        <v>298</v>
+      </c>
+      <c r="H181" t="s">
+        <v>300</v>
+      </c>
+      <c r="I181" t="s">
+        <v>19</v>
+      </c>
+      <c r="J181">
+        <v>1</v>
+      </c>
+      <c r="K181">
+        <v>1205000</v>
+      </c>
+      <c r="L181">
+        <v>1205000</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12">
+      <c r="A182">
+        <v>179</v>
+      </c>
+      <c r="B182">
+        <v>626402</v>
+      </c>
+      <c r="C182" t="s">
+        <v>13</v>
+      </c>
+      <c r="D182" t="s">
+        <v>295</v>
+      </c>
+      <c r="E182" t="s">
+        <v>296</v>
+      </c>
+      <c r="F182" t="s">
+        <v>297</v>
+      </c>
+      <c r="G182" t="s">
+        <v>298</v>
+      </c>
+      <c r="H182" t="s">
+        <v>301</v>
+      </c>
+      <c r="I182" t="s">
+        <v>19</v>
+      </c>
+      <c r="J182">
+        <v>1</v>
+      </c>
+      <c r="K182">
+        <v>630000</v>
+      </c>
+      <c r="L182">
+        <v>630000</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12">
+      <c r="A183">
+        <v>180</v>
+      </c>
+      <c r="B183">
+        <v>626402</v>
+      </c>
+      <c r="C183" t="s">
+        <v>13</v>
+      </c>
+      <c r="D183" t="s">
+        <v>295</v>
+      </c>
+      <c r="E183" t="s">
+        <v>296</v>
+      </c>
+      <c r="F183" t="s">
+        <v>297</v>
+      </c>
+      <c r="G183" t="s">
+        <v>298</v>
+      </c>
+      <c r="H183" t="s">
+        <v>302</v>
+      </c>
+      <c r="I183" t="s">
+        <v>19</v>
+      </c>
+      <c r="J183">
+        <v>1</v>
+      </c>
+      <c r="K183">
+        <v>510000</v>
+      </c>
+      <c r="L183">
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12">
+      <c r="A184">
+        <v>181</v>
+      </c>
+      <c r="B184">
+        <v>626402</v>
+      </c>
+      <c r="C184" t="s">
+        <v>13</v>
+      </c>
+      <c r="D184" t="s">
+        <v>295</v>
+      </c>
+      <c r="E184" t="s">
+        <v>303</v>
+      </c>
+      <c r="F184" t="s">
+        <v>304</v>
+      </c>
+      <c r="G184" t="s">
+        <v>305</v>
+      </c>
+      <c r="H184" t="s">
+        <v>306</v>
+      </c>
+      <c r="I184" t="s">
+        <v>19</v>
+      </c>
+      <c r="J184">
+        <v>1</v>
+      </c>
+      <c r="K184">
+        <v>1700000</v>
+      </c>
+      <c r="L184">
+        <v>1700000</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12">
+      <c r="A185">
+        <v>182</v>
+      </c>
+      <c r="B185">
+        <v>626402</v>
+      </c>
+      <c r="C185" t="s">
+        <v>13</v>
+      </c>
+      <c r="D185" t="s">
+        <v>295</v>
+      </c>
+      <c r="E185" t="s">
+        <v>307</v>
+      </c>
+      <c r="F185" t="s">
+        <v>308</v>
+      </c>
+      <c r="G185" t="s">
+        <v>309</v>
+      </c>
+      <c r="H185" t="s">
+        <v>274</v>
+      </c>
+      <c r="I185" t="s">
+        <v>19</v>
+      </c>
+      <c r="J185">
+        <v>1</v>
+      </c>
+      <c r="K185">
+        <v>5907000</v>
+      </c>
+      <c r="L185">
+        <v>5907000</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12">
+      <c r="A186">
+        <v>183</v>
+      </c>
+      <c r="B186">
+        <v>626402</v>
+      </c>
+      <c r="C186" t="s">
+        <v>13</v>
+      </c>
+      <c r="D186" t="s">
+        <v>295</v>
+      </c>
+      <c r="E186" t="s">
+        <v>310</v>
+      </c>
+      <c r="F186" t="s">
+        <v>311</v>
+      </c>
+      <c r="G186" t="s">
+        <v>312</v>
+      </c>
+      <c r="H186" t="s">
+        <v>313</v>
+      </c>
+      <c r="I186" t="s">
+        <v>19</v>
+      </c>
+      <c r="J186">
+        <v>1</v>
+      </c>
+      <c r="K186">
+        <v>3897000</v>
+      </c>
+      <c r="L186">
+        <v>3897000</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12">
+      <c r="A187">
+        <v>184</v>
+      </c>
+      <c r="B187">
+        <v>626402</v>
+      </c>
+      <c r="C187" t="s">
+        <v>13</v>
+      </c>
+      <c r="D187" t="s">
+        <v>295</v>
+      </c>
+      <c r="E187" t="s">
+        <v>314</v>
+      </c>
+      <c r="F187" t="s">
+        <v>315</v>
+      </c>
+      <c r="G187" t="s">
+        <v>316</v>
+      </c>
+      <c r="H187" t="s">
+        <v>131</v>
+      </c>
+      <c r="I187" t="s">
+        <v>19</v>
+      </c>
+      <c r="J187">
+        <v>1</v>
+      </c>
+      <c r="K187">
+        <v>5410000</v>
+      </c>
+      <c r="L187">
+        <v>5410000</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12">
+      <c r="A188">
+        <v>185</v>
+      </c>
+      <c r="B188">
+        <v>626402</v>
+      </c>
+      <c r="C188" t="s">
+        <v>13</v>
+      </c>
+      <c r="D188" t="s">
+        <v>295</v>
+      </c>
+      <c r="E188" t="s">
+        <v>317</v>
+      </c>
+      <c r="F188" t="s">
+        <v>318</v>
+      </c>
+      <c r="G188" t="s">
+        <v>319</v>
+      </c>
+      <c r="H188" t="s">
+        <v>290</v>
+      </c>
+      <c r="I188" t="s">
+        <v>19</v>
+      </c>
+      <c r="J188">
+        <v>1</v>
+      </c>
+      <c r="K188">
+        <v>520000</v>
+      </c>
+      <c r="L188">
+        <v>520000</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12">
+      <c r="A189">
+        <v>186</v>
+      </c>
+      <c r="B189">
+        <v>626402</v>
+      </c>
+      <c r="C189" t="s">
+        <v>13</v>
+      </c>
+      <c r="D189" t="s">
+        <v>295</v>
+      </c>
+      <c r="E189" t="s">
+        <v>317</v>
+      </c>
+      <c r="F189" t="s">
+        <v>318</v>
+      </c>
+      <c r="G189" t="s">
+        <v>319</v>
+      </c>
+      <c r="H189" t="s">
+        <v>291</v>
+      </c>
+      <c r="I189" t="s">
+        <v>19</v>
+      </c>
+      <c r="J189">
+        <v>1</v>
+      </c>
+      <c r="K189">
+        <v>850000</v>
+      </c>
+      <c r="L189">
+        <v>850000</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12">
+      <c r="A190">
+        <v>187</v>
+      </c>
+      <c r="B190">
+        <v>626402</v>
+      </c>
+      <c r="C190" t="s">
+        <v>13</v>
+      </c>
+      <c r="D190" t="s">
+        <v>295</v>
+      </c>
+      <c r="E190" t="s">
+        <v>320</v>
+      </c>
+      <c r="F190" t="s">
+        <v>321</v>
+      </c>
+      <c r="G190" t="s">
+        <v>322</v>
+      </c>
+      <c r="H190" t="s">
+        <v>118</v>
+      </c>
+      <c r="I190" t="s">
+        <v>19</v>
+      </c>
+      <c r="J190">
+        <v>1</v>
+      </c>
+      <c r="K190">
+        <v>29064400</v>
+      </c>
+      <c r="L190">
+        <v>29064400</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12">
+      <c r="A191">
+        <v>188</v>
+      </c>
+      <c r="B191">
+        <v>626402</v>
+      </c>
+      <c r="C191" t="s">
+        <v>13</v>
+      </c>
+      <c r="D191" t="s">
+        <v>295</v>
+      </c>
+      <c r="E191" t="s">
+        <v>323</v>
+      </c>
+      <c r="F191" t="s">
+        <v>324</v>
+      </c>
+      <c r="G191" t="s">
+        <v>325</v>
+      </c>
+      <c r="H191" t="s">
+        <v>326</v>
+      </c>
+      <c r="I191" t="s">
+        <v>19</v>
+      </c>
+      <c r="J191">
+        <v>1</v>
+      </c>
+      <c r="K191">
+        <v>40120000</v>
+      </c>
+      <c r="L191">
+        <v>40120000</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12">
+      <c r="A192">
+        <v>189</v>
+      </c>
+      <c r="B192">
+        <v>626402</v>
+      </c>
+      <c r="C192" t="s">
+        <v>13</v>
+      </c>
+      <c r="D192" t="s">
+        <v>295</v>
+      </c>
+      <c r="E192" t="s">
+        <v>323</v>
+      </c>
+      <c r="F192" t="s">
+        <v>324</v>
+      </c>
+      <c r="G192" t="s">
+        <v>325</v>
+      </c>
+      <c r="H192" t="s">
+        <v>109</v>
+      </c>
+      <c r="I192" t="s">
+        <v>19</v>
+      </c>
+      <c r="J192">
+        <v>1</v>
+      </c>
+      <c r="K192">
+        <v>17650000</v>
+      </c>
+      <c r="L192">
+        <v>17650000</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12">
+      <c r="A193">
+        <v>190</v>
+      </c>
+      <c r="B193">
+        <v>626402</v>
+      </c>
+      <c r="C193" t="s">
+        <v>13</v>
+      </c>
+      <c r="D193" t="s">
+        <v>295</v>
+      </c>
+      <c r="E193" t="s">
+        <v>327</v>
+      </c>
+      <c r="F193" t="s">
+        <v>328</v>
+      </c>
+      <c r="G193" t="s">
+        <v>329</v>
+      </c>
+      <c r="H193" t="s">
+        <v>330</v>
+      </c>
+      <c r="I193" t="s">
+        <v>19</v>
+      </c>
+      <c r="J193">
+        <v>1</v>
+      </c>
+      <c r="K193">
+        <v>20000000</v>
+      </c>
+      <c r="L193">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12">
+      <c r="A194">
+        <v>191</v>
+      </c>
+      <c r="B194">
+        <v>626402</v>
+      </c>
+      <c r="C194" t="s">
+        <v>13</v>
+      </c>
+      <c r="D194" t="s">
+        <v>295</v>
+      </c>
+      <c r="E194" t="s">
+        <v>331</v>
+      </c>
+      <c r="F194" t="s">
+        <v>332</v>
+      </c>
+      <c r="G194" t="s">
+        <v>333</v>
+      </c>
+      <c r="H194" t="s">
+        <v>268</v>
+      </c>
+      <c r="I194" t="s">
+        <v>19</v>
+      </c>
+      <c r="J194">
+        <v>1</v>
+      </c>
+      <c r="K194">
+        <v>23931600</v>
+      </c>
+      <c r="L194">
+        <v>23931600</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12">
+      <c r="A195">
+        <v>192</v>
+      </c>
+      <c r="B195">
+        <v>626402</v>
+      </c>
+      <c r="C195" t="s">
+        <v>13</v>
+      </c>
+      <c r="D195" t="s">
+        <v>334</v>
+      </c>
+      <c r="E195" t="s">
+        <v>335</v>
+      </c>
+      <c r="F195" t="s">
+        <v>336</v>
+      </c>
+      <c r="G195" t="s">
+        <v>337</v>
+      </c>
+      <c r="H195" t="s">
+        <v>338</v>
+      </c>
+      <c r="I195" t="s">
+        <v>19</v>
+      </c>
+      <c r="J195">
+        <v>1</v>
+      </c>
+      <c r="K195">
+        <v>28720670</v>
+      </c>
+      <c r="L195">
+        <v>28720670</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12">
+      <c r="A196">
+        <v>193</v>
+      </c>
+      <c r="B196">
+        <v>626402</v>
+      </c>
+      <c r="C196" t="s">
+        <v>13</v>
+      </c>
+      <c r="D196" t="s">
+        <v>334</v>
+      </c>
+      <c r="E196" t="s">
+        <v>339</v>
+      </c>
+      <c r="F196" t="s">
+        <v>340</v>
+      </c>
+      <c r="G196" t="s">
+        <v>341</v>
+      </c>
+      <c r="H196" t="s">
+        <v>342</v>
+      </c>
+      <c r="I196" t="s">
+        <v>19</v>
+      </c>
+      <c r="J196">
+        <v>1</v>
+      </c>
+      <c r="K196">
+        <v>28720670</v>
+      </c>
+      <c r="L196">
+        <v>28720670</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12">
+      <c r="A197">
+        <v>194</v>
+      </c>
+      <c r="B197">
+        <v>626402</v>
+      </c>
+      <c r="C197" t="s">
+        <v>13</v>
+      </c>
+      <c r="D197" t="s">
+        <v>334</v>
+      </c>
+      <c r="E197" t="s">
+        <v>343</v>
+      </c>
+      <c r="F197" t="s">
+        <v>344</v>
+      </c>
+      <c r="G197" t="s">
+        <v>345</v>
+      </c>
+      <c r="H197" t="s">
+        <v>342</v>
+      </c>
+      <c r="I197" t="s">
+        <v>19</v>
+      </c>
+      <c r="J197">
+        <v>1</v>
+      </c>
+      <c r="K197">
+        <v>7428768</v>
+      </c>
+      <c r="L197">
+        <v>7428768</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12">
+      <c r="A198">
+        <v>195</v>
+      </c>
+      <c r="B198">
+        <v>626402</v>
+      </c>
+      <c r="C198" t="s">
+        <v>13</v>
+      </c>
+      <c r="D198" t="s">
+        <v>346</v>
+      </c>
+      <c r="E198" t="s">
+        <v>347</v>
+      </c>
+      <c r="F198" t="s">
+        <v>348</v>
+      </c>
+      <c r="G198" t="s">
+        <v>349</v>
+      </c>
+      <c r="H198" t="s">
+        <v>198</v>
+      </c>
+      <c r="I198" t="s">
+        <v>19</v>
+      </c>
+      <c r="J198">
+        <v>1</v>
+      </c>
+      <c r="K198">
+        <v>14600000</v>
+      </c>
+      <c r="L198">
+        <v>14600000</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12">
+      <c r="A199">
+        <v>196</v>
+      </c>
+      <c r="B199">
+        <v>626402</v>
+      </c>
+      <c r="C199" t="s">
+        <v>13</v>
+      </c>
+      <c r="D199" t="s">
+        <v>334</v>
+      </c>
+      <c r="E199" t="s">
+        <v>350</v>
+      </c>
+      <c r="F199" t="s">
+        <v>351</v>
+      </c>
+      <c r="G199" t="s">
+        <v>352</v>
+      </c>
+      <c r="H199" t="s">
+        <v>128</v>
+      </c>
+      <c r="I199" t="s">
+        <v>19</v>
+      </c>
+      <c r="J199">
+        <v>1</v>
+      </c>
+      <c r="K199">
+        <v>1356500</v>
+      </c>
+      <c r="L199">
+        <v>1356500</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12">
+      <c r="A200">
+        <v>197</v>
+      </c>
+      <c r="B200">
+        <v>626402</v>
+      </c>
+      <c r="C200" t="s">
+        <v>13</v>
+      </c>
+      <c r="D200" t="s">
+        <v>334</v>
+      </c>
+      <c r="E200" t="s">
+        <v>353</v>
+      </c>
+      <c r="F200" t="s">
+        <v>354</v>
+      </c>
+      <c r="G200" t="s">
+        <v>177</v>
+      </c>
+      <c r="H200" t="s">
+        <v>355</v>
+      </c>
+      <c r="I200" t="s">
+        <v>19</v>
+      </c>
+      <c r="J200">
+        <v>1</v>
+      </c>
+      <c r="K200">
+        <v>8099000</v>
+      </c>
+      <c r="L200">
+        <v>8099000</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12">
+      <c r="A201">
+        <v>198</v>
+      </c>
+      <c r="B201">
+        <v>626402</v>
+      </c>
+      <c r="C201" t="s">
+        <v>13</v>
+      </c>
+      <c r="D201" t="s">
+        <v>334</v>
+      </c>
+      <c r="E201" t="s">
+        <v>353</v>
+      </c>
+      <c r="F201" t="s">
+        <v>354</v>
+      </c>
+      <c r="G201" t="s">
+        <v>177</v>
+      </c>
+      <c r="H201" t="s">
+        <v>356</v>
+      </c>
+      <c r="I201" t="s">
+        <v>19</v>
+      </c>
+      <c r="J201">
+        <v>1</v>
+      </c>
+      <c r="K201">
+        <v>2054100</v>
+      </c>
+      <c r="L201">
+        <v>2054100</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12">
+      <c r="A202">
+        <v>199</v>
+      </c>
+      <c r="B202">
+        <v>626402</v>
+      </c>
+      <c r="C202" t="s">
+        <v>13</v>
+      </c>
+      <c r="D202" t="s">
+        <v>334</v>
+      </c>
+      <c r="E202" t="s">
+        <v>353</v>
+      </c>
+      <c r="F202" t="s">
+        <v>354</v>
+      </c>
+      <c r="G202" t="s">
+        <v>177</v>
+      </c>
+      <c r="H202" t="s">
+        <v>357</v>
+      </c>
+      <c r="I202" t="s">
+        <v>19</v>
+      </c>
+      <c r="J202">
+        <v>1</v>
+      </c>
+      <c r="K202">
+        <v>3485000</v>
+      </c>
+      <c r="L202">
+        <v>3485000</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12">
+      <c r="A203">
+        <v>200</v>
+      </c>
+      <c r="B203">
+        <v>626402</v>
+      </c>
+      <c r="C203" t="s">
+        <v>13</v>
+      </c>
+      <c r="D203" t="s">
+        <v>334</v>
+      </c>
+      <c r="E203" t="s">
+        <v>353</v>
+      </c>
+      <c r="F203" t="s">
+        <v>354</v>
+      </c>
+      <c r="G203" t="s">
+        <v>177</v>
+      </c>
+      <c r="H203" t="s">
+        <v>358</v>
+      </c>
+      <c r="I203" t="s">
+        <v>19</v>
+      </c>
+      <c r="J203">
+        <v>1</v>
+      </c>
+      <c r="K203">
+        <v>1560000</v>
+      </c>
+      <c r="L203">
+        <v>1560000</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12">
+      <c r="A204">
+        <v>201</v>
+      </c>
+      <c r="B204">
+        <v>626402</v>
+      </c>
+      <c r="C204" t="s">
+        <v>13</v>
+      </c>
+      <c r="D204" t="s">
+        <v>346</v>
+      </c>
+      <c r="E204" t="s">
+        <v>359</v>
+      </c>
+      <c r="F204" t="s">
+        <v>360</v>
+      </c>
+      <c r="G204" t="s">
+        <v>361</v>
+      </c>
+      <c r="H204" t="s">
+        <v>362</v>
+      </c>
+      <c r="I204" t="s">
+        <v>19</v>
+      </c>
+      <c r="J204">
+        <v>1</v>
+      </c>
+      <c r="K204">
+        <v>2935600</v>
+      </c>
+      <c r="L204">
+        <v>2935600</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12">
+      <c r="A205">
+        <v>202</v>
+      </c>
+      <c r="B205">
+        <v>626402</v>
+      </c>
+      <c r="C205" t="s">
+        <v>13</v>
+      </c>
+      <c r="D205" t="s">
+        <v>346</v>
+      </c>
+      <c r="E205" t="s">
+        <v>359</v>
+      </c>
+      <c r="F205" t="s">
+        <v>360</v>
+      </c>
+      <c r="G205" t="s">
+        <v>361</v>
+      </c>
+      <c r="H205" t="s">
+        <v>363</v>
+      </c>
+      <c r="I205" t="s">
+        <v>19</v>
+      </c>
+      <c r="J205">
+        <v>1</v>
+      </c>
+      <c r="K205">
+        <v>108631940</v>
+      </c>
+      <c r="L205">
+        <v>108631940</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12">
+      <c r="A206">
+        <v>203</v>
+      </c>
+      <c r="B206">
+        <v>626402</v>
+      </c>
+      <c r="C206" t="s">
+        <v>13</v>
+      </c>
+      <c r="D206" t="s">
+        <v>346</v>
+      </c>
+      <c r="E206" t="s">
+        <v>359</v>
+      </c>
+      <c r="F206" t="s">
+        <v>360</v>
+      </c>
+      <c r="G206" t="s">
+        <v>361</v>
+      </c>
+      <c r="H206" t="s">
+        <v>364</v>
+      </c>
+      <c r="I206" t="s">
+        <v>19</v>
+      </c>
+      <c r="J206">
+        <v>1</v>
+      </c>
+      <c r="K206">
+        <v>150000</v>
+      </c>
+      <c r="L206">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12">
+      <c r="A207">
+        <v>204</v>
+      </c>
+      <c r="B207">
+        <v>626402</v>
+      </c>
+      <c r="C207" t="s">
+        <v>13</v>
+      </c>
+      <c r="D207" t="s">
+        <v>346</v>
+      </c>
+      <c r="E207" t="s">
+        <v>365</v>
+      </c>
+      <c r="F207" t="s">
+        <v>366</v>
+      </c>
+      <c r="G207" t="s">
+        <v>367</v>
+      </c>
+      <c r="H207" t="s">
+        <v>368</v>
+      </c>
+      <c r="I207" t="s">
+        <v>19</v>
+      </c>
+      <c r="J207">
+        <v>1</v>
+      </c>
+      <c r="K207">
+        <v>198871146</v>
+      </c>
+      <c r="L207">
+        <v>198871146</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12">
+      <c r="A208">
+        <v>205</v>
+      </c>
+      <c r="B208">
+        <v>626402</v>
+      </c>
+      <c r="C208" t="s">
+        <v>13</v>
+      </c>
+      <c r="D208" t="s">
+        <v>346</v>
+      </c>
+      <c r="E208" t="s">
+        <v>369</v>
+      </c>
+      <c r="F208" t="s">
+        <v>370</v>
+      </c>
+      <c r="G208" t="s">
+        <v>371</v>
+      </c>
+      <c r="H208" t="s">
+        <v>372</v>
+      </c>
+      <c r="I208" t="s">
+        <v>19</v>
+      </c>
+      <c r="J208">
+        <v>1</v>
+      </c>
+      <c r="K208">
+        <v>412680289</v>
+      </c>
+      <c r="L208">
+        <v>412680289</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12">
+      <c r="A209">
+        <v>206</v>
+      </c>
+      <c r="B209">
+        <v>626402</v>
+      </c>
+      <c r="C209" t="s">
+        <v>13</v>
+      </c>
+      <c r="D209" t="s">
+        <v>346</v>
+      </c>
+      <c r="E209" t="s">
+        <v>373</v>
+      </c>
+      <c r="F209" t="s">
+        <v>374</v>
+      </c>
+      <c r="G209" t="s">
+        <v>375</v>
+      </c>
+      <c r="H209" t="s">
+        <v>80</v>
+      </c>
+      <c r="I209" t="s">
+        <v>19</v>
+      </c>
+      <c r="J209">
+        <v>1</v>
+      </c>
+      <c r="K209">
+        <v>203211317</v>
+      </c>
+      <c r="L209">
+        <v>203211317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 15 feb 2024
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="494">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -902,6 +902,21 @@
     <t>Pembayaran belanja barang berupa biaya perjadin sesuai ST No. B.829/BPPSDM.1/KP.440/I/2024 Tanggal 26 Januari 2024 a.n Rizky Hendriansyah, dkk</t>
   </si>
   <si>
+    <t>2024-02-13</t>
+  </si>
+  <si>
+    <t>'00062T</t>
+  </si>
+  <si>
+    <t>'241751303001743</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang.Prog Dr FITB-ITB Serdik KKP Sem 2 TA 2023/2024,Sem 1 TA 2024/2025 an.Freshty,dkk,SPK No:531/PPK.PUSDIK/PL.530/I/2024 tgl 19-1-2024,BAST No:85/PPK.PUSDIK/PL.530/I/2024 tgl 31-1-2024,BAP No:86/PPK.PUSDIK/PL.530/I/2024 tgl 31-1-2024</t>
+  </si>
+  <si>
+    <t>'626402.175.521219.03212WA.4345EBC.A000000001.00000.1.0151.2.000000.000000.996.301.0A.001332</t>
+  </si>
+  <si>
     <t>2024-02-06</t>
   </si>
   <si>
@@ -1094,6 +1109,60 @@
     <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0D.001479</t>
   </si>
   <si>
+    <t>2024-02-15</t>
+  </si>
+  <si>
+    <t>'00079T</t>
+  </si>
+  <si>
+    <t>'241751303001768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.92/BPPSDM.5/KP.440/I/2024 Tgl.18 Januari 2024 </t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0D.001477</t>
+  </si>
+  <si>
+    <t>'00080T</t>
+  </si>
+  <si>
+    <t>'241751303001796</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.115/BPPSDM.5/KP.440/I/2024 Tgl.23 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0D.000987</t>
+  </si>
+  <si>
+    <t>'00081T</t>
+  </si>
+  <si>
+    <t>'241751303001797</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.122/BPPSDM.5/KP.440/I/2024 Tgl.23 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0B.000964</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0B.001471</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0B.001472</t>
+  </si>
+  <si>
+    <t>'00082T</t>
+  </si>
+  <si>
+    <t>'241751303001798</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.121/BPPSDM.5/KP.440/I/2024 Tgl.23 Januari 2024</t>
+  </si>
+  <si>
     <t>'00083T</t>
   </si>
   <si>
@@ -1112,6 +1181,18 @@
     <t>'626402.175.524114.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.103.0A.000860</t>
   </si>
   <si>
+    <t>'00084T</t>
+  </si>
+  <si>
+    <t>'241751301002101</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:009/PE/KWT/I/2024 Tgl.30-1-2024</t>
+  </si>
+  <si>
+    <t>'626402.175.523111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BC.000508</t>
+  </si>
+  <si>
     <t>'00085T</t>
   </si>
   <si>
@@ -1143,6 +1224,279 @@
   </si>
   <si>
     <t>Pembayaran tunjangan kinerja susulan bulan Januari tahun 2024 untuk 40 Pegawai/Anggota Polri/Prajurit TNI (Pusdik KP)</t>
+  </si>
+  <si>
+    <t>'00088T</t>
+  </si>
+  <si>
+    <t>'241751303001715</t>
+  </si>
+  <si>
+    <t>Penggantian uang persediaan KKP untuk keperluan belanja barang (BPP 001 Set. BRSDM)</t>
+  </si>
+  <si>
+    <t>'00089T</t>
+  </si>
+  <si>
+    <t>'241751302001895</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai SPK No:3/PPK/BRSDM.1/I/2024 Tgl.2-1-2024,BAST No:BAST.221/PPK/BRSDM.1/I/2024 Tgl.31-1-2024,BAP No:222/PPK/BRSDM.1/I/2024 Tgl.31-1-2024 Pengadaan Jasa tenaga kebersihan sekretariat BRSDM TA 2024 Termin 1</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BA.000499</t>
+  </si>
+  <si>
+    <t>'00090T</t>
+  </si>
+  <si>
+    <t>'241751301002103</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai SPK No:4/PPK/BRSDM.1/I/2024 Tgl.2-1-2024,BAST No:BAST.223/PPK/BRSDM.1/I/2024 Tgl.31-1-2024,BAP No:224/PPK/BRSDM.1/I/2024 Tgl.31-1-2024 Pengadaan jasa satuan pegamanan sekretariat BRSDM TA 2024 Termin 1</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BA.000498</t>
+  </si>
+  <si>
+    <t>'00091T</t>
+  </si>
+  <si>
+    <t>'241751303001727</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No. B.226,B.311/BPPSDM.1/KP.440/I/2024 Tanggal 10 dan 15 Januari 2024 a.n Don Bapkas Nisnoni, dkk</t>
+  </si>
+  <si>
+    <t>'626402.175.524113.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0A.000879</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.101.0A.000881</t>
+  </si>
+  <si>
+    <t>'00092T</t>
+  </si>
+  <si>
+    <t>'241751303001737</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor 001/KWT-2/AMA/I/2024 Tanggal 31 Januari 2024</t>
+  </si>
+  <si>
+    <t>'00093T</t>
+  </si>
+  <si>
+    <t>'241751303001738</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor 002/KWT-2/AMA/I/2024 Tanggal 31 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.523121.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AC.000453</t>
+  </si>
+  <si>
+    <t>'00094T</t>
+  </si>
+  <si>
+    <t>'241751303001714</t>
+  </si>
+  <si>
+    <t>Penggantian uang persediaan untuk keperluan belanja barang (BPP 001 Set.BRSDM)</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BA.001607</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BA.001608</t>
+  </si>
+  <si>
+    <t>'626402.175.522191.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000440</t>
+  </si>
+  <si>
+    <t>'00097T</t>
+  </si>
+  <si>
+    <t>'241751303001934</t>
+  </si>
+  <si>
+    <t>Penggantian uang persediaan untuk keperluan belanja barang (BPP001 Puslatluh KP)</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.DA.000528</t>
+  </si>
+  <si>
+    <t>'626402.175.521111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.DD.000553</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0D.000044</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0F.000061</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0E.000090</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.000096</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.000109</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0C.000155</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0D.000979</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0E.000091</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0E.000092</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0B.001428</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0B.001429</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0E.001455</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0E.001456</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.201.0C.001143</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.201.0C.001500</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.201.0C.001501</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0B.000079</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0E.000093</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.000104</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.000115</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0C.000162</t>
+  </si>
+  <si>
+    <t>'626402.175.524119.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.952.201.0C.000976</t>
+  </si>
+  <si>
+    <t>'00098T</t>
+  </si>
+  <si>
+    <t>'241751303001799</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.247/BRSDM/KP.440/I/2024 Tgl.15 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.962.101.0A.000603</t>
+  </si>
+  <si>
+    <t>'00099T</t>
+  </si>
+  <si>
+    <t>'241751302001937</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:003 Tanggal 02 Februari 2024</t>
+  </si>
+  <si>
+    <t>'00100T</t>
+  </si>
+  <si>
+    <t>'241751301002187</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai SPK No:2/PPK/BRSDM.1/I/2024 Tgl.2-1-2024,BAST No:BAST.225/BRSDM.1/I/2024 Tgl.31-1-2024,BAP No:226/PPK/BRSDM.1/I/2024 Tgl.31-1-2024 Pengadaan jasa internet provider sekretariat BRSDM TA 2024 Termin 1</t>
+  </si>
+  <si>
+    <t>'626402.175.522119.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BB.000503</t>
+  </si>
+  <si>
+    <t>'00101T</t>
+  </si>
+  <si>
+    <t>'241751301002182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai SPK No:161/PPK/BRSDM.1/I/2024 Tgl.23-1-2024,BAST No:BAST.191//PPK/BRSDM.1/I/2024 Tgl.26-1-2024,BAP No:192/PPK/BRSDM.1/I/2024 Tgl.26-1-2024 </t>
+  </si>
+  <si>
+    <t>'626402.175.524119.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AA.001367</t>
+  </si>
+  <si>
+    <t>'00102T</t>
+  </si>
+  <si>
+    <t>'241751301002183</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai SPK No:162/PPK/BRSDM.1/I/2024 Tgl.23-1-2024,BAST No:BAST.193/PPK/BRSDM.1/I/2024 Tgl.26-1-2024,BAP No:194/PPK/BRSDM.1/I/2024 Tgl.26-1-2024 Paket Fullboard Meeting Pengelolaan Kepegawaian dan PNBP Lingkup BPPSDM</t>
+  </si>
+  <si>
+    <t>'626402.175.524119.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.101.0B.000836</t>
+  </si>
+  <si>
+    <t>'00103T</t>
+  </si>
+  <si>
+    <t>'241751302001917</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai SPK NO:171/PPK/BRSDM.1/I/2024 Tgl.24-1-2024,BAST NO:BAST.194/PPK/BRSDM.1/I/2024 Tgl.26-1-2024, BAP No:195/PPK/BRSDM.1/I/2024 Tgl.26-1-2024 Jasa Penyelenggaraan Kegiatan Peningkatan Kapasitas Pegawai BRSDM</t>
+  </si>
+  <si>
+    <t>'626402.175.522191.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.101.0B.000834</t>
+  </si>
+  <si>
+    <t>'00104T</t>
+  </si>
+  <si>
+    <t>'241751303001852</t>
+  </si>
+  <si>
+    <t>Penggantian uang persediaan KKP untuk keperluan belanja modal (BPP 001 Set.BRSDM)</t>
+  </si>
+  <si>
+    <t>'626402.175.532111.03212WA.2378EBB.A000000001.00000.1.0151.2.000000.000000.951.103.0A.000818</t>
+  </si>
+  <si>
+    <t>'00105T</t>
+  </si>
+  <si>
+    <t>'241751303001851</t>
+  </si>
+  <si>
+    <t>Penggantian Uang Persediaan KKP Untuk Keperluan Pembayaran Belanja Barang (BPP 001 Set.BRSDM)</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AC.001085</t>
+  </si>
+  <si>
+    <t>'626402.175.522119.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AB.000443</t>
+  </si>
+  <si>
+    <t>'00110T</t>
+  </si>
+  <si>
+    <t>'241751303001935</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AC.001090</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1838,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L209"/>
+  <dimension ref="A1:L284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -8258,10 +8612,10 @@
         <v>1</v>
       </c>
       <c r="K180">
-        <v>2316500</v>
+        <v>360000000</v>
       </c>
       <c r="L180">
-        <v>2316500</v>
+        <v>360000000</v>
       </c>
     </row>
     <row r="181" spans="1:12">
@@ -8275,19 +8629,19 @@
         <v>13</v>
       </c>
       <c r="D181" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E181" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="F181" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="G181" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="H181" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="I181" t="s">
         <v>19</v>
@@ -8296,10 +8650,10 @@
         <v>1</v>
       </c>
       <c r="K181">
-        <v>1205000</v>
+        <v>2316500</v>
       </c>
       <c r="L181">
-        <v>1205000</v>
+        <v>2316500</v>
       </c>
     </row>
     <row r="182" spans="1:12">
@@ -8313,19 +8667,19 @@
         <v>13</v>
       </c>
       <c r="D182" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E182" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="F182" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="G182" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="H182" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="I182" t="s">
         <v>19</v>
@@ -8334,10 +8688,10 @@
         <v>1</v>
       </c>
       <c r="K182">
-        <v>630000</v>
+        <v>1205000</v>
       </c>
       <c r="L182">
-        <v>630000</v>
+        <v>1205000</v>
       </c>
     </row>
     <row r="183" spans="1:12">
@@ -8351,19 +8705,19 @@
         <v>13</v>
       </c>
       <c r="D183" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E183" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="F183" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="G183" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="H183" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I183" t="s">
         <v>19</v>
@@ -8372,10 +8726,10 @@
         <v>1</v>
       </c>
       <c r="K183">
-        <v>510000</v>
+        <v>630000</v>
       </c>
       <c r="L183">
-        <v>510000</v>
+        <v>630000</v>
       </c>
     </row>
     <row r="184" spans="1:12">
@@ -8389,19 +8743,19 @@
         <v>13</v>
       </c>
       <c r="D184" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E184" t="s">
+        <v>301</v>
+      </c>
+      <c r="F184" t="s">
+        <v>302</v>
+      </c>
+      <c r="G184" t="s">
         <v>303</v>
       </c>
-      <c r="F184" t="s">
-        <v>304</v>
-      </c>
-      <c r="G184" t="s">
-        <v>305</v>
-      </c>
       <c r="H184" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I184" t="s">
         <v>19</v>
@@ -8410,10 +8764,10 @@
         <v>1</v>
       </c>
       <c r="K184">
-        <v>1700000</v>
+        <v>510000</v>
       </c>
       <c r="L184">
-        <v>1700000</v>
+        <v>510000</v>
       </c>
     </row>
     <row r="185" spans="1:12">
@@ -8427,19 +8781,19 @@
         <v>13</v>
       </c>
       <c r="D185" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E185" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F185" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G185" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H185" t="s">
-        <v>274</v>
+        <v>311</v>
       </c>
       <c r="I185" t="s">
         <v>19</v>
@@ -8448,10 +8802,10 @@
         <v>1</v>
       </c>
       <c r="K185">
-        <v>5907000</v>
+        <v>1700000</v>
       </c>
       <c r="L185">
-        <v>5907000</v>
+        <v>1700000</v>
       </c>
     </row>
     <row r="186" spans="1:12">
@@ -8465,19 +8819,19 @@
         <v>13</v>
       </c>
       <c r="D186" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E186" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="F186" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="G186" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="H186" t="s">
-        <v>313</v>
+        <v>274</v>
       </c>
       <c r="I186" t="s">
         <v>19</v>
@@ -8486,10 +8840,10 @@
         <v>1</v>
       </c>
       <c r="K186">
-        <v>3897000</v>
+        <v>5907000</v>
       </c>
       <c r="L186">
-        <v>3897000</v>
+        <v>5907000</v>
       </c>
     </row>
     <row r="187" spans="1:12">
@@ -8503,19 +8857,19 @@
         <v>13</v>
       </c>
       <c r="D187" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E187" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F187" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G187" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H187" t="s">
-        <v>131</v>
+        <v>318</v>
       </c>
       <c r="I187" t="s">
         <v>19</v>
@@ -8524,10 +8878,10 @@
         <v>1</v>
       </c>
       <c r="K187">
-        <v>5410000</v>
+        <v>3897000</v>
       </c>
       <c r="L187">
-        <v>5410000</v>
+        <v>3897000</v>
       </c>
     </row>
     <row r="188" spans="1:12">
@@ -8541,19 +8895,19 @@
         <v>13</v>
       </c>
       <c r="D188" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E188" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F188" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="G188" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="H188" t="s">
-        <v>290</v>
+        <v>131</v>
       </c>
       <c r="I188" t="s">
         <v>19</v>
@@ -8562,10 +8916,10 @@
         <v>1</v>
       </c>
       <c r="K188">
-        <v>520000</v>
+        <v>5410000</v>
       </c>
       <c r="L188">
-        <v>520000</v>
+        <v>5410000</v>
       </c>
     </row>
     <row r="189" spans="1:12">
@@ -8579,19 +8933,19 @@
         <v>13</v>
       </c>
       <c r="D189" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E189" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="F189" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="G189" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="H189" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I189" t="s">
         <v>19</v>
@@ -8600,10 +8954,10 @@
         <v>1</v>
       </c>
       <c r="K189">
-        <v>850000</v>
+        <v>520000</v>
       </c>
       <c r="L189">
-        <v>850000</v>
+        <v>520000</v>
       </c>
     </row>
     <row r="190" spans="1:12">
@@ -8617,19 +8971,19 @@
         <v>13</v>
       </c>
       <c r="D190" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E190" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F190" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G190" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="H190" t="s">
-        <v>118</v>
+        <v>291</v>
       </c>
       <c r="I190" t="s">
         <v>19</v>
@@ -8638,10 +8992,10 @@
         <v>1</v>
       </c>
       <c r="K190">
-        <v>29064400</v>
+        <v>850000</v>
       </c>
       <c r="L190">
-        <v>29064400</v>
+        <v>850000</v>
       </c>
     </row>
     <row r="191" spans="1:12">
@@ -8655,19 +9009,19 @@
         <v>13</v>
       </c>
       <c r="D191" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E191" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F191" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G191" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="H191" t="s">
-        <v>326</v>
+        <v>118</v>
       </c>
       <c r="I191" t="s">
         <v>19</v>
@@ -8676,10 +9030,10 @@
         <v>1</v>
       </c>
       <c r="K191">
-        <v>40120000</v>
+        <v>29064400</v>
       </c>
       <c r="L191">
-        <v>40120000</v>
+        <v>29064400</v>
       </c>
     </row>
     <row r="192" spans="1:12">
@@ -8693,19 +9047,19 @@
         <v>13</v>
       </c>
       <c r="D192" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E192" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="F192" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="G192" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="H192" t="s">
-        <v>109</v>
+        <v>331</v>
       </c>
       <c r="I192" t="s">
         <v>19</v>
@@ -8714,10 +9068,10 @@
         <v>1</v>
       </c>
       <c r="K192">
-        <v>17650000</v>
+        <v>40120000</v>
       </c>
       <c r="L192">
-        <v>17650000</v>
+        <v>40120000</v>
       </c>
     </row>
     <row r="193" spans="1:12">
@@ -8731,19 +9085,19 @@
         <v>13</v>
       </c>
       <c r="D193" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E193" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F193" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G193" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H193" t="s">
-        <v>330</v>
+        <v>109</v>
       </c>
       <c r="I193" t="s">
         <v>19</v>
@@ -8752,10 +9106,10 @@
         <v>1</v>
       </c>
       <c r="K193">
-        <v>20000000</v>
+        <v>17650000</v>
       </c>
       <c r="L193">
-        <v>20000000</v>
+        <v>17650000</v>
       </c>
     </row>
     <row r="194" spans="1:12">
@@ -8769,19 +9123,19 @@
         <v>13</v>
       </c>
       <c r="D194" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E194" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F194" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G194" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H194" t="s">
-        <v>268</v>
+        <v>335</v>
       </c>
       <c r="I194" t="s">
         <v>19</v>
@@ -8790,10 +9144,10 @@
         <v>1</v>
       </c>
       <c r="K194">
-        <v>23931600</v>
+        <v>20000000</v>
       </c>
       <c r="L194">
-        <v>23931600</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="195" spans="1:12">
@@ -8807,19 +9161,19 @@
         <v>13</v>
       </c>
       <c r="D195" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
       <c r="E195" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F195" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G195" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H195" t="s">
-        <v>338</v>
+        <v>268</v>
       </c>
       <c r="I195" t="s">
         <v>19</v>
@@ -8828,10 +9182,10 @@
         <v>1</v>
       </c>
       <c r="K195">
-        <v>28720670</v>
+        <v>23931600</v>
       </c>
       <c r="L195">
-        <v>28720670</v>
+        <v>23931600</v>
       </c>
     </row>
     <row r="196" spans="1:12">
@@ -8845,19 +9199,19 @@
         <v>13</v>
       </c>
       <c r="D196" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="E196" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F196" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G196" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="H196" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="I196" t="s">
         <v>19</v>
@@ -8883,19 +9237,19 @@
         <v>13</v>
       </c>
       <c r="D197" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="E197" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F197" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="G197" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H197" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="I197" t="s">
         <v>19</v>
@@ -8904,10 +9258,10 @@
         <v>1</v>
       </c>
       <c r="K197">
-        <v>7428768</v>
+        <v>28720670</v>
       </c>
       <c r="L197">
-        <v>7428768</v>
+        <v>28720670</v>
       </c>
     </row>
     <row r="198" spans="1:12">
@@ -8921,20 +9275,20 @@
         <v>13</v>
       </c>
       <c r="D198" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E198" t="s">
+        <v>348</v>
+      </c>
+      <c r="F198" t="s">
+        <v>349</v>
+      </c>
+      <c r="G198" t="s">
+        <v>350</v>
+      </c>
+      <c r="H198" t="s">
         <v>347</v>
       </c>
-      <c r="F198" t="s">
-        <v>348</v>
-      </c>
-      <c r="G198" t="s">
-        <v>349</v>
-      </c>
-      <c r="H198" t="s">
-        <v>198</v>
-      </c>
       <c r="I198" t="s">
         <v>19</v>
       </c>
@@ -8942,10 +9296,10 @@
         <v>1</v>
       </c>
       <c r="K198">
-        <v>14600000</v>
+        <v>7428768</v>
       </c>
       <c r="L198">
-        <v>14600000</v>
+        <v>7428768</v>
       </c>
     </row>
     <row r="199" spans="1:12">
@@ -8959,19 +9313,19 @@
         <v>13</v>
       </c>
       <c r="D199" t="s">
-        <v>334</v>
+        <v>351</v>
       </c>
       <c r="E199" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F199" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G199" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="H199" t="s">
-        <v>128</v>
+        <v>198</v>
       </c>
       <c r="I199" t="s">
         <v>19</v>
@@ -8980,10 +9334,10 @@
         <v>1</v>
       </c>
       <c r="K199">
-        <v>1356500</v>
+        <v>14600000</v>
       </c>
       <c r="L199">
-        <v>1356500</v>
+        <v>14600000</v>
       </c>
     </row>
     <row r="200" spans="1:12">
@@ -8997,19 +9351,19 @@
         <v>13</v>
       </c>
       <c r="D200" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="E200" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F200" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="G200" t="s">
-        <v>177</v>
+        <v>357</v>
       </c>
       <c r="H200" t="s">
-        <v>355</v>
+        <v>128</v>
       </c>
       <c r="I200" t="s">
         <v>19</v>
@@ -9018,10 +9372,10 @@
         <v>1</v>
       </c>
       <c r="K200">
-        <v>8099000</v>
+        <v>1356500</v>
       </c>
       <c r="L200">
-        <v>8099000</v>
+        <v>1356500</v>
       </c>
     </row>
     <row r="201" spans="1:12">
@@ -9035,19 +9389,19 @@
         <v>13</v>
       </c>
       <c r="D201" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="E201" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="F201" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="G201" t="s">
         <v>177</v>
       </c>
       <c r="H201" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="I201" t="s">
         <v>19</v>
@@ -9056,10 +9410,10 @@
         <v>1</v>
       </c>
       <c r="K201">
-        <v>2054100</v>
+        <v>8099000</v>
       </c>
       <c r="L201">
-        <v>2054100</v>
+        <v>8099000</v>
       </c>
     </row>
     <row r="202" spans="1:12">
@@ -9073,19 +9427,19 @@
         <v>13</v>
       </c>
       <c r="D202" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="E202" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="F202" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="G202" t="s">
         <v>177</v>
       </c>
       <c r="H202" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="I202" t="s">
         <v>19</v>
@@ -9094,10 +9448,10 @@
         <v>1</v>
       </c>
       <c r="K202">
-        <v>3485000</v>
+        <v>2054100</v>
       </c>
       <c r="L202">
-        <v>3485000</v>
+        <v>2054100</v>
       </c>
     </row>
     <row r="203" spans="1:12">
@@ -9111,19 +9465,19 @@
         <v>13</v>
       </c>
       <c r="D203" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="E203" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="F203" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="G203" t="s">
         <v>177</v>
       </c>
       <c r="H203" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="I203" t="s">
         <v>19</v>
@@ -9132,10 +9486,10 @@
         <v>1</v>
       </c>
       <c r="K203">
-        <v>1560000</v>
+        <v>3485000</v>
       </c>
       <c r="L203">
-        <v>1560000</v>
+        <v>3485000</v>
       </c>
     </row>
     <row r="204" spans="1:12">
@@ -9149,19 +9503,19 @@
         <v>13</v>
       </c>
       <c r="D204" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E204" t="s">
+        <v>358</v>
+      </c>
+      <c r="F204" t="s">
         <v>359</v>
       </c>
-      <c r="F204" t="s">
-        <v>360</v>
-      </c>
       <c r="G204" t="s">
-        <v>361</v>
+        <v>177</v>
       </c>
       <c r="H204" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="I204" t="s">
         <v>19</v>
@@ -9170,10 +9524,10 @@
         <v>1</v>
       </c>
       <c r="K204">
-        <v>2935600</v>
+        <v>1560000</v>
       </c>
       <c r="L204">
-        <v>2935600</v>
+        <v>1560000</v>
       </c>
     </row>
     <row r="205" spans="1:12">
@@ -9187,19 +9541,19 @@
         <v>13</v>
       </c>
       <c r="D205" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="E205" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="F205" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="G205" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="H205" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="I205" t="s">
         <v>19</v>
@@ -9208,10 +9562,10 @@
         <v>1</v>
       </c>
       <c r="K205">
-        <v>108631940</v>
+        <v>1110000</v>
       </c>
       <c r="L205">
-        <v>108631940</v>
+        <v>1110000</v>
       </c>
     </row>
     <row r="206" spans="1:12">
@@ -9225,19 +9579,19 @@
         <v>13</v>
       </c>
       <c r="D206" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="E206" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="F206" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="G206" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="H206" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I206" t="s">
         <v>19</v>
@@ -9246,10 +9600,10 @@
         <v>1</v>
       </c>
       <c r="K206">
-        <v>150000</v>
+        <v>1498000</v>
       </c>
       <c r="L206">
-        <v>150000</v>
+        <v>1498000</v>
       </c>
     </row>
     <row r="207" spans="1:12">
@@ -9263,7 +9617,7 @@
         <v>13</v>
       </c>
       <c r="D207" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="E207" t="s">
         <v>365</v>
@@ -9275,7 +9629,7 @@
         <v>367</v>
       </c>
       <c r="H207" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="I207" t="s">
         <v>19</v>
@@ -9284,10 +9638,10 @@
         <v>1</v>
       </c>
       <c r="K207">
-        <v>198871146</v>
+        <v>691700</v>
       </c>
       <c r="L207">
-        <v>198871146</v>
+        <v>691700</v>
       </c>
     </row>
     <row r="208" spans="1:12">
@@ -9301,7 +9655,7 @@
         <v>13</v>
       </c>
       <c r="D208" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="E208" t="s">
         <v>369</v>
@@ -9322,10 +9676,10 @@
         <v>1</v>
       </c>
       <c r="K208">
-        <v>412680289</v>
+        <v>590000</v>
       </c>
       <c r="L208">
-        <v>412680289</v>
+        <v>590000</v>
       </c>
     </row>
     <row r="209" spans="1:12">
@@ -9339,31 +9693,2881 @@
         <v>13</v>
       </c>
       <c r="D209" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="E209" t="s">
+        <v>369</v>
+      </c>
+      <c r="F209" t="s">
+        <v>370</v>
+      </c>
+      <c r="G209" t="s">
+        <v>371</v>
+      </c>
+      <c r="H209" t="s">
+        <v>368</v>
+      </c>
+      <c r="I209" t="s">
+        <v>19</v>
+      </c>
+      <c r="J209">
+        <v>1</v>
+      </c>
+      <c r="K209">
+        <v>1850000</v>
+      </c>
+      <c r="L209">
+        <v>1850000</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12">
+      <c r="A210">
+        <v>207</v>
+      </c>
+      <c r="B210">
+        <v>626402</v>
+      </c>
+      <c r="C210" t="s">
+        <v>13</v>
+      </c>
+      <c r="D210" t="s">
+        <v>364</v>
+      </c>
+      <c r="E210" t="s">
+        <v>369</v>
+      </c>
+      <c r="F210" t="s">
+        <v>370</v>
+      </c>
+      <c r="G210" t="s">
+        <v>371</v>
+      </c>
+      <c r="H210" t="s">
+        <v>362</v>
+      </c>
+      <c r="I210" t="s">
+        <v>19</v>
+      </c>
+      <c r="J210">
+        <v>1</v>
+      </c>
+      <c r="K210">
+        <v>2067000</v>
+      </c>
+      <c r="L210">
+        <v>2067000</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12">
+      <c r="A211">
+        <v>208</v>
+      </c>
+      <c r="B211">
+        <v>626402</v>
+      </c>
+      <c r="C211" t="s">
+        <v>13</v>
+      </c>
+      <c r="D211" t="s">
+        <v>364</v>
+      </c>
+      <c r="E211" t="s">
+        <v>369</v>
+      </c>
+      <c r="F211" t="s">
+        <v>370</v>
+      </c>
+      <c r="G211" t="s">
+        <v>371</v>
+      </c>
+      <c r="H211" t="s">
+        <v>363</v>
+      </c>
+      <c r="I211" t="s">
+        <v>19</v>
+      </c>
+      <c r="J211">
+        <v>1</v>
+      </c>
+      <c r="K211">
+        <v>574500</v>
+      </c>
+      <c r="L211">
+        <v>574500</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12">
+      <c r="A212">
+        <v>209</v>
+      </c>
+      <c r="B212">
+        <v>626402</v>
+      </c>
+      <c r="C212" t="s">
+        <v>13</v>
+      </c>
+      <c r="D212" t="s">
+        <v>364</v>
+      </c>
+      <c r="E212" t="s">
         <v>373</v>
       </c>
-      <c r="F209" t="s">
+      <c r="F212" t="s">
         <v>374</v>
       </c>
-      <c r="G209" t="s">
+      <c r="G212" t="s">
         <v>375</v>
       </c>
-      <c r="H209" t="s">
+      <c r="H212" t="s">
+        <v>376</v>
+      </c>
+      <c r="I212" t="s">
+        <v>19</v>
+      </c>
+      <c r="J212">
+        <v>1</v>
+      </c>
+      <c r="K212">
+        <v>1110300</v>
+      </c>
+      <c r="L212">
+        <v>1110300</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12">
+      <c r="A213">
+        <v>210</v>
+      </c>
+      <c r="B213">
+        <v>626402</v>
+      </c>
+      <c r="C213" t="s">
+        <v>13</v>
+      </c>
+      <c r="D213" t="s">
+        <v>364</v>
+      </c>
+      <c r="E213" t="s">
+        <v>373</v>
+      </c>
+      <c r="F213" t="s">
+        <v>374</v>
+      </c>
+      <c r="G213" t="s">
+        <v>375</v>
+      </c>
+      <c r="H213" t="s">
+        <v>377</v>
+      </c>
+      <c r="I213" t="s">
+        <v>19</v>
+      </c>
+      <c r="J213">
+        <v>1</v>
+      </c>
+      <c r="K213">
+        <v>760000</v>
+      </c>
+      <c r="L213">
+        <v>760000</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12">
+      <c r="A214">
+        <v>211</v>
+      </c>
+      <c r="B214">
+        <v>626402</v>
+      </c>
+      <c r="C214" t="s">
+        <v>13</v>
+      </c>
+      <c r="D214" t="s">
+        <v>364</v>
+      </c>
+      <c r="E214" t="s">
+        <v>373</v>
+      </c>
+      <c r="F214" t="s">
+        <v>374</v>
+      </c>
+      <c r="G214" t="s">
+        <v>375</v>
+      </c>
+      <c r="H214" t="s">
+        <v>378</v>
+      </c>
+      <c r="I214" t="s">
+        <v>19</v>
+      </c>
+      <c r="J214">
+        <v>1</v>
+      </c>
+      <c r="K214">
+        <v>750000</v>
+      </c>
+      <c r="L214">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12">
+      <c r="A215">
+        <v>212</v>
+      </c>
+      <c r="B215">
+        <v>626402</v>
+      </c>
+      <c r="C215" t="s">
+        <v>13</v>
+      </c>
+      <c r="D215" t="s">
+        <v>364</v>
+      </c>
+      <c r="E215" t="s">
+        <v>379</v>
+      </c>
+      <c r="F215" t="s">
+        <v>380</v>
+      </c>
+      <c r="G215" t="s">
+        <v>381</v>
+      </c>
+      <c r="H215" t="s">
+        <v>376</v>
+      </c>
+      <c r="I215" t="s">
+        <v>19</v>
+      </c>
+      <c r="J215">
+        <v>1</v>
+      </c>
+      <c r="K215">
+        <v>1466300</v>
+      </c>
+      <c r="L215">
+        <v>1466300</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12">
+      <c r="A216">
+        <v>213</v>
+      </c>
+      <c r="B216">
+        <v>626402</v>
+      </c>
+      <c r="C216" t="s">
+        <v>13</v>
+      </c>
+      <c r="D216" t="s">
+        <v>364</v>
+      </c>
+      <c r="E216" t="s">
+        <v>379</v>
+      </c>
+      <c r="F216" t="s">
+        <v>380</v>
+      </c>
+      <c r="G216" t="s">
+        <v>381</v>
+      </c>
+      <c r="H216" t="s">
+        <v>377</v>
+      </c>
+      <c r="I216" t="s">
+        <v>19</v>
+      </c>
+      <c r="J216">
+        <v>1</v>
+      </c>
+      <c r="K216">
+        <v>2960000</v>
+      </c>
+      <c r="L216">
+        <v>2960000</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12">
+      <c r="A217">
+        <v>214</v>
+      </c>
+      <c r="B217">
+        <v>626402</v>
+      </c>
+      <c r="C217" t="s">
+        <v>13</v>
+      </c>
+      <c r="D217" t="s">
+        <v>364</v>
+      </c>
+      <c r="E217" t="s">
+        <v>379</v>
+      </c>
+      <c r="F217" t="s">
+        <v>380</v>
+      </c>
+      <c r="G217" t="s">
+        <v>381</v>
+      </c>
+      <c r="H217" t="s">
+        <v>378</v>
+      </c>
+      <c r="I217" t="s">
+        <v>19</v>
+      </c>
+      <c r="J217">
+        <v>1</v>
+      </c>
+      <c r="K217">
+        <v>3576000</v>
+      </c>
+      <c r="L217">
+        <v>3576000</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12">
+      <c r="A218">
+        <v>215</v>
+      </c>
+      <c r="B218">
+        <v>626402</v>
+      </c>
+      <c r="C218" t="s">
+        <v>13</v>
+      </c>
+      <c r="D218" t="s">
+        <v>364</v>
+      </c>
+      <c r="E218" t="s">
+        <v>379</v>
+      </c>
+      <c r="F218" t="s">
+        <v>380</v>
+      </c>
+      <c r="G218" t="s">
+        <v>381</v>
+      </c>
+      <c r="H218" t="s">
+        <v>361</v>
+      </c>
+      <c r="I218" t="s">
+        <v>19</v>
+      </c>
+      <c r="J218">
+        <v>1</v>
+      </c>
+      <c r="K218">
+        <v>210000</v>
+      </c>
+      <c r="L218">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12">
+      <c r="A219">
+        <v>216</v>
+      </c>
+      <c r="B219">
+        <v>626402</v>
+      </c>
+      <c r="C219" t="s">
+        <v>13</v>
+      </c>
+      <c r="D219" t="s">
+        <v>351</v>
+      </c>
+      <c r="E219" t="s">
+        <v>382</v>
+      </c>
+      <c r="F219" t="s">
+        <v>383</v>
+      </c>
+      <c r="G219" t="s">
+        <v>384</v>
+      </c>
+      <c r="H219" t="s">
+        <v>385</v>
+      </c>
+      <c r="I219" t="s">
+        <v>19</v>
+      </c>
+      <c r="J219">
+        <v>1</v>
+      </c>
+      <c r="K219">
+        <v>2935600</v>
+      </c>
+      <c r="L219">
+        <v>2935600</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12">
+      <c r="A220">
+        <v>217</v>
+      </c>
+      <c r="B220">
+        <v>626402</v>
+      </c>
+      <c r="C220" t="s">
+        <v>13</v>
+      </c>
+      <c r="D220" t="s">
+        <v>351</v>
+      </c>
+      <c r="E220" t="s">
+        <v>382</v>
+      </c>
+      <c r="F220" t="s">
+        <v>383</v>
+      </c>
+      <c r="G220" t="s">
+        <v>384</v>
+      </c>
+      <c r="H220" t="s">
+        <v>386</v>
+      </c>
+      <c r="I220" t="s">
+        <v>19</v>
+      </c>
+      <c r="J220">
+        <v>1</v>
+      </c>
+      <c r="K220">
+        <v>108631940</v>
+      </c>
+      <c r="L220">
+        <v>108631940</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12">
+      <c r="A221">
+        <v>218</v>
+      </c>
+      <c r="B221">
+        <v>626402</v>
+      </c>
+      <c r="C221" t="s">
+        <v>13</v>
+      </c>
+      <c r="D221" t="s">
+        <v>351</v>
+      </c>
+      <c r="E221" t="s">
+        <v>382</v>
+      </c>
+      <c r="F221" t="s">
+        <v>383</v>
+      </c>
+      <c r="G221" t="s">
+        <v>384</v>
+      </c>
+      <c r="H221" t="s">
+        <v>387</v>
+      </c>
+      <c r="I221" t="s">
+        <v>19</v>
+      </c>
+      <c r="J221">
+        <v>1</v>
+      </c>
+      <c r="K221">
+        <v>150000</v>
+      </c>
+      <c r="L221">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12">
+      <c r="A222">
+        <v>219</v>
+      </c>
+      <c r="B222">
+        <v>626402</v>
+      </c>
+      <c r="C222" t="s">
+        <v>13</v>
+      </c>
+      <c r="D222" t="s">
+        <v>364</v>
+      </c>
+      <c r="E222" t="s">
+        <v>388</v>
+      </c>
+      <c r="F222" t="s">
+        <v>389</v>
+      </c>
+      <c r="G222" t="s">
+        <v>390</v>
+      </c>
+      <c r="H222" t="s">
+        <v>391</v>
+      </c>
+      <c r="I222" t="s">
+        <v>19</v>
+      </c>
+      <c r="J222">
+        <v>1</v>
+      </c>
+      <c r="K222">
+        <v>5311350</v>
+      </c>
+      <c r="L222">
+        <v>5311350</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12">
+      <c r="A223">
+        <v>220</v>
+      </c>
+      <c r="B223">
+        <v>626402</v>
+      </c>
+      <c r="C223" t="s">
+        <v>13</v>
+      </c>
+      <c r="D223" t="s">
+        <v>351</v>
+      </c>
+      <c r="E223" t="s">
+        <v>392</v>
+      </c>
+      <c r="F223" t="s">
+        <v>393</v>
+      </c>
+      <c r="G223" t="s">
+        <v>394</v>
+      </c>
+      <c r="H223" t="s">
+        <v>395</v>
+      </c>
+      <c r="I223" t="s">
+        <v>19</v>
+      </c>
+      <c r="J223">
+        <v>1</v>
+      </c>
+      <c r="K223">
+        <v>198871146</v>
+      </c>
+      <c r="L223">
+        <v>198871146</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12">
+      <c r="A224">
+        <v>221</v>
+      </c>
+      <c r="B224">
+        <v>626402</v>
+      </c>
+      <c r="C224" t="s">
+        <v>13</v>
+      </c>
+      <c r="D224" t="s">
+        <v>351</v>
+      </c>
+      <c r="E224" t="s">
+        <v>396</v>
+      </c>
+      <c r="F224" t="s">
+        <v>397</v>
+      </c>
+      <c r="G224" t="s">
+        <v>398</v>
+      </c>
+      <c r="H224" t="s">
+        <v>399</v>
+      </c>
+      <c r="I224" t="s">
+        <v>19</v>
+      </c>
+      <c r="J224">
+        <v>1</v>
+      </c>
+      <c r="K224">
+        <v>412680289</v>
+      </c>
+      <c r="L224">
+        <v>412680289</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12">
+      <c r="A225">
+        <v>222</v>
+      </c>
+      <c r="B225">
+        <v>626402</v>
+      </c>
+      <c r="C225" t="s">
+        <v>13</v>
+      </c>
+      <c r="D225" t="s">
+        <v>351</v>
+      </c>
+      <c r="E225" t="s">
+        <v>400</v>
+      </c>
+      <c r="F225" t="s">
+        <v>401</v>
+      </c>
+      <c r="G225" t="s">
+        <v>402</v>
+      </c>
+      <c r="H225" t="s">
         <v>80</v>
       </c>
-      <c r="I209" t="s">
-        <v>19</v>
-      </c>
-      <c r="J209">
-        <v>1</v>
-      </c>
-      <c r="K209">
+      <c r="I225" t="s">
+        <v>19</v>
+      </c>
+      <c r="J225">
+        <v>1</v>
+      </c>
+      <c r="K225">
         <v>203211317</v>
       </c>
-      <c r="L209">
+      <c r="L225">
         <v>203211317</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12">
+      <c r="A226">
+        <v>223</v>
+      </c>
+      <c r="B226">
+        <v>626402</v>
+      </c>
+      <c r="C226" t="s">
+        <v>13</v>
+      </c>
+      <c r="D226" t="s">
+        <v>351</v>
+      </c>
+      <c r="E226" t="s">
+        <v>403</v>
+      </c>
+      <c r="F226" t="s">
+        <v>404</v>
+      </c>
+      <c r="G226" t="s">
+        <v>405</v>
+      </c>
+      <c r="H226" t="s">
+        <v>318</v>
+      </c>
+      <c r="I226" t="s">
+        <v>19</v>
+      </c>
+      <c r="J226">
+        <v>1</v>
+      </c>
+      <c r="K226">
+        <v>4931320</v>
+      </c>
+      <c r="L226">
+        <v>4931320</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12">
+      <c r="A227">
+        <v>224</v>
+      </c>
+      <c r="B227">
+        <v>626402</v>
+      </c>
+      <c r="C227" t="s">
+        <v>13</v>
+      </c>
+      <c r="D227" t="s">
+        <v>351</v>
+      </c>
+      <c r="E227" t="s">
+        <v>403</v>
+      </c>
+      <c r="F227" t="s">
+        <v>404</v>
+      </c>
+      <c r="G227" t="s">
+        <v>405</v>
+      </c>
+      <c r="H227" t="s">
+        <v>274</v>
+      </c>
+      <c r="I227" t="s">
+        <v>19</v>
+      </c>
+      <c r="J227">
+        <v>1</v>
+      </c>
+      <c r="K227">
+        <v>27862906</v>
+      </c>
+      <c r="L227">
+        <v>27862906</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12">
+      <c r="A228">
+        <v>225</v>
+      </c>
+      <c r="B228">
+        <v>626402</v>
+      </c>
+      <c r="C228" t="s">
+        <v>13</v>
+      </c>
+      <c r="D228" t="s">
+        <v>364</v>
+      </c>
+      <c r="E228" t="s">
+        <v>406</v>
+      </c>
+      <c r="F228" t="s">
+        <v>407</v>
+      </c>
+      <c r="G228" t="s">
+        <v>408</v>
+      </c>
+      <c r="H228" t="s">
+        <v>409</v>
+      </c>
+      <c r="I228" t="s">
+        <v>19</v>
+      </c>
+      <c r="J228">
+        <v>1</v>
+      </c>
+      <c r="K228">
+        <v>219712619</v>
+      </c>
+      <c r="L228">
+        <v>219712619</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12">
+      <c r="A229">
+        <v>226</v>
+      </c>
+      <c r="B229">
+        <v>626402</v>
+      </c>
+      <c r="C229" t="s">
+        <v>13</v>
+      </c>
+      <c r="D229" t="s">
+        <v>364</v>
+      </c>
+      <c r="E229" t="s">
+        <v>410</v>
+      </c>
+      <c r="F229" t="s">
+        <v>411</v>
+      </c>
+      <c r="G229" t="s">
+        <v>412</v>
+      </c>
+      <c r="H229" t="s">
+        <v>413</v>
+      </c>
+      <c r="I229" t="s">
+        <v>19</v>
+      </c>
+      <c r="J229">
+        <v>1</v>
+      </c>
+      <c r="K229">
+        <v>162678384</v>
+      </c>
+      <c r="L229">
+        <v>162678384</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12">
+      <c r="A230">
+        <v>227</v>
+      </c>
+      <c r="B230">
+        <v>626402</v>
+      </c>
+      <c r="C230" t="s">
+        <v>13</v>
+      </c>
+      <c r="D230" t="s">
+        <v>364</v>
+      </c>
+      <c r="E230" t="s">
+        <v>414</v>
+      </c>
+      <c r="F230" t="s">
+        <v>415</v>
+      </c>
+      <c r="G230" t="s">
+        <v>416</v>
+      </c>
+      <c r="H230" t="s">
+        <v>417</v>
+      </c>
+      <c r="I230" t="s">
+        <v>19</v>
+      </c>
+      <c r="J230">
+        <v>1</v>
+      </c>
+      <c r="K230">
+        <v>680000</v>
+      </c>
+      <c r="L230">
+        <v>680000</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12">
+      <c r="A231">
+        <v>228</v>
+      </c>
+      <c r="B231">
+        <v>626402</v>
+      </c>
+      <c r="C231" t="s">
+        <v>13</v>
+      </c>
+      <c r="D231" t="s">
+        <v>364</v>
+      </c>
+      <c r="E231" t="s">
+        <v>414</v>
+      </c>
+      <c r="F231" t="s">
+        <v>415</v>
+      </c>
+      <c r="G231" t="s">
+        <v>416</v>
+      </c>
+      <c r="H231" t="s">
+        <v>418</v>
+      </c>
+      <c r="I231" t="s">
+        <v>19</v>
+      </c>
+      <c r="J231">
+        <v>1</v>
+      </c>
+      <c r="K231">
+        <v>520000</v>
+      </c>
+      <c r="L231">
+        <v>520000</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12">
+      <c r="A232">
+        <v>229</v>
+      </c>
+      <c r="B232">
+        <v>626402</v>
+      </c>
+      <c r="C232" t="s">
+        <v>13</v>
+      </c>
+      <c r="D232" t="s">
+        <v>364</v>
+      </c>
+      <c r="E232" t="s">
+        <v>414</v>
+      </c>
+      <c r="F232" t="s">
+        <v>415</v>
+      </c>
+      <c r="G232" t="s">
+        <v>416</v>
+      </c>
+      <c r="H232" t="s">
+        <v>331</v>
+      </c>
+      <c r="I232" t="s">
+        <v>19</v>
+      </c>
+      <c r="J232">
+        <v>1</v>
+      </c>
+      <c r="K232">
+        <v>23600000</v>
+      </c>
+      <c r="L232">
+        <v>23600000</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12">
+      <c r="A233">
+        <v>230</v>
+      </c>
+      <c r="B233">
+        <v>626402</v>
+      </c>
+      <c r="C233" t="s">
+        <v>13</v>
+      </c>
+      <c r="D233" t="s">
+        <v>364</v>
+      </c>
+      <c r="E233" t="s">
+        <v>414</v>
+      </c>
+      <c r="F233" t="s">
+        <v>415</v>
+      </c>
+      <c r="G233" t="s">
+        <v>416</v>
+      </c>
+      <c r="H233" t="s">
+        <v>109</v>
+      </c>
+      <c r="I233" t="s">
+        <v>19</v>
+      </c>
+      <c r="J233">
+        <v>1</v>
+      </c>
+      <c r="K233">
+        <v>6610000</v>
+      </c>
+      <c r="L233">
+        <v>6610000</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12">
+      <c r="A234">
+        <v>231</v>
+      </c>
+      <c r="B234">
+        <v>626402</v>
+      </c>
+      <c r="C234" t="s">
+        <v>13</v>
+      </c>
+      <c r="D234" t="s">
+        <v>364</v>
+      </c>
+      <c r="E234" t="s">
+        <v>419</v>
+      </c>
+      <c r="F234" t="s">
+        <v>420</v>
+      </c>
+      <c r="G234" t="s">
+        <v>421</v>
+      </c>
+      <c r="H234" t="s">
+        <v>269</v>
+      </c>
+      <c r="I234" t="s">
+        <v>19</v>
+      </c>
+      <c r="J234">
+        <v>1</v>
+      </c>
+      <c r="K234">
+        <v>4828500</v>
+      </c>
+      <c r="L234">
+        <v>4828500</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12">
+      <c r="A235">
+        <v>232</v>
+      </c>
+      <c r="B235">
+        <v>626402</v>
+      </c>
+      <c r="C235" t="s">
+        <v>13</v>
+      </c>
+      <c r="D235" t="s">
+        <v>364</v>
+      </c>
+      <c r="E235" t="s">
+        <v>422</v>
+      </c>
+      <c r="F235" t="s">
+        <v>423</v>
+      </c>
+      <c r="G235" t="s">
+        <v>424</v>
+      </c>
+      <c r="H235" t="s">
+        <v>425</v>
+      </c>
+      <c r="I235" t="s">
+        <v>19</v>
+      </c>
+      <c r="J235">
+        <v>1</v>
+      </c>
+      <c r="K235">
+        <v>825000</v>
+      </c>
+      <c r="L235">
+        <v>825000</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12">
+      <c r="A236">
+        <v>233</v>
+      </c>
+      <c r="B236">
+        <v>626402</v>
+      </c>
+      <c r="C236" t="s">
+        <v>13</v>
+      </c>
+      <c r="D236" t="s">
+        <v>351</v>
+      </c>
+      <c r="E236" t="s">
+        <v>426</v>
+      </c>
+      <c r="F236" t="s">
+        <v>427</v>
+      </c>
+      <c r="G236" t="s">
+        <v>428</v>
+      </c>
+      <c r="H236" t="s">
+        <v>254</v>
+      </c>
+      <c r="I236" t="s">
+        <v>19</v>
+      </c>
+      <c r="J236">
+        <v>1</v>
+      </c>
+      <c r="K236">
+        <v>23400000</v>
+      </c>
+      <c r="L236">
+        <v>23400000</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12">
+      <c r="A237">
+        <v>234</v>
+      </c>
+      <c r="B237">
+        <v>626402</v>
+      </c>
+      <c r="C237" t="s">
+        <v>13</v>
+      </c>
+      <c r="D237" t="s">
+        <v>351</v>
+      </c>
+      <c r="E237" t="s">
+        <v>426</v>
+      </c>
+      <c r="F237" t="s">
+        <v>427</v>
+      </c>
+      <c r="G237" t="s">
+        <v>428</v>
+      </c>
+      <c r="H237" t="s">
+        <v>429</v>
+      </c>
+      <c r="I237" t="s">
+        <v>19</v>
+      </c>
+      <c r="J237">
+        <v>1</v>
+      </c>
+      <c r="K237">
+        <v>22460000</v>
+      </c>
+      <c r="L237">
+        <v>22460000</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12">
+      <c r="A238">
+        <v>235</v>
+      </c>
+      <c r="B238">
+        <v>626402</v>
+      </c>
+      <c r="C238" t="s">
+        <v>13</v>
+      </c>
+      <c r="D238" t="s">
+        <v>351</v>
+      </c>
+      <c r="E238" t="s">
+        <v>426</v>
+      </c>
+      <c r="F238" t="s">
+        <v>427</v>
+      </c>
+      <c r="G238" t="s">
+        <v>428</v>
+      </c>
+      <c r="H238" t="s">
+        <v>430</v>
+      </c>
+      <c r="I238" t="s">
+        <v>19</v>
+      </c>
+      <c r="J238">
+        <v>1</v>
+      </c>
+      <c r="K238">
+        <v>40832000</v>
+      </c>
+      <c r="L238">
+        <v>40832000</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12">
+      <c r="A239">
+        <v>236</v>
+      </c>
+      <c r="B239">
+        <v>626402</v>
+      </c>
+      <c r="C239" t="s">
+        <v>13</v>
+      </c>
+      <c r="D239" t="s">
+        <v>351</v>
+      </c>
+      <c r="E239" t="s">
+        <v>426</v>
+      </c>
+      <c r="F239" t="s">
+        <v>427</v>
+      </c>
+      <c r="G239" t="s">
+        <v>428</v>
+      </c>
+      <c r="H239" t="s">
+        <v>431</v>
+      </c>
+      <c r="I239" t="s">
+        <v>19</v>
+      </c>
+      <c r="J239">
+        <v>1</v>
+      </c>
+      <c r="K239">
+        <v>750000</v>
+      </c>
+      <c r="L239">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12">
+      <c r="A240">
+        <v>237</v>
+      </c>
+      <c r="B240">
+        <v>626402</v>
+      </c>
+      <c r="C240" t="s">
+        <v>13</v>
+      </c>
+      <c r="D240" t="s">
+        <v>351</v>
+      </c>
+      <c r="E240" t="s">
+        <v>426</v>
+      </c>
+      <c r="F240" t="s">
+        <v>427</v>
+      </c>
+      <c r="G240" t="s">
+        <v>428</v>
+      </c>
+      <c r="H240" t="s">
+        <v>391</v>
+      </c>
+      <c r="I240" t="s">
+        <v>19</v>
+      </c>
+      <c r="J240">
+        <v>1</v>
+      </c>
+      <c r="K240">
+        <v>12243300</v>
+      </c>
+      <c r="L240">
+        <v>12243300</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12">
+      <c r="A241">
+        <v>238</v>
+      </c>
+      <c r="B241">
+        <v>626402</v>
+      </c>
+      <c r="C241" t="s">
+        <v>13</v>
+      </c>
+      <c r="D241" t="s">
+        <v>351</v>
+      </c>
+      <c r="E241" t="s">
+        <v>426</v>
+      </c>
+      <c r="F241" t="s">
+        <v>427</v>
+      </c>
+      <c r="G241" t="s">
+        <v>428</v>
+      </c>
+      <c r="H241" t="s">
+        <v>269</v>
+      </c>
+      <c r="I241" t="s">
+        <v>19</v>
+      </c>
+      <c r="J241">
+        <v>1</v>
+      </c>
+      <c r="K241">
+        <v>152000</v>
+      </c>
+      <c r="L241">
+        <v>152000</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12">
+      <c r="A242">
+        <v>239</v>
+      </c>
+      <c r="B242">
+        <v>626402</v>
+      </c>
+      <c r="C242" t="s">
+        <v>13</v>
+      </c>
+      <c r="D242" t="s">
+        <v>364</v>
+      </c>
+      <c r="E242" t="s">
+        <v>432</v>
+      </c>
+      <c r="F242" t="s">
+        <v>433</v>
+      </c>
+      <c r="G242" t="s">
+        <v>434</v>
+      </c>
+      <c r="H242" t="s">
+        <v>435</v>
+      </c>
+      <c r="I242" t="s">
+        <v>19</v>
+      </c>
+      <c r="J242">
+        <v>1</v>
+      </c>
+      <c r="K242">
+        <v>4828000</v>
+      </c>
+      <c r="L242">
+        <v>4828000</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12">
+      <c r="A243">
+        <v>240</v>
+      </c>
+      <c r="B243">
+        <v>626402</v>
+      </c>
+      <c r="C243" t="s">
+        <v>13</v>
+      </c>
+      <c r="D243" t="s">
+        <v>364</v>
+      </c>
+      <c r="E243" t="s">
+        <v>432</v>
+      </c>
+      <c r="F243" t="s">
+        <v>433</v>
+      </c>
+      <c r="G243" t="s">
+        <v>434</v>
+      </c>
+      <c r="H243" t="s">
+        <v>436</v>
+      </c>
+      <c r="I243" t="s">
+        <v>19</v>
+      </c>
+      <c r="J243">
+        <v>1</v>
+      </c>
+      <c r="K243">
+        <v>516000</v>
+      </c>
+      <c r="L243">
+        <v>516000</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12">
+      <c r="A244">
+        <v>241</v>
+      </c>
+      <c r="B244">
+        <v>626402</v>
+      </c>
+      <c r="C244" t="s">
+        <v>13</v>
+      </c>
+      <c r="D244" t="s">
+        <v>364</v>
+      </c>
+      <c r="E244" t="s">
+        <v>432</v>
+      </c>
+      <c r="F244" t="s">
+        <v>433</v>
+      </c>
+      <c r="G244" t="s">
+        <v>434</v>
+      </c>
+      <c r="H244" t="s">
+        <v>437</v>
+      </c>
+      <c r="I244" t="s">
+        <v>19</v>
+      </c>
+      <c r="J244">
+        <v>1</v>
+      </c>
+      <c r="K244">
+        <v>220000</v>
+      </c>
+      <c r="L244">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12">
+      <c r="A245">
+        <v>242</v>
+      </c>
+      <c r="B245">
+        <v>626402</v>
+      </c>
+      <c r="C245" t="s">
+        <v>13</v>
+      </c>
+      <c r="D245" t="s">
+        <v>364</v>
+      </c>
+      <c r="E245" t="s">
+        <v>432</v>
+      </c>
+      <c r="F245" t="s">
+        <v>433</v>
+      </c>
+      <c r="G245" t="s">
+        <v>434</v>
+      </c>
+      <c r="H245" t="s">
+        <v>438</v>
+      </c>
+      <c r="I245" t="s">
+        <v>19</v>
+      </c>
+      <c r="J245">
+        <v>1</v>
+      </c>
+      <c r="K245">
+        <v>1680000</v>
+      </c>
+      <c r="L245">
+        <v>1680000</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12">
+      <c r="A246">
+        <v>243</v>
+      </c>
+      <c r="B246">
+        <v>626402</v>
+      </c>
+      <c r="C246" t="s">
+        <v>13</v>
+      </c>
+      <c r="D246" t="s">
+        <v>364</v>
+      </c>
+      <c r="E246" t="s">
+        <v>432</v>
+      </c>
+      <c r="F246" t="s">
+        <v>433</v>
+      </c>
+      <c r="G246" t="s">
+        <v>434</v>
+      </c>
+      <c r="H246" t="s">
+        <v>439</v>
+      </c>
+      <c r="I246" t="s">
+        <v>19</v>
+      </c>
+      <c r="J246">
+        <v>1</v>
+      </c>
+      <c r="K246">
+        <v>3000000</v>
+      </c>
+      <c r="L246">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12">
+      <c r="A247">
+        <v>244</v>
+      </c>
+      <c r="B247">
+        <v>626402</v>
+      </c>
+      <c r="C247" t="s">
+        <v>13</v>
+      </c>
+      <c r="D247" t="s">
+        <v>364</v>
+      </c>
+      <c r="E247" t="s">
+        <v>432</v>
+      </c>
+      <c r="F247" t="s">
+        <v>433</v>
+      </c>
+      <c r="G247" t="s">
+        <v>434</v>
+      </c>
+      <c r="H247" t="s">
+        <v>440</v>
+      </c>
+      <c r="I247" t="s">
+        <v>19</v>
+      </c>
+      <c r="J247">
+        <v>1</v>
+      </c>
+      <c r="K247">
+        <v>1870000</v>
+      </c>
+      <c r="L247">
+        <v>1870000</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12">
+      <c r="A248">
+        <v>245</v>
+      </c>
+      <c r="B248">
+        <v>626402</v>
+      </c>
+      <c r="C248" t="s">
+        <v>13</v>
+      </c>
+      <c r="D248" t="s">
+        <v>364</v>
+      </c>
+      <c r="E248" t="s">
+        <v>432</v>
+      </c>
+      <c r="F248" t="s">
+        <v>433</v>
+      </c>
+      <c r="G248" t="s">
+        <v>434</v>
+      </c>
+      <c r="H248" t="s">
+        <v>441</v>
+      </c>
+      <c r="I248" t="s">
+        <v>19</v>
+      </c>
+      <c r="J248">
+        <v>1</v>
+      </c>
+      <c r="K248">
+        <v>876000</v>
+      </c>
+      <c r="L248">
+        <v>876000</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12">
+      <c r="A249">
+        <v>246</v>
+      </c>
+      <c r="B249">
+        <v>626402</v>
+      </c>
+      <c r="C249" t="s">
+        <v>13</v>
+      </c>
+      <c r="D249" t="s">
+        <v>364</v>
+      </c>
+      <c r="E249" t="s">
+        <v>432</v>
+      </c>
+      <c r="F249" t="s">
+        <v>433</v>
+      </c>
+      <c r="G249" t="s">
+        <v>434</v>
+      </c>
+      <c r="H249" t="s">
+        <v>442</v>
+      </c>
+      <c r="I249" t="s">
+        <v>19</v>
+      </c>
+      <c r="J249">
+        <v>1</v>
+      </c>
+      <c r="K249">
+        <v>1077500</v>
+      </c>
+      <c r="L249">
+        <v>1077500</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12">
+      <c r="A250">
+        <v>247</v>
+      </c>
+      <c r="B250">
+        <v>626402</v>
+      </c>
+      <c r="C250" t="s">
+        <v>13</v>
+      </c>
+      <c r="D250" t="s">
+        <v>364</v>
+      </c>
+      <c r="E250" t="s">
+        <v>432</v>
+      </c>
+      <c r="F250" t="s">
+        <v>433</v>
+      </c>
+      <c r="G250" t="s">
+        <v>434</v>
+      </c>
+      <c r="H250" t="s">
+        <v>443</v>
+      </c>
+      <c r="I250" t="s">
+        <v>19</v>
+      </c>
+      <c r="J250">
+        <v>1</v>
+      </c>
+      <c r="K250">
+        <v>2360000</v>
+      </c>
+      <c r="L250">
+        <v>2360000</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12">
+      <c r="A251">
+        <v>248</v>
+      </c>
+      <c r="B251">
+        <v>626402</v>
+      </c>
+      <c r="C251" t="s">
+        <v>13</v>
+      </c>
+      <c r="D251" t="s">
+        <v>364</v>
+      </c>
+      <c r="E251" t="s">
+        <v>432</v>
+      </c>
+      <c r="F251" t="s">
+        <v>433</v>
+      </c>
+      <c r="G251" t="s">
+        <v>434</v>
+      </c>
+      <c r="H251" t="s">
+        <v>444</v>
+      </c>
+      <c r="I251" t="s">
+        <v>19</v>
+      </c>
+      <c r="J251">
+        <v>1</v>
+      </c>
+      <c r="K251">
+        <v>990000</v>
+      </c>
+      <c r="L251">
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12">
+      <c r="A252">
+        <v>249</v>
+      </c>
+      <c r="B252">
+        <v>626402</v>
+      </c>
+      <c r="C252" t="s">
+        <v>13</v>
+      </c>
+      <c r="D252" t="s">
+        <v>364</v>
+      </c>
+      <c r="E252" t="s">
+        <v>432</v>
+      </c>
+      <c r="F252" t="s">
+        <v>433</v>
+      </c>
+      <c r="G252" t="s">
+        <v>434</v>
+      </c>
+      <c r="H252" t="s">
+        <v>445</v>
+      </c>
+      <c r="I252" t="s">
+        <v>19</v>
+      </c>
+      <c r="J252">
+        <v>1</v>
+      </c>
+      <c r="K252">
+        <v>1000000</v>
+      </c>
+      <c r="L252">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12">
+      <c r="A253">
+        <v>250</v>
+      </c>
+      <c r="B253">
+        <v>626402</v>
+      </c>
+      <c r="C253" t="s">
+        <v>13</v>
+      </c>
+      <c r="D253" t="s">
+        <v>364</v>
+      </c>
+      <c r="E253" t="s">
+        <v>432</v>
+      </c>
+      <c r="F253" t="s">
+        <v>433</v>
+      </c>
+      <c r="G253" t="s">
+        <v>434</v>
+      </c>
+      <c r="H253" t="s">
+        <v>446</v>
+      </c>
+      <c r="I253" t="s">
+        <v>19</v>
+      </c>
+      <c r="J253">
+        <v>1</v>
+      </c>
+      <c r="K253">
+        <v>1720000</v>
+      </c>
+      <c r="L253">
+        <v>1720000</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12">
+      <c r="A254">
+        <v>251</v>
+      </c>
+      <c r="B254">
+        <v>626402</v>
+      </c>
+      <c r="C254" t="s">
+        <v>13</v>
+      </c>
+      <c r="D254" t="s">
+        <v>364</v>
+      </c>
+      <c r="E254" t="s">
+        <v>432</v>
+      </c>
+      <c r="F254" t="s">
+        <v>433</v>
+      </c>
+      <c r="G254" t="s">
+        <v>434</v>
+      </c>
+      <c r="H254" t="s">
+        <v>447</v>
+      </c>
+      <c r="I254" t="s">
+        <v>19</v>
+      </c>
+      <c r="J254">
+        <v>1</v>
+      </c>
+      <c r="K254">
+        <v>798900</v>
+      </c>
+      <c r="L254">
+        <v>798900</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12">
+      <c r="A255">
+        <v>252</v>
+      </c>
+      <c r="B255">
+        <v>626402</v>
+      </c>
+      <c r="C255" t="s">
+        <v>13</v>
+      </c>
+      <c r="D255" t="s">
+        <v>364</v>
+      </c>
+      <c r="E255" t="s">
+        <v>432</v>
+      </c>
+      <c r="F255" t="s">
+        <v>433</v>
+      </c>
+      <c r="G255" t="s">
+        <v>434</v>
+      </c>
+      <c r="H255" t="s">
+        <v>234</v>
+      </c>
+      <c r="I255" t="s">
+        <v>19</v>
+      </c>
+      <c r="J255">
+        <v>1</v>
+      </c>
+      <c r="K255">
+        <v>2496920</v>
+      </c>
+      <c r="L255">
+        <v>2496920</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12">
+      <c r="A256">
+        <v>253</v>
+      </c>
+      <c r="B256">
+        <v>626402</v>
+      </c>
+      <c r="C256" t="s">
+        <v>13</v>
+      </c>
+      <c r="D256" t="s">
+        <v>364</v>
+      </c>
+      <c r="E256" t="s">
+        <v>432</v>
+      </c>
+      <c r="F256" t="s">
+        <v>433</v>
+      </c>
+      <c r="G256" t="s">
+        <v>434</v>
+      </c>
+      <c r="H256" t="s">
+        <v>236</v>
+      </c>
+      <c r="I256" t="s">
+        <v>19</v>
+      </c>
+      <c r="J256">
+        <v>1</v>
+      </c>
+      <c r="K256">
+        <v>1080000</v>
+      </c>
+      <c r="L256">
+        <v>1080000</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12">
+      <c r="A257">
+        <v>254</v>
+      </c>
+      <c r="B257">
+        <v>626402</v>
+      </c>
+      <c r="C257" t="s">
+        <v>13</v>
+      </c>
+      <c r="D257" t="s">
+        <v>364</v>
+      </c>
+      <c r="E257" t="s">
+        <v>432</v>
+      </c>
+      <c r="F257" t="s">
+        <v>433</v>
+      </c>
+      <c r="G257" t="s">
+        <v>434</v>
+      </c>
+      <c r="H257" t="s">
+        <v>237</v>
+      </c>
+      <c r="I257" t="s">
+        <v>19</v>
+      </c>
+      <c r="J257">
+        <v>1</v>
+      </c>
+      <c r="K257">
+        <v>205500</v>
+      </c>
+      <c r="L257">
+        <v>205500</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12">
+      <c r="A258">
+        <v>255</v>
+      </c>
+      <c r="B258">
+        <v>626402</v>
+      </c>
+      <c r="C258" t="s">
+        <v>13</v>
+      </c>
+      <c r="D258" t="s">
+        <v>364</v>
+      </c>
+      <c r="E258" t="s">
+        <v>432</v>
+      </c>
+      <c r="F258" t="s">
+        <v>433</v>
+      </c>
+      <c r="G258" t="s">
+        <v>434</v>
+      </c>
+      <c r="H258" t="s">
+        <v>448</v>
+      </c>
+      <c r="I258" t="s">
+        <v>19</v>
+      </c>
+      <c r="J258">
+        <v>1</v>
+      </c>
+      <c r="K258">
+        <v>370000</v>
+      </c>
+      <c r="L258">
+        <v>370000</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12">
+      <c r="A259">
+        <v>256</v>
+      </c>
+      <c r="B259">
+        <v>626402</v>
+      </c>
+      <c r="C259" t="s">
+        <v>13</v>
+      </c>
+      <c r="D259" t="s">
+        <v>364</v>
+      </c>
+      <c r="E259" t="s">
+        <v>432</v>
+      </c>
+      <c r="F259" t="s">
+        <v>433</v>
+      </c>
+      <c r="G259" t="s">
+        <v>434</v>
+      </c>
+      <c r="H259" t="s">
+        <v>449</v>
+      </c>
+      <c r="I259" t="s">
+        <v>19</v>
+      </c>
+      <c r="J259">
+        <v>1</v>
+      </c>
+      <c r="K259">
+        <v>517500</v>
+      </c>
+      <c r="L259">
+        <v>517500</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12">
+      <c r="A260">
+        <v>257</v>
+      </c>
+      <c r="B260">
+        <v>626402</v>
+      </c>
+      <c r="C260" t="s">
+        <v>13</v>
+      </c>
+      <c r="D260" t="s">
+        <v>364</v>
+      </c>
+      <c r="E260" t="s">
+        <v>432</v>
+      </c>
+      <c r="F260" t="s">
+        <v>433</v>
+      </c>
+      <c r="G260" t="s">
+        <v>434</v>
+      </c>
+      <c r="H260" t="s">
+        <v>368</v>
+      </c>
+      <c r="I260" t="s">
+        <v>19</v>
+      </c>
+      <c r="J260">
+        <v>1</v>
+      </c>
+      <c r="K260">
+        <v>2340000</v>
+      </c>
+      <c r="L260">
+        <v>2340000</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12">
+      <c r="A261">
+        <v>258</v>
+      </c>
+      <c r="B261">
+        <v>626402</v>
+      </c>
+      <c r="C261" t="s">
+        <v>13</v>
+      </c>
+      <c r="D261" t="s">
+        <v>364</v>
+      </c>
+      <c r="E261" t="s">
+        <v>432</v>
+      </c>
+      <c r="F261" t="s">
+        <v>433</v>
+      </c>
+      <c r="G261" t="s">
+        <v>434</v>
+      </c>
+      <c r="H261" t="s">
+        <v>363</v>
+      </c>
+      <c r="I261" t="s">
+        <v>19</v>
+      </c>
+      <c r="J261">
+        <v>1</v>
+      </c>
+      <c r="K261">
+        <v>3060000</v>
+      </c>
+      <c r="L261">
+        <v>3060000</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12">
+      <c r="A262">
+        <v>259</v>
+      </c>
+      <c r="B262">
+        <v>626402</v>
+      </c>
+      <c r="C262" t="s">
+        <v>13</v>
+      </c>
+      <c r="D262" t="s">
+        <v>364</v>
+      </c>
+      <c r="E262" t="s">
+        <v>432</v>
+      </c>
+      <c r="F262" t="s">
+        <v>433</v>
+      </c>
+      <c r="G262" t="s">
+        <v>434</v>
+      </c>
+      <c r="H262" t="s">
+        <v>450</v>
+      </c>
+      <c r="I262" t="s">
+        <v>19</v>
+      </c>
+      <c r="J262">
+        <v>1</v>
+      </c>
+      <c r="K262">
+        <v>3430000</v>
+      </c>
+      <c r="L262">
+        <v>3430000</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12">
+      <c r="A263">
+        <v>260</v>
+      </c>
+      <c r="B263">
+        <v>626402</v>
+      </c>
+      <c r="C263" t="s">
+        <v>13</v>
+      </c>
+      <c r="D263" t="s">
+        <v>364</v>
+      </c>
+      <c r="E263" t="s">
+        <v>432</v>
+      </c>
+      <c r="F263" t="s">
+        <v>433</v>
+      </c>
+      <c r="G263" t="s">
+        <v>434</v>
+      </c>
+      <c r="H263" t="s">
+        <v>451</v>
+      </c>
+      <c r="I263" t="s">
+        <v>19</v>
+      </c>
+      <c r="J263">
+        <v>1</v>
+      </c>
+      <c r="K263">
+        <v>3000000</v>
+      </c>
+      <c r="L263">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12">
+      <c r="A264">
+        <v>261</v>
+      </c>
+      <c r="B264">
+        <v>626402</v>
+      </c>
+      <c r="C264" t="s">
+        <v>13</v>
+      </c>
+      <c r="D264" t="s">
+        <v>364</v>
+      </c>
+      <c r="E264" t="s">
+        <v>432</v>
+      </c>
+      <c r="F264" t="s">
+        <v>433</v>
+      </c>
+      <c r="G264" t="s">
+        <v>434</v>
+      </c>
+      <c r="H264" t="s">
+        <v>452</v>
+      </c>
+      <c r="I264" t="s">
+        <v>19</v>
+      </c>
+      <c r="J264">
+        <v>1</v>
+      </c>
+      <c r="K264">
+        <v>4618753</v>
+      </c>
+      <c r="L264">
+        <v>4618753</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12">
+      <c r="A265">
+        <v>262</v>
+      </c>
+      <c r="B265">
+        <v>626402</v>
+      </c>
+      <c r="C265" t="s">
+        <v>13</v>
+      </c>
+      <c r="D265" t="s">
+        <v>364</v>
+      </c>
+      <c r="E265" t="s">
+        <v>432</v>
+      </c>
+      <c r="F265" t="s">
+        <v>433</v>
+      </c>
+      <c r="G265" t="s">
+        <v>434</v>
+      </c>
+      <c r="H265" t="s">
+        <v>453</v>
+      </c>
+      <c r="I265" t="s">
+        <v>19</v>
+      </c>
+      <c r="J265">
+        <v>1</v>
+      </c>
+      <c r="K265">
+        <v>510000</v>
+      </c>
+      <c r="L265">
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12">
+      <c r="A266">
+        <v>263</v>
+      </c>
+      <c r="B266">
+        <v>626402</v>
+      </c>
+      <c r="C266" t="s">
+        <v>13</v>
+      </c>
+      <c r="D266" t="s">
+        <v>364</v>
+      </c>
+      <c r="E266" t="s">
+        <v>432</v>
+      </c>
+      <c r="F266" t="s">
+        <v>433</v>
+      </c>
+      <c r="G266" t="s">
+        <v>434</v>
+      </c>
+      <c r="H266" t="s">
+        <v>454</v>
+      </c>
+      <c r="I266" t="s">
+        <v>19</v>
+      </c>
+      <c r="J266">
+        <v>1</v>
+      </c>
+      <c r="K266">
+        <v>9081490</v>
+      </c>
+      <c r="L266">
+        <v>9081490</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12">
+      <c r="A267">
+        <v>264</v>
+      </c>
+      <c r="B267">
+        <v>626402</v>
+      </c>
+      <c r="C267" t="s">
+        <v>13</v>
+      </c>
+      <c r="D267" t="s">
+        <v>364</v>
+      </c>
+      <c r="E267" t="s">
+        <v>432</v>
+      </c>
+      <c r="F267" t="s">
+        <v>433</v>
+      </c>
+      <c r="G267" t="s">
+        <v>434</v>
+      </c>
+      <c r="H267" t="s">
+        <v>455</v>
+      </c>
+      <c r="I267" t="s">
+        <v>19</v>
+      </c>
+      <c r="J267">
+        <v>1</v>
+      </c>
+      <c r="K267">
+        <v>2380000</v>
+      </c>
+      <c r="L267">
+        <v>2380000</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12">
+      <c r="A268">
+        <v>265</v>
+      </c>
+      <c r="B268">
+        <v>626402</v>
+      </c>
+      <c r="C268" t="s">
+        <v>13</v>
+      </c>
+      <c r="D268" t="s">
+        <v>364</v>
+      </c>
+      <c r="E268" t="s">
+        <v>432</v>
+      </c>
+      <c r="F268" t="s">
+        <v>433</v>
+      </c>
+      <c r="G268" t="s">
+        <v>434</v>
+      </c>
+      <c r="H268" t="s">
+        <v>456</v>
+      </c>
+      <c r="I268" t="s">
+        <v>19</v>
+      </c>
+      <c r="J268">
+        <v>1</v>
+      </c>
+      <c r="K268">
+        <v>680000</v>
+      </c>
+      <c r="L268">
+        <v>680000</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12">
+      <c r="A269">
+        <v>266</v>
+      </c>
+      <c r="B269">
+        <v>626402</v>
+      </c>
+      <c r="C269" t="s">
+        <v>13</v>
+      </c>
+      <c r="D269" t="s">
+        <v>364</v>
+      </c>
+      <c r="E269" t="s">
+        <v>432</v>
+      </c>
+      <c r="F269" t="s">
+        <v>433</v>
+      </c>
+      <c r="G269" t="s">
+        <v>434</v>
+      </c>
+      <c r="H269" t="s">
+        <v>457</v>
+      </c>
+      <c r="I269" t="s">
+        <v>19</v>
+      </c>
+      <c r="J269">
+        <v>1</v>
+      </c>
+      <c r="K269">
+        <v>1190000</v>
+      </c>
+      <c r="L269">
+        <v>1190000</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12">
+      <c r="A270">
+        <v>267</v>
+      </c>
+      <c r="B270">
+        <v>626402</v>
+      </c>
+      <c r="C270" t="s">
+        <v>13</v>
+      </c>
+      <c r="D270" t="s">
+        <v>364</v>
+      </c>
+      <c r="E270" t="s">
+        <v>432</v>
+      </c>
+      <c r="F270" t="s">
+        <v>433</v>
+      </c>
+      <c r="G270" t="s">
+        <v>434</v>
+      </c>
+      <c r="H270" t="s">
+        <v>458</v>
+      </c>
+      <c r="I270" t="s">
+        <v>19</v>
+      </c>
+      <c r="J270">
+        <v>1</v>
+      </c>
+      <c r="K270">
+        <v>34500000</v>
+      </c>
+      <c r="L270">
+        <v>34500000</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12">
+      <c r="A271">
+        <v>268</v>
+      </c>
+      <c r="B271">
+        <v>626402</v>
+      </c>
+      <c r="C271" t="s">
+        <v>13</v>
+      </c>
+      <c r="D271" t="s">
+        <v>364</v>
+      </c>
+      <c r="E271" t="s">
+        <v>459</v>
+      </c>
+      <c r="F271" t="s">
+        <v>460</v>
+      </c>
+      <c r="G271" t="s">
+        <v>461</v>
+      </c>
+      <c r="H271" t="s">
+        <v>311</v>
+      </c>
+      <c r="I271" t="s">
+        <v>19</v>
+      </c>
+      <c r="J271">
+        <v>1</v>
+      </c>
+      <c r="K271">
+        <v>510000</v>
+      </c>
+      <c r="L271">
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12">
+      <c r="A272">
+        <v>269</v>
+      </c>
+      <c r="B272">
+        <v>626402</v>
+      </c>
+      <c r="C272" t="s">
+        <v>13</v>
+      </c>
+      <c r="D272" t="s">
+        <v>364</v>
+      </c>
+      <c r="E272" t="s">
+        <v>459</v>
+      </c>
+      <c r="F272" t="s">
+        <v>460</v>
+      </c>
+      <c r="G272" t="s">
+        <v>461</v>
+      </c>
+      <c r="H272" t="s">
+        <v>462</v>
+      </c>
+      <c r="I272" t="s">
+        <v>19</v>
+      </c>
+      <c r="J272">
+        <v>1</v>
+      </c>
+      <c r="K272">
+        <v>630000</v>
+      </c>
+      <c r="L272">
+        <v>630000</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12">
+      <c r="A273">
+        <v>270</v>
+      </c>
+      <c r="B273">
+        <v>626402</v>
+      </c>
+      <c r="C273" t="s">
+        <v>13</v>
+      </c>
+      <c r="D273" t="s">
+        <v>364</v>
+      </c>
+      <c r="E273" t="s">
+        <v>463</v>
+      </c>
+      <c r="F273" t="s">
+        <v>464</v>
+      </c>
+      <c r="G273" t="s">
+        <v>465</v>
+      </c>
+      <c r="H273" t="s">
+        <v>198</v>
+      </c>
+      <c r="I273" t="s">
+        <v>19</v>
+      </c>
+      <c r="J273">
+        <v>1</v>
+      </c>
+      <c r="K273">
+        <v>23018070</v>
+      </c>
+      <c r="L273">
+        <v>23018070</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12">
+      <c r="A274">
+        <v>271</v>
+      </c>
+      <c r="B274">
+        <v>626402</v>
+      </c>
+      <c r="C274" t="s">
+        <v>13</v>
+      </c>
+      <c r="D274" t="s">
+        <v>364</v>
+      </c>
+      <c r="E274" t="s">
+        <v>466</v>
+      </c>
+      <c r="F274" t="s">
+        <v>467</v>
+      </c>
+      <c r="G274" t="s">
+        <v>468</v>
+      </c>
+      <c r="H274" t="s">
+        <v>469</v>
+      </c>
+      <c r="I274" t="s">
+        <v>19</v>
+      </c>
+      <c r="J274">
+        <v>1</v>
+      </c>
+      <c r="K274">
+        <v>53000000</v>
+      </c>
+      <c r="L274">
+        <v>53000000</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12">
+      <c r="A275">
+        <v>272</v>
+      </c>
+      <c r="B275">
+        <v>626402</v>
+      </c>
+      <c r="C275" t="s">
+        <v>13</v>
+      </c>
+      <c r="D275" t="s">
+        <v>364</v>
+      </c>
+      <c r="E275" t="s">
+        <v>470</v>
+      </c>
+      <c r="F275" t="s">
+        <v>471</v>
+      </c>
+      <c r="G275" t="s">
+        <v>472</v>
+      </c>
+      <c r="H275" t="s">
+        <v>473</v>
+      </c>
+      <c r="I275" t="s">
+        <v>19</v>
+      </c>
+      <c r="J275">
+        <v>1</v>
+      </c>
+      <c r="K275">
+        <v>336000000</v>
+      </c>
+      <c r="L275">
+        <v>336000000</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12">
+      <c r="A276">
+        <v>273</v>
+      </c>
+      <c r="B276">
+        <v>626402</v>
+      </c>
+      <c r="C276" t="s">
+        <v>13</v>
+      </c>
+      <c r="D276" t="s">
+        <v>364</v>
+      </c>
+      <c r="E276" t="s">
+        <v>474</v>
+      </c>
+      <c r="F276" t="s">
+        <v>475</v>
+      </c>
+      <c r="G276" t="s">
+        <v>476</v>
+      </c>
+      <c r="H276" t="s">
+        <v>477</v>
+      </c>
+      <c r="I276" t="s">
+        <v>19</v>
+      </c>
+      <c r="J276">
+        <v>1</v>
+      </c>
+      <c r="K276">
+        <v>182000000</v>
+      </c>
+      <c r="L276">
+        <v>182000000</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12">
+      <c r="A277">
+        <v>274</v>
+      </c>
+      <c r="B277">
+        <v>626402</v>
+      </c>
+      <c r="C277" t="s">
+        <v>13</v>
+      </c>
+      <c r="D277" t="s">
+        <v>364</v>
+      </c>
+      <c r="E277" t="s">
+        <v>478</v>
+      </c>
+      <c r="F277" t="s">
+        <v>479</v>
+      </c>
+      <c r="G277" t="s">
+        <v>480</v>
+      </c>
+      <c r="H277" t="s">
+        <v>481</v>
+      </c>
+      <c r="I277" t="s">
+        <v>19</v>
+      </c>
+      <c r="J277">
+        <v>1</v>
+      </c>
+      <c r="K277">
+        <v>196700000</v>
+      </c>
+      <c r="L277">
+        <v>196700000</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12">
+      <c r="A278">
+        <v>275</v>
+      </c>
+      <c r="B278">
+        <v>626402</v>
+      </c>
+      <c r="C278" t="s">
+        <v>13</v>
+      </c>
+      <c r="D278" t="s">
+        <v>295</v>
+      </c>
+      <c r="E278" t="s">
+        <v>482</v>
+      </c>
+      <c r="F278" t="s">
+        <v>483</v>
+      </c>
+      <c r="G278" t="s">
+        <v>484</v>
+      </c>
+      <c r="H278" t="s">
+        <v>485</v>
+      </c>
+      <c r="I278" t="s">
+        <v>19</v>
+      </c>
+      <c r="J278">
+        <v>1</v>
+      </c>
+      <c r="K278">
+        <v>1129000</v>
+      </c>
+      <c r="L278">
+        <v>1129000</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12">
+      <c r="A279">
+        <v>276</v>
+      </c>
+      <c r="B279">
+        <v>626402</v>
+      </c>
+      <c r="C279" t="s">
+        <v>13</v>
+      </c>
+      <c r="D279" t="s">
+        <v>295</v>
+      </c>
+      <c r="E279" t="s">
+        <v>486</v>
+      </c>
+      <c r="F279" t="s">
+        <v>487</v>
+      </c>
+      <c r="G279" t="s">
+        <v>488</v>
+      </c>
+      <c r="H279" t="s">
+        <v>254</v>
+      </c>
+      <c r="I279" t="s">
+        <v>19</v>
+      </c>
+      <c r="J279">
+        <v>1</v>
+      </c>
+      <c r="K279">
+        <v>8145611</v>
+      </c>
+      <c r="L279">
+        <v>8145611</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12">
+      <c r="A280">
+        <v>277</v>
+      </c>
+      <c r="B280">
+        <v>626402</v>
+      </c>
+      <c r="C280" t="s">
+        <v>13</v>
+      </c>
+      <c r="D280" t="s">
+        <v>295</v>
+      </c>
+      <c r="E280" t="s">
+        <v>486</v>
+      </c>
+      <c r="F280" t="s">
+        <v>487</v>
+      </c>
+      <c r="G280" t="s">
+        <v>488</v>
+      </c>
+      <c r="H280" t="s">
+        <v>489</v>
+      </c>
+      <c r="I280" t="s">
+        <v>19</v>
+      </c>
+      <c r="J280">
+        <v>1</v>
+      </c>
+      <c r="K280">
+        <v>391600</v>
+      </c>
+      <c r="L280">
+        <v>391600</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12">
+      <c r="A281">
+        <v>278</v>
+      </c>
+      <c r="B281">
+        <v>626402</v>
+      </c>
+      <c r="C281" t="s">
+        <v>13</v>
+      </c>
+      <c r="D281" t="s">
+        <v>295</v>
+      </c>
+      <c r="E281" t="s">
+        <v>486</v>
+      </c>
+      <c r="F281" t="s">
+        <v>487</v>
+      </c>
+      <c r="G281" t="s">
+        <v>488</v>
+      </c>
+      <c r="H281" t="s">
+        <v>490</v>
+      </c>
+      <c r="I281" t="s">
+        <v>19</v>
+      </c>
+      <c r="J281">
+        <v>1</v>
+      </c>
+      <c r="K281">
+        <v>22121588</v>
+      </c>
+      <c r="L281">
+        <v>22121588</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12">
+      <c r="A282">
+        <v>279</v>
+      </c>
+      <c r="B282">
+        <v>626402</v>
+      </c>
+      <c r="C282" t="s">
+        <v>13</v>
+      </c>
+      <c r="D282" t="s">
+        <v>295</v>
+      </c>
+      <c r="E282" t="s">
+        <v>486</v>
+      </c>
+      <c r="F282" t="s">
+        <v>487</v>
+      </c>
+      <c r="G282" t="s">
+        <v>488</v>
+      </c>
+      <c r="H282" t="s">
+        <v>274</v>
+      </c>
+      <c r="I282" t="s">
+        <v>19</v>
+      </c>
+      <c r="J282">
+        <v>1</v>
+      </c>
+      <c r="K282">
+        <v>436583</v>
+      </c>
+      <c r="L282">
+        <v>436583</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12">
+      <c r="A283">
+        <v>280</v>
+      </c>
+      <c r="B283">
+        <v>626402</v>
+      </c>
+      <c r="C283" t="s">
+        <v>13</v>
+      </c>
+      <c r="D283" t="s">
+        <v>364</v>
+      </c>
+      <c r="E283" t="s">
+        <v>491</v>
+      </c>
+      <c r="F283" t="s">
+        <v>492</v>
+      </c>
+      <c r="G283" t="s">
+        <v>121</v>
+      </c>
+      <c r="H283" t="s">
+        <v>128</v>
+      </c>
+      <c r="I283" t="s">
+        <v>19</v>
+      </c>
+      <c r="J283">
+        <v>1</v>
+      </c>
+      <c r="K283">
+        <v>6893713</v>
+      </c>
+      <c r="L283">
+        <v>6893713</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12">
+      <c r="A284">
+        <v>281</v>
+      </c>
+      <c r="B284">
+        <v>626402</v>
+      </c>
+      <c r="C284" t="s">
+        <v>13</v>
+      </c>
+      <c r="D284" t="s">
+        <v>364</v>
+      </c>
+      <c r="E284" t="s">
+        <v>491</v>
+      </c>
+      <c r="F284" t="s">
+        <v>492</v>
+      </c>
+      <c r="G284" t="s">
+        <v>121</v>
+      </c>
+      <c r="H284" t="s">
+        <v>493</v>
+      </c>
+      <c r="I284" t="s">
+        <v>19</v>
+      </c>
+      <c r="J284">
+        <v>1</v>
+      </c>
+      <c r="K284">
+        <v>2187190</v>
+      </c>
+      <c r="L284">
+        <v>2187190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 16 feb 2024
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="513">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -1313,6 +1313,30 @@
     <t>'626402.175.522191.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000440</t>
   </si>
   <si>
+    <t>2024-02-16</t>
+  </si>
+  <si>
+    <t>'00095T</t>
+  </si>
+  <si>
+    <t>'241751303002023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.83/BPPSDM.5/KP.440/I/2024 Tgl.18 Januari 2024 </t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.201.0B.001139</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.201.0B.001497</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.201.0B.001498</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.201.0B.001499</t>
+  </si>
+  <si>
     <t>'00097T</t>
   </si>
   <si>
@@ -1488,6 +1512,39 @@
   </si>
   <si>
     <t>'626402.175.522119.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AB.000443</t>
+  </si>
+  <si>
+    <t>'00106T</t>
+  </si>
+  <si>
+    <t>'241751303002064</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang.Fullboard Meeting Ev.Penyelenggaraan PTKL dan Lemb. Pemerintah Non Kementerian, SPK No:33/PPK.PUSDIK/PL.430/I/2024 tgl.12/1/2024,BAST No:50/PPK.PUSDIK/PL.450/I/2024 tgl 18/1/2024,BAP No:51/PPK.PUSDIK/PL.450/I/2024 tgl 18/1/2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524119.03212DL.2376AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.001380</t>
+  </si>
+  <si>
+    <t>'00107T</t>
+  </si>
+  <si>
+    <t>'241751305000184</t>
+  </si>
+  <si>
+    <t>Pembayaran tunjangan kinerja susulan Pegawai Sekretariat bulan Januari tahun 2024 untuk 1 Pegawai/Anggota Polri/Prajurit TNI.</t>
+  </si>
+  <si>
+    <t>'00108T</t>
+  </si>
+  <si>
+    <t>'241751303002198</t>
+  </si>
+  <si>
+    <t>Pembayaran tunjangan kinerja susulan bulan Januari tahun 2024 untuk 2 Pegawai/Anggota Polri/Prajurit TNI.</t>
+  </si>
+  <si>
+    <t>'626402.175.512414.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.AA.001366</t>
   </si>
   <si>
     <t>'00110T</t>
@@ -1838,7 +1895,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L284"/>
+  <dimension ref="A1:L291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -10947,19 +11004,19 @@
         <v>13</v>
       </c>
       <c r="D242" t="s">
-        <v>364</v>
+        <v>432</v>
       </c>
       <c r="E242" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F242" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G242" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H242" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="I242" t="s">
         <v>19</v>
@@ -10968,10 +11025,10 @@
         <v>1</v>
       </c>
       <c r="K242">
-        <v>4828000</v>
+        <v>5097100</v>
       </c>
       <c r="L242">
-        <v>4828000</v>
+        <v>5097100</v>
       </c>
     </row>
     <row r="243" spans="1:12">
@@ -10985,19 +11042,19 @@
         <v>13</v>
       </c>
       <c r="D243" t="s">
-        <v>364</v>
+        <v>432</v>
       </c>
       <c r="E243" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F243" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G243" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H243" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="I243" t="s">
         <v>19</v>
@@ -11006,10 +11063,10 @@
         <v>1</v>
       </c>
       <c r="K243">
-        <v>516000</v>
+        <v>3010000</v>
       </c>
       <c r="L243">
-        <v>516000</v>
+        <v>3010000</v>
       </c>
     </row>
     <row r="244" spans="1:12">
@@ -11023,19 +11080,19 @@
         <v>13</v>
       </c>
       <c r="D244" t="s">
-        <v>364</v>
+        <v>432</v>
       </c>
       <c r="E244" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F244" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G244" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H244" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="I244" t="s">
         <v>19</v>
@@ -11044,10 +11101,10 @@
         <v>1</v>
       </c>
       <c r="K244">
-        <v>220000</v>
+        <v>2300000</v>
       </c>
       <c r="L244">
-        <v>220000</v>
+        <v>2300000</v>
       </c>
     </row>
     <row r="245" spans="1:12">
@@ -11061,19 +11118,19 @@
         <v>13</v>
       </c>
       <c r="D245" t="s">
-        <v>364</v>
+        <v>432</v>
       </c>
       <c r="E245" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F245" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G245" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H245" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="I245" t="s">
         <v>19</v>
@@ -11082,10 +11139,10 @@
         <v>1</v>
       </c>
       <c r="K245">
-        <v>1680000</v>
+        <v>245500</v>
       </c>
       <c r="L245">
-        <v>1680000</v>
+        <v>245500</v>
       </c>
     </row>
     <row r="246" spans="1:12">
@@ -11102,16 +11159,16 @@
         <v>364</v>
       </c>
       <c r="E246" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F246" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G246" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H246" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="I246" t="s">
         <v>19</v>
@@ -11120,10 +11177,10 @@
         <v>1</v>
       </c>
       <c r="K246">
-        <v>3000000</v>
+        <v>4828000</v>
       </c>
       <c r="L246">
-        <v>3000000</v>
+        <v>4828000</v>
       </c>
     </row>
     <row r="247" spans="1:12">
@@ -11140,16 +11197,16 @@
         <v>364</v>
       </c>
       <c r="E247" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F247" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G247" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H247" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="I247" t="s">
         <v>19</v>
@@ -11158,10 +11215,10 @@
         <v>1</v>
       </c>
       <c r="K247">
-        <v>1870000</v>
+        <v>516000</v>
       </c>
       <c r="L247">
-        <v>1870000</v>
+        <v>516000</v>
       </c>
     </row>
     <row r="248" spans="1:12">
@@ -11178,16 +11235,16 @@
         <v>364</v>
       </c>
       <c r="E248" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F248" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G248" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H248" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="I248" t="s">
         <v>19</v>
@@ -11196,10 +11253,10 @@
         <v>1</v>
       </c>
       <c r="K248">
-        <v>876000</v>
+        <v>220000</v>
       </c>
       <c r="L248">
-        <v>876000</v>
+        <v>220000</v>
       </c>
     </row>
     <row r="249" spans="1:12">
@@ -11216,16 +11273,16 @@
         <v>364</v>
       </c>
       <c r="E249" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F249" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G249" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H249" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="I249" t="s">
         <v>19</v>
@@ -11234,10 +11291,10 @@
         <v>1</v>
       </c>
       <c r="K249">
-        <v>1077500</v>
+        <v>1680000</v>
       </c>
       <c r="L249">
-        <v>1077500</v>
+        <v>1680000</v>
       </c>
     </row>
     <row r="250" spans="1:12">
@@ -11254,16 +11311,16 @@
         <v>364</v>
       </c>
       <c r="E250" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F250" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G250" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H250" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="I250" t="s">
         <v>19</v>
@@ -11272,10 +11329,10 @@
         <v>1</v>
       </c>
       <c r="K250">
-        <v>2360000</v>
+        <v>3000000</v>
       </c>
       <c r="L250">
-        <v>2360000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="251" spans="1:12">
@@ -11292,16 +11349,16 @@
         <v>364</v>
       </c>
       <c r="E251" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F251" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G251" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H251" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="I251" t="s">
         <v>19</v>
@@ -11310,10 +11367,10 @@
         <v>1</v>
       </c>
       <c r="K251">
-        <v>990000</v>
+        <v>1870000</v>
       </c>
       <c r="L251">
-        <v>990000</v>
+        <v>1870000</v>
       </c>
     </row>
     <row r="252" spans="1:12">
@@ -11330,16 +11387,16 @@
         <v>364</v>
       </c>
       <c r="E252" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F252" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G252" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H252" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="I252" t="s">
         <v>19</v>
@@ -11348,10 +11405,10 @@
         <v>1</v>
       </c>
       <c r="K252">
-        <v>1000000</v>
+        <v>876000</v>
       </c>
       <c r="L252">
-        <v>1000000</v>
+        <v>876000</v>
       </c>
     </row>
     <row r="253" spans="1:12">
@@ -11368,16 +11425,16 @@
         <v>364</v>
       </c>
       <c r="E253" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F253" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G253" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H253" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="I253" t="s">
         <v>19</v>
@@ -11386,10 +11443,10 @@
         <v>1</v>
       </c>
       <c r="K253">
-        <v>1720000</v>
+        <v>1077500</v>
       </c>
       <c r="L253">
-        <v>1720000</v>
+        <v>1077500</v>
       </c>
     </row>
     <row r="254" spans="1:12">
@@ -11406,16 +11463,16 @@
         <v>364</v>
       </c>
       <c r="E254" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F254" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G254" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H254" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="I254" t="s">
         <v>19</v>
@@ -11424,10 +11481,10 @@
         <v>1</v>
       </c>
       <c r="K254">
-        <v>798900</v>
+        <v>2360000</v>
       </c>
       <c r="L254">
-        <v>798900</v>
+        <v>2360000</v>
       </c>
     </row>
     <row r="255" spans="1:12">
@@ -11444,16 +11501,16 @@
         <v>364</v>
       </c>
       <c r="E255" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F255" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G255" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H255" t="s">
-        <v>234</v>
+        <v>452</v>
       </c>
       <c r="I255" t="s">
         <v>19</v>
@@ -11462,10 +11519,10 @@
         <v>1</v>
       </c>
       <c r="K255">
-        <v>2496920</v>
+        <v>990000</v>
       </c>
       <c r="L255">
-        <v>2496920</v>
+        <v>990000</v>
       </c>
     </row>
     <row r="256" spans="1:12">
@@ -11482,16 +11539,16 @@
         <v>364</v>
       </c>
       <c r="E256" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F256" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G256" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H256" t="s">
-        <v>236</v>
+        <v>453</v>
       </c>
       <c r="I256" t="s">
         <v>19</v>
@@ -11500,10 +11557,10 @@
         <v>1</v>
       </c>
       <c r="K256">
-        <v>1080000</v>
+        <v>1000000</v>
       </c>
       <c r="L256">
-        <v>1080000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="257" spans="1:12">
@@ -11520,16 +11577,16 @@
         <v>364</v>
       </c>
       <c r="E257" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F257" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G257" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H257" t="s">
-        <v>237</v>
+        <v>454</v>
       </c>
       <c r="I257" t="s">
         <v>19</v>
@@ -11538,10 +11595,10 @@
         <v>1</v>
       </c>
       <c r="K257">
-        <v>205500</v>
+        <v>1720000</v>
       </c>
       <c r="L257">
-        <v>205500</v>
+        <v>1720000</v>
       </c>
     </row>
     <row r="258" spans="1:12">
@@ -11558,16 +11615,16 @@
         <v>364</v>
       </c>
       <c r="E258" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F258" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G258" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H258" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="I258" t="s">
         <v>19</v>
@@ -11576,10 +11633,10 @@
         <v>1</v>
       </c>
       <c r="K258">
-        <v>370000</v>
+        <v>798900</v>
       </c>
       <c r="L258">
-        <v>370000</v>
+        <v>798900</v>
       </c>
     </row>
     <row r="259" spans="1:12">
@@ -11596,16 +11653,16 @@
         <v>364</v>
       </c>
       <c r="E259" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F259" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G259" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H259" t="s">
-        <v>449</v>
+        <v>234</v>
       </c>
       <c r="I259" t="s">
         <v>19</v>
@@ -11614,10 +11671,10 @@
         <v>1</v>
       </c>
       <c r="K259">
-        <v>517500</v>
+        <v>2496920</v>
       </c>
       <c r="L259">
-        <v>517500</v>
+        <v>2496920</v>
       </c>
     </row>
     <row r="260" spans="1:12">
@@ -11634,16 +11691,16 @@
         <v>364</v>
       </c>
       <c r="E260" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F260" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G260" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H260" t="s">
-        <v>368</v>
+        <v>236</v>
       </c>
       <c r="I260" t="s">
         <v>19</v>
@@ -11652,10 +11709,10 @@
         <v>1</v>
       </c>
       <c r="K260">
-        <v>2340000</v>
+        <v>1080000</v>
       </c>
       <c r="L260">
-        <v>2340000</v>
+        <v>1080000</v>
       </c>
     </row>
     <row r="261" spans="1:12">
@@ -11672,16 +11729,16 @@
         <v>364</v>
       </c>
       <c r="E261" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F261" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G261" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H261" t="s">
-        <v>363</v>
+        <v>237</v>
       </c>
       <c r="I261" t="s">
         <v>19</v>
@@ -11690,10 +11747,10 @@
         <v>1</v>
       </c>
       <c r="K261">
-        <v>3060000</v>
+        <v>205500</v>
       </c>
       <c r="L261">
-        <v>3060000</v>
+        <v>205500</v>
       </c>
     </row>
     <row r="262" spans="1:12">
@@ -11710,16 +11767,16 @@
         <v>364</v>
       </c>
       <c r="E262" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F262" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G262" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H262" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="I262" t="s">
         <v>19</v>
@@ -11728,10 +11785,10 @@
         <v>1</v>
       </c>
       <c r="K262">
-        <v>3430000</v>
+        <v>370000</v>
       </c>
       <c r="L262">
-        <v>3430000</v>
+        <v>370000</v>
       </c>
     </row>
     <row r="263" spans="1:12">
@@ -11748,16 +11805,16 @@
         <v>364</v>
       </c>
       <c r="E263" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F263" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G263" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H263" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="I263" t="s">
         <v>19</v>
@@ -11766,10 +11823,10 @@
         <v>1</v>
       </c>
       <c r="K263">
-        <v>3000000</v>
+        <v>517500</v>
       </c>
       <c r="L263">
-        <v>3000000</v>
+        <v>517500</v>
       </c>
     </row>
     <row r="264" spans="1:12">
@@ -11786,16 +11843,16 @@
         <v>364</v>
       </c>
       <c r="E264" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F264" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G264" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H264" t="s">
-        <v>452</v>
+        <v>368</v>
       </c>
       <c r="I264" t="s">
         <v>19</v>
@@ -11804,10 +11861,10 @@
         <v>1</v>
       </c>
       <c r="K264">
-        <v>4618753</v>
+        <v>2340000</v>
       </c>
       <c r="L264">
-        <v>4618753</v>
+        <v>2340000</v>
       </c>
     </row>
     <row r="265" spans="1:12">
@@ -11824,16 +11881,16 @@
         <v>364</v>
       </c>
       <c r="E265" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F265" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G265" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H265" t="s">
-        <v>453</v>
+        <v>363</v>
       </c>
       <c r="I265" t="s">
         <v>19</v>
@@ -11842,10 +11899,10 @@
         <v>1</v>
       </c>
       <c r="K265">
-        <v>510000</v>
+        <v>3060000</v>
       </c>
       <c r="L265">
-        <v>510000</v>
+        <v>3060000</v>
       </c>
     </row>
     <row r="266" spans="1:12">
@@ -11862,16 +11919,16 @@
         <v>364</v>
       </c>
       <c r="E266" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F266" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G266" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H266" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="I266" t="s">
         <v>19</v>
@@ -11880,10 +11937,10 @@
         <v>1</v>
       </c>
       <c r="K266">
-        <v>9081490</v>
+        <v>3430000</v>
       </c>
       <c r="L266">
-        <v>9081490</v>
+        <v>3430000</v>
       </c>
     </row>
     <row r="267" spans="1:12">
@@ -11900,16 +11957,16 @@
         <v>364</v>
       </c>
       <c r="E267" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F267" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G267" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H267" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="I267" t="s">
         <v>19</v>
@@ -11918,10 +11975,10 @@
         <v>1</v>
       </c>
       <c r="K267">
-        <v>2380000</v>
+        <v>3000000</v>
       </c>
       <c r="L267">
-        <v>2380000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="268" spans="1:12">
@@ -11938,16 +11995,16 @@
         <v>364</v>
       </c>
       <c r="E268" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F268" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G268" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H268" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="I268" t="s">
         <v>19</v>
@@ -11956,10 +12013,10 @@
         <v>1</v>
       </c>
       <c r="K268">
-        <v>680000</v>
+        <v>4618753</v>
       </c>
       <c r="L268">
-        <v>680000</v>
+        <v>4618753</v>
       </c>
     </row>
     <row r="269" spans="1:12">
@@ -11976,16 +12033,16 @@
         <v>364</v>
       </c>
       <c r="E269" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F269" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G269" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H269" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I269" t="s">
         <v>19</v>
@@ -11994,10 +12051,10 @@
         <v>1</v>
       </c>
       <c r="K269">
-        <v>1190000</v>
+        <v>510000</v>
       </c>
       <c r="L269">
-        <v>1190000</v>
+        <v>510000</v>
       </c>
     </row>
     <row r="270" spans="1:12">
@@ -12014,16 +12071,16 @@
         <v>364</v>
       </c>
       <c r="E270" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F270" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G270" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="H270" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="I270" t="s">
         <v>19</v>
@@ -12032,10 +12089,10 @@
         <v>1</v>
       </c>
       <c r="K270">
-        <v>34500000</v>
+        <v>9081490</v>
       </c>
       <c r="L270">
-        <v>34500000</v>
+        <v>9081490</v>
       </c>
     </row>
     <row r="271" spans="1:12">
@@ -12052,16 +12109,16 @@
         <v>364</v>
       </c>
       <c r="E271" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="F271" t="s">
-        <v>460</v>
+        <v>441</v>
       </c>
       <c r="G271" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="H271" t="s">
-        <v>311</v>
+        <v>463</v>
       </c>
       <c r="I271" t="s">
         <v>19</v>
@@ -12070,10 +12127,10 @@
         <v>1</v>
       </c>
       <c r="K271">
-        <v>510000</v>
+        <v>2380000</v>
       </c>
       <c r="L271">
-        <v>510000</v>
+        <v>2380000</v>
       </c>
     </row>
     <row r="272" spans="1:12">
@@ -12090,16 +12147,16 @@
         <v>364</v>
       </c>
       <c r="E272" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="F272" t="s">
-        <v>460</v>
+        <v>441</v>
       </c>
       <c r="G272" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="H272" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="I272" t="s">
         <v>19</v>
@@ -12108,10 +12165,10 @@
         <v>1</v>
       </c>
       <c r="K272">
-        <v>630000</v>
+        <v>680000</v>
       </c>
       <c r="L272">
-        <v>630000</v>
+        <v>680000</v>
       </c>
     </row>
     <row r="273" spans="1:12">
@@ -12128,17 +12185,17 @@
         <v>364</v>
       </c>
       <c r="E273" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="F273" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="G273" t="s">
+        <v>442</v>
+      </c>
+      <c r="H273" t="s">
         <v>465</v>
       </c>
-      <c r="H273" t="s">
-        <v>198</v>
-      </c>
       <c r="I273" t="s">
         <v>19</v>
       </c>
@@ -12146,10 +12203,10 @@
         <v>1</v>
       </c>
       <c r="K273">
-        <v>23018070</v>
+        <v>1190000</v>
       </c>
       <c r="L273">
-        <v>23018070</v>
+        <v>1190000</v>
       </c>
     </row>
     <row r="274" spans="1:12">
@@ -12166,17 +12223,17 @@
         <v>364</v>
       </c>
       <c r="E274" t="s">
+        <v>440</v>
+      </c>
+      <c r="F274" t="s">
+        <v>441</v>
+      </c>
+      <c r="G274" t="s">
+        <v>442</v>
+      </c>
+      <c r="H274" t="s">
         <v>466</v>
       </c>
-      <c r="F274" t="s">
-        <v>467</v>
-      </c>
-      <c r="G274" t="s">
-        <v>468</v>
-      </c>
-      <c r="H274" t="s">
-        <v>469</v>
-      </c>
       <c r="I274" t="s">
         <v>19</v>
       </c>
@@ -12184,10 +12241,10 @@
         <v>1</v>
       </c>
       <c r="K274">
-        <v>53000000</v>
+        <v>34500000</v>
       </c>
       <c r="L274">
-        <v>53000000</v>
+        <v>34500000</v>
       </c>
     </row>
     <row r="275" spans="1:12">
@@ -12204,16 +12261,16 @@
         <v>364</v>
       </c>
       <c r="E275" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F275" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G275" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="H275" t="s">
-        <v>473</v>
+        <v>311</v>
       </c>
       <c r="I275" t="s">
         <v>19</v>
@@ -12222,10 +12279,10 @@
         <v>1</v>
       </c>
       <c r="K275">
-        <v>336000000</v>
+        <v>510000</v>
       </c>
       <c r="L275">
-        <v>336000000</v>
+        <v>510000</v>
       </c>
     </row>
     <row r="276" spans="1:12">
@@ -12242,16 +12299,16 @@
         <v>364</v>
       </c>
       <c r="E276" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="F276" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="G276" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="H276" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="I276" t="s">
         <v>19</v>
@@ -12260,10 +12317,10 @@
         <v>1</v>
       </c>
       <c r="K276">
-        <v>182000000</v>
+        <v>630000</v>
       </c>
       <c r="L276">
-        <v>182000000</v>
+        <v>630000</v>
       </c>
     </row>
     <row r="277" spans="1:12">
@@ -12280,16 +12337,16 @@
         <v>364</v>
       </c>
       <c r="E277" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="F277" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="G277" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="H277" t="s">
-        <v>481</v>
+        <v>198</v>
       </c>
       <c r="I277" t="s">
         <v>19</v>
@@ -12298,10 +12355,10 @@
         <v>1</v>
       </c>
       <c r="K277">
-        <v>196700000</v>
+        <v>23018070</v>
       </c>
       <c r="L277">
-        <v>196700000</v>
+        <v>23018070</v>
       </c>
     </row>
     <row r="278" spans="1:12">
@@ -12315,19 +12372,19 @@
         <v>13</v>
       </c>
       <c r="D278" t="s">
-        <v>295</v>
+        <v>364</v>
       </c>
       <c r="E278" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="F278" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="G278" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="H278" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="I278" t="s">
         <v>19</v>
@@ -12336,10 +12393,10 @@
         <v>1</v>
       </c>
       <c r="K278">
-        <v>1129000</v>
+        <v>53000000</v>
       </c>
       <c r="L278">
-        <v>1129000</v>
+        <v>53000000</v>
       </c>
     </row>
     <row r="279" spans="1:12">
@@ -12353,19 +12410,19 @@
         <v>13</v>
       </c>
       <c r="D279" t="s">
-        <v>295</v>
+        <v>364</v>
       </c>
       <c r="E279" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="F279" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="G279" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="H279" t="s">
-        <v>254</v>
+        <v>481</v>
       </c>
       <c r="I279" t="s">
         <v>19</v>
@@ -12374,10 +12431,10 @@
         <v>1</v>
       </c>
       <c r="K279">
-        <v>8145611</v>
+        <v>336000000</v>
       </c>
       <c r="L279">
-        <v>8145611</v>
+        <v>336000000</v>
       </c>
     </row>
     <row r="280" spans="1:12">
@@ -12391,19 +12448,19 @@
         <v>13</v>
       </c>
       <c r="D280" t="s">
-        <v>295</v>
+        <v>364</v>
       </c>
       <c r="E280" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="F280" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="G280" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="H280" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="I280" t="s">
         <v>19</v>
@@ -12412,10 +12469,10 @@
         <v>1</v>
       </c>
       <c r="K280">
-        <v>391600</v>
+        <v>182000000</v>
       </c>
       <c r="L280">
-        <v>391600</v>
+        <v>182000000</v>
       </c>
     </row>
     <row r="281" spans="1:12">
@@ -12429,7 +12486,7 @@
         <v>13</v>
       </c>
       <c r="D281" t="s">
-        <v>295</v>
+        <v>364</v>
       </c>
       <c r="E281" t="s">
         <v>486</v>
@@ -12441,7 +12498,7 @@
         <v>488</v>
       </c>
       <c r="H281" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I281" t="s">
         <v>19</v>
@@ -12450,10 +12507,10 @@
         <v>1</v>
       </c>
       <c r="K281">
-        <v>22121588</v>
+        <v>196700000</v>
       </c>
       <c r="L281">
-        <v>22121588</v>
+        <v>196700000</v>
       </c>
     </row>
     <row r="282" spans="1:12">
@@ -12470,16 +12527,16 @@
         <v>295</v>
       </c>
       <c r="E282" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="F282" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="G282" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="H282" t="s">
-        <v>274</v>
+        <v>493</v>
       </c>
       <c r="I282" t="s">
         <v>19</v>
@@ -12488,10 +12545,10 @@
         <v>1</v>
       </c>
       <c r="K282">
-        <v>436583</v>
+        <v>1129000</v>
       </c>
       <c r="L282">
-        <v>436583</v>
+        <v>1129000</v>
       </c>
     </row>
     <row r="283" spans="1:12">
@@ -12505,19 +12562,19 @@
         <v>13</v>
       </c>
       <c r="D283" t="s">
-        <v>364</v>
+        <v>295</v>
       </c>
       <c r="E283" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="F283" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="G283" t="s">
-        <v>121</v>
+        <v>496</v>
       </c>
       <c r="H283" t="s">
-        <v>128</v>
+        <v>254</v>
       </c>
       <c r="I283" t="s">
         <v>19</v>
@@ -12526,10 +12583,10 @@
         <v>1</v>
       </c>
       <c r="K283">
-        <v>6893713</v>
+        <v>8145611</v>
       </c>
       <c r="L283">
-        <v>6893713</v>
+        <v>8145611</v>
       </c>
     </row>
     <row r="284" spans="1:12">
@@ -12543,30 +12600,296 @@
         <v>13</v>
       </c>
       <c r="D284" t="s">
+        <v>295</v>
+      </c>
+      <c r="E284" t="s">
+        <v>494</v>
+      </c>
+      <c r="F284" t="s">
+        <v>495</v>
+      </c>
+      <c r="G284" t="s">
+        <v>496</v>
+      </c>
+      <c r="H284" t="s">
+        <v>497</v>
+      </c>
+      <c r="I284" t="s">
+        <v>19</v>
+      </c>
+      <c r="J284">
+        <v>1</v>
+      </c>
+      <c r="K284">
+        <v>391600</v>
+      </c>
+      <c r="L284">
+        <v>391600</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12">
+      <c r="A285">
+        <v>282</v>
+      </c>
+      <c r="B285">
+        <v>626402</v>
+      </c>
+      <c r="C285" t="s">
+        <v>13</v>
+      </c>
+      <c r="D285" t="s">
+        <v>295</v>
+      </c>
+      <c r="E285" t="s">
+        <v>494</v>
+      </c>
+      <c r="F285" t="s">
+        <v>495</v>
+      </c>
+      <c r="G285" t="s">
+        <v>496</v>
+      </c>
+      <c r="H285" t="s">
+        <v>498</v>
+      </c>
+      <c r="I285" t="s">
+        <v>19</v>
+      </c>
+      <c r="J285">
+        <v>1</v>
+      </c>
+      <c r="K285">
+        <v>22121588</v>
+      </c>
+      <c r="L285">
+        <v>22121588</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12">
+      <c r="A286">
+        <v>283</v>
+      </c>
+      <c r="B286">
+        <v>626402</v>
+      </c>
+      <c r="C286" t="s">
+        <v>13</v>
+      </c>
+      <c r="D286" t="s">
+        <v>295</v>
+      </c>
+      <c r="E286" t="s">
+        <v>494</v>
+      </c>
+      <c r="F286" t="s">
+        <v>495</v>
+      </c>
+      <c r="G286" t="s">
+        <v>496</v>
+      </c>
+      <c r="H286" t="s">
+        <v>274</v>
+      </c>
+      <c r="I286" t="s">
+        <v>19</v>
+      </c>
+      <c r="J286">
+        <v>1</v>
+      </c>
+      <c r="K286">
+        <v>436583</v>
+      </c>
+      <c r="L286">
+        <v>436583</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12">
+      <c r="A287">
+        <v>284</v>
+      </c>
+      <c r="B287">
+        <v>626402</v>
+      </c>
+      <c r="C287" t="s">
+        <v>13</v>
+      </c>
+      <c r="D287" t="s">
+        <v>432</v>
+      </c>
+      <c r="E287" t="s">
+        <v>499</v>
+      </c>
+      <c r="F287" t="s">
+        <v>500</v>
+      </c>
+      <c r="G287" t="s">
+        <v>501</v>
+      </c>
+      <c r="H287" t="s">
+        <v>502</v>
+      </c>
+      <c r="I287" t="s">
+        <v>19</v>
+      </c>
+      <c r="J287">
+        <v>1</v>
+      </c>
+      <c r="K287">
+        <v>268240000</v>
+      </c>
+      <c r="L287">
+        <v>268240000</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12">
+      <c r="A288">
+        <v>285</v>
+      </c>
+      <c r="B288">
+        <v>626402</v>
+      </c>
+      <c r="C288" t="s">
+        <v>13</v>
+      </c>
+      <c r="D288" t="s">
+        <v>432</v>
+      </c>
+      <c r="E288" t="s">
+        <v>503</v>
+      </c>
+      <c r="F288" t="s">
+        <v>504</v>
+      </c>
+      <c r="G288" t="s">
+        <v>505</v>
+      </c>
+      <c r="H288" t="s">
+        <v>399</v>
+      </c>
+      <c r="I288" t="s">
+        <v>19</v>
+      </c>
+      <c r="J288">
+        <v>1</v>
+      </c>
+      <c r="K288">
+        <v>5305483</v>
+      </c>
+      <c r="L288">
+        <v>5305483</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12">
+      <c r="A289">
+        <v>286</v>
+      </c>
+      <c r="B289">
+        <v>626402</v>
+      </c>
+      <c r="C289" t="s">
+        <v>13</v>
+      </c>
+      <c r="D289" t="s">
+        <v>432</v>
+      </c>
+      <c r="E289" t="s">
+        <v>506</v>
+      </c>
+      <c r="F289" t="s">
+        <v>507</v>
+      </c>
+      <c r="G289" t="s">
+        <v>508</v>
+      </c>
+      <c r="H289" t="s">
+        <v>509</v>
+      </c>
+      <c r="I289" t="s">
+        <v>19</v>
+      </c>
+      <c r="J289">
+        <v>1</v>
+      </c>
+      <c r="K289">
+        <v>9190300</v>
+      </c>
+      <c r="L289">
+        <v>9190300</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12">
+      <c r="A290">
+        <v>287</v>
+      </c>
+      <c r="B290">
+        <v>626402</v>
+      </c>
+      <c r="C290" t="s">
+        <v>13</v>
+      </c>
+      <c r="D290" t="s">
         <v>364</v>
       </c>
-      <c r="E284" t="s">
-        <v>491</v>
-      </c>
-      <c r="F284" t="s">
-        <v>492</v>
-      </c>
-      <c r="G284" t="s">
+      <c r="E290" t="s">
+        <v>510</v>
+      </c>
+      <c r="F290" t="s">
+        <v>511</v>
+      </c>
+      <c r="G290" t="s">
         <v>121</v>
       </c>
-      <c r="H284" t="s">
-        <v>493</v>
-      </c>
-      <c r="I284" t="s">
-        <v>19</v>
-      </c>
-      <c r="J284">
-        <v>1</v>
-      </c>
-      <c r="K284">
+      <c r="H290" t="s">
+        <v>128</v>
+      </c>
+      <c r="I290" t="s">
+        <v>19</v>
+      </c>
+      <c r="J290">
+        <v>1</v>
+      </c>
+      <c r="K290">
+        <v>6893713</v>
+      </c>
+      <c r="L290">
+        <v>6893713</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12">
+      <c r="A291">
+        <v>288</v>
+      </c>
+      <c r="B291">
+        <v>626402</v>
+      </c>
+      <c r="C291" t="s">
+        <v>13</v>
+      </c>
+      <c r="D291" t="s">
+        <v>364</v>
+      </c>
+      <c r="E291" t="s">
+        <v>510</v>
+      </c>
+      <c r="F291" t="s">
+        <v>511</v>
+      </c>
+      <c r="G291" t="s">
+        <v>121</v>
+      </c>
+      <c r="H291" t="s">
+        <v>512</v>
+      </c>
+      <c r="I291" t="s">
+        <v>19</v>
+      </c>
+      <c r="J291">
+        <v>1</v>
+      </c>
+      <c r="K291">
         <v>2187190</v>
       </c>
-      <c r="L284">
+      <c r="L291">
         <v>2187190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Realisasi s.d 6 Maret 2024
Penambahan rekap realisasi sesuai OMSPAN dan SAKTI :

OMSPAN : 14,68%
SAKTI : 15,87%
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1034">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -2780,6 +2780,33 @@
     <t>'626402.175.522141.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AB.000444</t>
   </si>
   <si>
+    <t>2024-03-07</t>
+  </si>
+  <si>
+    <t>'00196T</t>
+  </si>
+  <si>
+    <t>'241751301005158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Kuitansi Nomor:122/SERA/TRAC-JKT1/AH/II/2024 Tanggal 1 Februari 2024 </t>
+  </si>
+  <si>
+    <t>'626402.175.522141.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AB.001605</t>
+  </si>
+  <si>
+    <t>'00197T</t>
+  </si>
+  <si>
+    <t>'241751302005109</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:015/KW/PT-HAM/II/2024 Tanggal 15 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.522191.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BC.000507</t>
+  </si>
+  <si>
     <t>'00199T</t>
   </si>
   <si>
@@ -2862,6 +2889,234 @@
   </si>
   <si>
     <t>'626402.175.524113.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.962.301.0C.000667</t>
+  </si>
+  <si>
+    <t>'00201T</t>
+  </si>
+  <si>
+    <t>'241751303004755</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran Uang makan pegawai Puslatluh bulan Februari 2024 untuk 33 pegawai)</t>
+  </si>
+  <si>
+    <t>'00202T</t>
+  </si>
+  <si>
+    <t>'241751303004756</t>
+  </si>
+  <si>
+    <t>Pembayaran tunjangan kinerja susulan pegawai Puslatluh bulan Februari tahun 2024 untuk 33 Pegawai/Anggota Polri/Prajurit TNI.</t>
+  </si>
+  <si>
+    <t>'00203T</t>
+  </si>
+  <si>
+    <t>'241751303004754</t>
+  </si>
+  <si>
+    <t>2024-03-06</t>
+  </si>
+  <si>
+    <t>'00204T</t>
+  </si>
+  <si>
+    <t>'241751303004646</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:AWH-AR/24/01/00093 Tanggal 31 Januari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.052.0E.000094</t>
+  </si>
+  <si>
+    <t>'00205T</t>
+  </si>
+  <si>
+    <t>'241751301004859</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:2024/II/MKU/0129 Tanggal 12 Februari 2024</t>
+  </si>
+  <si>
+    <t>'626402.175.523121.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BC.000514</t>
+  </si>
+  <si>
+    <t>'00206T</t>
+  </si>
+  <si>
+    <t>'241751301004881</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:043/NNI/II/24 Tanggal 29 Februari 2024</t>
+  </si>
+  <si>
+    <t>'00207T</t>
+  </si>
+  <si>
+    <t>'241751302004948</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor: 016 Tanggal 15 Februari 2024</t>
+  </si>
+  <si>
+    <t>'00209T</t>
+  </si>
+  <si>
+    <t>'241751303004917</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.346/BPPSDM.5/KP.440/II/2024 Tgl. 26 Februari 2024 a.n Supriyadi dkk</t>
+  </si>
+  <si>
+    <t>'00210T</t>
+  </si>
+  <si>
+    <t>'241751303004918</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.243,284/BPPSDM.5/KP.440/II/2024 Tgl. 16 Februari 2024 a.n Lilly aprilya pregiwati dkk</t>
+  </si>
+  <si>
+    <t>'00211T</t>
+  </si>
+  <si>
+    <t>'241751303004863</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.283,284/BPPSDM.5/KP.440/II/2024 Tgl. 16 Februari 2024 a.n Riza Satriawan dkk</t>
+  </si>
+  <si>
+    <t>'00212T</t>
+  </si>
+  <si>
+    <t>'241751303004990</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000470</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000471</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000472</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000473</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000474</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000475</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000478</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000479</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000480</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000481</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000484</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000485</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000486</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000487</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000488</t>
+  </si>
+  <si>
+    <t>'626402.175.521115.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AD.000489</t>
+  </si>
+  <si>
+    <t>'626402.175.524113.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AB.001082</t>
+  </si>
+  <si>
+    <t>'00213T</t>
+  </si>
+  <si>
+    <t>'241751303004991</t>
+  </si>
+  <si>
+    <t>Penggantian Uang Persediaan Untuk Keperluan Pembayaran Belanja Barang (BPP 001 Puslatluhkp)</t>
+  </si>
+  <si>
+    <t>'626402.175.521119.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.DD.000558</t>
+  </si>
+  <si>
+    <t>'626402.175.521119.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.DD.000559</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0B.000024</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0E.000052</t>
+  </si>
+  <si>
+    <t>'626402.175.522141.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.DB.000546</t>
+  </si>
+  <si>
+    <t>'626402.175.522141.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.DB.000547</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0A.001411</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0A.001412</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0E.001421</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.051.0E.001422</t>
+  </si>
+  <si>
+    <t>'00214T</t>
+  </si>
+  <si>
+    <t>'241751303004887</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Biaya hidup (Jan-Juni 2024) peserta tubel S3-IPB an. Herry sesuai SK KaBRSDMKP No 107/KEP-BRSDM/2020 Tgl 18/8/2020 dan SK PPK No KEP 16/BRSDM.4/I/2024 Tgl 3/1/2024</t>
+  </si>
+  <si>
+    <t>'00215T</t>
+  </si>
+  <si>
+    <t>'241751303004845</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Biaya hidup (Jan-Juni 2024) peserta tubel S2-AUP,IPB an. Banar,dkk sesuai SK KaBRSDMKP No 520 Tahun 2022 Tgl 11/8/2022 dan SK PPK No KEP 16/BRSDM.4/I/2024 Tgl 3/1/2024</t>
+  </si>
+  <si>
+    <t>'00216T</t>
+  </si>
+  <si>
+    <t>'241751303004848</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Biaya hidup (Jan-Juni 2024) peserta tubel S3-IPB, S2-IPB,UGM,ITS an. Defra,dkk sesuai SK KaBRSDMKP No 380 Tahun 2023 Tgl 1/8/2023 dan SK PPK No KEP 16/BRSDM.4/I/2024 Tgl 3/1/2024</t>
+  </si>
+  <si>
+    <t>'00217T</t>
+  </si>
+  <si>
+    <t>'241751303004846</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Biaya penelitian peserta tubel S2-UNDIP an. Hilman Adi S sesuai SK KaBRSDMKP No 520 Tahun 2022 Tgl 11/8/2022 dan SK PPK No KEP 16/BRSDM.4/I/2024 Tgl 3/1/2024</t>
   </si>
 </sst>
 </file>
@@ -3203,7 +3458,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L678"/>
+  <dimension ref="A1:L732"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -27968,19 +28223,19 @@
         <v>13</v>
       </c>
       <c r="D654" t="s">
-        <v>901</v>
+        <v>921</v>
       </c>
       <c r="E654" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F654" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="G654" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="H654" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="I654" t="s">
         <v>19</v>
@@ -27989,10 +28244,10 @@
         <v>1</v>
       </c>
       <c r="K654">
-        <v>8300000</v>
+        <v>25000000</v>
       </c>
       <c r="L654">
-        <v>8300000</v>
+        <v>25000000</v>
       </c>
     </row>
     <row r="655" spans="1:12">
@@ -28006,19 +28261,19 @@
         <v>13</v>
       </c>
       <c r="D655" t="s">
-        <v>839</v>
+        <v>921</v>
       </c>
       <c r="E655" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="F655" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="G655" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="H655" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="I655" t="s">
         <v>19</v>
@@ -28027,10 +28282,10 @@
         <v>1</v>
       </c>
       <c r="K655">
-        <v>7387700</v>
+        <v>6474000</v>
       </c>
       <c r="L655">
-        <v>7387700</v>
+        <v>6474000</v>
       </c>
     </row>
     <row r="656" spans="1:12">
@@ -28044,19 +28299,19 @@
         <v>13</v>
       </c>
       <c r="D656" t="s">
-        <v>839</v>
+        <v>901</v>
       </c>
       <c r="E656" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
       <c r="F656" t="s">
-        <v>926</v>
+        <v>931</v>
       </c>
       <c r="G656" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="H656" t="s">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c r="I656" t="s">
         <v>19</v>
@@ -28065,10 +28320,10 @@
         <v>1</v>
       </c>
       <c r="K656">
-        <v>3152000</v>
+        <v>8300000</v>
       </c>
       <c r="L656">
-        <v>3152000</v>
+        <v>8300000</v>
       </c>
     </row>
     <row r="657" spans="1:12">
@@ -28085,16 +28340,16 @@
         <v>839</v>
       </c>
       <c r="E657" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F657" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G657" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H657" t="s">
-        <v>930</v>
+        <v>937</v>
       </c>
       <c r="I657" t="s">
         <v>19</v>
@@ -28103,10 +28358,10 @@
         <v>1</v>
       </c>
       <c r="K657">
-        <v>526235</v>
+        <v>7387700</v>
       </c>
       <c r="L657">
-        <v>526235</v>
+        <v>7387700</v>
       </c>
     </row>
     <row r="658" spans="1:12">
@@ -28123,16 +28378,16 @@
         <v>839</v>
       </c>
       <c r="E658" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F658" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G658" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H658" t="s">
-        <v>931</v>
+        <v>938</v>
       </c>
       <c r="I658" t="s">
         <v>19</v>
@@ -28141,10 +28396,10 @@
         <v>1</v>
       </c>
       <c r="K658">
-        <v>5232072</v>
+        <v>3152000</v>
       </c>
       <c r="L658">
-        <v>5232072</v>
+        <v>3152000</v>
       </c>
     </row>
     <row r="659" spans="1:12">
@@ -28161,16 +28416,16 @@
         <v>839</v>
       </c>
       <c r="E659" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F659" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G659" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H659" t="s">
-        <v>932</v>
+        <v>939</v>
       </c>
       <c r="I659" t="s">
         <v>19</v>
@@ -28179,10 +28434,10 @@
         <v>1</v>
       </c>
       <c r="K659">
-        <v>1190000</v>
+        <v>526235</v>
       </c>
       <c r="L659">
-        <v>1190000</v>
+        <v>526235</v>
       </c>
     </row>
     <row r="660" spans="1:12">
@@ -28199,16 +28454,16 @@
         <v>839</v>
       </c>
       <c r="E660" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F660" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G660" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H660" t="s">
-        <v>933</v>
+        <v>940</v>
       </c>
       <c r="I660" t="s">
         <v>19</v>
@@ -28217,10 +28472,10 @@
         <v>1</v>
       </c>
       <c r="K660">
-        <v>160000</v>
+        <v>5232072</v>
       </c>
       <c r="L660">
-        <v>160000</v>
+        <v>5232072</v>
       </c>
     </row>
     <row r="661" spans="1:12">
@@ -28237,16 +28492,16 @@
         <v>839</v>
       </c>
       <c r="E661" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F661" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G661" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H661" t="s">
-        <v>934</v>
+        <v>941</v>
       </c>
       <c r="I661" t="s">
         <v>19</v>
@@ -28255,10 +28510,10 @@
         <v>1</v>
       </c>
       <c r="K661">
-        <v>1495000</v>
+        <v>1190000</v>
       </c>
       <c r="L661">
-        <v>1495000</v>
+        <v>1190000</v>
       </c>
     </row>
     <row r="662" spans="1:12">
@@ -28275,16 +28530,16 @@
         <v>839</v>
       </c>
       <c r="E662" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F662" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G662" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H662" t="s">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="I662" t="s">
         <v>19</v>
@@ -28293,10 +28548,10 @@
         <v>1</v>
       </c>
       <c r="K662">
-        <v>5951150</v>
+        <v>160000</v>
       </c>
       <c r="L662">
-        <v>5951150</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="663" spans="1:12">
@@ -28313,16 +28568,16 @@
         <v>839</v>
       </c>
       <c r="E663" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F663" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G663" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H663" t="s">
-        <v>936</v>
+        <v>943</v>
       </c>
       <c r="I663" t="s">
         <v>19</v>
@@ -28331,10 +28586,10 @@
         <v>1</v>
       </c>
       <c r="K663">
-        <v>1500000</v>
+        <v>1495000</v>
       </c>
       <c r="L663">
-        <v>1500000</v>
+        <v>1495000</v>
       </c>
     </row>
     <row r="664" spans="1:12">
@@ -28351,16 +28606,16 @@
         <v>839</v>
       </c>
       <c r="E664" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F664" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G664" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H664" t="s">
-        <v>937</v>
+        <v>944</v>
       </c>
       <c r="I664" t="s">
         <v>19</v>
@@ -28369,10 +28624,10 @@
         <v>1</v>
       </c>
       <c r="K664">
-        <v>998000</v>
+        <v>5951150</v>
       </c>
       <c r="L664">
-        <v>998000</v>
+        <v>5951150</v>
       </c>
     </row>
     <row r="665" spans="1:12">
@@ -28389,16 +28644,16 @@
         <v>839</v>
       </c>
       <c r="E665" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F665" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G665" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H665" t="s">
-        <v>938</v>
+        <v>945</v>
       </c>
       <c r="I665" t="s">
         <v>19</v>
@@ -28427,16 +28682,16 @@
         <v>839</v>
       </c>
       <c r="E666" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F666" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G666" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H666" t="s">
-        <v>939</v>
+        <v>946</v>
       </c>
       <c r="I666" t="s">
         <v>19</v>
@@ -28445,10 +28700,10 @@
         <v>1</v>
       </c>
       <c r="K666">
-        <v>1490000</v>
+        <v>998000</v>
       </c>
       <c r="L666">
-        <v>1490000</v>
+        <v>998000</v>
       </c>
     </row>
     <row r="667" spans="1:12">
@@ -28465,16 +28720,16 @@
         <v>839</v>
       </c>
       <c r="E667" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F667" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G667" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H667" t="s">
-        <v>940</v>
+        <v>947</v>
       </c>
       <c r="I667" t="s">
         <v>19</v>
@@ -28483,10 +28738,10 @@
         <v>1</v>
       </c>
       <c r="K667">
-        <v>1400000</v>
+        <v>1500000</v>
       </c>
       <c r="L667">
-        <v>1400000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="668" spans="1:12">
@@ -28503,16 +28758,16 @@
         <v>839</v>
       </c>
       <c r="E668" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F668" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G668" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H668" t="s">
-        <v>941</v>
+        <v>948</v>
       </c>
       <c r="I668" t="s">
         <v>19</v>
@@ -28521,10 +28776,10 @@
         <v>1</v>
       </c>
       <c r="K668">
-        <v>6700000</v>
+        <v>1490000</v>
       </c>
       <c r="L668">
-        <v>6700000</v>
+        <v>1490000</v>
       </c>
     </row>
     <row r="669" spans="1:12">
@@ -28541,16 +28796,16 @@
         <v>839</v>
       </c>
       <c r="E669" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F669" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G669" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H669" t="s">
-        <v>942</v>
+        <v>949</v>
       </c>
       <c r="I669" t="s">
         <v>19</v>
@@ -28559,10 +28814,10 @@
         <v>1</v>
       </c>
       <c r="K669">
-        <v>3702000</v>
+        <v>1400000</v>
       </c>
       <c r="L669">
-        <v>3702000</v>
+        <v>1400000</v>
       </c>
     </row>
     <row r="670" spans="1:12">
@@ -28579,16 +28834,16 @@
         <v>839</v>
       </c>
       <c r="E670" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F670" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G670" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H670" t="s">
-        <v>943</v>
+        <v>950</v>
       </c>
       <c r="I670" t="s">
         <v>19</v>
@@ -28597,10 +28852,10 @@
         <v>1</v>
       </c>
       <c r="K670">
-        <v>10238934</v>
+        <v>6700000</v>
       </c>
       <c r="L670">
-        <v>10238934</v>
+        <v>6700000</v>
       </c>
     </row>
     <row r="671" spans="1:12">
@@ -28617,16 +28872,16 @@
         <v>839</v>
       </c>
       <c r="E671" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F671" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G671" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H671" t="s">
-        <v>944</v>
+        <v>951</v>
       </c>
       <c r="I671" t="s">
         <v>19</v>
@@ -28635,10 +28890,10 @@
         <v>1</v>
       </c>
       <c r="K671">
-        <v>2807600</v>
+        <v>3702000</v>
       </c>
       <c r="L671">
-        <v>2807600</v>
+        <v>3702000</v>
       </c>
     </row>
     <row r="672" spans="1:12">
@@ -28655,16 +28910,16 @@
         <v>839</v>
       </c>
       <c r="E672" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F672" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G672" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H672" t="s">
-        <v>945</v>
+        <v>952</v>
       </c>
       <c r="I672" t="s">
         <v>19</v>
@@ -28673,10 +28928,10 @@
         <v>1</v>
       </c>
       <c r="K672">
-        <v>564123</v>
+        <v>10238934</v>
       </c>
       <c r="L672">
-        <v>564123</v>
+        <v>10238934</v>
       </c>
     </row>
     <row r="673" spans="1:12">
@@ -28693,16 +28948,16 @@
         <v>839</v>
       </c>
       <c r="E673" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F673" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G673" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H673" t="s">
-        <v>704</v>
+        <v>953</v>
       </c>
       <c r="I673" t="s">
         <v>19</v>
@@ -28711,10 +28966,10 @@
         <v>1</v>
       </c>
       <c r="K673">
-        <v>6689000</v>
+        <v>2807600</v>
       </c>
       <c r="L673">
-        <v>6689000</v>
+        <v>2807600</v>
       </c>
     </row>
     <row r="674" spans="1:12">
@@ -28731,16 +28986,16 @@
         <v>839</v>
       </c>
       <c r="E674" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F674" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G674" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H674" t="s">
-        <v>946</v>
+        <v>954</v>
       </c>
       <c r="I674" t="s">
         <v>19</v>
@@ -28749,10 +29004,10 @@
         <v>1</v>
       </c>
       <c r="K674">
-        <v>5098500</v>
+        <v>564123</v>
       </c>
       <c r="L674">
-        <v>5098500</v>
+        <v>564123</v>
       </c>
     </row>
     <row r="675" spans="1:12">
@@ -28769,16 +29024,16 @@
         <v>839</v>
       </c>
       <c r="E675" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F675" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G675" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H675" t="s">
-        <v>212</v>
+        <v>704</v>
       </c>
       <c r="I675" t="s">
         <v>19</v>
@@ -28787,10 +29042,10 @@
         <v>1</v>
       </c>
       <c r="K675">
-        <v>332500</v>
+        <v>6689000</v>
       </c>
       <c r="L675">
-        <v>332500</v>
+        <v>6689000</v>
       </c>
     </row>
     <row r="676" spans="1:12">
@@ -28807,16 +29062,16 @@
         <v>839</v>
       </c>
       <c r="E676" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F676" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G676" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H676" t="s">
-        <v>213</v>
+        <v>955</v>
       </c>
       <c r="I676" t="s">
         <v>19</v>
@@ -28825,10 +29080,10 @@
         <v>1</v>
       </c>
       <c r="K676">
-        <v>7135469</v>
+        <v>5098500</v>
       </c>
       <c r="L676">
-        <v>7135469</v>
+        <v>5098500</v>
       </c>
     </row>
     <row r="677" spans="1:12">
@@ -28845,16 +29100,16 @@
         <v>839</v>
       </c>
       <c r="E677" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F677" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G677" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H677" t="s">
-        <v>947</v>
+        <v>212</v>
       </c>
       <c r="I677" t="s">
         <v>19</v>
@@ -28863,10 +29118,10 @@
         <v>1</v>
       </c>
       <c r="K677">
-        <v>300000</v>
+        <v>332500</v>
       </c>
       <c r="L677">
-        <v>300000</v>
+        <v>332500</v>
       </c>
     </row>
     <row r="678" spans="1:12">
@@ -28883,16 +29138,16 @@
         <v>839</v>
       </c>
       <c r="E678" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="F678" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="G678" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="H678" t="s">
-        <v>948</v>
+        <v>213</v>
       </c>
       <c r="I678" t="s">
         <v>19</v>
@@ -28901,10 +29156,2062 @@
         <v>1</v>
       </c>
       <c r="K678">
+        <v>7135469</v>
+      </c>
+      <c r="L678">
+        <v>7135469</v>
+      </c>
+    </row>
+    <row r="679" spans="1:12">
+      <c r="A679">
+        <v>676</v>
+      </c>
+      <c r="B679">
+        <v>626402</v>
+      </c>
+      <c r="C679" t="s">
+        <v>13</v>
+      </c>
+      <c r="D679" t="s">
+        <v>839</v>
+      </c>
+      <c r="E679" t="s">
+        <v>934</v>
+      </c>
+      <c r="F679" t="s">
+        <v>935</v>
+      </c>
+      <c r="G679" t="s">
+        <v>936</v>
+      </c>
+      <c r="H679" t="s">
+        <v>956</v>
+      </c>
+      <c r="I679" t="s">
+        <v>19</v>
+      </c>
+      <c r="J679">
+        <v>1</v>
+      </c>
+      <c r="K679">
         <v>300000</v>
       </c>
-      <c r="L678">
+      <c r="L679">
         <v>300000</v>
+      </c>
+    </row>
+    <row r="680" spans="1:12">
+      <c r="A680">
+        <v>677</v>
+      </c>
+      <c r="B680">
+        <v>626402</v>
+      </c>
+      <c r="C680" t="s">
+        <v>13</v>
+      </c>
+      <c r="D680" t="s">
+        <v>839</v>
+      </c>
+      <c r="E680" t="s">
+        <v>934</v>
+      </c>
+      <c r="F680" t="s">
+        <v>935</v>
+      </c>
+      <c r="G680" t="s">
+        <v>936</v>
+      </c>
+      <c r="H680" t="s">
+        <v>957</v>
+      </c>
+      <c r="I680" t="s">
+        <v>19</v>
+      </c>
+      <c r="J680">
+        <v>1</v>
+      </c>
+      <c r="K680">
+        <v>300000</v>
+      </c>
+      <c r="L680">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="681" spans="1:12">
+      <c r="A681">
+        <v>678</v>
+      </c>
+      <c r="B681">
+        <v>626402</v>
+      </c>
+      <c r="C681" t="s">
+        <v>13</v>
+      </c>
+      <c r="D681" t="s">
+        <v>901</v>
+      </c>
+      <c r="E681" t="s">
+        <v>958</v>
+      </c>
+      <c r="F681" t="s">
+        <v>959</v>
+      </c>
+      <c r="G681" t="s">
+        <v>960</v>
+      </c>
+      <c r="H681" t="s">
+        <v>783</v>
+      </c>
+      <c r="I681" t="s">
+        <v>19</v>
+      </c>
+      <c r="J681">
+        <v>1</v>
+      </c>
+      <c r="K681">
+        <v>12891000</v>
+      </c>
+      <c r="L681">
+        <v>12891000</v>
+      </c>
+    </row>
+    <row r="682" spans="1:12">
+      <c r="A682">
+        <v>679</v>
+      </c>
+      <c r="B682">
+        <v>626402</v>
+      </c>
+      <c r="C682" t="s">
+        <v>13</v>
+      </c>
+      <c r="D682" t="s">
+        <v>901</v>
+      </c>
+      <c r="E682" t="s">
+        <v>961</v>
+      </c>
+      <c r="F682" t="s">
+        <v>962</v>
+      </c>
+      <c r="G682" t="s">
+        <v>963</v>
+      </c>
+      <c r="H682" t="s">
+        <v>396</v>
+      </c>
+      <c r="I682" t="s">
+        <v>19</v>
+      </c>
+      <c r="J682">
+        <v>1</v>
+      </c>
+      <c r="K682">
+        <v>198905755</v>
+      </c>
+      <c r="L682">
+        <v>198905755</v>
+      </c>
+    </row>
+    <row r="683" spans="1:12">
+      <c r="A683">
+        <v>680</v>
+      </c>
+      <c r="B683">
+        <v>626402</v>
+      </c>
+      <c r="C683" t="s">
+        <v>13</v>
+      </c>
+      <c r="D683" t="s">
+        <v>901</v>
+      </c>
+      <c r="E683" t="s">
+        <v>964</v>
+      </c>
+      <c r="F683" t="s">
+        <v>965</v>
+      </c>
+      <c r="G683" t="s">
+        <v>121</v>
+      </c>
+      <c r="H683" t="s">
+        <v>255</v>
+      </c>
+      <c r="I683" t="s">
+        <v>19</v>
+      </c>
+      <c r="J683">
+        <v>1</v>
+      </c>
+      <c r="K683">
+        <v>2581400</v>
+      </c>
+      <c r="L683">
+        <v>2581400</v>
+      </c>
+    </row>
+    <row r="684" spans="1:12">
+      <c r="A684">
+        <v>681</v>
+      </c>
+      <c r="B684">
+        <v>626402</v>
+      </c>
+      <c r="C684" t="s">
+        <v>13</v>
+      </c>
+      <c r="D684" t="s">
+        <v>901</v>
+      </c>
+      <c r="E684" t="s">
+        <v>964</v>
+      </c>
+      <c r="F684" t="s">
+        <v>965</v>
+      </c>
+      <c r="G684" t="s">
+        <v>121</v>
+      </c>
+      <c r="H684" t="s">
+        <v>518</v>
+      </c>
+      <c r="I684" t="s">
+        <v>19</v>
+      </c>
+      <c r="J684">
+        <v>1</v>
+      </c>
+      <c r="K684">
+        <v>2361857</v>
+      </c>
+      <c r="L684">
+        <v>2361857</v>
+      </c>
+    </row>
+    <row r="685" spans="1:12">
+      <c r="A685">
+        <v>682</v>
+      </c>
+      <c r="B685">
+        <v>626402</v>
+      </c>
+      <c r="C685" t="s">
+        <v>13</v>
+      </c>
+      <c r="D685" t="s">
+        <v>966</v>
+      </c>
+      <c r="E685" t="s">
+        <v>967</v>
+      </c>
+      <c r="F685" t="s">
+        <v>968</v>
+      </c>
+      <c r="G685" t="s">
+        <v>969</v>
+      </c>
+      <c r="H685" t="s">
+        <v>970</v>
+      </c>
+      <c r="I685" t="s">
+        <v>19</v>
+      </c>
+      <c r="J685">
+        <v>1</v>
+      </c>
+      <c r="K685">
+        <v>19000000</v>
+      </c>
+      <c r="L685">
+        <v>19000000</v>
+      </c>
+    </row>
+    <row r="686" spans="1:12">
+      <c r="A686">
+        <v>683</v>
+      </c>
+      <c r="B686">
+        <v>626402</v>
+      </c>
+      <c r="C686" t="s">
+        <v>13</v>
+      </c>
+      <c r="D686" t="s">
+        <v>966</v>
+      </c>
+      <c r="E686" t="s">
+        <v>971</v>
+      </c>
+      <c r="F686" t="s">
+        <v>972</v>
+      </c>
+      <c r="G686" t="s">
+        <v>973</v>
+      </c>
+      <c r="H686" t="s">
+        <v>974</v>
+      </c>
+      <c r="I686" t="s">
+        <v>19</v>
+      </c>
+      <c r="J686">
+        <v>1</v>
+      </c>
+      <c r="K686">
+        <v>22311000</v>
+      </c>
+      <c r="L686">
+        <v>22311000</v>
+      </c>
+    </row>
+    <row r="687" spans="1:12">
+      <c r="A687">
+        <v>684</v>
+      </c>
+      <c r="B687">
+        <v>626402</v>
+      </c>
+      <c r="C687" t="s">
+        <v>13</v>
+      </c>
+      <c r="D687" t="s">
+        <v>966</v>
+      </c>
+      <c r="E687" t="s">
+        <v>975</v>
+      </c>
+      <c r="F687" t="s">
+        <v>976</v>
+      </c>
+      <c r="G687" t="s">
+        <v>977</v>
+      </c>
+      <c r="H687" t="s">
+        <v>336</v>
+      </c>
+      <c r="I687" t="s">
+        <v>19</v>
+      </c>
+      <c r="J687">
+        <v>1</v>
+      </c>
+      <c r="K687">
+        <v>20000000</v>
+      </c>
+      <c r="L687">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="688" spans="1:12">
+      <c r="A688">
+        <v>685</v>
+      </c>
+      <c r="B688">
+        <v>626402</v>
+      </c>
+      <c r="C688" t="s">
+        <v>13</v>
+      </c>
+      <c r="D688" t="s">
+        <v>966</v>
+      </c>
+      <c r="E688" t="s">
+        <v>978</v>
+      </c>
+      <c r="F688" t="s">
+        <v>979</v>
+      </c>
+      <c r="G688" t="s">
+        <v>980</v>
+      </c>
+      <c r="H688" t="s">
+        <v>256</v>
+      </c>
+      <c r="I688" t="s">
+        <v>19</v>
+      </c>
+      <c r="J688">
+        <v>1</v>
+      </c>
+      <c r="K688">
+        <v>18636900</v>
+      </c>
+      <c r="L688">
+        <v>18636900</v>
+      </c>
+    </row>
+    <row r="689" spans="1:12">
+      <c r="A689">
+        <v>686</v>
+      </c>
+      <c r="B689">
+        <v>626402</v>
+      </c>
+      <c r="C689" t="s">
+        <v>13</v>
+      </c>
+      <c r="D689" t="s">
+        <v>921</v>
+      </c>
+      <c r="E689" t="s">
+        <v>981</v>
+      </c>
+      <c r="F689" t="s">
+        <v>982</v>
+      </c>
+      <c r="G689" t="s">
+        <v>983</v>
+      </c>
+      <c r="H689" t="s">
+        <v>373</v>
+      </c>
+      <c r="I689" t="s">
+        <v>19</v>
+      </c>
+      <c r="J689">
+        <v>1</v>
+      </c>
+      <c r="K689">
+        <v>4402600</v>
+      </c>
+      <c r="L689">
+        <v>4402600</v>
+      </c>
+    </row>
+    <row r="690" spans="1:12">
+      <c r="A690">
+        <v>687</v>
+      </c>
+      <c r="B690">
+        <v>626402</v>
+      </c>
+      <c r="C690" t="s">
+        <v>13</v>
+      </c>
+      <c r="D690" t="s">
+        <v>921</v>
+      </c>
+      <c r="E690" t="s">
+        <v>984</v>
+      </c>
+      <c r="F690" t="s">
+        <v>985</v>
+      </c>
+      <c r="G690" t="s">
+        <v>986</v>
+      </c>
+      <c r="H690" t="s">
+        <v>218</v>
+      </c>
+      <c r="I690" t="s">
+        <v>19</v>
+      </c>
+      <c r="J690">
+        <v>1</v>
+      </c>
+      <c r="K690">
+        <v>30969218</v>
+      </c>
+      <c r="L690">
+        <v>30969218</v>
+      </c>
+    </row>
+    <row r="691" spans="1:12">
+      <c r="A691">
+        <v>688</v>
+      </c>
+      <c r="B691">
+        <v>626402</v>
+      </c>
+      <c r="C691" t="s">
+        <v>13</v>
+      </c>
+      <c r="D691" t="s">
+        <v>921</v>
+      </c>
+      <c r="E691" t="s">
+        <v>987</v>
+      </c>
+      <c r="F691" t="s">
+        <v>988</v>
+      </c>
+      <c r="G691" t="s">
+        <v>989</v>
+      </c>
+      <c r="H691" t="s">
+        <v>218</v>
+      </c>
+      <c r="I691" t="s">
+        <v>19</v>
+      </c>
+      <c r="J691">
+        <v>1</v>
+      </c>
+      <c r="K691">
+        <v>14328133</v>
+      </c>
+      <c r="L691">
+        <v>14328133</v>
+      </c>
+    </row>
+    <row r="692" spans="1:12">
+      <c r="A692">
+        <v>689</v>
+      </c>
+      <c r="B692">
+        <v>626402</v>
+      </c>
+      <c r="C692" t="s">
+        <v>13</v>
+      </c>
+      <c r="D692" t="s">
+        <v>966</v>
+      </c>
+      <c r="E692" t="s">
+        <v>990</v>
+      </c>
+      <c r="F692" t="s">
+        <v>991</v>
+      </c>
+      <c r="G692" t="s">
+        <v>429</v>
+      </c>
+      <c r="H692" t="s">
+        <v>255</v>
+      </c>
+      <c r="I692" t="s">
+        <v>19</v>
+      </c>
+      <c r="J692">
+        <v>1</v>
+      </c>
+      <c r="K692">
+        <v>12429300</v>
+      </c>
+      <c r="L692">
+        <v>12429300</v>
+      </c>
+    </row>
+    <row r="693" spans="1:12">
+      <c r="A693">
+        <v>690</v>
+      </c>
+      <c r="B693">
+        <v>626402</v>
+      </c>
+      <c r="C693" t="s">
+        <v>13</v>
+      </c>
+      <c r="D693" t="s">
+        <v>966</v>
+      </c>
+      <c r="E693" t="s">
+        <v>990</v>
+      </c>
+      <c r="F693" t="s">
+        <v>991</v>
+      </c>
+      <c r="G693" t="s">
+        <v>429</v>
+      </c>
+      <c r="H693" t="s">
+        <v>430</v>
+      </c>
+      <c r="I693" t="s">
+        <v>19</v>
+      </c>
+      <c r="J693">
+        <v>1</v>
+      </c>
+      <c r="K693">
+        <v>22460000</v>
+      </c>
+      <c r="L693">
+        <v>22460000</v>
+      </c>
+    </row>
+    <row r="694" spans="1:12">
+      <c r="A694">
+        <v>691</v>
+      </c>
+      <c r="B694">
+        <v>626402</v>
+      </c>
+      <c r="C694" t="s">
+        <v>13</v>
+      </c>
+      <c r="D694" t="s">
+        <v>966</v>
+      </c>
+      <c r="E694" t="s">
+        <v>990</v>
+      </c>
+      <c r="F694" t="s">
+        <v>991</v>
+      </c>
+      <c r="G694" t="s">
+        <v>429</v>
+      </c>
+      <c r="H694" t="s">
+        <v>431</v>
+      </c>
+      <c r="I694" t="s">
+        <v>19</v>
+      </c>
+      <c r="J694">
+        <v>1</v>
+      </c>
+      <c r="K694">
+        <v>40832000</v>
+      </c>
+      <c r="L694">
+        <v>40832000</v>
+      </c>
+    </row>
+    <row r="695" spans="1:12">
+      <c r="A695">
+        <v>692</v>
+      </c>
+      <c r="B695">
+        <v>626402</v>
+      </c>
+      <c r="C695" t="s">
+        <v>13</v>
+      </c>
+      <c r="D695" t="s">
+        <v>966</v>
+      </c>
+      <c r="E695" t="s">
+        <v>990</v>
+      </c>
+      <c r="F695" t="s">
+        <v>991</v>
+      </c>
+      <c r="G695" t="s">
+        <v>429</v>
+      </c>
+      <c r="H695" t="s">
+        <v>992</v>
+      </c>
+      <c r="I695" t="s">
+        <v>19</v>
+      </c>
+      <c r="J695">
+        <v>1</v>
+      </c>
+      <c r="K695">
+        <v>1952000</v>
+      </c>
+      <c r="L695">
+        <v>1952000</v>
+      </c>
+    </row>
+    <row r="696" spans="1:12">
+      <c r="A696">
+        <v>693</v>
+      </c>
+      <c r="B696">
+        <v>626402</v>
+      </c>
+      <c r="C696" t="s">
+        <v>13</v>
+      </c>
+      <c r="D696" t="s">
+        <v>966</v>
+      </c>
+      <c r="E696" t="s">
+        <v>990</v>
+      </c>
+      <c r="F696" t="s">
+        <v>991</v>
+      </c>
+      <c r="G696" t="s">
+        <v>429</v>
+      </c>
+      <c r="H696" t="s">
+        <v>993</v>
+      </c>
+      <c r="I696" t="s">
+        <v>19</v>
+      </c>
+      <c r="J696">
+        <v>1</v>
+      </c>
+      <c r="K696">
+        <v>3816000</v>
+      </c>
+      <c r="L696">
+        <v>3816000</v>
+      </c>
+    </row>
+    <row r="697" spans="1:12">
+      <c r="A697">
+        <v>694</v>
+      </c>
+      <c r="B697">
+        <v>626402</v>
+      </c>
+      <c r="C697" t="s">
+        <v>13</v>
+      </c>
+      <c r="D697" t="s">
+        <v>966</v>
+      </c>
+      <c r="E697" t="s">
+        <v>990</v>
+      </c>
+      <c r="F697" t="s">
+        <v>991</v>
+      </c>
+      <c r="G697" t="s">
+        <v>429</v>
+      </c>
+      <c r="H697" t="s">
+        <v>994</v>
+      </c>
+      <c r="I697" t="s">
+        <v>19</v>
+      </c>
+      <c r="J697">
+        <v>1</v>
+      </c>
+      <c r="K697">
+        <v>1696000</v>
+      </c>
+      <c r="L697">
+        <v>1696000</v>
+      </c>
+    </row>
+    <row r="698" spans="1:12">
+      <c r="A698">
+        <v>695</v>
+      </c>
+      <c r="B698">
+        <v>626402</v>
+      </c>
+      <c r="C698" t="s">
+        <v>13</v>
+      </c>
+      <c r="D698" t="s">
+        <v>966</v>
+      </c>
+      <c r="E698" t="s">
+        <v>990</v>
+      </c>
+      <c r="F698" t="s">
+        <v>991</v>
+      </c>
+      <c r="G698" t="s">
+        <v>429</v>
+      </c>
+      <c r="H698" t="s">
+        <v>995</v>
+      </c>
+      <c r="I698" t="s">
+        <v>19</v>
+      </c>
+      <c r="J698">
+        <v>1</v>
+      </c>
+      <c r="K698">
+        <v>2976000</v>
+      </c>
+      <c r="L698">
+        <v>2976000</v>
+      </c>
+    </row>
+    <row r="699" spans="1:12">
+      <c r="A699">
+        <v>696</v>
+      </c>
+      <c r="B699">
+        <v>626402</v>
+      </c>
+      <c r="C699" t="s">
+        <v>13</v>
+      </c>
+      <c r="D699" t="s">
+        <v>966</v>
+      </c>
+      <c r="E699" t="s">
+        <v>990</v>
+      </c>
+      <c r="F699" t="s">
+        <v>991</v>
+      </c>
+      <c r="G699" t="s">
+        <v>429</v>
+      </c>
+      <c r="H699" t="s">
+        <v>996</v>
+      </c>
+      <c r="I699" t="s">
+        <v>19</v>
+      </c>
+      <c r="J699">
+        <v>1</v>
+      </c>
+      <c r="K699">
+        <v>2844000</v>
+      </c>
+      <c r="L699">
+        <v>2844000</v>
+      </c>
+    </row>
+    <row r="700" spans="1:12">
+      <c r="A700">
+        <v>697</v>
+      </c>
+      <c r="B700">
+        <v>626402</v>
+      </c>
+      <c r="C700" t="s">
+        <v>13</v>
+      </c>
+      <c r="D700" t="s">
+        <v>966</v>
+      </c>
+      <c r="E700" t="s">
+        <v>990</v>
+      </c>
+      <c r="F700" t="s">
+        <v>991</v>
+      </c>
+      <c r="G700" t="s">
+        <v>429</v>
+      </c>
+      <c r="H700" t="s">
+        <v>997</v>
+      </c>
+      <c r="I700" t="s">
+        <v>19</v>
+      </c>
+      <c r="J700">
+        <v>1</v>
+      </c>
+      <c r="K700">
+        <v>2184000</v>
+      </c>
+      <c r="L700">
+        <v>2184000</v>
+      </c>
+    </row>
+    <row r="701" spans="1:12">
+      <c r="A701">
+        <v>698</v>
+      </c>
+      <c r="B701">
+        <v>626402</v>
+      </c>
+      <c r="C701" t="s">
+        <v>13</v>
+      </c>
+      <c r="D701" t="s">
+        <v>966</v>
+      </c>
+      <c r="E701" t="s">
+        <v>990</v>
+      </c>
+      <c r="F701" t="s">
+        <v>991</v>
+      </c>
+      <c r="G701" t="s">
+        <v>429</v>
+      </c>
+      <c r="H701" t="s">
+        <v>998</v>
+      </c>
+      <c r="I701" t="s">
+        <v>19</v>
+      </c>
+      <c r="J701">
+        <v>1</v>
+      </c>
+      <c r="K701">
+        <v>160000</v>
+      </c>
+      <c r="L701">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="702" spans="1:12">
+      <c r="A702">
+        <v>699</v>
+      </c>
+      <c r="B702">
+        <v>626402</v>
+      </c>
+      <c r="C702" t="s">
+        <v>13</v>
+      </c>
+      <c r="D702" t="s">
+        <v>966</v>
+      </c>
+      <c r="E702" t="s">
+        <v>990</v>
+      </c>
+      <c r="F702" t="s">
+        <v>991</v>
+      </c>
+      <c r="G702" t="s">
+        <v>429</v>
+      </c>
+      <c r="H702" t="s">
+        <v>999</v>
+      </c>
+      <c r="I702" t="s">
+        <v>19</v>
+      </c>
+      <c r="J702">
+        <v>1</v>
+      </c>
+      <c r="K702">
+        <v>200000</v>
+      </c>
+      <c r="L702">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="703" spans="1:12">
+      <c r="A703">
+        <v>700</v>
+      </c>
+      <c r="B703">
+        <v>626402</v>
+      </c>
+      <c r="C703" t="s">
+        <v>13</v>
+      </c>
+      <c r="D703" t="s">
+        <v>966</v>
+      </c>
+      <c r="E703" t="s">
+        <v>990</v>
+      </c>
+      <c r="F703" t="s">
+        <v>991</v>
+      </c>
+      <c r="G703" t="s">
+        <v>429</v>
+      </c>
+      <c r="H703" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I703" t="s">
+        <v>19</v>
+      </c>
+      <c r="J703">
+        <v>1</v>
+      </c>
+      <c r="K703">
+        <v>784000</v>
+      </c>
+      <c r="L703">
+        <v>784000</v>
+      </c>
+    </row>
+    <row r="704" spans="1:12">
+      <c r="A704">
+        <v>701</v>
+      </c>
+      <c r="B704">
+        <v>626402</v>
+      </c>
+      <c r="C704" t="s">
+        <v>13</v>
+      </c>
+      <c r="D704" t="s">
+        <v>966</v>
+      </c>
+      <c r="E704" t="s">
+        <v>990</v>
+      </c>
+      <c r="F704" t="s">
+        <v>991</v>
+      </c>
+      <c r="G704" t="s">
+        <v>429</v>
+      </c>
+      <c r="H704" t="s">
+        <v>1001</v>
+      </c>
+      <c r="I704" t="s">
+        <v>19</v>
+      </c>
+      <c r="J704">
+        <v>1</v>
+      </c>
+      <c r="K704">
+        <v>240000</v>
+      </c>
+      <c r="L704">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="705" spans="1:12">
+      <c r="A705">
+        <v>702</v>
+      </c>
+      <c r="B705">
+        <v>626402</v>
+      </c>
+      <c r="C705" t="s">
+        <v>13</v>
+      </c>
+      <c r="D705" t="s">
+        <v>966</v>
+      </c>
+      <c r="E705" t="s">
+        <v>990</v>
+      </c>
+      <c r="F705" t="s">
+        <v>991</v>
+      </c>
+      <c r="G705" t="s">
+        <v>429</v>
+      </c>
+      <c r="H705" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I705" t="s">
+        <v>19</v>
+      </c>
+      <c r="J705">
+        <v>1</v>
+      </c>
+      <c r="K705">
+        <v>320000</v>
+      </c>
+      <c r="L705">
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="706" spans="1:12">
+      <c r="A706">
+        <v>703</v>
+      </c>
+      <c r="B706">
+        <v>626402</v>
+      </c>
+      <c r="C706" t="s">
+        <v>13</v>
+      </c>
+      <c r="D706" t="s">
+        <v>966</v>
+      </c>
+      <c r="E706" t="s">
+        <v>990</v>
+      </c>
+      <c r="F706" t="s">
+        <v>991</v>
+      </c>
+      <c r="G706" t="s">
+        <v>429</v>
+      </c>
+      <c r="H706" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I706" t="s">
+        <v>19</v>
+      </c>
+      <c r="J706">
+        <v>1</v>
+      </c>
+      <c r="K706">
+        <v>280000</v>
+      </c>
+      <c r="L706">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="707" spans="1:12">
+      <c r="A707">
+        <v>704</v>
+      </c>
+      <c r="B707">
+        <v>626402</v>
+      </c>
+      <c r="C707" t="s">
+        <v>13</v>
+      </c>
+      <c r="D707" t="s">
+        <v>966</v>
+      </c>
+      <c r="E707" t="s">
+        <v>990</v>
+      </c>
+      <c r="F707" t="s">
+        <v>991</v>
+      </c>
+      <c r="G707" t="s">
+        <v>429</v>
+      </c>
+      <c r="H707" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I707" t="s">
+        <v>19</v>
+      </c>
+      <c r="J707">
+        <v>1</v>
+      </c>
+      <c r="K707">
+        <v>720000</v>
+      </c>
+      <c r="L707">
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="708" spans="1:12">
+      <c r="A708">
+        <v>705</v>
+      </c>
+      <c r="B708">
+        <v>626402</v>
+      </c>
+      <c r="C708" t="s">
+        <v>13</v>
+      </c>
+      <c r="D708" t="s">
+        <v>966</v>
+      </c>
+      <c r="E708" t="s">
+        <v>990</v>
+      </c>
+      <c r="F708" t="s">
+        <v>991</v>
+      </c>
+      <c r="G708" t="s">
+        <v>429</v>
+      </c>
+      <c r="H708" t="s">
+        <v>1005</v>
+      </c>
+      <c r="I708" t="s">
+        <v>19</v>
+      </c>
+      <c r="J708">
+        <v>1</v>
+      </c>
+      <c r="K708">
+        <v>784000</v>
+      </c>
+      <c r="L708">
+        <v>784000</v>
+      </c>
+    </row>
+    <row r="709" spans="1:12">
+      <c r="A709">
+        <v>706</v>
+      </c>
+      <c r="B709">
+        <v>626402</v>
+      </c>
+      <c r="C709" t="s">
+        <v>13</v>
+      </c>
+      <c r="D709" t="s">
+        <v>966</v>
+      </c>
+      <c r="E709" t="s">
+        <v>990</v>
+      </c>
+      <c r="F709" t="s">
+        <v>991</v>
+      </c>
+      <c r="G709" t="s">
+        <v>429</v>
+      </c>
+      <c r="H709" t="s">
+        <v>1006</v>
+      </c>
+      <c r="I709" t="s">
+        <v>19</v>
+      </c>
+      <c r="J709">
+        <v>1</v>
+      </c>
+      <c r="K709">
+        <v>240000</v>
+      </c>
+      <c r="L709">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="710" spans="1:12">
+      <c r="A710">
+        <v>707</v>
+      </c>
+      <c r="B710">
+        <v>626402</v>
+      </c>
+      <c r="C710" t="s">
+        <v>13</v>
+      </c>
+      <c r="D710" t="s">
+        <v>966</v>
+      </c>
+      <c r="E710" t="s">
+        <v>990</v>
+      </c>
+      <c r="F710" t="s">
+        <v>991</v>
+      </c>
+      <c r="G710" t="s">
+        <v>429</v>
+      </c>
+      <c r="H710" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I710" t="s">
+        <v>19</v>
+      </c>
+      <c r="J710">
+        <v>1</v>
+      </c>
+      <c r="K710">
+        <v>816000</v>
+      </c>
+      <c r="L710">
+        <v>816000</v>
+      </c>
+    </row>
+    <row r="711" spans="1:12">
+      <c r="A711">
+        <v>708</v>
+      </c>
+      <c r="B711">
+        <v>626402</v>
+      </c>
+      <c r="C711" t="s">
+        <v>13</v>
+      </c>
+      <c r="D711" t="s">
+        <v>966</v>
+      </c>
+      <c r="E711" t="s">
+        <v>990</v>
+      </c>
+      <c r="F711" t="s">
+        <v>991</v>
+      </c>
+      <c r="G711" t="s">
+        <v>429</v>
+      </c>
+      <c r="H711" t="s">
+        <v>261</v>
+      </c>
+      <c r="I711" t="s">
+        <v>19</v>
+      </c>
+      <c r="J711">
+        <v>1</v>
+      </c>
+      <c r="K711">
+        <v>412000</v>
+      </c>
+      <c r="L711">
+        <v>412000</v>
+      </c>
+    </row>
+    <row r="712" spans="1:12">
+      <c r="A712">
+        <v>709</v>
+      </c>
+      <c r="B712">
+        <v>626402</v>
+      </c>
+      <c r="C712" t="s">
+        <v>13</v>
+      </c>
+      <c r="D712" t="s">
+        <v>966</v>
+      </c>
+      <c r="E712" t="s">
+        <v>990</v>
+      </c>
+      <c r="F712" t="s">
+        <v>991</v>
+      </c>
+      <c r="G712" t="s">
+        <v>429</v>
+      </c>
+      <c r="H712" t="s">
+        <v>432</v>
+      </c>
+      <c r="I712" t="s">
+        <v>19</v>
+      </c>
+      <c r="J712">
+        <v>1</v>
+      </c>
+      <c r="K712">
+        <v>750000</v>
+      </c>
+      <c r="L712">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="713" spans="1:12">
+      <c r="A713">
+        <v>710</v>
+      </c>
+      <c r="B713">
+        <v>626402</v>
+      </c>
+      <c r="C713" t="s">
+        <v>13</v>
+      </c>
+      <c r="D713" t="s">
+        <v>966</v>
+      </c>
+      <c r="E713" t="s">
+        <v>990</v>
+      </c>
+      <c r="F713" t="s">
+        <v>991</v>
+      </c>
+      <c r="G713" t="s">
+        <v>429</v>
+      </c>
+      <c r="H713" t="s">
+        <v>270</v>
+      </c>
+      <c r="I713" t="s">
+        <v>19</v>
+      </c>
+      <c r="J713">
+        <v>1</v>
+      </c>
+      <c r="K713">
+        <v>96000</v>
+      </c>
+      <c r="L713">
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="714" spans="1:12">
+      <c r="A714">
+        <v>711</v>
+      </c>
+      <c r="B714">
+        <v>626402</v>
+      </c>
+      <c r="C714" t="s">
+        <v>13</v>
+      </c>
+      <c r="D714" t="s">
+        <v>966</v>
+      </c>
+      <c r="E714" t="s">
+        <v>990</v>
+      </c>
+      <c r="F714" t="s">
+        <v>991</v>
+      </c>
+      <c r="G714" t="s">
+        <v>429</v>
+      </c>
+      <c r="H714" t="s">
+        <v>128</v>
+      </c>
+      <c r="I714" t="s">
+        <v>19</v>
+      </c>
+      <c r="J714">
+        <v>1</v>
+      </c>
+      <c r="K714">
+        <v>1715708</v>
+      </c>
+      <c r="L714">
+        <v>1715708</v>
+      </c>
+    </row>
+    <row r="715" spans="1:12">
+      <c r="A715">
+        <v>712</v>
+      </c>
+      <c r="B715">
+        <v>626402</v>
+      </c>
+      <c r="C715" t="s">
+        <v>13</v>
+      </c>
+      <c r="D715" t="s">
+        <v>966</v>
+      </c>
+      <c r="E715" t="s">
+        <v>990</v>
+      </c>
+      <c r="F715" t="s">
+        <v>991</v>
+      </c>
+      <c r="G715" t="s">
+        <v>429</v>
+      </c>
+      <c r="H715" t="s">
+        <v>518</v>
+      </c>
+      <c r="I715" t="s">
+        <v>19</v>
+      </c>
+      <c r="J715">
+        <v>1</v>
+      </c>
+      <c r="K715">
+        <v>360000</v>
+      </c>
+      <c r="L715">
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="716" spans="1:12">
+      <c r="A716">
+        <v>713</v>
+      </c>
+      <c r="B716">
+        <v>626402</v>
+      </c>
+      <c r="C716" t="s">
+        <v>13</v>
+      </c>
+      <c r="D716" t="s">
+        <v>966</v>
+      </c>
+      <c r="E716" t="s">
+        <v>990</v>
+      </c>
+      <c r="F716" t="s">
+        <v>991</v>
+      </c>
+      <c r="G716" t="s">
+        <v>429</v>
+      </c>
+      <c r="H716" t="s">
+        <v>1008</v>
+      </c>
+      <c r="I716" t="s">
+        <v>19</v>
+      </c>
+      <c r="J716">
+        <v>1</v>
+      </c>
+      <c r="K716">
+        <v>510000</v>
+      </c>
+      <c r="L716">
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="717" spans="1:12">
+      <c r="A717">
+        <v>714</v>
+      </c>
+      <c r="B717">
+        <v>626402</v>
+      </c>
+      <c r="C717" t="s">
+        <v>13</v>
+      </c>
+      <c r="D717" t="s">
+        <v>966</v>
+      </c>
+      <c r="E717" t="s">
+        <v>990</v>
+      </c>
+      <c r="F717" t="s">
+        <v>991</v>
+      </c>
+      <c r="G717" t="s">
+        <v>429</v>
+      </c>
+      <c r="H717" t="s">
+        <v>312</v>
+      </c>
+      <c r="I717" t="s">
+        <v>19</v>
+      </c>
+      <c r="J717">
+        <v>1</v>
+      </c>
+      <c r="K717">
+        <v>340000</v>
+      </c>
+      <c r="L717">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="718" spans="1:12">
+      <c r="A718">
+        <v>715</v>
+      </c>
+      <c r="B718">
+        <v>626402</v>
+      </c>
+      <c r="C718" t="s">
+        <v>13</v>
+      </c>
+      <c r="D718" t="s">
+        <v>966</v>
+      </c>
+      <c r="E718" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F718" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G718" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H718" t="s">
+        <v>1012</v>
+      </c>
+      <c r="I718" t="s">
+        <v>19</v>
+      </c>
+      <c r="J718">
+        <v>1</v>
+      </c>
+      <c r="K718">
+        <v>27654000</v>
+      </c>
+      <c r="L718">
+        <v>27654000</v>
+      </c>
+    </row>
+    <row r="719" spans="1:12">
+      <c r="A719">
+        <v>716</v>
+      </c>
+      <c r="B719">
+        <v>626402</v>
+      </c>
+      <c r="C719" t="s">
+        <v>13</v>
+      </c>
+      <c r="D719" t="s">
+        <v>966</v>
+      </c>
+      <c r="E719" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F719" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G719" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H719" t="s">
+        <v>1013</v>
+      </c>
+      <c r="I719" t="s">
+        <v>19</v>
+      </c>
+      <c r="J719">
+        <v>1</v>
+      </c>
+      <c r="K719">
+        <v>11070000</v>
+      </c>
+      <c r="L719">
+        <v>11070000</v>
+      </c>
+    </row>
+    <row r="720" spans="1:12">
+      <c r="A720">
+        <v>717</v>
+      </c>
+      <c r="B720">
+        <v>626402</v>
+      </c>
+      <c r="C720" t="s">
+        <v>13</v>
+      </c>
+      <c r="D720" t="s">
+        <v>966</v>
+      </c>
+      <c r="E720" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F720" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G720" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H720" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I720" t="s">
+        <v>19</v>
+      </c>
+      <c r="J720">
+        <v>1</v>
+      </c>
+      <c r="K720">
+        <v>161500</v>
+      </c>
+      <c r="L720">
+        <v>161500</v>
+      </c>
+    </row>
+    <row r="721" spans="1:12">
+      <c r="A721">
+        <v>718</v>
+      </c>
+      <c r="B721">
+        <v>626402</v>
+      </c>
+      <c r="C721" t="s">
+        <v>13</v>
+      </c>
+      <c r="D721" t="s">
+        <v>966</v>
+      </c>
+      <c r="E721" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F721" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G721" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H721" t="s">
+        <v>1015</v>
+      </c>
+      <c r="I721" t="s">
+        <v>19</v>
+      </c>
+      <c r="J721">
+        <v>1</v>
+      </c>
+      <c r="K721">
+        <v>2175985</v>
+      </c>
+      <c r="L721">
+        <v>2175985</v>
+      </c>
+    </row>
+    <row r="722" spans="1:12">
+      <c r="A722">
+        <v>719</v>
+      </c>
+      <c r="B722">
+        <v>626402</v>
+      </c>
+      <c r="C722" t="s">
+        <v>13</v>
+      </c>
+      <c r="D722" t="s">
+        <v>966</v>
+      </c>
+      <c r="E722" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F722" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G722" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H722" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I722" t="s">
+        <v>19</v>
+      </c>
+      <c r="J722">
+        <v>1</v>
+      </c>
+      <c r="K722">
+        <v>3000000</v>
+      </c>
+      <c r="L722">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="723" spans="1:12">
+      <c r="A723">
+        <v>720</v>
+      </c>
+      <c r="B723">
+        <v>626402</v>
+      </c>
+      <c r="C723" t="s">
+        <v>13</v>
+      </c>
+      <c r="D723" t="s">
+        <v>966</v>
+      </c>
+      <c r="E723" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F723" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G723" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H723" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I723" t="s">
+        <v>19</v>
+      </c>
+      <c r="J723">
+        <v>1</v>
+      </c>
+      <c r="K723">
+        <v>49000000</v>
+      </c>
+      <c r="L723">
+        <v>49000000</v>
+      </c>
+    </row>
+    <row r="724" spans="1:12">
+      <c r="A724">
+        <v>721</v>
+      </c>
+      <c r="B724">
+        <v>626402</v>
+      </c>
+      <c r="C724" t="s">
+        <v>13</v>
+      </c>
+      <c r="D724" t="s">
+        <v>966</v>
+      </c>
+      <c r="E724" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F724" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G724" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H724" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I724" t="s">
+        <v>19</v>
+      </c>
+      <c r="J724">
+        <v>1</v>
+      </c>
+      <c r="K724">
+        <v>315000</v>
+      </c>
+      <c r="L724">
+        <v>315000</v>
+      </c>
+    </row>
+    <row r="725" spans="1:12">
+      <c r="A725">
+        <v>722</v>
+      </c>
+      <c r="B725">
+        <v>626402</v>
+      </c>
+      <c r="C725" t="s">
+        <v>13</v>
+      </c>
+      <c r="D725" t="s">
+        <v>966</v>
+      </c>
+      <c r="E725" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F725" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G725" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H725" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I725" t="s">
+        <v>19</v>
+      </c>
+      <c r="J725">
+        <v>1</v>
+      </c>
+      <c r="K725">
+        <v>385000</v>
+      </c>
+      <c r="L725">
+        <v>385000</v>
+      </c>
+    </row>
+    <row r="726" spans="1:12">
+      <c r="A726">
+        <v>723</v>
+      </c>
+      <c r="B726">
+        <v>626402</v>
+      </c>
+      <c r="C726" t="s">
+        <v>13</v>
+      </c>
+      <c r="D726" t="s">
+        <v>966</v>
+      </c>
+      <c r="E726" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F726" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G726" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H726" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I726" t="s">
+        <v>19</v>
+      </c>
+      <c r="J726">
+        <v>1</v>
+      </c>
+      <c r="K726">
+        <v>2610000</v>
+      </c>
+      <c r="L726">
+        <v>2610000</v>
+      </c>
+    </row>
+    <row r="727" spans="1:12">
+      <c r="A727">
+        <v>724</v>
+      </c>
+      <c r="B727">
+        <v>626402</v>
+      </c>
+      <c r="C727" t="s">
+        <v>13</v>
+      </c>
+      <c r="D727" t="s">
+        <v>966</v>
+      </c>
+      <c r="E727" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F727" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G727" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H727" t="s">
+        <v>1021</v>
+      </c>
+      <c r="I727" t="s">
+        <v>19</v>
+      </c>
+      <c r="J727">
+        <v>1</v>
+      </c>
+      <c r="K727">
+        <v>3016434</v>
+      </c>
+      <c r="L727">
+        <v>3016434</v>
+      </c>
+    </row>
+    <row r="728" spans="1:12">
+      <c r="A728">
+        <v>725</v>
+      </c>
+      <c r="B728">
+        <v>626402</v>
+      </c>
+      <c r="C728" t="s">
+        <v>13</v>
+      </c>
+      <c r="D728" t="s">
+        <v>966</v>
+      </c>
+      <c r="E728" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F728" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G728" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H728" t="s">
+        <v>616</v>
+      </c>
+      <c r="I728" t="s">
+        <v>19</v>
+      </c>
+      <c r="J728">
+        <v>1</v>
+      </c>
+      <c r="K728">
+        <v>600000</v>
+      </c>
+      <c r="L728">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="729" spans="1:12">
+      <c r="A729">
+        <v>726</v>
+      </c>
+      <c r="B729">
+        <v>626402</v>
+      </c>
+      <c r="C729" t="s">
+        <v>13</v>
+      </c>
+      <c r="D729" t="s">
+        <v>921</v>
+      </c>
+      <c r="E729" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F729" t="s">
+        <v>1023</v>
+      </c>
+      <c r="G729" t="s">
+        <v>1024</v>
+      </c>
+      <c r="H729" t="s">
+        <v>545</v>
+      </c>
+      <c r="I729" t="s">
+        <v>19</v>
+      </c>
+      <c r="J729">
+        <v>1</v>
+      </c>
+      <c r="K729">
+        <v>12440000</v>
+      </c>
+      <c r="L729">
+        <v>12440000</v>
+      </c>
+    </row>
+    <row r="730" spans="1:12">
+      <c r="A730">
+        <v>727</v>
+      </c>
+      <c r="B730">
+        <v>626402</v>
+      </c>
+      <c r="C730" t="s">
+        <v>13</v>
+      </c>
+      <c r="D730" t="s">
+        <v>921</v>
+      </c>
+      <c r="E730" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F730" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G730" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H730" t="s">
+        <v>545</v>
+      </c>
+      <c r="I730" t="s">
+        <v>19</v>
+      </c>
+      <c r="J730">
+        <v>1</v>
+      </c>
+      <c r="K730">
+        <v>36930000</v>
+      </c>
+      <c r="L730">
+        <v>36930000</v>
+      </c>
+    </row>
+    <row r="731" spans="1:12">
+      <c r="A731">
+        <v>728</v>
+      </c>
+      <c r="B731">
+        <v>626402</v>
+      </c>
+      <c r="C731" t="s">
+        <v>13</v>
+      </c>
+      <c r="D731" t="s">
+        <v>921</v>
+      </c>
+      <c r="E731" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F731" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G731" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H731" t="s">
+        <v>545</v>
+      </c>
+      <c r="I731" t="s">
+        <v>19</v>
+      </c>
+      <c r="J731">
+        <v>1</v>
+      </c>
+      <c r="K731">
+        <v>86300000</v>
+      </c>
+      <c r="L731">
+        <v>86300000</v>
+      </c>
+    </row>
+    <row r="732" spans="1:12">
+      <c r="A732">
+        <v>729</v>
+      </c>
+      <c r="B732">
+        <v>626402</v>
+      </c>
+      <c r="C732" t="s">
+        <v>13</v>
+      </c>
+      <c r="D732" t="s">
+        <v>921</v>
+      </c>
+      <c r="E732" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F732" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G732" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H732" t="s">
+        <v>545</v>
+      </c>
+      <c r="I732" t="s">
+        <v>19</v>
+      </c>
+      <c r="J732">
+        <v>1</v>
+      </c>
+      <c r="K732">
+        <v>15000000</v>
+      </c>
+      <c r="L732">
+        <v>15000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updtate 13 mar 23
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1142">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -2960,6 +2960,18 @@
     <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor: 016 Tanggal 15 Februari 2024</t>
   </si>
   <si>
+    <t>2024-03-08</t>
+  </si>
+  <si>
+    <t>'00208T</t>
+  </si>
+  <si>
+    <t>'241751303005574</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran gaji susulan an VIda bulan Maret 2024 untuk 1 pegawai)</t>
+  </si>
+  <si>
     <t>'00209T</t>
   </si>
   <si>
@@ -3119,7 +3131,124 @@
     <t>Pembayaran Belanja Barang. Biaya penelitian peserta tubel S2-UNDIP an. Hilman Adi S sesuai SK KaBRSDMKP No 520 Tahun 2022 Tgl 11/8/2022 dan SK PPK No KEP 16/BRSDM.4/I/2024 Tgl 3/1/2024</t>
   </si>
   <si>
-    <t>2024-03-08</t>
+    <t>'00218T</t>
+  </si>
+  <si>
+    <t>'241751303005571</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran gaji susulan pegawai an. Devy bulan Januari s.d Maret 2024 untuk 1 pegawai)</t>
+  </si>
+  <si>
+    <t>'00219T</t>
+  </si>
+  <si>
+    <t>'241751303005385</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran kekurangan gaji pegawai Pusdik sesuai PP tarif baru bulan Januari-Februari 2024 untuk 30 pegawai)</t>
+  </si>
+  <si>
+    <t>'00220T</t>
+  </si>
+  <si>
+    <t>'241751303005376</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran uang makan pegawai pusdik bulan februari 2024 untuk 37 pegawai)</t>
+  </si>
+  <si>
+    <t>'00221T</t>
+  </si>
+  <si>
+    <t>'241751303005584</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran uang makan pegawai Sekretariat BRSDM bulan Februari 2024 untuk 72 pegawai)</t>
+  </si>
+  <si>
+    <t>'00222T</t>
+  </si>
+  <si>
+    <t>'241751303005370</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa Perjalanan Dinas untuk 2 pegawai sesuai ST Nomor B.1303/BPPSDM.1/KP.440/III/2024 Tanggal 27 Februari 2023.</t>
+  </si>
+  <si>
+    <t>'00223T</t>
+  </si>
+  <si>
+    <t>'241751303005373</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.337/BPPSDM.5/KP.440/II/2024 Tgl. 23 Februari 2024 a.n Drs.Mas Adi Pranggono</t>
+  </si>
+  <si>
+    <t>'00224T</t>
+  </si>
+  <si>
+    <t>'241751303005374</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.258/BPPSDM.5/KP.440/II/2024 Tgl. 15 Februari 2024 a.n Supriyadi,S.Pi dkk</t>
+  </si>
+  <si>
+    <t>'00225T</t>
+  </si>
+  <si>
+    <t>'241751303005369</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.258/BPPSDM.5/KP.440/II/2024 Tgl. 15 Februari 2024 a.n Fitra Aditama</t>
+  </si>
+  <si>
+    <t>'00226T</t>
+  </si>
+  <si>
+    <t>'241751303005371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.389/BPPSDM.5/KP.440/III/2024 Tgl. 01 Maret 2024 a.n Lilly Aprilya Pregiwati </t>
+  </si>
+  <si>
+    <t>'00227T</t>
+  </si>
+  <si>
+    <t>'241751303005368</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.389/BPPSDM.5/KP.440/III/2024 Tgl. 01 Maret 2024 a.n Riza Satriawan dkk</t>
+  </si>
+  <si>
+    <t>'00228T</t>
+  </si>
+  <si>
+    <t>'241751303005375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.352/BPPSDM.5/KP.440/I/2024 Tgl. 27 Februari 2024 a.n Ary Budhy Purwoko S Ap </t>
+  </si>
+  <si>
+    <t>'00230T</t>
+  </si>
+  <si>
+    <t>'241751303005372</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang berupa biaya perjadin sesuai ST No.B.369/BPPSDM.5/KP.440/II/2024 Tgl. 28 Februari 2024 a.n Drs Mas Adi Pranggono,MM</t>
+  </si>
+  <si>
+    <t>'00231T</t>
+  </si>
+  <si>
+    <t>'241751301005484</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor 033/BSM/SET.BPPSDM/III/202 Tanggal 1 Maret 2024.</t>
+  </si>
+  <si>
+    <t>'626402.175.523121.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BC.000523</t>
   </si>
   <si>
     <t>'00232T</t>
@@ -3131,9 +3260,6 @@
     <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor 034/BSM/SET.BPPSDM/II/2024 Tanggal 4 Maret 2024.</t>
   </si>
   <si>
-    <t>'626402.175.523121.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.BC.000523</t>
-  </si>
-  <si>
     <t>'00233T</t>
   </si>
   <si>
@@ -3216,6 +3342,105 @@
   </si>
   <si>
     <t>Pembayaran belanja pegawai(pembayaran uang makan pegawai Sekretariat BRSDM bulan Februari 2024 untuk 2 pegawai)</t>
+  </si>
+  <si>
+    <t>'00242T</t>
+  </si>
+  <si>
+    <t>'241751303005543</t>
+  </si>
+  <si>
+    <t>'00243T</t>
+  </si>
+  <si>
+    <t>'241751303005572</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran uang makan pegawai PPPK bulan Januari untuk 2 pegawai)</t>
+  </si>
+  <si>
+    <t>'626402.175.511628.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.001.AA.001365</t>
+  </si>
+  <si>
+    <t>2024-03-13</t>
+  </si>
+  <si>
+    <t>'00244T</t>
+  </si>
+  <si>
+    <t>'241751303005455</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perjalanan Dinas untuk 3 pegawai sesuai ST No. B.1459/BPPSDM.1/KP.440/III/2024 Tanggal 1 Maret 2024 a.n Yatin Agus, dkk</t>
+  </si>
+  <si>
+    <t>'00245T</t>
+  </si>
+  <si>
+    <t>'241751303005456</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perjalanan Dinas untuk 1 pegawai sesuai ST Nomor B.1459/BPPSDM.1/KP.440/III/2024 Tanggal 1 Maret 2024 a.n Nina Lusmiati</t>
+  </si>
+  <si>
+    <t>'00246T</t>
+  </si>
+  <si>
+    <t>'241751303005454</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perjalanan Dinas untuk 1 pegawai sesuai ST Nomor B.1269/BPPSDM.1/KP.440/III/2024 Tanggal 26 Februari 2024.</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.101.0A.000829</t>
+  </si>
+  <si>
+    <t>'00247T</t>
+  </si>
+  <si>
+    <t>'241751303005573</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran uang makan pegawai PPPK bulan Februari 2024 untuk 2 pegawai)</t>
+  </si>
+  <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
+    <t>'00248T</t>
+  </si>
+  <si>
+    <t>'241751301005835</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai SPK No:2/PPK/BRSDM.1/I/2024 Tgl.2-1-2024,BAST No:BAST.606/PPK/BRSDM.1/II/2024 Tgl.29-2-2-24,BAP No:607/PPK/BRSDM.1/II/2024 Tgl.29-2-2024 Pengadaan jasa internet provider sekretariat BRSDM TA 2024 TERMIN 2</t>
+  </si>
+  <si>
+    <t>'00249T</t>
+  </si>
+  <si>
+    <t>'241751301005899</t>
+  </si>
+  <si>
+    <t>Pembayara Belanja Barang Sesuai Kuitansi Nomor:0490/AGA.04.02/F06010000/2024 Tanggal 4 Maret 2024 Tagihan listrik Bln. Maret 2024 untuk Pemakaian Energi Listrik Bln. Februari 2024 GD.BSRDM ANCOL</t>
+  </si>
+  <si>
+    <t>'00250T</t>
+  </si>
+  <si>
+    <t>'241751304000045</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kuitansi Nomor:0006/AGA.04.02/020700/2024 Tgl.5 maret 2024 Tagihan Listrik Bln.Maret 2023 untuk pemakaian energi listrik Bln.Februari 2024 Gd.ARSIP BRSDM Depok</t>
+  </si>
+  <si>
+    <t>'00251T</t>
+  </si>
+  <si>
+    <t>'241751303005657</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran rapel kekurangan gaji pegawai Puslatluh bulan januari-februari 2024 untuk 37 pegawa/105 Jiwa)</t>
   </si>
 </sst>
 </file>
@@ -3557,7 +3782,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L742"/>
+  <dimension ref="A1:L786"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -29652,19 +29877,19 @@
         <v>13</v>
       </c>
       <c r="D689" t="s">
-        <v>921</v>
+        <v>981</v>
       </c>
       <c r="E689" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="F689" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="G689" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="H689" t="s">
-        <v>373</v>
+        <v>18</v>
       </c>
       <c r="I689" t="s">
         <v>19</v>
@@ -29673,10 +29898,10 @@
         <v>1</v>
       </c>
       <c r="K689">
-        <v>4402600</v>
+        <v>2564200</v>
       </c>
       <c r="L689">
-        <v>4402600</v>
+        <v>2564200</v>
       </c>
     </row>
     <row r="690" spans="1:12">
@@ -29690,19 +29915,19 @@
         <v>13</v>
       </c>
       <c r="D690" t="s">
-        <v>921</v>
+        <v>981</v>
       </c>
       <c r="E690" t="s">
+        <v>982</v>
+      </c>
+      <c r="F690" t="s">
+        <v>983</v>
+      </c>
+      <c r="G690" t="s">
         <v>984</v>
       </c>
-      <c r="F690" t="s">
-        <v>985</v>
-      </c>
-      <c r="G690" t="s">
-        <v>986</v>
-      </c>
       <c r="H690" t="s">
-        <v>218</v>
+        <v>20</v>
       </c>
       <c r="I690" t="s">
         <v>19</v>
@@ -29711,10 +29936,10 @@
         <v>1</v>
       </c>
       <c r="K690">
-        <v>30969218</v>
+        <v>99</v>
       </c>
       <c r="L690">
-        <v>30969218</v>
+        <v>99</v>
       </c>
     </row>
     <row r="691" spans="1:12">
@@ -29728,19 +29953,19 @@
         <v>13</v>
       </c>
       <c r="D691" t="s">
-        <v>921</v>
+        <v>981</v>
       </c>
       <c r="E691" t="s">
-        <v>987</v>
+        <v>982</v>
       </c>
       <c r="F691" t="s">
-        <v>988</v>
+        <v>983</v>
       </c>
       <c r="G691" t="s">
-        <v>989</v>
+        <v>984</v>
       </c>
       <c r="H691" t="s">
-        <v>218</v>
+        <v>21</v>
       </c>
       <c r="I691" t="s">
         <v>19</v>
@@ -29749,10 +29974,10 @@
         <v>1</v>
       </c>
       <c r="K691">
-        <v>14328133</v>
+        <v>256420</v>
       </c>
       <c r="L691">
-        <v>14328133</v>
+        <v>256420</v>
       </c>
     </row>
     <row r="692" spans="1:12">
@@ -29766,19 +29991,19 @@
         <v>13</v>
       </c>
       <c r="D692" t="s">
-        <v>966</v>
+        <v>981</v>
       </c>
       <c r="E692" t="s">
-        <v>990</v>
+        <v>982</v>
       </c>
       <c r="F692" t="s">
-        <v>991</v>
+        <v>983</v>
       </c>
       <c r="G692" t="s">
-        <v>429</v>
+        <v>984</v>
       </c>
       <c r="H692" t="s">
-        <v>255</v>
+        <v>23</v>
       </c>
       <c r="I692" t="s">
         <v>19</v>
@@ -29787,10 +30012,10 @@
         <v>1</v>
       </c>
       <c r="K692">
-        <v>12429300</v>
+        <v>330000</v>
       </c>
       <c r="L692">
-        <v>12429300</v>
+        <v>330000</v>
       </c>
     </row>
     <row r="693" spans="1:12">
@@ -29804,19 +30029,19 @@
         <v>13</v>
       </c>
       <c r="D693" t="s">
-        <v>966</v>
+        <v>981</v>
       </c>
       <c r="E693" t="s">
-        <v>990</v>
+        <v>982</v>
       </c>
       <c r="F693" t="s">
-        <v>991</v>
+        <v>983</v>
       </c>
       <c r="G693" t="s">
-        <v>429</v>
+        <v>984</v>
       </c>
       <c r="H693" t="s">
-        <v>430</v>
+        <v>25</v>
       </c>
       <c r="I693" t="s">
         <v>19</v>
@@ -29825,10 +30050,10 @@
         <v>1</v>
       </c>
       <c r="K693">
-        <v>22460000</v>
+        <v>144840</v>
       </c>
       <c r="L693">
-        <v>22460000</v>
+        <v>144840</v>
       </c>
     </row>
     <row r="694" spans="1:12">
@@ -29842,19 +30067,19 @@
         <v>13</v>
       </c>
       <c r="D694" t="s">
-        <v>966</v>
+        <v>921</v>
       </c>
       <c r="E694" t="s">
-        <v>990</v>
+        <v>985</v>
       </c>
       <c r="F694" t="s">
-        <v>991</v>
+        <v>986</v>
       </c>
       <c r="G694" t="s">
-        <v>429</v>
+        <v>987</v>
       </c>
       <c r="H694" t="s">
-        <v>431</v>
+        <v>373</v>
       </c>
       <c r="I694" t="s">
         <v>19</v>
@@ -29863,10 +30088,10 @@
         <v>1</v>
       </c>
       <c r="K694">
-        <v>40832000</v>
+        <v>4402600</v>
       </c>
       <c r="L694">
-        <v>40832000</v>
+        <v>4402600</v>
       </c>
     </row>
     <row r="695" spans="1:12">
@@ -29880,19 +30105,19 @@
         <v>13</v>
       </c>
       <c r="D695" t="s">
-        <v>966</v>
+        <v>921</v>
       </c>
       <c r="E695" t="s">
+        <v>988</v>
+      </c>
+      <c r="F695" t="s">
+        <v>989</v>
+      </c>
+      <c r="G695" t="s">
         <v>990</v>
       </c>
-      <c r="F695" t="s">
-        <v>991</v>
-      </c>
-      <c r="G695" t="s">
-        <v>429</v>
-      </c>
       <c r="H695" t="s">
-        <v>992</v>
+        <v>218</v>
       </c>
       <c r="I695" t="s">
         <v>19</v>
@@ -29901,10 +30126,10 @@
         <v>1</v>
       </c>
       <c r="K695">
-        <v>1952000</v>
+        <v>30969218</v>
       </c>
       <c r="L695">
-        <v>1952000</v>
+        <v>30969218</v>
       </c>
     </row>
     <row r="696" spans="1:12">
@@ -29918,19 +30143,19 @@
         <v>13</v>
       </c>
       <c r="D696" t="s">
-        <v>966</v>
+        <v>921</v>
       </c>
       <c r="E696" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="F696" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="G696" t="s">
-        <v>429</v>
+        <v>993</v>
       </c>
       <c r="H696" t="s">
-        <v>993</v>
+        <v>218</v>
       </c>
       <c r="I696" t="s">
         <v>19</v>
@@ -29939,10 +30164,10 @@
         <v>1</v>
       </c>
       <c r="K696">
-        <v>3816000</v>
+        <v>14328133</v>
       </c>
       <c r="L696">
-        <v>3816000</v>
+        <v>14328133</v>
       </c>
     </row>
     <row r="697" spans="1:12">
@@ -29959,16 +30184,16 @@
         <v>966</v>
       </c>
       <c r="E697" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F697" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G697" t="s">
         <v>429</v>
       </c>
       <c r="H697" t="s">
-        <v>994</v>
+        <v>255</v>
       </c>
       <c r="I697" t="s">
         <v>19</v>
@@ -29977,10 +30202,10 @@
         <v>1</v>
       </c>
       <c r="K697">
-        <v>1696000</v>
+        <v>12429300</v>
       </c>
       <c r="L697">
-        <v>1696000</v>
+        <v>12429300</v>
       </c>
     </row>
     <row r="698" spans="1:12">
@@ -29997,16 +30222,16 @@
         <v>966</v>
       </c>
       <c r="E698" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F698" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G698" t="s">
         <v>429</v>
       </c>
       <c r="H698" t="s">
-        <v>995</v>
+        <v>430</v>
       </c>
       <c r="I698" t="s">
         <v>19</v>
@@ -30015,10 +30240,10 @@
         <v>1</v>
       </c>
       <c r="K698">
-        <v>2976000</v>
+        <v>22460000</v>
       </c>
       <c r="L698">
-        <v>2976000</v>
+        <v>22460000</v>
       </c>
     </row>
     <row r="699" spans="1:12">
@@ -30035,16 +30260,16 @@
         <v>966</v>
       </c>
       <c r="E699" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F699" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G699" t="s">
         <v>429</v>
       </c>
       <c r="H699" t="s">
-        <v>996</v>
+        <v>431</v>
       </c>
       <c r="I699" t="s">
         <v>19</v>
@@ -30053,10 +30278,10 @@
         <v>1</v>
       </c>
       <c r="K699">
-        <v>2844000</v>
+        <v>40832000</v>
       </c>
       <c r="L699">
-        <v>2844000</v>
+        <v>40832000</v>
       </c>
     </row>
     <row r="700" spans="1:12">
@@ -30073,16 +30298,16 @@
         <v>966</v>
       </c>
       <c r="E700" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F700" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G700" t="s">
         <v>429</v>
       </c>
       <c r="H700" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="I700" t="s">
         <v>19</v>
@@ -30091,10 +30316,10 @@
         <v>1</v>
       </c>
       <c r="K700">
-        <v>2184000</v>
+        <v>1952000</v>
       </c>
       <c r="L700">
-        <v>2184000</v>
+        <v>1952000</v>
       </c>
     </row>
     <row r="701" spans="1:12">
@@ -30111,16 +30336,16 @@
         <v>966</v>
       </c>
       <c r="E701" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F701" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G701" t="s">
         <v>429</v>
       </c>
       <c r="H701" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I701" t="s">
         <v>19</v>
@@ -30129,10 +30354,10 @@
         <v>1</v>
       </c>
       <c r="K701">
-        <v>160000</v>
+        <v>3816000</v>
       </c>
       <c r="L701">
-        <v>160000</v>
+        <v>3816000</v>
       </c>
     </row>
     <row r="702" spans="1:12">
@@ -30149,16 +30374,16 @@
         <v>966</v>
       </c>
       <c r="E702" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F702" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G702" t="s">
         <v>429</v>
       </c>
       <c r="H702" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I702" t="s">
         <v>19</v>
@@ -30167,10 +30392,10 @@
         <v>1</v>
       </c>
       <c r="K702">
-        <v>200000</v>
+        <v>1696000</v>
       </c>
       <c r="L702">
-        <v>200000</v>
+        <v>1696000</v>
       </c>
     </row>
     <row r="703" spans="1:12">
@@ -30187,16 +30412,16 @@
         <v>966</v>
       </c>
       <c r="E703" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F703" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G703" t="s">
         <v>429</v>
       </c>
       <c r="H703" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I703" t="s">
         <v>19</v>
@@ -30205,10 +30430,10 @@
         <v>1</v>
       </c>
       <c r="K703">
-        <v>784000</v>
+        <v>2976000</v>
       </c>
       <c r="L703">
-        <v>784000</v>
+        <v>2976000</v>
       </c>
     </row>
     <row r="704" spans="1:12">
@@ -30225,16 +30450,16 @@
         <v>966</v>
       </c>
       <c r="E704" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F704" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G704" t="s">
         <v>429</v>
       </c>
       <c r="H704" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I704" t="s">
         <v>19</v>
@@ -30243,10 +30468,10 @@
         <v>1</v>
       </c>
       <c r="K704">
-        <v>240000</v>
+        <v>2844000</v>
       </c>
       <c r="L704">
-        <v>240000</v>
+        <v>2844000</v>
       </c>
     </row>
     <row r="705" spans="1:12">
@@ -30263,16 +30488,16 @@
         <v>966</v>
       </c>
       <c r="E705" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F705" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G705" t="s">
         <v>429</v>
       </c>
       <c r="H705" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="I705" t="s">
         <v>19</v>
@@ -30281,10 +30506,10 @@
         <v>1</v>
       </c>
       <c r="K705">
-        <v>320000</v>
+        <v>2184000</v>
       </c>
       <c r="L705">
-        <v>320000</v>
+        <v>2184000</v>
       </c>
     </row>
     <row r="706" spans="1:12">
@@ -30301,16 +30526,16 @@
         <v>966</v>
       </c>
       <c r="E706" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F706" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G706" t="s">
         <v>429</v>
       </c>
       <c r="H706" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I706" t="s">
         <v>19</v>
@@ -30319,10 +30544,10 @@
         <v>1</v>
       </c>
       <c r="K706">
-        <v>280000</v>
+        <v>160000</v>
       </c>
       <c r="L706">
-        <v>280000</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="707" spans="1:12">
@@ -30339,16 +30564,16 @@
         <v>966</v>
       </c>
       <c r="E707" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F707" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G707" t="s">
         <v>429</v>
       </c>
       <c r="H707" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="I707" t="s">
         <v>19</v>
@@ -30357,10 +30582,10 @@
         <v>1</v>
       </c>
       <c r="K707">
-        <v>720000</v>
+        <v>200000</v>
       </c>
       <c r="L707">
-        <v>720000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="708" spans="1:12">
@@ -30377,16 +30602,16 @@
         <v>966</v>
       </c>
       <c r="E708" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F708" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G708" t="s">
         <v>429</v>
       </c>
       <c r="H708" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="I708" t="s">
         <v>19</v>
@@ -30415,16 +30640,16 @@
         <v>966</v>
       </c>
       <c r="E709" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F709" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G709" t="s">
         <v>429</v>
       </c>
       <c r="H709" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="I709" t="s">
         <v>19</v>
@@ -30453,16 +30678,16 @@
         <v>966</v>
       </c>
       <c r="E710" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F710" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G710" t="s">
         <v>429</v>
       </c>
       <c r="H710" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="I710" t="s">
         <v>19</v>
@@ -30471,10 +30696,10 @@
         <v>1</v>
       </c>
       <c r="K710">
-        <v>816000</v>
+        <v>320000</v>
       </c>
       <c r="L710">
-        <v>816000</v>
+        <v>320000</v>
       </c>
     </row>
     <row r="711" spans="1:12">
@@ -30491,16 +30716,16 @@
         <v>966</v>
       </c>
       <c r="E711" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F711" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G711" t="s">
         <v>429</v>
       </c>
       <c r="H711" t="s">
-        <v>261</v>
+        <v>1007</v>
       </c>
       <c r="I711" t="s">
         <v>19</v>
@@ -30509,10 +30734,10 @@
         <v>1</v>
       </c>
       <c r="K711">
-        <v>412000</v>
+        <v>280000</v>
       </c>
       <c r="L711">
-        <v>412000</v>
+        <v>280000</v>
       </c>
     </row>
     <row r="712" spans="1:12">
@@ -30529,16 +30754,16 @@
         <v>966</v>
       </c>
       <c r="E712" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F712" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G712" t="s">
         <v>429</v>
       </c>
       <c r="H712" t="s">
-        <v>432</v>
+        <v>1008</v>
       </c>
       <c r="I712" t="s">
         <v>19</v>
@@ -30547,10 +30772,10 @@
         <v>1</v>
       </c>
       <c r="K712">
-        <v>750000</v>
+        <v>720000</v>
       </c>
       <c r="L712">
-        <v>750000</v>
+        <v>720000</v>
       </c>
     </row>
     <row r="713" spans="1:12">
@@ -30567,16 +30792,16 @@
         <v>966</v>
       </c>
       <c r="E713" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F713" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G713" t="s">
         <v>429</v>
       </c>
       <c r="H713" t="s">
-        <v>270</v>
+        <v>1009</v>
       </c>
       <c r="I713" t="s">
         <v>19</v>
@@ -30585,10 +30810,10 @@
         <v>1</v>
       </c>
       <c r="K713">
-        <v>96000</v>
+        <v>784000</v>
       </c>
       <c r="L713">
-        <v>96000</v>
+        <v>784000</v>
       </c>
     </row>
     <row r="714" spans="1:12">
@@ -30605,16 +30830,16 @@
         <v>966</v>
       </c>
       <c r="E714" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F714" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G714" t="s">
         <v>429</v>
       </c>
       <c r="H714" t="s">
-        <v>128</v>
+        <v>1010</v>
       </c>
       <c r="I714" t="s">
         <v>19</v>
@@ -30623,10 +30848,10 @@
         <v>1</v>
       </c>
       <c r="K714">
-        <v>1715708</v>
+        <v>240000</v>
       </c>
       <c r="L714">
-        <v>1715708</v>
+        <v>240000</v>
       </c>
     </row>
     <row r="715" spans="1:12">
@@ -30643,16 +30868,16 @@
         <v>966</v>
       </c>
       <c r="E715" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F715" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G715" t="s">
         <v>429</v>
       </c>
       <c r="H715" t="s">
-        <v>518</v>
+        <v>1011</v>
       </c>
       <c r="I715" t="s">
         <v>19</v>
@@ -30661,10 +30886,10 @@
         <v>1</v>
       </c>
       <c r="K715">
-        <v>360000</v>
+        <v>816000</v>
       </c>
       <c r="L715">
-        <v>360000</v>
+        <v>816000</v>
       </c>
     </row>
     <row r="716" spans="1:12">
@@ -30681,16 +30906,16 @@
         <v>966</v>
       </c>
       <c r="E716" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F716" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G716" t="s">
         <v>429</v>
       </c>
       <c r="H716" t="s">
-        <v>1008</v>
+        <v>261</v>
       </c>
       <c r="I716" t="s">
         <v>19</v>
@@ -30699,10 +30924,10 @@
         <v>1</v>
       </c>
       <c r="K716">
-        <v>510000</v>
+        <v>412000</v>
       </c>
       <c r="L716">
-        <v>510000</v>
+        <v>412000</v>
       </c>
     </row>
     <row r="717" spans="1:12">
@@ -30719,16 +30944,16 @@
         <v>966</v>
       </c>
       <c r="E717" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="F717" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="G717" t="s">
         <v>429</v>
       </c>
       <c r="H717" t="s">
-        <v>312</v>
+        <v>432</v>
       </c>
       <c r="I717" t="s">
         <v>19</v>
@@ -30737,10 +30962,10 @@
         <v>1</v>
       </c>
       <c r="K717">
-        <v>340000</v>
+        <v>750000</v>
       </c>
       <c r="L717">
-        <v>340000</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="718" spans="1:12">
@@ -30757,16 +30982,16 @@
         <v>966</v>
       </c>
       <c r="E718" t="s">
-        <v>1009</v>
+        <v>994</v>
       </c>
       <c r="F718" t="s">
-        <v>1010</v>
+        <v>995</v>
       </c>
       <c r="G718" t="s">
-        <v>1011</v>
+        <v>429</v>
       </c>
       <c r="H718" t="s">
-        <v>1012</v>
+        <v>270</v>
       </c>
       <c r="I718" t="s">
         <v>19</v>
@@ -30775,10 +31000,10 @@
         <v>1</v>
       </c>
       <c r="K718">
-        <v>27654000</v>
+        <v>96000</v>
       </c>
       <c r="L718">
-        <v>27654000</v>
+        <v>96000</v>
       </c>
     </row>
     <row r="719" spans="1:12">
@@ -30795,16 +31020,16 @@
         <v>966</v>
       </c>
       <c r="E719" t="s">
-        <v>1009</v>
+        <v>994</v>
       </c>
       <c r="F719" t="s">
-        <v>1010</v>
+        <v>995</v>
       </c>
       <c r="G719" t="s">
-        <v>1011</v>
+        <v>429</v>
       </c>
       <c r="H719" t="s">
-        <v>1013</v>
+        <v>128</v>
       </c>
       <c r="I719" t="s">
         <v>19</v>
@@ -30813,10 +31038,10 @@
         <v>1</v>
       </c>
       <c r="K719">
-        <v>11070000</v>
+        <v>1715708</v>
       </c>
       <c r="L719">
-        <v>11070000</v>
+        <v>1715708</v>
       </c>
     </row>
     <row r="720" spans="1:12">
@@ -30833,16 +31058,16 @@
         <v>966</v>
       </c>
       <c r="E720" t="s">
-        <v>1009</v>
+        <v>994</v>
       </c>
       <c r="F720" t="s">
-        <v>1010</v>
+        <v>995</v>
       </c>
       <c r="G720" t="s">
-        <v>1011</v>
+        <v>429</v>
       </c>
       <c r="H720" t="s">
-        <v>1014</v>
+        <v>518</v>
       </c>
       <c r="I720" t="s">
         <v>19</v>
@@ -30851,10 +31076,10 @@
         <v>1</v>
       </c>
       <c r="K720">
-        <v>161500</v>
+        <v>360000</v>
       </c>
       <c r="L720">
-        <v>161500</v>
+        <v>360000</v>
       </c>
     </row>
     <row r="721" spans="1:12">
@@ -30871,16 +31096,16 @@
         <v>966</v>
       </c>
       <c r="E721" t="s">
-        <v>1009</v>
+        <v>994</v>
       </c>
       <c r="F721" t="s">
-        <v>1010</v>
+        <v>995</v>
       </c>
       <c r="G721" t="s">
-        <v>1011</v>
+        <v>429</v>
       </c>
       <c r="H721" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="I721" t="s">
         <v>19</v>
@@ -30889,10 +31114,10 @@
         <v>1</v>
       </c>
       <c r="K721">
-        <v>2175985</v>
+        <v>510000</v>
       </c>
       <c r="L721">
-        <v>2175985</v>
+        <v>510000</v>
       </c>
     </row>
     <row r="722" spans="1:12">
@@ -30909,16 +31134,16 @@
         <v>966</v>
       </c>
       <c r="E722" t="s">
-        <v>1009</v>
+        <v>994</v>
       </c>
       <c r="F722" t="s">
-        <v>1010</v>
+        <v>995</v>
       </c>
       <c r="G722" t="s">
-        <v>1011</v>
+        <v>429</v>
       </c>
       <c r="H722" t="s">
-        <v>1016</v>
+        <v>312</v>
       </c>
       <c r="I722" t="s">
         <v>19</v>
@@ -30927,10 +31152,10 @@
         <v>1</v>
       </c>
       <c r="K722">
-        <v>3000000</v>
+        <v>340000</v>
       </c>
       <c r="L722">
-        <v>3000000</v>
+        <v>340000</v>
       </c>
     </row>
     <row r="723" spans="1:12">
@@ -30947,16 +31172,16 @@
         <v>966</v>
       </c>
       <c r="E723" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="F723" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="G723" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="H723" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="I723" t="s">
         <v>19</v>
@@ -30965,10 +31190,10 @@
         <v>1</v>
       </c>
       <c r="K723">
-        <v>49000000</v>
+        <v>27654000</v>
       </c>
       <c r="L723">
-        <v>49000000</v>
+        <v>27654000</v>
       </c>
     </row>
     <row r="724" spans="1:12">
@@ -30985,16 +31210,16 @@
         <v>966</v>
       </c>
       <c r="E724" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="F724" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="G724" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="H724" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I724" t="s">
         <v>19</v>
@@ -31003,10 +31228,10 @@
         <v>1</v>
       </c>
       <c r="K724">
-        <v>315000</v>
+        <v>11070000</v>
       </c>
       <c r="L724">
-        <v>315000</v>
+        <v>11070000</v>
       </c>
     </row>
     <row r="725" spans="1:12">
@@ -31023,16 +31248,16 @@
         <v>966</v>
       </c>
       <c r="E725" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="F725" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="G725" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="H725" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="I725" t="s">
         <v>19</v>
@@ -31041,10 +31266,10 @@
         <v>1</v>
       </c>
       <c r="K725">
-        <v>385000</v>
+        <v>161500</v>
       </c>
       <c r="L725">
-        <v>385000</v>
+        <v>161500</v>
       </c>
     </row>
     <row r="726" spans="1:12">
@@ -31061,16 +31286,16 @@
         <v>966</v>
       </c>
       <c r="E726" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="F726" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="G726" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="H726" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I726" t="s">
         <v>19</v>
@@ -31079,10 +31304,10 @@
         <v>1</v>
       </c>
       <c r="K726">
-        <v>2610000</v>
+        <v>2175985</v>
       </c>
       <c r="L726">
-        <v>2610000</v>
+        <v>2175985</v>
       </c>
     </row>
     <row r="727" spans="1:12">
@@ -31099,16 +31324,16 @@
         <v>966</v>
       </c>
       <c r="E727" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="F727" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="G727" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="H727" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I727" t="s">
         <v>19</v>
@@ -31117,10 +31342,10 @@
         <v>1</v>
       </c>
       <c r="K727">
-        <v>3016434</v>
+        <v>3000000</v>
       </c>
       <c r="L727">
-        <v>3016434</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="728" spans="1:12">
@@ -31137,16 +31362,16 @@
         <v>966</v>
       </c>
       <c r="E728" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="F728" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="G728" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="H728" t="s">
-        <v>616</v>
+        <v>1021</v>
       </c>
       <c r="I728" t="s">
         <v>19</v>
@@ -31155,10 +31380,10 @@
         <v>1</v>
       </c>
       <c r="K728">
-        <v>600000</v>
+        <v>49000000</v>
       </c>
       <c r="L728">
-        <v>600000</v>
+        <v>49000000</v>
       </c>
     </row>
     <row r="729" spans="1:12">
@@ -31172,20 +31397,20 @@
         <v>13</v>
       </c>
       <c r="D729" t="s">
-        <v>921</v>
+        <v>966</v>
       </c>
       <c r="E729" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F729" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G729" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H729" t="s">
         <v>1022</v>
       </c>
-      <c r="F729" t="s">
-        <v>1023</v>
-      </c>
-      <c r="G729" t="s">
-        <v>1024</v>
-      </c>
-      <c r="H729" t="s">
-        <v>545</v>
-      </c>
       <c r="I729" t="s">
         <v>19</v>
       </c>
@@ -31193,10 +31418,10 @@
         <v>1</v>
       </c>
       <c r="K729">
-        <v>12440000</v>
+        <v>315000</v>
       </c>
       <c r="L729">
-        <v>12440000</v>
+        <v>315000</v>
       </c>
     </row>
     <row r="730" spans="1:12">
@@ -31210,19 +31435,19 @@
         <v>13</v>
       </c>
       <c r="D730" t="s">
-        <v>921</v>
+        <v>966</v>
       </c>
       <c r="E730" t="s">
-        <v>1025</v>
+        <v>1013</v>
       </c>
       <c r="F730" t="s">
-        <v>1026</v>
+        <v>1014</v>
       </c>
       <c r="G730" t="s">
-        <v>1027</v>
+        <v>1015</v>
       </c>
       <c r="H730" t="s">
-        <v>545</v>
+        <v>1023</v>
       </c>
       <c r="I730" t="s">
         <v>19</v>
@@ -31231,10 +31456,10 @@
         <v>1</v>
       </c>
       <c r="K730">
-        <v>36930000</v>
+        <v>385000</v>
       </c>
       <c r="L730">
-        <v>36930000</v>
+        <v>385000</v>
       </c>
     </row>
     <row r="731" spans="1:12">
@@ -31248,19 +31473,19 @@
         <v>13</v>
       </c>
       <c r="D731" t="s">
-        <v>921</v>
+        <v>966</v>
       </c>
       <c r="E731" t="s">
-        <v>1028</v>
+        <v>1013</v>
       </c>
       <c r="F731" t="s">
-        <v>1029</v>
+        <v>1014</v>
       </c>
       <c r="G731" t="s">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="H731" t="s">
-        <v>545</v>
+        <v>1024</v>
       </c>
       <c r="I731" t="s">
         <v>19</v>
@@ -31269,10 +31494,10 @@
         <v>1</v>
       </c>
       <c r="K731">
-        <v>86300000</v>
+        <v>2610000</v>
       </c>
       <c r="L731">
-        <v>86300000</v>
+        <v>2610000</v>
       </c>
     </row>
     <row r="732" spans="1:12">
@@ -31286,19 +31511,19 @@
         <v>13</v>
       </c>
       <c r="D732" t="s">
-        <v>921</v>
+        <v>966</v>
       </c>
       <c r="E732" t="s">
-        <v>1031</v>
+        <v>1013</v>
       </c>
       <c r="F732" t="s">
-        <v>1032</v>
+        <v>1014</v>
       </c>
       <c r="G732" t="s">
-        <v>1033</v>
+        <v>1015</v>
       </c>
       <c r="H732" t="s">
-        <v>545</v>
+        <v>1025</v>
       </c>
       <c r="I732" t="s">
         <v>19</v>
@@ -31307,10 +31532,10 @@
         <v>1</v>
       </c>
       <c r="K732">
-        <v>15000000</v>
+        <v>3016434</v>
       </c>
       <c r="L732">
-        <v>15000000</v>
+        <v>3016434</v>
       </c>
     </row>
     <row r="733" spans="1:12">
@@ -31324,19 +31549,19 @@
         <v>13</v>
       </c>
       <c r="D733" t="s">
-        <v>1034</v>
+        <v>966</v>
       </c>
       <c r="E733" t="s">
-        <v>1035</v>
+        <v>1013</v>
       </c>
       <c r="F733" t="s">
-        <v>1036</v>
+        <v>1014</v>
       </c>
       <c r="G733" t="s">
-        <v>1037</v>
+        <v>1015</v>
       </c>
       <c r="H733" t="s">
-        <v>1038</v>
+        <v>616</v>
       </c>
       <c r="I733" t="s">
         <v>19</v>
@@ -31345,10 +31570,10 @@
         <v>1</v>
       </c>
       <c r="K733">
-        <v>28651320</v>
+        <v>600000</v>
       </c>
       <c r="L733">
-        <v>28651320</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="734" spans="1:12">
@@ -31362,19 +31587,19 @@
         <v>13</v>
       </c>
       <c r="D734" t="s">
-        <v>1034</v>
+        <v>921</v>
       </c>
       <c r="E734" t="s">
-        <v>1039</v>
+        <v>1026</v>
       </c>
       <c r="F734" t="s">
-        <v>1040</v>
+        <v>1027</v>
       </c>
       <c r="G734" t="s">
-        <v>1041</v>
+        <v>1028</v>
       </c>
       <c r="H734" t="s">
-        <v>613</v>
+        <v>545</v>
       </c>
       <c r="I734" t="s">
         <v>19</v>
@@ -31383,10 +31608,10 @@
         <v>1</v>
       </c>
       <c r="K734">
-        <v>3449500</v>
+        <v>12440000</v>
       </c>
       <c r="L734">
-        <v>3449500</v>
+        <v>12440000</v>
       </c>
     </row>
     <row r="735" spans="1:12">
@@ -31400,19 +31625,19 @@
         <v>13</v>
       </c>
       <c r="D735" t="s">
-        <v>1034</v>
+        <v>921</v>
       </c>
       <c r="E735" t="s">
-        <v>1042</v>
+        <v>1029</v>
       </c>
       <c r="F735" t="s">
-        <v>1043</v>
+        <v>1030</v>
       </c>
       <c r="G735" t="s">
-        <v>1044</v>
+        <v>1031</v>
       </c>
       <c r="H735" t="s">
-        <v>1045</v>
+        <v>545</v>
       </c>
       <c r="I735" t="s">
         <v>19</v>
@@ -31421,10 +31646,10 @@
         <v>1</v>
       </c>
       <c r="K735">
-        <v>35908500</v>
+        <v>36930000</v>
       </c>
       <c r="L735">
-        <v>35908500</v>
+        <v>36930000</v>
       </c>
     </row>
     <row r="736" spans="1:12">
@@ -31438,19 +31663,19 @@
         <v>13</v>
       </c>
       <c r="D736" t="s">
+        <v>921</v>
+      </c>
+      <c r="E736" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F736" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G736" t="s">
         <v>1034</v>
       </c>
-      <c r="E736" t="s">
-        <v>1046</v>
-      </c>
-      <c r="F736" t="s">
-        <v>1047</v>
-      </c>
-      <c r="G736" t="s">
-        <v>1048</v>
-      </c>
       <c r="H736" t="s">
-        <v>257</v>
+        <v>545</v>
       </c>
       <c r="I736" t="s">
         <v>19</v>
@@ -31459,10 +31684,10 @@
         <v>1</v>
       </c>
       <c r="K736">
-        <v>2053500</v>
+        <v>86300000</v>
       </c>
       <c r="L736">
-        <v>2053500</v>
+        <v>86300000</v>
       </c>
     </row>
     <row r="737" spans="1:12">
@@ -31476,19 +31701,19 @@
         <v>13</v>
       </c>
       <c r="D737" t="s">
-        <v>1034</v>
+        <v>921</v>
       </c>
       <c r="E737" t="s">
-        <v>1049</v>
+        <v>1035</v>
       </c>
       <c r="F737" t="s">
-        <v>1050</v>
+        <v>1036</v>
       </c>
       <c r="G737" t="s">
-        <v>1051</v>
+        <v>1037</v>
       </c>
       <c r="H737" t="s">
-        <v>275</v>
+        <v>545</v>
       </c>
       <c r="I737" t="s">
         <v>19</v>
@@ -31497,10 +31722,10 @@
         <v>1</v>
       </c>
       <c r="K737">
-        <v>4076500</v>
+        <v>15000000</v>
       </c>
       <c r="L737">
-        <v>4076500</v>
+        <v>15000000</v>
       </c>
     </row>
     <row r="738" spans="1:12">
@@ -31514,19 +31739,19 @@
         <v>13</v>
       </c>
       <c r="D738" t="s">
-        <v>921</v>
+        <v>981</v>
       </c>
       <c r="E738" t="s">
-        <v>1052</v>
+        <v>1038</v>
       </c>
       <c r="F738" t="s">
-        <v>1053</v>
+        <v>1039</v>
       </c>
       <c r="G738" t="s">
-        <v>1054</v>
+        <v>1040</v>
       </c>
       <c r="H738" t="s">
-        <v>400</v>
+        <v>46</v>
       </c>
       <c r="I738" t="s">
         <v>19</v>
@@ -31535,10 +31760,10 @@
         <v>1</v>
       </c>
       <c r="K738">
-        <v>414643586</v>
+        <v>8985000</v>
       </c>
       <c r="L738">
-        <v>414643586</v>
+        <v>8985000</v>
       </c>
     </row>
     <row r="739" spans="1:12">
@@ -31552,19 +31777,19 @@
         <v>13</v>
       </c>
       <c r="D739" t="s">
-        <v>921</v>
+        <v>981</v>
       </c>
       <c r="E739" t="s">
-        <v>1055</v>
+        <v>1038</v>
       </c>
       <c r="F739" t="s">
-        <v>1056</v>
+        <v>1039</v>
       </c>
       <c r="G739" t="s">
-        <v>1057</v>
+        <v>1040</v>
       </c>
       <c r="H739" t="s">
-        <v>510</v>
+        <v>47</v>
       </c>
       <c r="I739" t="s">
         <v>19</v>
@@ -31573,10 +31798,10 @@
         <v>1</v>
       </c>
       <c r="K739">
-        <v>9177893</v>
+        <v>33</v>
       </c>
       <c r="L739">
-        <v>9177893</v>
+        <v>33</v>
       </c>
     </row>
     <row r="740" spans="1:12">
@@ -31590,19 +31815,19 @@
         <v>13</v>
       </c>
       <c r="D740" t="s">
-        <v>921</v>
+        <v>981</v>
       </c>
       <c r="E740" t="s">
-        <v>1058</v>
+        <v>1038</v>
       </c>
       <c r="F740" t="s">
-        <v>1059</v>
+        <v>1039</v>
       </c>
       <c r="G740" t="s">
-        <v>1060</v>
+        <v>1040</v>
       </c>
       <c r="H740" t="s">
-        <v>400</v>
+        <v>48</v>
       </c>
       <c r="I740" t="s">
         <v>19</v>
@@ -31611,10 +31836,10 @@
         <v>1</v>
       </c>
       <c r="K740">
-        <v>5305483</v>
+        <v>898500</v>
       </c>
       <c r="L740">
-        <v>5305483</v>
+        <v>898500</v>
       </c>
     </row>
     <row r="741" spans="1:12">
@@ -31628,19 +31853,19 @@
         <v>13</v>
       </c>
       <c r="D741" t="s">
-        <v>921</v>
+        <v>981</v>
       </c>
       <c r="E741" t="s">
-        <v>1061</v>
+        <v>1038</v>
       </c>
       <c r="F741" t="s">
-        <v>1062</v>
+        <v>1039</v>
       </c>
       <c r="G741" t="s">
-        <v>1063</v>
+        <v>1040</v>
       </c>
       <c r="H741" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="I741" t="s">
         <v>19</v>
@@ -31649,10 +31874,10 @@
         <v>1</v>
       </c>
       <c r="K741">
-        <v>203332962</v>
+        <v>359400</v>
       </c>
       <c r="L741">
-        <v>203332962</v>
+        <v>359400</v>
       </c>
     </row>
     <row r="742" spans="1:12">
@@ -31666,31 +31891,1703 @@
         <v>13</v>
       </c>
       <c r="D742" t="s">
+        <v>981</v>
+      </c>
+      <c r="E742" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F742" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G742" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H742" t="s">
+        <v>52</v>
+      </c>
+      <c r="I742" t="s">
+        <v>19</v>
+      </c>
+      <c r="J742">
+        <v>1</v>
+      </c>
+      <c r="K742">
+        <v>350010</v>
+      </c>
+      <c r="L742">
+        <v>350010</v>
+      </c>
+    </row>
+    <row r="743" spans="1:12">
+      <c r="A743">
+        <v>740</v>
+      </c>
+      <c r="B743">
+        <v>626402</v>
+      </c>
+      <c r="C743" t="s">
+        <v>13</v>
+      </c>
+      <c r="D743" t="s">
+        <v>981</v>
+      </c>
+      <c r="E743" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F743" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G743" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H743" t="s">
+        <v>53</v>
+      </c>
+      <c r="I743" t="s">
+        <v>19</v>
+      </c>
+      <c r="J743">
+        <v>1</v>
+      </c>
+      <c r="K743">
+        <v>869040</v>
+      </c>
+      <c r="L743">
+        <v>869040</v>
+      </c>
+    </row>
+    <row r="744" spans="1:12">
+      <c r="A744">
+        <v>741</v>
+      </c>
+      <c r="B744">
+        <v>626402</v>
+      </c>
+      <c r="C744" t="s">
+        <v>13</v>
+      </c>
+      <c r="D744" t="s">
+        <v>981</v>
+      </c>
+      <c r="E744" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F744" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G744" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H744" t="s">
+        <v>54</v>
+      </c>
+      <c r="I744" t="s">
+        <v>19</v>
+      </c>
+      <c r="J744">
+        <v>1</v>
+      </c>
+      <c r="K744">
+        <v>555000</v>
+      </c>
+      <c r="L744">
+        <v>555000</v>
+      </c>
+    </row>
+    <row r="745" spans="1:12">
+      <c r="A745">
+        <v>742</v>
+      </c>
+      <c r="B745">
+        <v>626402</v>
+      </c>
+      <c r="C745" t="s">
+        <v>13</v>
+      </c>
+      <c r="D745" t="s">
         <v>921</v>
       </c>
-      <c r="E742" t="s">
+      <c r="E745" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F745" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G745" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H745" t="s">
+        <v>46</v>
+      </c>
+      <c r="I745" t="s">
+        <v>19</v>
+      </c>
+      <c r="J745">
+        <v>1</v>
+      </c>
+      <c r="K745">
+        <v>17178600</v>
+      </c>
+      <c r="L745">
+        <v>17178600</v>
+      </c>
+    </row>
+    <row r="746" spans="1:12">
+      <c r="A746">
+        <v>743</v>
+      </c>
+      <c r="B746">
+        <v>626402</v>
+      </c>
+      <c r="C746" t="s">
+        <v>13</v>
+      </c>
+      <c r="D746" t="s">
+        <v>921</v>
+      </c>
+      <c r="E746" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F746" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G746" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H746" t="s">
+        <v>47</v>
+      </c>
+      <c r="I746" t="s">
+        <v>19</v>
+      </c>
+      <c r="J746">
+        <v>1</v>
+      </c>
+      <c r="K746">
+        <v>1199</v>
+      </c>
+      <c r="L746">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="747" spans="1:12">
+      <c r="A747">
+        <v>744</v>
+      </c>
+      <c r="B747">
+        <v>626402</v>
+      </c>
+      <c r="C747" t="s">
+        <v>13</v>
+      </c>
+      <c r="D747" t="s">
+        <v>921</v>
+      </c>
+      <c r="E747" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F747" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G747" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H747" t="s">
+        <v>48</v>
+      </c>
+      <c r="I747" t="s">
+        <v>19</v>
+      </c>
+      <c r="J747">
+        <v>1</v>
+      </c>
+      <c r="K747">
+        <v>1122800</v>
+      </c>
+      <c r="L747">
+        <v>1122800</v>
+      </c>
+    </row>
+    <row r="748" spans="1:12">
+      <c r="A748">
+        <v>745</v>
+      </c>
+      <c r="B748">
+        <v>626402</v>
+      </c>
+      <c r="C748" t="s">
+        <v>13</v>
+      </c>
+      <c r="D748" t="s">
+        <v>921</v>
+      </c>
+      <c r="E748" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F748" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G748" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H748" t="s">
+        <v>49</v>
+      </c>
+      <c r="I748" t="s">
+        <v>19</v>
+      </c>
+      <c r="J748">
+        <v>1</v>
+      </c>
+      <c r="K748">
+        <v>338460</v>
+      </c>
+      <c r="L748">
+        <v>338460</v>
+      </c>
+    </row>
+    <row r="749" spans="1:12">
+      <c r="A749">
+        <v>746</v>
+      </c>
+      <c r="B749">
+        <v>626402</v>
+      </c>
+      <c r="C749" t="s">
+        <v>13</v>
+      </c>
+      <c r="D749" t="s">
+        <v>921</v>
+      </c>
+      <c r="E749" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F749" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G749" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H749" t="s">
+        <v>52</v>
+      </c>
+      <c r="I749" t="s">
+        <v>19</v>
+      </c>
+      <c r="J749">
+        <v>1</v>
+      </c>
+      <c r="K749">
+        <v>262602</v>
+      </c>
+      <c r="L749">
+        <v>262602</v>
+      </c>
+    </row>
+    <row r="750" spans="1:12">
+      <c r="A750">
+        <v>747</v>
+      </c>
+      <c r="B750">
+        <v>626402</v>
+      </c>
+      <c r="C750" t="s">
+        <v>13</v>
+      </c>
+      <c r="D750" t="s">
+        <v>921</v>
+      </c>
+      <c r="E750" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F750" t="s">
+        <v>1045</v>
+      </c>
+      <c r="G750" t="s">
+        <v>1046</v>
+      </c>
+      <c r="H750" t="s">
+        <v>85</v>
+      </c>
+      <c r="I750" t="s">
+        <v>19</v>
+      </c>
+      <c r="J750">
+        <v>1</v>
+      </c>
+      <c r="K750">
+        <v>18837000</v>
+      </c>
+      <c r="L750">
+        <v>18837000</v>
+      </c>
+    </row>
+    <row r="751" spans="1:12">
+      <c r="A751">
+        <v>748</v>
+      </c>
+      <c r="B751">
+        <v>626402</v>
+      </c>
+      <c r="C751" t="s">
+        <v>13</v>
+      </c>
+      <c r="D751" t="s">
+        <v>981</v>
+      </c>
+      <c r="E751" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F751" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G751" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H751" t="s">
+        <v>793</v>
+      </c>
+      <c r="I751" t="s">
+        <v>19</v>
+      </c>
+      <c r="J751">
+        <v>1</v>
+      </c>
+      <c r="K751">
+        <v>29407000</v>
+      </c>
+      <c r="L751">
+        <v>29407000</v>
+      </c>
+    </row>
+    <row r="752" spans="1:12">
+      <c r="A752">
+        <v>749</v>
+      </c>
+      <c r="B752">
+        <v>626402</v>
+      </c>
+      <c r="C752" t="s">
+        <v>13</v>
+      </c>
+      <c r="D752" t="s">
+        <v>981</v>
+      </c>
+      <c r="E752" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F752" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G752" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H752" t="s">
+        <v>183</v>
+      </c>
+      <c r="I752" t="s">
+        <v>19</v>
+      </c>
+      <c r="J752">
+        <v>1</v>
+      </c>
+      <c r="K752">
+        <v>5543000</v>
+      </c>
+      <c r="L752">
+        <v>5543000</v>
+      </c>
+    </row>
+    <row r="753" spans="1:12">
+      <c r="A753">
+        <v>750</v>
+      </c>
+      <c r="B753">
+        <v>626402</v>
+      </c>
+      <c r="C753" t="s">
+        <v>13</v>
+      </c>
+      <c r="D753" t="s">
+        <v>981</v>
+      </c>
+      <c r="E753" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F753" t="s">
+        <v>1054</v>
+      </c>
+      <c r="G753" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H753" t="s">
+        <v>373</v>
+      </c>
+      <c r="I753" t="s">
+        <v>19</v>
+      </c>
+      <c r="J753">
+        <v>1</v>
+      </c>
+      <c r="K753">
+        <v>3754500</v>
+      </c>
+      <c r="L753">
+        <v>3754500</v>
+      </c>
+    </row>
+    <row r="754" spans="1:12">
+      <c r="A754">
+        <v>751</v>
+      </c>
+      <c r="B754">
+        <v>626402</v>
+      </c>
+      <c r="C754" t="s">
+        <v>13</v>
+      </c>
+      <c r="D754" t="s">
+        <v>981</v>
+      </c>
+      <c r="E754" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F754" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G754" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H754" t="s">
+        <v>614</v>
+      </c>
+      <c r="I754" t="s">
+        <v>19</v>
+      </c>
+      <c r="J754">
+        <v>1</v>
+      </c>
+      <c r="K754">
+        <v>1876600</v>
+      </c>
+      <c r="L754">
+        <v>1876600</v>
+      </c>
+    </row>
+    <row r="755" spans="1:12">
+      <c r="A755">
+        <v>752</v>
+      </c>
+      <c r="B755">
+        <v>626402</v>
+      </c>
+      <c r="C755" t="s">
+        <v>13</v>
+      </c>
+      <c r="D755" t="s">
+        <v>981</v>
+      </c>
+      <c r="E755" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F755" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G755" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H755" t="s">
+        <v>614</v>
+      </c>
+      <c r="I755" t="s">
+        <v>19</v>
+      </c>
+      <c r="J755">
+        <v>1</v>
+      </c>
+      <c r="K755">
+        <v>338000</v>
+      </c>
+      <c r="L755">
+        <v>338000</v>
+      </c>
+    </row>
+    <row r="756" spans="1:12">
+      <c r="A756">
+        <v>753</v>
+      </c>
+      <c r="B756">
+        <v>626402</v>
+      </c>
+      <c r="C756" t="s">
+        <v>13</v>
+      </c>
+      <c r="D756" t="s">
+        <v>981</v>
+      </c>
+      <c r="E756" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F756" t="s">
+        <v>1063</v>
+      </c>
+      <c r="G756" t="s">
         <v>1064</v>
       </c>
-      <c r="F742" t="s">
+      <c r="H756" t="s">
+        <v>872</v>
+      </c>
+      <c r="I756" t="s">
+        <v>19</v>
+      </c>
+      <c r="J756">
+        <v>1</v>
+      </c>
+      <c r="K756">
+        <v>580000</v>
+      </c>
+      <c r="L756">
+        <v>580000</v>
+      </c>
+    </row>
+    <row r="757" spans="1:12">
+      <c r="A757">
+        <v>754</v>
+      </c>
+      <c r="B757">
+        <v>626402</v>
+      </c>
+      <c r="C757" t="s">
+        <v>13</v>
+      </c>
+      <c r="D757" t="s">
+        <v>981</v>
+      </c>
+      <c r="E757" t="s">
         <v>1065</v>
       </c>
-      <c r="G742" t="s">
+      <c r="F757" t="s">
         <v>1066</v>
       </c>
-      <c r="H742" t="s">
+      <c r="G757" t="s">
+        <v>1067</v>
+      </c>
+      <c r="H757" t="s">
+        <v>872</v>
+      </c>
+      <c r="I757" t="s">
+        <v>19</v>
+      </c>
+      <c r="J757">
+        <v>1</v>
+      </c>
+      <c r="K757">
+        <v>860000</v>
+      </c>
+      <c r="L757">
+        <v>860000</v>
+      </c>
+    </row>
+    <row r="758" spans="1:12">
+      <c r="A758">
+        <v>755</v>
+      </c>
+      <c r="B758">
+        <v>626402</v>
+      </c>
+      <c r="C758" t="s">
+        <v>13</v>
+      </c>
+      <c r="D758" t="s">
+        <v>981</v>
+      </c>
+      <c r="E758" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F758" t="s">
+        <v>1069</v>
+      </c>
+      <c r="G758" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H758" t="s">
+        <v>369</v>
+      </c>
+      <c r="I758" t="s">
+        <v>19</v>
+      </c>
+      <c r="J758">
+        <v>1</v>
+      </c>
+      <c r="K758">
+        <v>1274500</v>
+      </c>
+      <c r="L758">
+        <v>1274500</v>
+      </c>
+    </row>
+    <row r="759" spans="1:12">
+      <c r="A759">
+        <v>756</v>
+      </c>
+      <c r="B759">
+        <v>626402</v>
+      </c>
+      <c r="C759" t="s">
+        <v>13</v>
+      </c>
+      <c r="D759" t="s">
+        <v>981</v>
+      </c>
+      <c r="E759" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F759" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G759" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H759" t="s">
+        <v>373</v>
+      </c>
+      <c r="I759" t="s">
+        <v>19</v>
+      </c>
+      <c r="J759">
+        <v>1</v>
+      </c>
+      <c r="K759">
+        <v>10054800</v>
+      </c>
+      <c r="L759">
+        <v>10054800</v>
+      </c>
+    </row>
+    <row r="760" spans="1:12">
+      <c r="A760">
+        <v>757</v>
+      </c>
+      <c r="B760">
+        <v>626402</v>
+      </c>
+      <c r="C760" t="s">
+        <v>13</v>
+      </c>
+      <c r="D760" t="s">
+        <v>981</v>
+      </c>
+      <c r="E760" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F760" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G760" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H760" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I760" t="s">
+        <v>19</v>
+      </c>
+      <c r="J760">
+        <v>1</v>
+      </c>
+      <c r="K760">
+        <v>14468850</v>
+      </c>
+      <c r="L760">
+        <v>14468850</v>
+      </c>
+    </row>
+    <row r="761" spans="1:12">
+      <c r="A761">
+        <v>758</v>
+      </c>
+      <c r="B761">
+        <v>626402</v>
+      </c>
+      <c r="C761" t="s">
+        <v>13</v>
+      </c>
+      <c r="D761" t="s">
+        <v>981</v>
+      </c>
+      <c r="E761" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F761" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G761" t="s">
+        <v>1080</v>
+      </c>
+      <c r="H761" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I761" t="s">
+        <v>19</v>
+      </c>
+      <c r="J761">
+        <v>1</v>
+      </c>
+      <c r="K761">
+        <v>28651320</v>
+      </c>
+      <c r="L761">
+        <v>28651320</v>
+      </c>
+    </row>
+    <row r="762" spans="1:12">
+      <c r="A762">
+        <v>759</v>
+      </c>
+      <c r="B762">
+        <v>626402</v>
+      </c>
+      <c r="C762" t="s">
+        <v>13</v>
+      </c>
+      <c r="D762" t="s">
+        <v>981</v>
+      </c>
+      <c r="E762" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F762" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G762" t="s">
+        <v>1083</v>
+      </c>
+      <c r="H762" t="s">
+        <v>613</v>
+      </c>
+      <c r="I762" t="s">
+        <v>19</v>
+      </c>
+      <c r="J762">
+        <v>1</v>
+      </c>
+      <c r="K762">
+        <v>3449500</v>
+      </c>
+      <c r="L762">
+        <v>3449500</v>
+      </c>
+    </row>
+    <row r="763" spans="1:12">
+      <c r="A763">
+        <v>760</v>
+      </c>
+      <c r="B763">
+        <v>626402</v>
+      </c>
+      <c r="C763" t="s">
+        <v>13</v>
+      </c>
+      <c r="D763" t="s">
+        <v>981</v>
+      </c>
+      <c r="E763" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F763" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G763" t="s">
+        <v>1086</v>
+      </c>
+      <c r="H763" t="s">
+        <v>1087</v>
+      </c>
+      <c r="I763" t="s">
+        <v>19</v>
+      </c>
+      <c r="J763">
+        <v>1</v>
+      </c>
+      <c r="K763">
+        <v>35908500</v>
+      </c>
+      <c r="L763">
+        <v>35908500</v>
+      </c>
+    </row>
+    <row r="764" spans="1:12">
+      <c r="A764">
+        <v>761</v>
+      </c>
+      <c r="B764">
+        <v>626402</v>
+      </c>
+      <c r="C764" t="s">
+        <v>13</v>
+      </c>
+      <c r="D764" t="s">
+        <v>981</v>
+      </c>
+      <c r="E764" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F764" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G764" t="s">
+        <v>1090</v>
+      </c>
+      <c r="H764" t="s">
+        <v>257</v>
+      </c>
+      <c r="I764" t="s">
+        <v>19</v>
+      </c>
+      <c r="J764">
+        <v>1</v>
+      </c>
+      <c r="K764">
+        <v>2053500</v>
+      </c>
+      <c r="L764">
+        <v>2053500</v>
+      </c>
+    </row>
+    <row r="765" spans="1:12">
+      <c r="A765">
+        <v>762</v>
+      </c>
+      <c r="B765">
+        <v>626402</v>
+      </c>
+      <c r="C765" t="s">
+        <v>13</v>
+      </c>
+      <c r="D765" t="s">
+        <v>981</v>
+      </c>
+      <c r="E765" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F765" t="s">
+        <v>1092</v>
+      </c>
+      <c r="G765" t="s">
+        <v>1093</v>
+      </c>
+      <c r="H765" t="s">
+        <v>275</v>
+      </c>
+      <c r="I765" t="s">
+        <v>19</v>
+      </c>
+      <c r="J765">
+        <v>1</v>
+      </c>
+      <c r="K765">
+        <v>4076500</v>
+      </c>
+      <c r="L765">
+        <v>4076500</v>
+      </c>
+    </row>
+    <row r="766" spans="1:12">
+      <c r="A766">
+        <v>763</v>
+      </c>
+      <c r="B766">
+        <v>626402</v>
+      </c>
+      <c r="C766" t="s">
+        <v>13</v>
+      </c>
+      <c r="D766" t="s">
+        <v>921</v>
+      </c>
+      <c r="E766" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F766" t="s">
+        <v>1095</v>
+      </c>
+      <c r="G766" t="s">
+        <v>1096</v>
+      </c>
+      <c r="H766" t="s">
+        <v>400</v>
+      </c>
+      <c r="I766" t="s">
+        <v>19</v>
+      </c>
+      <c r="J766">
+        <v>1</v>
+      </c>
+      <c r="K766">
+        <v>414643586</v>
+      </c>
+      <c r="L766">
+        <v>414643586</v>
+      </c>
+    </row>
+    <row r="767" spans="1:12">
+      <c r="A767">
+        <v>764</v>
+      </c>
+      <c r="B767">
+        <v>626402</v>
+      </c>
+      <c r="C767" t="s">
+        <v>13</v>
+      </c>
+      <c r="D767" t="s">
+        <v>921</v>
+      </c>
+      <c r="E767" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F767" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G767" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H767" t="s">
+        <v>510</v>
+      </c>
+      <c r="I767" t="s">
+        <v>19</v>
+      </c>
+      <c r="J767">
+        <v>1</v>
+      </c>
+      <c r="K767">
+        <v>9177893</v>
+      </c>
+      <c r="L767">
+        <v>9177893</v>
+      </c>
+    </row>
+    <row r="768" spans="1:12">
+      <c r="A768">
+        <v>765</v>
+      </c>
+      <c r="B768">
+        <v>626402</v>
+      </c>
+      <c r="C768" t="s">
+        <v>13</v>
+      </c>
+      <c r="D768" t="s">
+        <v>921</v>
+      </c>
+      <c r="E768" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F768" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G768" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H768" t="s">
+        <v>400</v>
+      </c>
+      <c r="I768" t="s">
+        <v>19</v>
+      </c>
+      <c r="J768">
+        <v>1</v>
+      </c>
+      <c r="K768">
+        <v>5305483</v>
+      </c>
+      <c r="L768">
+        <v>5305483</v>
+      </c>
+    </row>
+    <row r="769" spans="1:12">
+      <c r="A769">
+        <v>766</v>
+      </c>
+      <c r="B769">
+        <v>626402</v>
+      </c>
+      <c r="C769" t="s">
+        <v>13</v>
+      </c>
+      <c r="D769" t="s">
+        <v>921</v>
+      </c>
+      <c r="E769" t="s">
+        <v>1103</v>
+      </c>
+      <c r="F769" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G769" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H769" t="s">
+        <v>80</v>
+      </c>
+      <c r="I769" t="s">
+        <v>19</v>
+      </c>
+      <c r="J769">
+        <v>1</v>
+      </c>
+      <c r="K769">
+        <v>203332962</v>
+      </c>
+      <c r="L769">
+        <v>203332962</v>
+      </c>
+    </row>
+    <row r="770" spans="1:12">
+      <c r="A770">
+        <v>767</v>
+      </c>
+      <c r="B770">
+        <v>626402</v>
+      </c>
+      <c r="C770" t="s">
+        <v>13</v>
+      </c>
+      <c r="D770" t="s">
+        <v>921</v>
+      </c>
+      <c r="E770" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F770" t="s">
+        <v>1107</v>
+      </c>
+      <c r="G770" t="s">
+        <v>1108</v>
+      </c>
+      <c r="H770" t="s">
         <v>793</v>
       </c>
-      <c r="I742" t="s">
-        <v>19</v>
-      </c>
-      <c r="J742">
-        <v>1</v>
-      </c>
-      <c r="K742">
+      <c r="I770" t="s">
+        <v>19</v>
+      </c>
+      <c r="J770">
+        <v>1</v>
+      </c>
+      <c r="K770">
         <v>883000</v>
       </c>
-      <c r="L742">
+      <c r="L770">
         <v>883000</v>
+      </c>
+    </row>
+    <row r="771" spans="1:12">
+      <c r="A771">
+        <v>768</v>
+      </c>
+      <c r="B771">
+        <v>626402</v>
+      </c>
+      <c r="C771" t="s">
+        <v>13</v>
+      </c>
+      <c r="D771" t="s">
+        <v>981</v>
+      </c>
+      <c r="E771" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F771" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G771" t="s">
+        <v>121</v>
+      </c>
+      <c r="H771" t="s">
+        <v>499</v>
+      </c>
+      <c r="I771" t="s">
+        <v>19</v>
+      </c>
+      <c r="J771">
+        <v>1</v>
+      </c>
+      <c r="K771">
+        <v>161547</v>
+      </c>
+      <c r="L771">
+        <v>161547</v>
+      </c>
+    </row>
+    <row r="772" spans="1:12">
+      <c r="A772">
+        <v>769</v>
+      </c>
+      <c r="B772">
+        <v>626402</v>
+      </c>
+      <c r="C772" t="s">
+        <v>13</v>
+      </c>
+      <c r="D772" t="s">
+        <v>981</v>
+      </c>
+      <c r="E772" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F772" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G772" t="s">
+        <v>121</v>
+      </c>
+      <c r="H772" t="s">
+        <v>123</v>
+      </c>
+      <c r="I772" t="s">
+        <v>19</v>
+      </c>
+      <c r="J772">
+        <v>1</v>
+      </c>
+      <c r="K772">
+        <v>271119</v>
+      </c>
+      <c r="L772">
+        <v>271119</v>
+      </c>
+    </row>
+    <row r="773" spans="1:12">
+      <c r="A773">
+        <v>770</v>
+      </c>
+      <c r="B773">
+        <v>626402</v>
+      </c>
+      <c r="C773" t="s">
+        <v>13</v>
+      </c>
+      <c r="D773" t="s">
+        <v>981</v>
+      </c>
+      <c r="E773" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F773" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G773" t="s">
+        <v>121</v>
+      </c>
+      <c r="H773" t="s">
+        <v>275</v>
+      </c>
+      <c r="I773" t="s">
+        <v>19</v>
+      </c>
+      <c r="J773">
+        <v>1</v>
+      </c>
+      <c r="K773">
+        <v>13457981</v>
+      </c>
+      <c r="L773">
+        <v>13457981</v>
+      </c>
+    </row>
+    <row r="774" spans="1:12">
+      <c r="A774">
+        <v>771</v>
+      </c>
+      <c r="B774">
+        <v>626402</v>
+      </c>
+      <c r="C774" t="s">
+        <v>13</v>
+      </c>
+      <c r="D774" t="s">
+        <v>981</v>
+      </c>
+      <c r="E774" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F774" t="s">
+        <v>1112</v>
+      </c>
+      <c r="G774" t="s">
+        <v>1113</v>
+      </c>
+      <c r="H774" t="s">
+        <v>1114</v>
+      </c>
+      <c r="I774" t="s">
+        <v>19</v>
+      </c>
+      <c r="J774">
+        <v>1</v>
+      </c>
+      <c r="K774">
+        <v>777000</v>
+      </c>
+      <c r="L774">
+        <v>777000</v>
+      </c>
+    </row>
+    <row r="775" spans="1:12">
+      <c r="A775">
+        <v>772</v>
+      </c>
+      <c r="B775">
+        <v>626402</v>
+      </c>
+      <c r="C775" t="s">
+        <v>13</v>
+      </c>
+      <c r="D775" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E775" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F775" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G775" t="s">
+        <v>1118</v>
+      </c>
+      <c r="H775" t="s">
+        <v>131</v>
+      </c>
+      <c r="I775" t="s">
+        <v>19</v>
+      </c>
+      <c r="J775">
+        <v>1</v>
+      </c>
+      <c r="K775">
+        <v>2383500</v>
+      </c>
+      <c r="L775">
+        <v>2383500</v>
+      </c>
+    </row>
+    <row r="776" spans="1:12">
+      <c r="A776">
+        <v>773</v>
+      </c>
+      <c r="B776">
+        <v>626402</v>
+      </c>
+      <c r="C776" t="s">
+        <v>13</v>
+      </c>
+      <c r="D776" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E776" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F776" t="s">
+        <v>1120</v>
+      </c>
+      <c r="G776" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H776" t="s">
+        <v>131</v>
+      </c>
+      <c r="I776" t="s">
+        <v>19</v>
+      </c>
+      <c r="J776">
+        <v>1</v>
+      </c>
+      <c r="K776">
+        <v>524500</v>
+      </c>
+      <c r="L776">
+        <v>524500</v>
+      </c>
+    </row>
+    <row r="777" spans="1:12">
+      <c r="A777">
+        <v>774</v>
+      </c>
+      <c r="B777">
+        <v>626402</v>
+      </c>
+      <c r="C777" t="s">
+        <v>13</v>
+      </c>
+      <c r="D777" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E777" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F777" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G777" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H777" t="s">
+        <v>1125</v>
+      </c>
+      <c r="I777" t="s">
+        <v>19</v>
+      </c>
+      <c r="J777">
+        <v>1</v>
+      </c>
+      <c r="K777">
+        <v>1757500</v>
+      </c>
+      <c r="L777">
+        <v>1757500</v>
+      </c>
+    </row>
+    <row r="778" spans="1:12">
+      <c r="A778">
+        <v>775</v>
+      </c>
+      <c r="B778">
+        <v>626402</v>
+      </c>
+      <c r="C778" t="s">
+        <v>13</v>
+      </c>
+      <c r="D778" t="s">
+        <v>981</v>
+      </c>
+      <c r="E778" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F778" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G778" t="s">
+        <v>1128</v>
+      </c>
+      <c r="H778" t="s">
+        <v>1114</v>
+      </c>
+      <c r="I778" t="s">
+        <v>19</v>
+      </c>
+      <c r="J778">
+        <v>1</v>
+      </c>
+      <c r="K778">
+        <v>703000</v>
+      </c>
+      <c r="L778">
+        <v>703000</v>
+      </c>
+    </row>
+    <row r="779" spans="1:12">
+      <c r="A779">
+        <v>776</v>
+      </c>
+      <c r="B779">
+        <v>626402</v>
+      </c>
+      <c r="C779" t="s">
+        <v>13</v>
+      </c>
+      <c r="D779" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E779" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F779" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G779" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H779" t="s">
+        <v>478</v>
+      </c>
+      <c r="I779" t="s">
+        <v>19</v>
+      </c>
+      <c r="J779">
+        <v>1</v>
+      </c>
+      <c r="K779">
+        <v>53000000</v>
+      </c>
+      <c r="L779">
+        <v>53000000</v>
+      </c>
+    </row>
+    <row r="780" spans="1:12">
+      <c r="A780">
+        <v>777</v>
+      </c>
+      <c r="B780">
+        <v>626402</v>
+      </c>
+      <c r="C780" t="s">
+        <v>13</v>
+      </c>
+      <c r="D780" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E780" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F780" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G780" t="s">
+        <v>1135</v>
+      </c>
+      <c r="H780" t="s">
+        <v>59</v>
+      </c>
+      <c r="I780" t="s">
+        <v>19</v>
+      </c>
+      <c r="J780">
+        <v>1</v>
+      </c>
+      <c r="K780">
+        <v>147618183</v>
+      </c>
+      <c r="L780">
+        <v>147618183</v>
+      </c>
+    </row>
+    <row r="781" spans="1:12">
+      <c r="A781">
+        <v>778</v>
+      </c>
+      <c r="B781">
+        <v>626402</v>
+      </c>
+      <c r="C781" t="s">
+        <v>13</v>
+      </c>
+      <c r="D781" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E781" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F781" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G781" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H781" t="s">
+        <v>59</v>
+      </c>
+      <c r="I781" t="s">
+        <v>19</v>
+      </c>
+      <c r="J781">
+        <v>1</v>
+      </c>
+      <c r="K781">
+        <v>1777878</v>
+      </c>
+      <c r="L781">
+        <v>1777878</v>
+      </c>
+    </row>
+    <row r="782" spans="1:12">
+      <c r="A782">
+        <v>779</v>
+      </c>
+      <c r="B782">
+        <v>626402</v>
+      </c>
+      <c r="C782" t="s">
+        <v>13</v>
+      </c>
+      <c r="D782" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E782" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F782" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G782" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H782" t="s">
+        <v>34</v>
+      </c>
+      <c r="I782" t="s">
+        <v>19</v>
+      </c>
+      <c r="J782">
+        <v>1</v>
+      </c>
+      <c r="K782">
+        <v>23424000</v>
+      </c>
+      <c r="L782">
+        <v>23424000</v>
+      </c>
+    </row>
+    <row r="783" spans="1:12">
+      <c r="A783">
+        <v>780</v>
+      </c>
+      <c r="B783">
+        <v>626402</v>
+      </c>
+      <c r="C783" t="s">
+        <v>13</v>
+      </c>
+      <c r="D783" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E783" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F783" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G783" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H783" t="s">
+        <v>35</v>
+      </c>
+      <c r="I783" t="s">
+        <v>19</v>
+      </c>
+      <c r="J783">
+        <v>1</v>
+      </c>
+      <c r="K783">
+        <v>1910</v>
+      </c>
+      <c r="L783">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="784" spans="1:12">
+      <c r="A784">
+        <v>781</v>
+      </c>
+      <c r="B784">
+        <v>626402</v>
+      </c>
+      <c r="C784" t="s">
+        <v>13</v>
+      </c>
+      <c r="D784" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E784" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F784" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G784" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H784" t="s">
+        <v>36</v>
+      </c>
+      <c r="I784" t="s">
+        <v>19</v>
+      </c>
+      <c r="J784">
+        <v>1</v>
+      </c>
+      <c r="K784">
+        <v>1722840</v>
+      </c>
+      <c r="L784">
+        <v>1722840</v>
+      </c>
+    </row>
+    <row r="785" spans="1:12">
+      <c r="A785">
+        <v>782</v>
+      </c>
+      <c r="B785">
+        <v>626402</v>
+      </c>
+      <c r="C785" t="s">
+        <v>13</v>
+      </c>
+      <c r="D785" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E785" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F785" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G785" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H785" t="s">
+        <v>37</v>
+      </c>
+      <c r="I785" t="s">
+        <v>19</v>
+      </c>
+      <c r="J785">
+        <v>1</v>
+      </c>
+      <c r="K785">
+        <v>514080</v>
+      </c>
+      <c r="L785">
+        <v>514080</v>
+      </c>
+    </row>
+    <row r="786" spans="1:12">
+      <c r="A786">
+        <v>783</v>
+      </c>
+      <c r="B786">
+        <v>626402</v>
+      </c>
+      <c r="C786" t="s">
+        <v>13</v>
+      </c>
+      <c r="D786" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E786" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F786" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G786" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H786" t="s">
+        <v>40</v>
+      </c>
+      <c r="I786" t="s">
+        <v>19</v>
+      </c>
+      <c r="J786">
+        <v>1</v>
+      </c>
+      <c r="K786">
+        <v>679047</v>
+      </c>
+      <c r="L786">
+        <v>679047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SP2d 18 Maret (8 Timja)
</commit_message>
<xml_diff>
--- a/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
+++ b/Database/MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1260">
   <si>
     <t>MONITORING DETAIL TRANSAKSI FA 16 SEGMEN VERSI SP2D</t>
   </si>
@@ -3441,6 +3441,360 @@
   </si>
   <si>
     <t>Pembayaran belanja pegawai(pembayaran rapel kekurangan gaji pegawai Puslatluh bulan januari-februari 2024 untuk 37 pegawa/105 Jiwa)</t>
+  </si>
+  <si>
+    <t>'00253T</t>
+  </si>
+  <si>
+    <t>'241751303005956</t>
+  </si>
+  <si>
+    <t>Pembayaran tunjangan kinerja susulan bulan Januari tahun 2024 an  DEvy untuk 1 Pegawai/Anggota Polri/Prajurit TNI.</t>
+  </si>
+  <si>
+    <t>'00254T</t>
+  </si>
+  <si>
+    <t>'241751303005957</t>
+  </si>
+  <si>
+    <t>Pembayaran tunjangan kinerja susulan bulan Februari tahun 2024 an Devy untuk 1 Pegawai/Anggota Polri/Prajurit TNI.</t>
+  </si>
+  <si>
+    <t>'00255T</t>
+  </si>
+  <si>
+    <t>'241751303005958</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran uang makan bulan Januari 2024 an Devy untuk 1 pegawai)</t>
+  </si>
+  <si>
+    <t>'00256T</t>
+  </si>
+  <si>
+    <t>'241751303005959</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai (pembayaran uang makan bulan Februari an Devy untuk 1 pegawai)</t>
+  </si>
+  <si>
+    <t>2024-03-18</t>
+  </si>
+  <si>
+    <t>'00257T</t>
+  </si>
+  <si>
+    <t>'241751303006450</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perjalanan Dinas untuk 4 pegawai sesuai ST No. B.404/BPPSDM.5/KP.440/III/2024 Tanggal 5 Maret 2024 a.n Supriyadi,dkk</t>
+  </si>
+  <si>
+    <t>'00258T</t>
+  </si>
+  <si>
+    <t>'241751303006428</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perjalanan Dinas untuk 2 pegawai sesuai ST No. B.404/BPPSDM.5/KP.440/III/2024 Tanggal 5 Maret 2024 a.n Firdaus,dkk</t>
+  </si>
+  <si>
+    <t>'00260T</t>
+  </si>
+  <si>
+    <t>'241751303006448</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.000106</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0B.000107</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0C.000120</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0C.000121</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0B.000147</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.202.0A.001286</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.000098</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0A.000099</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0B.000149</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0B.000150</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0C.000158</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0C.000159</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0D.000167</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0D.000168</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0E.000173</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0E.000174</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.201.0A.001277</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.201.0A.001278</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.202.0B.001290</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.202.0C.001294</t>
+  </si>
+  <si>
+    <t>'626402.175.522151.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0C.000123</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.054.0A.000142</t>
+  </si>
+  <si>
+    <t>'626402.175.524119.03212DL.2375AFA.A000000001.00000.1.0151.2.000000.000000.001.053.0C.000126</t>
+  </si>
+  <si>
+    <t>'00261T</t>
+  </si>
+  <si>
+    <t>'241751303006449</t>
+  </si>
+  <si>
+    <t>'626402.175.521211.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.956.101.AA.000251</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000434</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.103.0B.000862</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBC.A000000001.00000.1.0151.2.000000.000000.954.103.0B.000863</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AA.001063</t>
+  </si>
+  <si>
+    <t>'626402.175.521811.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AB.001589</t>
+  </si>
+  <si>
+    <t>'626402.175.522119.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.957.101.0A.001654</t>
+  </si>
+  <si>
+    <t>'626402.175.522151.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.955.101.AB.001078</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.960.101.0B.000799</t>
+  </si>
+  <si>
+    <t>'626402.175.524111.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.960.102.0B.000809</t>
+  </si>
+  <si>
+    <t>'626402.175.524113.03212WA.2378EBD.A000000001.00000.1.0151.2.000000.000000.953.101.0A.001511</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.956.101.AC.000268</t>
+  </si>
+  <si>
+    <t>'626402.175.524114.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.956.101.AC.000269</t>
+  </si>
+  <si>
+    <t>'00263T</t>
+  </si>
+  <si>
+    <t>'241751303006432</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 10 Pegawai sesuai ST Nomor B.2701/BPPSDM.1/KP.440/III/2024 tanggal 6 Maret 2024 a.n. Liana Sari, dkk</t>
+  </si>
+  <si>
+    <t>'00264T</t>
+  </si>
+  <si>
+    <t>'241751303006402</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 2 Pegawai sesuai ST Nomor B.2701/BPPSDM.1/KP.440/III/2024 tanggal 6 Maret 2024 a.n. Diwa Redina Tiurlan, dkk</t>
+  </si>
+  <si>
+    <t>'00265T</t>
+  </si>
+  <si>
+    <t>'241751303006403</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 1 Pegawai sesuai ST Nomor B.2715/BPPSDM.1/KP.440/III/2024 tanggal 6 Maret 2024 a.n. Priyo Purwanto</t>
+  </si>
+  <si>
+    <t>'00266T</t>
+  </si>
+  <si>
+    <t>'241751303006479</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 3 Pegawai sesuai ST Nomor B.2715/BPPSDM.1/KP.440/III/2024 tanggal 6 Maret 2024 a.n. Edwin Lutfi, dkk</t>
+  </si>
+  <si>
+    <t>'00267T</t>
+  </si>
+  <si>
+    <t>'241751303006401</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 1 Pegawai sesuai ST Nomor B.1244/BPPSDM.1/KP.440/II/2024 tanggal 22 Februari 2024 a.n. Rizky Hendriansyah</t>
+  </si>
+  <si>
+    <t>'00268T</t>
+  </si>
+  <si>
+    <t>'241751303006429</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 3 Pegawai sesuai ST Nomor B.1201/BPPSDM.1/KP.440/II/2024 tanggal 16 Februari 2024 a.n. I Wayan Purya Arnata, dkk</t>
+  </si>
+  <si>
+    <t>'00269T</t>
+  </si>
+  <si>
+    <t>'241751303006430</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 1 Pegawai sesuai ST Nomor B.298/BPPSDM/KP.440/II/2024 tanggal 22 Februari 2024 a.n. Rudi Alek Wahyudin</t>
+  </si>
+  <si>
+    <t>'00270T</t>
+  </si>
+  <si>
+    <t>'241751303006434</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Perdin Jkt-Solo (PP) tgl 23-26 Januari 2024 an Norma dan Dedy sesuai ST No B.183/BPPSDM.4/KP.440/I/2024 Tgl 22/01/2024 keg Rpt Koord Pengelolaan dan PNBP lingkup BPPSDM di Swiss-Belhotel Solo</t>
+  </si>
+  <si>
+    <t>'00271T</t>
+  </si>
+  <si>
+    <t>'241751303006433</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Perdin Jkt-Poltekkp Sidoarjo(PP) tgl 19-22 februari 2024 an Luh Dewi dan Mextaria sesuai ST No B.399/BPPSDM.4/KP.440/II/2024 Tgl 16/02/2024 keg Persiapan Pelaksanaan SFV UPT dan Desa Sumberdodol</t>
+  </si>
+  <si>
+    <t>'00272T</t>
+  </si>
+  <si>
+    <t>'241751303006468</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Perdin Jkt-Double Tree By Hilton Surabaya (PP) tgl 19-22 Feb 2024 an Irfan sesuai ST No B.404/BPPSDM.4/KP.440/II/2024 Tgl 16/02/2024 keg Rpt Menghadiri RAKERNIS BPPSDMKP</t>
+  </si>
+  <si>
+    <t>'00273T</t>
+  </si>
+  <si>
+    <t>'241751301006562</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai SPK No:4/PPK/BRSDM.1/I/2024 Tgl.2-1-2024,BAST No:BAST.602/PPK/BRSDM.1/II/2024 Tgl.29-2-2024,BAP No:603/PPK/BRSDM.1/II/2024 Tgl.29-2-2024 Pengadaan jasa satuan pegamanan sekretariat BRSDM TA 2024 TERMIN 2</t>
+  </si>
+  <si>
+    <t>'00274T</t>
+  </si>
+  <si>
+    <t>'241751303006431</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 5 Pegawai sesuai ST Nomor B.2647/BPPSDM.1/KP.440/III/2024 tanggal 4 Maret 2024 a.n. Rudi Alek Wahyudin, dkk</t>
+  </si>
+  <si>
+    <t>'00275T</t>
+  </si>
+  <si>
+    <t>'241751302006531</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai SPK No:301/PPK/BRSDM.1/II/2024 Tgl.6-2-2-2024,BAST No:BAST.522/PPK/BRSDM.1/II/2024 Tgl.23-2-2024,BAP No:523/PPK/BRSDM.1/II/2024 Tgl.23-2-2024 Jasa Pengadaan Pakaian Dinas Hitam Putih</t>
+  </si>
+  <si>
+    <t>'626402.175.521119.03212WA.2378EBA.A000000001.00000.1.0151.2.000000.000000.994.002.AA.000431</t>
+  </si>
+  <si>
+    <t>'00276T</t>
+  </si>
+  <si>
+    <t>'241751303006478</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 1 Pegawai sesuai ST Nomor B.826/BPPSDM.1/KP.440/II/2024 tanggal 26 Januari 2024 a.n. Rahmadi Sunoko</t>
+  </si>
+  <si>
+    <t>'00282T</t>
+  </si>
+  <si>
+    <t>'241751303006477</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perdin untuk 1 Pegawai sesuai ST Nomor B.2151/BPPSDM.1/KP.440/III/2024 tanggal 1 Maret 2024 a.n. Rahmadi Sunoko</t>
+  </si>
+  <si>
+    <t>2024-03-19</t>
+  </si>
+  <si>
+    <t>'00283T</t>
+  </si>
+  <si>
+    <t>'241751303006529</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perjalanan Dinas untuk 3 pegawai sesuai ST No. B.406/BPPSDM.5/KP.440/III/2024 Tanggal 5 Maret 2024 a.n Lilly Aprilya Pregiwati, dkk</t>
+  </si>
+  <si>
+    <t>'00284T</t>
+  </si>
+  <si>
+    <t>'241751303006530</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Perjalanan Dinas untuk 4 pegawai sesuai ST No. B.406/BPPSDM.5/KP.440/III/2024 Tanggal 5 Maret 2024 a.n Endah Septiani, dkk</t>
+  </si>
+  <si>
+    <t>'00288T</t>
+  </si>
+  <si>
+    <t>'241751303006427</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran kekurangan gaji pegawai Sekretariat BRSDM bulan Januari -Februari 2024 untuk 67 pegawai/179 Jiwa)</t>
+  </si>
+  <si>
+    <t>'00290T</t>
+  </si>
+  <si>
+    <t>'241751305000480</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja pegawai(pembayaran kekurangan gaji bulan januari s.d februari 2024 an liana sari)</t>
   </si>
 </sst>
 </file>
@@ -3782,7 +4136,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L786"/>
+  <dimension ref="A1:L896"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -33588,6 +33942,4186 @@
       </c>
       <c r="L786">
         <v>679047</v>
+      </c>
+    </row>
+    <row r="787" spans="1:12">
+      <c r="A787">
+        <v>784</v>
+      </c>
+      <c r="B787">
+        <v>626402</v>
+      </c>
+      <c r="C787" t="s">
+        <v>13</v>
+      </c>
+      <c r="D787" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E787" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F787" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G787" t="s">
+        <v>1144</v>
+      </c>
+      <c r="H787" t="s">
+        <v>80</v>
+      </c>
+      <c r="I787" t="s">
+        <v>19</v>
+      </c>
+      <c r="J787">
+        <v>1</v>
+      </c>
+      <c r="K787">
+        <v>3915950</v>
+      </c>
+      <c r="L787">
+        <v>3915950</v>
+      </c>
+    </row>
+    <row r="788" spans="1:12">
+      <c r="A788">
+        <v>785</v>
+      </c>
+      <c r="B788">
+        <v>626402</v>
+      </c>
+      <c r="C788" t="s">
+        <v>13</v>
+      </c>
+      <c r="D788" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E788" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F788" t="s">
+        <v>1146</v>
+      </c>
+      <c r="G788" t="s">
+        <v>1147</v>
+      </c>
+      <c r="H788" t="s">
+        <v>80</v>
+      </c>
+      <c r="I788" t="s">
+        <v>19</v>
+      </c>
+      <c r="J788">
+        <v>1</v>
+      </c>
+      <c r="K788">
+        <v>3915950</v>
+      </c>
+      <c r="L788">
+        <v>3915950</v>
+      </c>
+    </row>
+    <row r="789" spans="1:12">
+      <c r="A789">
+        <v>786</v>
+      </c>
+      <c r="B789">
+        <v>626402</v>
+      </c>
+      <c r="C789" t="s">
+        <v>13</v>
+      </c>
+      <c r="D789" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E789" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F789" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G789" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H789" t="s">
+        <v>85</v>
+      </c>
+      <c r="I789" t="s">
+        <v>19</v>
+      </c>
+      <c r="J789">
+        <v>1</v>
+      </c>
+      <c r="K789">
+        <v>592000</v>
+      </c>
+      <c r="L789">
+        <v>592000</v>
+      </c>
+    </row>
+    <row r="790" spans="1:12">
+      <c r="A790">
+        <v>787</v>
+      </c>
+      <c r="B790">
+        <v>626402</v>
+      </c>
+      <c r="C790" t="s">
+        <v>13</v>
+      </c>
+      <c r="D790" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E790" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F790" t="s">
+        <v>1152</v>
+      </c>
+      <c r="G790" t="s">
+        <v>1153</v>
+      </c>
+      <c r="H790" t="s">
+        <v>85</v>
+      </c>
+      <c r="I790" t="s">
+        <v>19</v>
+      </c>
+      <c r="J790">
+        <v>1</v>
+      </c>
+      <c r="K790">
+        <v>518000</v>
+      </c>
+      <c r="L790">
+        <v>518000</v>
+      </c>
+    </row>
+    <row r="791" spans="1:12">
+      <c r="A791">
+        <v>788</v>
+      </c>
+      <c r="B791">
+        <v>626402</v>
+      </c>
+      <c r="C791" t="s">
+        <v>13</v>
+      </c>
+      <c r="D791" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E791" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F791" t="s">
+        <v>1156</v>
+      </c>
+      <c r="G791" t="s">
+        <v>1157</v>
+      </c>
+      <c r="H791" t="s">
+        <v>897</v>
+      </c>
+      <c r="I791" t="s">
+        <v>19</v>
+      </c>
+      <c r="J791">
+        <v>1</v>
+      </c>
+      <c r="K791">
+        <v>3440000</v>
+      </c>
+      <c r="L791">
+        <v>3440000</v>
+      </c>
+    </row>
+    <row r="792" spans="1:12">
+      <c r="A792">
+        <v>789</v>
+      </c>
+      <c r="B792">
+        <v>626402</v>
+      </c>
+      <c r="C792" t="s">
+        <v>13</v>
+      </c>
+      <c r="D792" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E792" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F792" t="s">
+        <v>1156</v>
+      </c>
+      <c r="G792" t="s">
+        <v>1157</v>
+      </c>
+      <c r="H792" t="s">
+        <v>898</v>
+      </c>
+      <c r="I792" t="s">
+        <v>19</v>
+      </c>
+      <c r="J792">
+        <v>1</v>
+      </c>
+      <c r="K792">
+        <v>566500</v>
+      </c>
+      <c r="L792">
+        <v>566500</v>
+      </c>
+    </row>
+    <row r="793" spans="1:12">
+      <c r="A793">
+        <v>790</v>
+      </c>
+      <c r="B793">
+        <v>626402</v>
+      </c>
+      <c r="C793" t="s">
+        <v>13</v>
+      </c>
+      <c r="D793" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E793" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F793" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G793" t="s">
+        <v>1160</v>
+      </c>
+      <c r="H793" t="s">
+        <v>897</v>
+      </c>
+      <c r="I793" t="s">
+        <v>19</v>
+      </c>
+      <c r="J793">
+        <v>1</v>
+      </c>
+      <c r="K793">
+        <v>860000</v>
+      </c>
+      <c r="L793">
+        <v>860000</v>
+      </c>
+    </row>
+    <row r="794" spans="1:12">
+      <c r="A794">
+        <v>791</v>
+      </c>
+      <c r="B794">
+        <v>626402</v>
+      </c>
+      <c r="C794" t="s">
+        <v>13</v>
+      </c>
+      <c r="D794" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E794" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F794" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G794" t="s">
+        <v>1160</v>
+      </c>
+      <c r="H794" t="s">
+        <v>898</v>
+      </c>
+      <c r="I794" t="s">
+        <v>19</v>
+      </c>
+      <c r="J794">
+        <v>1</v>
+      </c>
+      <c r="K794">
+        <v>31000</v>
+      </c>
+      <c r="L794">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="795" spans="1:12">
+      <c r="A795">
+        <v>792</v>
+      </c>
+      <c r="B795">
+        <v>626402</v>
+      </c>
+      <c r="C795" t="s">
+        <v>13</v>
+      </c>
+      <c r="D795" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E795" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F795" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G795" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H795" t="s">
+        <v>882</v>
+      </c>
+      <c r="I795" t="s">
+        <v>19</v>
+      </c>
+      <c r="J795">
+        <v>1</v>
+      </c>
+      <c r="K795">
+        <v>5615000</v>
+      </c>
+      <c r="L795">
+        <v>5615000</v>
+      </c>
+    </row>
+    <row r="796" spans="1:12">
+      <c r="A796">
+        <v>793</v>
+      </c>
+      <c r="B796">
+        <v>626402</v>
+      </c>
+      <c r="C796" t="s">
+        <v>13</v>
+      </c>
+      <c r="D796" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E796" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F796" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G796" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H796" t="s">
+        <v>1163</v>
+      </c>
+      <c r="I796" t="s">
+        <v>19</v>
+      </c>
+      <c r="J796">
+        <v>1</v>
+      </c>
+      <c r="K796">
+        <v>1000000</v>
+      </c>
+      <c r="L796">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="797" spans="1:12">
+      <c r="A797">
+        <v>794</v>
+      </c>
+      <c r="B797">
+        <v>626402</v>
+      </c>
+      <c r="C797" t="s">
+        <v>13</v>
+      </c>
+      <c r="D797" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E797" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F797" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G797" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H797" t="s">
+        <v>1164</v>
+      </c>
+      <c r="I797" t="s">
+        <v>19</v>
+      </c>
+      <c r="J797">
+        <v>1</v>
+      </c>
+      <c r="K797">
+        <v>1000000</v>
+      </c>
+      <c r="L797">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="798" spans="1:12">
+      <c r="A798">
+        <v>795</v>
+      </c>
+      <c r="B798">
+        <v>626402</v>
+      </c>
+      <c r="C798" t="s">
+        <v>13</v>
+      </c>
+      <c r="D798" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E798" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F798" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G798" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H798" t="s">
+        <v>450</v>
+      </c>
+      <c r="I798" t="s">
+        <v>19</v>
+      </c>
+      <c r="J798">
+        <v>1</v>
+      </c>
+      <c r="K798">
+        <v>1001600</v>
+      </c>
+      <c r="L798">
+        <v>1001600</v>
+      </c>
+    </row>
+    <row r="799" spans="1:12">
+      <c r="A799">
+        <v>796</v>
+      </c>
+      <c r="B799">
+        <v>626402</v>
+      </c>
+      <c r="C799" t="s">
+        <v>13</v>
+      </c>
+      <c r="D799" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E799" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F799" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G799" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H799" t="s">
+        <v>1165</v>
+      </c>
+      <c r="I799" t="s">
+        <v>19</v>
+      </c>
+      <c r="J799">
+        <v>1</v>
+      </c>
+      <c r="K799">
+        <v>2904000</v>
+      </c>
+      <c r="L799">
+        <v>2904000</v>
+      </c>
+    </row>
+    <row r="800" spans="1:12">
+      <c r="A800">
+        <v>797</v>
+      </c>
+      <c r="B800">
+        <v>626402</v>
+      </c>
+      <c r="C800" t="s">
+        <v>13</v>
+      </c>
+      <c r="D800" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E800" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F800" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G800" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H800" t="s">
+        <v>1166</v>
+      </c>
+      <c r="I800" t="s">
+        <v>19</v>
+      </c>
+      <c r="J800">
+        <v>1</v>
+      </c>
+      <c r="K800">
+        <v>15000000</v>
+      </c>
+      <c r="L800">
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="801" spans="1:12">
+      <c r="A801">
+        <v>798</v>
+      </c>
+      <c r="B801">
+        <v>626402</v>
+      </c>
+      <c r="C801" t="s">
+        <v>13</v>
+      </c>
+      <c r="D801" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E801" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F801" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G801" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H801" t="s">
+        <v>1167</v>
+      </c>
+      <c r="I801" t="s">
+        <v>19</v>
+      </c>
+      <c r="J801">
+        <v>1</v>
+      </c>
+      <c r="K801">
+        <v>1210000</v>
+      </c>
+      <c r="L801">
+        <v>1210000</v>
+      </c>
+    </row>
+    <row r="802" spans="1:12">
+      <c r="A802">
+        <v>799</v>
+      </c>
+      <c r="B802">
+        <v>626402</v>
+      </c>
+      <c r="C802" t="s">
+        <v>13</v>
+      </c>
+      <c r="D802" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E802" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F802" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G802" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H802" t="s">
+        <v>451</v>
+      </c>
+      <c r="I802" t="s">
+        <v>19</v>
+      </c>
+      <c r="J802">
+        <v>1</v>
+      </c>
+      <c r="K802">
+        <v>2927000</v>
+      </c>
+      <c r="L802">
+        <v>2927000</v>
+      </c>
+    </row>
+    <row r="803" spans="1:12">
+      <c r="A803">
+        <v>800</v>
+      </c>
+      <c r="B803">
+        <v>626402</v>
+      </c>
+      <c r="C803" t="s">
+        <v>13</v>
+      </c>
+      <c r="D803" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E803" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F803" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G803" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H803" t="s">
+        <v>452</v>
+      </c>
+      <c r="I803" t="s">
+        <v>19</v>
+      </c>
+      <c r="J803">
+        <v>1</v>
+      </c>
+      <c r="K803">
+        <v>4085900</v>
+      </c>
+      <c r="L803">
+        <v>4085900</v>
+      </c>
+    </row>
+    <row r="804" spans="1:12">
+      <c r="A804">
+        <v>801</v>
+      </c>
+      <c r="B804">
+        <v>626402</v>
+      </c>
+      <c r="C804" t="s">
+        <v>13</v>
+      </c>
+      <c r="D804" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E804" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F804" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G804" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H804" t="s">
+        <v>1168</v>
+      </c>
+      <c r="I804" t="s">
+        <v>19</v>
+      </c>
+      <c r="J804">
+        <v>1</v>
+      </c>
+      <c r="K804">
+        <v>1000000</v>
+      </c>
+      <c r="L804">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="805" spans="1:12">
+      <c r="A805">
+        <v>802</v>
+      </c>
+      <c r="B805">
+        <v>626402</v>
+      </c>
+      <c r="C805" t="s">
+        <v>13</v>
+      </c>
+      <c r="D805" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E805" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F805" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G805" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H805" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I805" t="s">
+        <v>19</v>
+      </c>
+      <c r="J805">
+        <v>1</v>
+      </c>
+      <c r="K805">
+        <v>1000000</v>
+      </c>
+      <c r="L805">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="806" spans="1:12">
+      <c r="A806">
+        <v>803</v>
+      </c>
+      <c r="B806">
+        <v>626402</v>
+      </c>
+      <c r="C806" t="s">
+        <v>13</v>
+      </c>
+      <c r="D806" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E806" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F806" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G806" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H806" t="s">
+        <v>1170</v>
+      </c>
+      <c r="I806" t="s">
+        <v>19</v>
+      </c>
+      <c r="J806">
+        <v>1</v>
+      </c>
+      <c r="K806">
+        <v>1000000</v>
+      </c>
+      <c r="L806">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="807" spans="1:12">
+      <c r="A807">
+        <v>804</v>
+      </c>
+      <c r="B807">
+        <v>626402</v>
+      </c>
+      <c r="C807" t="s">
+        <v>13</v>
+      </c>
+      <c r="D807" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E807" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F807" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G807" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H807" t="s">
+        <v>1171</v>
+      </c>
+      <c r="I807" t="s">
+        <v>19</v>
+      </c>
+      <c r="J807">
+        <v>1</v>
+      </c>
+      <c r="K807">
+        <v>1000000</v>
+      </c>
+      <c r="L807">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="808" spans="1:12">
+      <c r="A808">
+        <v>805</v>
+      </c>
+      <c r="B808">
+        <v>626402</v>
+      </c>
+      <c r="C808" t="s">
+        <v>13</v>
+      </c>
+      <c r="D808" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E808" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F808" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G808" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H808" t="s">
+        <v>1172</v>
+      </c>
+      <c r="I808" t="s">
+        <v>19</v>
+      </c>
+      <c r="J808">
+        <v>1</v>
+      </c>
+      <c r="K808">
+        <v>1000000</v>
+      </c>
+      <c r="L808">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="809" spans="1:12">
+      <c r="A809">
+        <v>806</v>
+      </c>
+      <c r="B809">
+        <v>626402</v>
+      </c>
+      <c r="C809" t="s">
+        <v>13</v>
+      </c>
+      <c r="D809" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E809" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F809" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G809" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H809" t="s">
+        <v>1173</v>
+      </c>
+      <c r="I809" t="s">
+        <v>19</v>
+      </c>
+      <c r="J809">
+        <v>1</v>
+      </c>
+      <c r="K809">
+        <v>1000000</v>
+      </c>
+      <c r="L809">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="810" spans="1:12">
+      <c r="A810">
+        <v>807</v>
+      </c>
+      <c r="B810">
+        <v>626402</v>
+      </c>
+      <c r="C810" t="s">
+        <v>13</v>
+      </c>
+      <c r="D810" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E810" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F810" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G810" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H810" t="s">
+        <v>1174</v>
+      </c>
+      <c r="I810" t="s">
+        <v>19</v>
+      </c>
+      <c r="J810">
+        <v>1</v>
+      </c>
+      <c r="K810">
+        <v>1000000</v>
+      </c>
+      <c r="L810">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="811" spans="1:12">
+      <c r="A811">
+        <v>808</v>
+      </c>
+      <c r="B811">
+        <v>626402</v>
+      </c>
+      <c r="C811" t="s">
+        <v>13</v>
+      </c>
+      <c r="D811" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E811" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F811" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G811" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H811" t="s">
+        <v>1175</v>
+      </c>
+      <c r="I811" t="s">
+        <v>19</v>
+      </c>
+      <c r="J811">
+        <v>1</v>
+      </c>
+      <c r="K811">
+        <v>1000000</v>
+      </c>
+      <c r="L811">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="812" spans="1:12">
+      <c r="A812">
+        <v>809</v>
+      </c>
+      <c r="B812">
+        <v>626402</v>
+      </c>
+      <c r="C812" t="s">
+        <v>13</v>
+      </c>
+      <c r="D812" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E812" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F812" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G812" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H812" t="s">
+        <v>1176</v>
+      </c>
+      <c r="I812" t="s">
+        <v>19</v>
+      </c>
+      <c r="J812">
+        <v>1</v>
+      </c>
+      <c r="K812">
+        <v>1000000</v>
+      </c>
+      <c r="L812">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="813" spans="1:12">
+      <c r="A813">
+        <v>810</v>
+      </c>
+      <c r="B813">
+        <v>626402</v>
+      </c>
+      <c r="C813" t="s">
+        <v>13</v>
+      </c>
+      <c r="D813" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E813" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F813" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G813" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H813" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I813" t="s">
+        <v>19</v>
+      </c>
+      <c r="J813">
+        <v>1</v>
+      </c>
+      <c r="K813">
+        <v>1000000</v>
+      </c>
+      <c r="L813">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="814" spans="1:12">
+      <c r="A814">
+        <v>811</v>
+      </c>
+      <c r="B814">
+        <v>626402</v>
+      </c>
+      <c r="C814" t="s">
+        <v>13</v>
+      </c>
+      <c r="D814" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E814" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F814" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G814" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H814" t="s">
+        <v>1178</v>
+      </c>
+      <c r="I814" t="s">
+        <v>19</v>
+      </c>
+      <c r="J814">
+        <v>1</v>
+      </c>
+      <c r="K814">
+        <v>1000000</v>
+      </c>
+      <c r="L814">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="815" spans="1:12">
+      <c r="A815">
+        <v>812</v>
+      </c>
+      <c r="B815">
+        <v>626402</v>
+      </c>
+      <c r="C815" t="s">
+        <v>13</v>
+      </c>
+      <c r="D815" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E815" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F815" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G815" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H815" t="s">
+        <v>1179</v>
+      </c>
+      <c r="I815" t="s">
+        <v>19</v>
+      </c>
+      <c r="J815">
+        <v>1</v>
+      </c>
+      <c r="K815">
+        <v>842000</v>
+      </c>
+      <c r="L815">
+        <v>842000</v>
+      </c>
+    </row>
+    <row r="816" spans="1:12">
+      <c r="A816">
+        <v>813</v>
+      </c>
+      <c r="B816">
+        <v>626402</v>
+      </c>
+      <c r="C816" t="s">
+        <v>13</v>
+      </c>
+      <c r="D816" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E816" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F816" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G816" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H816" t="s">
+        <v>1180</v>
+      </c>
+      <c r="I816" t="s">
+        <v>19</v>
+      </c>
+      <c r="J816">
+        <v>1</v>
+      </c>
+      <c r="K816">
+        <v>750000</v>
+      </c>
+      <c r="L816">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="817" spans="1:12">
+      <c r="A817">
+        <v>814</v>
+      </c>
+      <c r="B817">
+        <v>626402</v>
+      </c>
+      <c r="C817" t="s">
+        <v>13</v>
+      </c>
+      <c r="D817" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E817" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F817" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G817" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H817" t="s">
+        <v>1181</v>
+      </c>
+      <c r="I817" t="s">
+        <v>19</v>
+      </c>
+      <c r="J817">
+        <v>1</v>
+      </c>
+      <c r="K817">
+        <v>1500000</v>
+      </c>
+      <c r="L817">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="818" spans="1:12">
+      <c r="A818">
+        <v>815</v>
+      </c>
+      <c r="B818">
+        <v>626402</v>
+      </c>
+      <c r="C818" t="s">
+        <v>13</v>
+      </c>
+      <c r="D818" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E818" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F818" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G818" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H818" t="s">
+        <v>1182</v>
+      </c>
+      <c r="I818" t="s">
+        <v>19</v>
+      </c>
+      <c r="J818">
+        <v>1</v>
+      </c>
+      <c r="K818">
+        <v>1000000</v>
+      </c>
+      <c r="L818">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="819" spans="1:12">
+      <c r="A819">
+        <v>816</v>
+      </c>
+      <c r="B819">
+        <v>626402</v>
+      </c>
+      <c r="C819" t="s">
+        <v>13</v>
+      </c>
+      <c r="D819" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E819" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F819" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G819" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H819" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I819" t="s">
+        <v>19</v>
+      </c>
+      <c r="J819">
+        <v>1</v>
+      </c>
+      <c r="K819">
+        <v>3000000</v>
+      </c>
+      <c r="L819">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="820" spans="1:12">
+      <c r="A820">
+        <v>817</v>
+      </c>
+      <c r="B820">
+        <v>626402</v>
+      </c>
+      <c r="C820" t="s">
+        <v>13</v>
+      </c>
+      <c r="D820" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E820" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F820" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G820" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H820" t="s">
+        <v>1183</v>
+      </c>
+      <c r="I820" t="s">
+        <v>19</v>
+      </c>
+      <c r="J820">
+        <v>1</v>
+      </c>
+      <c r="K820">
+        <v>900000</v>
+      </c>
+      <c r="L820">
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="821" spans="1:12">
+      <c r="A821">
+        <v>818</v>
+      </c>
+      <c r="B821">
+        <v>626402</v>
+      </c>
+      <c r="C821" t="s">
+        <v>13</v>
+      </c>
+      <c r="D821" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E821" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F821" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G821" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H821" t="s">
+        <v>895</v>
+      </c>
+      <c r="I821" t="s">
+        <v>19</v>
+      </c>
+      <c r="J821">
+        <v>1</v>
+      </c>
+      <c r="K821">
+        <v>23546600</v>
+      </c>
+      <c r="L821">
+        <v>23546600</v>
+      </c>
+    </row>
+    <row r="822" spans="1:12">
+      <c r="A822">
+        <v>819</v>
+      </c>
+      <c r="B822">
+        <v>626402</v>
+      </c>
+      <c r="C822" t="s">
+        <v>13</v>
+      </c>
+      <c r="D822" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E822" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F822" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G822" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H822" t="s">
+        <v>231</v>
+      </c>
+      <c r="I822" t="s">
+        <v>19</v>
+      </c>
+      <c r="J822">
+        <v>1</v>
+      </c>
+      <c r="K822">
+        <v>260000</v>
+      </c>
+      <c r="L822">
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="823" spans="1:12">
+      <c r="A823">
+        <v>820</v>
+      </c>
+      <c r="B823">
+        <v>626402</v>
+      </c>
+      <c r="C823" t="s">
+        <v>13</v>
+      </c>
+      <c r="D823" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E823" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F823" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G823" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H823" t="s">
+        <v>232</v>
+      </c>
+      <c r="I823" t="s">
+        <v>19</v>
+      </c>
+      <c r="J823">
+        <v>1</v>
+      </c>
+      <c r="K823">
+        <v>340000</v>
+      </c>
+      <c r="L823">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="824" spans="1:12">
+      <c r="A824">
+        <v>821</v>
+      </c>
+      <c r="B824">
+        <v>626402</v>
+      </c>
+      <c r="C824" t="s">
+        <v>13</v>
+      </c>
+      <c r="D824" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E824" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F824" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G824" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H824" t="s">
+        <v>1184</v>
+      </c>
+      <c r="I824" t="s">
+        <v>19</v>
+      </c>
+      <c r="J824">
+        <v>1</v>
+      </c>
+      <c r="K824">
+        <v>2821234</v>
+      </c>
+      <c r="L824">
+        <v>2821234</v>
+      </c>
+    </row>
+    <row r="825" spans="1:12">
+      <c r="A825">
+        <v>822</v>
+      </c>
+      <c r="B825">
+        <v>626402</v>
+      </c>
+      <c r="C825" t="s">
+        <v>13</v>
+      </c>
+      <c r="D825" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E825" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F825" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G825" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H825" t="s">
+        <v>603</v>
+      </c>
+      <c r="I825" t="s">
+        <v>19</v>
+      </c>
+      <c r="J825">
+        <v>1</v>
+      </c>
+      <c r="K825">
+        <v>640000</v>
+      </c>
+      <c r="L825">
+        <v>640000</v>
+      </c>
+    </row>
+    <row r="826" spans="1:12">
+      <c r="A826">
+        <v>823</v>
+      </c>
+      <c r="B826">
+        <v>626402</v>
+      </c>
+      <c r="C826" t="s">
+        <v>13</v>
+      </c>
+      <c r="D826" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E826" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F826" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G826" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H826" t="s">
+        <v>604</v>
+      </c>
+      <c r="I826" t="s">
+        <v>19</v>
+      </c>
+      <c r="J826">
+        <v>1</v>
+      </c>
+      <c r="K826">
+        <v>1240000</v>
+      </c>
+      <c r="L826">
+        <v>1240000</v>
+      </c>
+    </row>
+    <row r="827" spans="1:12">
+      <c r="A827">
+        <v>824</v>
+      </c>
+      <c r="B827">
+        <v>626402</v>
+      </c>
+      <c r="C827" t="s">
+        <v>13</v>
+      </c>
+      <c r="D827" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E827" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F827" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G827" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H827" t="s">
+        <v>605</v>
+      </c>
+      <c r="I827" t="s">
+        <v>19</v>
+      </c>
+      <c r="J827">
+        <v>1</v>
+      </c>
+      <c r="K827">
+        <v>540000</v>
+      </c>
+      <c r="L827">
+        <v>540000</v>
+      </c>
+    </row>
+    <row r="828" spans="1:12">
+      <c r="A828">
+        <v>825</v>
+      </c>
+      <c r="B828">
+        <v>626402</v>
+      </c>
+      <c r="C828" t="s">
+        <v>13</v>
+      </c>
+      <c r="D828" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E828" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F828" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G828" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H828" t="s">
+        <v>373</v>
+      </c>
+      <c r="I828" t="s">
+        <v>19</v>
+      </c>
+      <c r="J828">
+        <v>1</v>
+      </c>
+      <c r="K828">
+        <v>8844575</v>
+      </c>
+      <c r="L828">
+        <v>8844575</v>
+      </c>
+    </row>
+    <row r="829" spans="1:12">
+      <c r="A829">
+        <v>826</v>
+      </c>
+      <c r="B829">
+        <v>626402</v>
+      </c>
+      <c r="C829" t="s">
+        <v>13</v>
+      </c>
+      <c r="D829" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E829" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F829" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G829" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H829" t="s">
+        <v>899</v>
+      </c>
+      <c r="I829" t="s">
+        <v>19</v>
+      </c>
+      <c r="J829">
+        <v>1</v>
+      </c>
+      <c r="K829">
+        <v>2550000</v>
+      </c>
+      <c r="L829">
+        <v>2550000</v>
+      </c>
+    </row>
+    <row r="830" spans="1:12">
+      <c r="A830">
+        <v>827</v>
+      </c>
+      <c r="B830">
+        <v>626402</v>
+      </c>
+      <c r="C830" t="s">
+        <v>13</v>
+      </c>
+      <c r="D830" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E830" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F830" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G830" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H830" t="s">
+        <v>1185</v>
+      </c>
+      <c r="I830" t="s">
+        <v>19</v>
+      </c>
+      <c r="J830">
+        <v>1</v>
+      </c>
+      <c r="K830">
+        <v>5400000</v>
+      </c>
+      <c r="L830">
+        <v>5400000</v>
+      </c>
+    </row>
+    <row r="831" spans="1:12">
+      <c r="A831">
+        <v>828</v>
+      </c>
+      <c r="B831">
+        <v>626402</v>
+      </c>
+      <c r="C831" t="s">
+        <v>13</v>
+      </c>
+      <c r="D831" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E831" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F831" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G831" t="s">
+        <v>429</v>
+      </c>
+      <c r="H831" t="s">
+        <v>255</v>
+      </c>
+      <c r="I831" t="s">
+        <v>19</v>
+      </c>
+      <c r="J831">
+        <v>1</v>
+      </c>
+      <c r="K831">
+        <v>26704500</v>
+      </c>
+      <c r="L831">
+        <v>26704500</v>
+      </c>
+    </row>
+    <row r="832" spans="1:12">
+      <c r="A832">
+        <v>829</v>
+      </c>
+      <c r="B832">
+        <v>626402</v>
+      </c>
+      <c r="C832" t="s">
+        <v>13</v>
+      </c>
+      <c r="D832" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E832" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F832" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G832" t="s">
+        <v>429</v>
+      </c>
+      <c r="H832" t="s">
+        <v>257</v>
+      </c>
+      <c r="I832" t="s">
+        <v>19</v>
+      </c>
+      <c r="J832">
+        <v>1</v>
+      </c>
+      <c r="K832">
+        <v>1598300</v>
+      </c>
+      <c r="L832">
+        <v>1598300</v>
+      </c>
+    </row>
+    <row r="833" spans="1:12">
+      <c r="A833">
+        <v>830</v>
+      </c>
+      <c r="B833">
+        <v>626402</v>
+      </c>
+      <c r="C833" t="s">
+        <v>13</v>
+      </c>
+      <c r="D833" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E833" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F833" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G833" t="s">
+        <v>429</v>
+      </c>
+      <c r="H833" t="s">
+        <v>258</v>
+      </c>
+      <c r="I833" t="s">
+        <v>19</v>
+      </c>
+      <c r="J833">
+        <v>1</v>
+      </c>
+      <c r="K833">
+        <v>854410</v>
+      </c>
+      <c r="L833">
+        <v>854410</v>
+      </c>
+    </row>
+    <row r="834" spans="1:12">
+      <c r="A834">
+        <v>831</v>
+      </c>
+      <c r="B834">
+        <v>626402</v>
+      </c>
+      <c r="C834" t="s">
+        <v>13</v>
+      </c>
+      <c r="D834" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E834" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F834" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G834" t="s">
+        <v>429</v>
+      </c>
+      <c r="H834" t="s">
+        <v>760</v>
+      </c>
+      <c r="I834" t="s">
+        <v>19</v>
+      </c>
+      <c r="J834">
+        <v>1</v>
+      </c>
+      <c r="K834">
+        <v>121284</v>
+      </c>
+      <c r="L834">
+        <v>121284</v>
+      </c>
+    </row>
+    <row r="835" spans="1:12">
+      <c r="A835">
+        <v>832</v>
+      </c>
+      <c r="B835">
+        <v>626402</v>
+      </c>
+      <c r="C835" t="s">
+        <v>13</v>
+      </c>
+      <c r="D835" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E835" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F835" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G835" t="s">
+        <v>429</v>
+      </c>
+      <c r="H835" t="s">
+        <v>761</v>
+      </c>
+      <c r="I835" t="s">
+        <v>19</v>
+      </c>
+      <c r="J835">
+        <v>1</v>
+      </c>
+      <c r="K835">
+        <v>220493</v>
+      </c>
+      <c r="L835">
+        <v>220493</v>
+      </c>
+    </row>
+    <row r="836" spans="1:12">
+      <c r="A836">
+        <v>833</v>
+      </c>
+      <c r="B836">
+        <v>626402</v>
+      </c>
+      <c r="C836" t="s">
+        <v>13</v>
+      </c>
+      <c r="D836" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E836" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F836" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G836" t="s">
+        <v>429</v>
+      </c>
+      <c r="H836" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I836" t="s">
+        <v>19</v>
+      </c>
+      <c r="J836">
+        <v>1</v>
+      </c>
+      <c r="K836">
+        <v>385000</v>
+      </c>
+      <c r="L836">
+        <v>385000</v>
+      </c>
+    </row>
+    <row r="837" spans="1:12">
+      <c r="A837">
+        <v>834</v>
+      </c>
+      <c r="B837">
+        <v>626402</v>
+      </c>
+      <c r="C837" t="s">
+        <v>13</v>
+      </c>
+      <c r="D837" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E837" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F837" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G837" t="s">
+        <v>429</v>
+      </c>
+      <c r="H837" t="s">
+        <v>1189</v>
+      </c>
+      <c r="I837" t="s">
+        <v>19</v>
+      </c>
+      <c r="J837">
+        <v>1</v>
+      </c>
+      <c r="K837">
+        <v>3577225</v>
+      </c>
+      <c r="L837">
+        <v>3577225</v>
+      </c>
+    </row>
+    <row r="838" spans="1:12">
+      <c r="A838">
+        <v>835</v>
+      </c>
+      <c r="B838">
+        <v>626402</v>
+      </c>
+      <c r="C838" t="s">
+        <v>13</v>
+      </c>
+      <c r="D838" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E838" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F838" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G838" t="s">
+        <v>429</v>
+      </c>
+      <c r="H838" t="s">
+        <v>267</v>
+      </c>
+      <c r="I838" t="s">
+        <v>19</v>
+      </c>
+      <c r="J838">
+        <v>1</v>
+      </c>
+      <c r="K838">
+        <v>1998500</v>
+      </c>
+      <c r="L838">
+        <v>1998500</v>
+      </c>
+    </row>
+    <row r="839" spans="1:12">
+      <c r="A839">
+        <v>836</v>
+      </c>
+      <c r="B839">
+        <v>626402</v>
+      </c>
+      <c r="C839" t="s">
+        <v>13</v>
+      </c>
+      <c r="D839" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E839" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F839" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G839" t="s">
+        <v>429</v>
+      </c>
+      <c r="H839" t="s">
+        <v>1190</v>
+      </c>
+      <c r="I839" t="s">
+        <v>19</v>
+      </c>
+      <c r="J839">
+        <v>1</v>
+      </c>
+      <c r="K839">
+        <v>926000</v>
+      </c>
+      <c r="L839">
+        <v>926000</v>
+      </c>
+    </row>
+    <row r="840" spans="1:12">
+      <c r="A840">
+        <v>837</v>
+      </c>
+      <c r="B840">
+        <v>626402</v>
+      </c>
+      <c r="C840" t="s">
+        <v>13</v>
+      </c>
+      <c r="D840" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E840" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F840" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G840" t="s">
+        <v>429</v>
+      </c>
+      <c r="H840" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I840" t="s">
+        <v>19</v>
+      </c>
+      <c r="J840">
+        <v>1</v>
+      </c>
+      <c r="K840">
+        <v>2800000</v>
+      </c>
+      <c r="L840">
+        <v>2800000</v>
+      </c>
+    </row>
+    <row r="841" spans="1:12">
+      <c r="A841">
+        <v>838</v>
+      </c>
+      <c r="B841">
+        <v>626402</v>
+      </c>
+      <c r="C841" t="s">
+        <v>13</v>
+      </c>
+      <c r="D841" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E841" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F841" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G841" t="s">
+        <v>429</v>
+      </c>
+      <c r="H841" t="s">
+        <v>1192</v>
+      </c>
+      <c r="I841" t="s">
+        <v>19</v>
+      </c>
+      <c r="J841">
+        <v>1</v>
+      </c>
+      <c r="K841">
+        <v>1400000</v>
+      </c>
+      <c r="L841">
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="842" spans="1:12">
+      <c r="A842">
+        <v>839</v>
+      </c>
+      <c r="B842">
+        <v>626402</v>
+      </c>
+      <c r="C842" t="s">
+        <v>13</v>
+      </c>
+      <c r="D842" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E842" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F842" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G842" t="s">
+        <v>429</v>
+      </c>
+      <c r="H842" t="s">
+        <v>1193</v>
+      </c>
+      <c r="I842" t="s">
+        <v>19</v>
+      </c>
+      <c r="J842">
+        <v>1</v>
+      </c>
+      <c r="K842">
+        <v>1996750</v>
+      </c>
+      <c r="L842">
+        <v>1996750</v>
+      </c>
+    </row>
+    <row r="843" spans="1:12">
+      <c r="A843">
+        <v>840</v>
+      </c>
+      <c r="B843">
+        <v>626402</v>
+      </c>
+      <c r="C843" t="s">
+        <v>13</v>
+      </c>
+      <c r="D843" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E843" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F843" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G843" t="s">
+        <v>429</v>
+      </c>
+      <c r="H843" t="s">
+        <v>1194</v>
+      </c>
+      <c r="I843" t="s">
+        <v>19</v>
+      </c>
+      <c r="J843">
+        <v>1</v>
+      </c>
+      <c r="K843">
+        <v>147000</v>
+      </c>
+      <c r="L843">
+        <v>147000</v>
+      </c>
+    </row>
+    <row r="844" spans="1:12">
+      <c r="A844">
+        <v>841</v>
+      </c>
+      <c r="B844">
+        <v>626402</v>
+      </c>
+      <c r="C844" t="s">
+        <v>13</v>
+      </c>
+      <c r="D844" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E844" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F844" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G844" t="s">
+        <v>429</v>
+      </c>
+      <c r="H844" t="s">
+        <v>768</v>
+      </c>
+      <c r="I844" t="s">
+        <v>19</v>
+      </c>
+      <c r="J844">
+        <v>1</v>
+      </c>
+      <c r="K844">
+        <v>1600000</v>
+      </c>
+      <c r="L844">
+        <v>1600000</v>
+      </c>
+    </row>
+    <row r="845" spans="1:12">
+      <c r="A845">
+        <v>842</v>
+      </c>
+      <c r="B845">
+        <v>626402</v>
+      </c>
+      <c r="C845" t="s">
+        <v>13</v>
+      </c>
+      <c r="D845" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E845" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F845" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G845" t="s">
+        <v>429</v>
+      </c>
+      <c r="H845" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I845" t="s">
+        <v>19</v>
+      </c>
+      <c r="J845">
+        <v>1</v>
+      </c>
+      <c r="K845">
+        <v>900000</v>
+      </c>
+      <c r="L845">
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="846" spans="1:12">
+      <c r="A846">
+        <v>843</v>
+      </c>
+      <c r="B846">
+        <v>626402</v>
+      </c>
+      <c r="C846" t="s">
+        <v>13</v>
+      </c>
+      <c r="D846" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E846" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F846" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G846" t="s">
+        <v>429</v>
+      </c>
+      <c r="H846" t="s">
+        <v>432</v>
+      </c>
+      <c r="I846" t="s">
+        <v>19</v>
+      </c>
+      <c r="J846">
+        <v>1</v>
+      </c>
+      <c r="K846">
+        <v>750000</v>
+      </c>
+      <c r="L846">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="847" spans="1:12">
+      <c r="A847">
+        <v>844</v>
+      </c>
+      <c r="B847">
+        <v>626402</v>
+      </c>
+      <c r="C847" t="s">
+        <v>13</v>
+      </c>
+      <c r="D847" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E847" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F847" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G847" t="s">
+        <v>429</v>
+      </c>
+      <c r="H847" t="s">
+        <v>270</v>
+      </c>
+      <c r="I847" t="s">
+        <v>19</v>
+      </c>
+      <c r="J847">
+        <v>1</v>
+      </c>
+      <c r="K847">
+        <v>490000</v>
+      </c>
+      <c r="L847">
+        <v>490000</v>
+      </c>
+    </row>
+    <row r="848" spans="1:12">
+      <c r="A848">
+        <v>845</v>
+      </c>
+      <c r="B848">
+        <v>626402</v>
+      </c>
+      <c r="C848" t="s">
+        <v>13</v>
+      </c>
+      <c r="D848" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E848" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F848" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G848" t="s">
+        <v>429</v>
+      </c>
+      <c r="H848" t="s">
+        <v>271</v>
+      </c>
+      <c r="I848" t="s">
+        <v>19</v>
+      </c>
+      <c r="J848">
+        <v>1</v>
+      </c>
+      <c r="K848">
+        <v>3275000</v>
+      </c>
+      <c r="L848">
+        <v>3275000</v>
+      </c>
+    </row>
+    <row r="849" spans="1:12">
+      <c r="A849">
+        <v>846</v>
+      </c>
+      <c r="B849">
+        <v>626402</v>
+      </c>
+      <c r="C849" t="s">
+        <v>13</v>
+      </c>
+      <c r="D849" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E849" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F849" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G849" t="s">
+        <v>429</v>
+      </c>
+      <c r="H849" t="s">
+        <v>772</v>
+      </c>
+      <c r="I849" t="s">
+        <v>19</v>
+      </c>
+      <c r="J849">
+        <v>1</v>
+      </c>
+      <c r="K849">
+        <v>608500</v>
+      </c>
+      <c r="L849">
+        <v>608500</v>
+      </c>
+    </row>
+    <row r="850" spans="1:12">
+      <c r="A850">
+        <v>847</v>
+      </c>
+      <c r="B850">
+        <v>626402</v>
+      </c>
+      <c r="C850" t="s">
+        <v>13</v>
+      </c>
+      <c r="D850" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E850" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F850" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G850" t="s">
+        <v>429</v>
+      </c>
+      <c r="H850" t="s">
+        <v>272</v>
+      </c>
+      <c r="I850" t="s">
+        <v>19</v>
+      </c>
+      <c r="J850">
+        <v>1</v>
+      </c>
+      <c r="K850">
+        <v>7247431</v>
+      </c>
+      <c r="L850">
+        <v>7247431</v>
+      </c>
+    </row>
+    <row r="851" spans="1:12">
+      <c r="A851">
+        <v>848</v>
+      </c>
+      <c r="B851">
+        <v>626402</v>
+      </c>
+      <c r="C851" t="s">
+        <v>13</v>
+      </c>
+      <c r="D851" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E851" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F851" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G851" t="s">
+        <v>429</v>
+      </c>
+      <c r="H851" t="s">
+        <v>305</v>
+      </c>
+      <c r="I851" t="s">
+        <v>19</v>
+      </c>
+      <c r="J851">
+        <v>1</v>
+      </c>
+      <c r="K851">
+        <v>276000</v>
+      </c>
+      <c r="L851">
+        <v>276000</v>
+      </c>
+    </row>
+    <row r="852" spans="1:12">
+      <c r="A852">
+        <v>849</v>
+      </c>
+      <c r="B852">
+        <v>626402</v>
+      </c>
+      <c r="C852" t="s">
+        <v>13</v>
+      </c>
+      <c r="D852" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E852" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F852" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G852" t="s">
+        <v>429</v>
+      </c>
+      <c r="H852" t="s">
+        <v>386</v>
+      </c>
+      <c r="I852" t="s">
+        <v>19</v>
+      </c>
+      <c r="J852">
+        <v>1</v>
+      </c>
+      <c r="K852">
+        <v>3291500</v>
+      </c>
+      <c r="L852">
+        <v>3291500</v>
+      </c>
+    </row>
+    <row r="853" spans="1:12">
+      <c r="A853">
+        <v>850</v>
+      </c>
+      <c r="B853">
+        <v>626402</v>
+      </c>
+      <c r="C853" t="s">
+        <v>13</v>
+      </c>
+      <c r="D853" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E853" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F853" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G853" t="s">
+        <v>429</v>
+      </c>
+      <c r="H853" t="s">
+        <v>1196</v>
+      </c>
+      <c r="I853" t="s">
+        <v>19</v>
+      </c>
+      <c r="J853">
+        <v>1</v>
+      </c>
+      <c r="K853">
+        <v>3365570</v>
+      </c>
+      <c r="L853">
+        <v>3365570</v>
+      </c>
+    </row>
+    <row r="854" spans="1:12">
+      <c r="A854">
+        <v>851</v>
+      </c>
+      <c r="B854">
+        <v>626402</v>
+      </c>
+      <c r="C854" t="s">
+        <v>13</v>
+      </c>
+      <c r="D854" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E854" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F854" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G854" t="s">
+        <v>429</v>
+      </c>
+      <c r="H854" t="s">
+        <v>387</v>
+      </c>
+      <c r="I854" t="s">
+        <v>19</v>
+      </c>
+      <c r="J854">
+        <v>1</v>
+      </c>
+      <c r="K854">
+        <v>2455000</v>
+      </c>
+      <c r="L854">
+        <v>2455000</v>
+      </c>
+    </row>
+    <row r="855" spans="1:12">
+      <c r="A855">
+        <v>852</v>
+      </c>
+      <c r="B855">
+        <v>626402</v>
+      </c>
+      <c r="C855" t="s">
+        <v>13</v>
+      </c>
+      <c r="D855" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E855" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F855" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G855" t="s">
+        <v>429</v>
+      </c>
+      <c r="H855" t="s">
+        <v>1197</v>
+      </c>
+      <c r="I855" t="s">
+        <v>19</v>
+      </c>
+      <c r="J855">
+        <v>1</v>
+      </c>
+      <c r="K855">
+        <v>7154500</v>
+      </c>
+      <c r="L855">
+        <v>7154500</v>
+      </c>
+    </row>
+    <row r="856" spans="1:12">
+      <c r="A856">
+        <v>853</v>
+      </c>
+      <c r="B856">
+        <v>626402</v>
+      </c>
+      <c r="C856" t="s">
+        <v>13</v>
+      </c>
+      <c r="D856" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E856" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F856" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G856" t="s">
+        <v>429</v>
+      </c>
+      <c r="H856" t="s">
+        <v>750</v>
+      </c>
+      <c r="I856" t="s">
+        <v>19</v>
+      </c>
+      <c r="J856">
+        <v>1</v>
+      </c>
+      <c r="K856">
+        <v>300000</v>
+      </c>
+      <c r="L856">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="857" spans="1:12">
+      <c r="A857">
+        <v>854</v>
+      </c>
+      <c r="B857">
+        <v>626402</v>
+      </c>
+      <c r="C857" t="s">
+        <v>13</v>
+      </c>
+      <c r="D857" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E857" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F857" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G857" t="s">
+        <v>429</v>
+      </c>
+      <c r="H857" t="s">
+        <v>667</v>
+      </c>
+      <c r="I857" t="s">
+        <v>19</v>
+      </c>
+      <c r="J857">
+        <v>1</v>
+      </c>
+      <c r="K857">
+        <v>6616700</v>
+      </c>
+      <c r="L857">
+        <v>6616700</v>
+      </c>
+    </row>
+    <row r="858" spans="1:12">
+      <c r="A858">
+        <v>855</v>
+      </c>
+      <c r="B858">
+        <v>626402</v>
+      </c>
+      <c r="C858" t="s">
+        <v>13</v>
+      </c>
+      <c r="D858" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E858" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F858" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G858" t="s">
+        <v>429</v>
+      </c>
+      <c r="H858" t="s">
+        <v>274</v>
+      </c>
+      <c r="I858" t="s">
+        <v>19</v>
+      </c>
+      <c r="J858">
+        <v>1</v>
+      </c>
+      <c r="K858">
+        <v>1651679</v>
+      </c>
+      <c r="L858">
+        <v>1651679</v>
+      </c>
+    </row>
+    <row r="859" spans="1:12">
+      <c r="A859">
+        <v>856</v>
+      </c>
+      <c r="B859">
+        <v>626402</v>
+      </c>
+      <c r="C859" t="s">
+        <v>13</v>
+      </c>
+      <c r="D859" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E859" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F859" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G859" t="s">
+        <v>429</v>
+      </c>
+      <c r="H859" t="s">
+        <v>518</v>
+      </c>
+      <c r="I859" t="s">
+        <v>19</v>
+      </c>
+      <c r="J859">
+        <v>1</v>
+      </c>
+      <c r="K859">
+        <v>6634200</v>
+      </c>
+      <c r="L859">
+        <v>6634200</v>
+      </c>
+    </row>
+    <row r="860" spans="1:12">
+      <c r="A860">
+        <v>857</v>
+      </c>
+      <c r="B860">
+        <v>626402</v>
+      </c>
+      <c r="C860" t="s">
+        <v>13</v>
+      </c>
+      <c r="D860" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E860" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F860" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G860" t="s">
+        <v>429</v>
+      </c>
+      <c r="H860" t="s">
+        <v>724</v>
+      </c>
+      <c r="I860" t="s">
+        <v>19</v>
+      </c>
+      <c r="J860">
+        <v>1</v>
+      </c>
+      <c r="K860">
+        <v>105000</v>
+      </c>
+      <c r="L860">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="861" spans="1:12">
+      <c r="A861">
+        <v>858</v>
+      </c>
+      <c r="B861">
+        <v>626402</v>
+      </c>
+      <c r="C861" t="s">
+        <v>13</v>
+      </c>
+      <c r="D861" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E861" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F861" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G861" t="s">
+        <v>429</v>
+      </c>
+      <c r="H861" t="s">
+        <v>275</v>
+      </c>
+      <c r="I861" t="s">
+        <v>19</v>
+      </c>
+      <c r="J861">
+        <v>1</v>
+      </c>
+      <c r="K861">
+        <v>1640000</v>
+      </c>
+      <c r="L861">
+        <v>1640000</v>
+      </c>
+    </row>
+    <row r="862" spans="1:12">
+      <c r="A862">
+        <v>859</v>
+      </c>
+      <c r="B862">
+        <v>626402</v>
+      </c>
+      <c r="C862" t="s">
+        <v>13</v>
+      </c>
+      <c r="D862" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E862" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F862" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G862" t="s">
+        <v>429</v>
+      </c>
+      <c r="H862" t="s">
+        <v>734</v>
+      </c>
+      <c r="I862" t="s">
+        <v>19</v>
+      </c>
+      <c r="J862">
+        <v>1</v>
+      </c>
+      <c r="K862">
+        <v>340000</v>
+      </c>
+      <c r="L862">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="863" spans="1:12">
+      <c r="A863">
+        <v>860</v>
+      </c>
+      <c r="B863">
+        <v>626402</v>
+      </c>
+      <c r="C863" t="s">
+        <v>13</v>
+      </c>
+      <c r="D863" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E863" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F863" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G863" t="s">
+        <v>429</v>
+      </c>
+      <c r="H863" t="s">
+        <v>307</v>
+      </c>
+      <c r="I863" t="s">
+        <v>19</v>
+      </c>
+      <c r="J863">
+        <v>1</v>
+      </c>
+      <c r="K863">
+        <v>840000</v>
+      </c>
+      <c r="L863">
+        <v>840000</v>
+      </c>
+    </row>
+    <row r="864" spans="1:12">
+      <c r="A864">
+        <v>861</v>
+      </c>
+      <c r="B864">
+        <v>626402</v>
+      </c>
+      <c r="C864" t="s">
+        <v>13</v>
+      </c>
+      <c r="D864" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E864" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F864" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G864" t="s">
+        <v>429</v>
+      </c>
+      <c r="H864" t="s">
+        <v>308</v>
+      </c>
+      <c r="I864" t="s">
+        <v>19</v>
+      </c>
+      <c r="J864">
+        <v>1</v>
+      </c>
+      <c r="K864">
+        <v>1530000</v>
+      </c>
+      <c r="L864">
+        <v>1530000</v>
+      </c>
+    </row>
+    <row r="865" spans="1:12">
+      <c r="A865">
+        <v>862</v>
+      </c>
+      <c r="B865">
+        <v>626402</v>
+      </c>
+      <c r="C865" t="s">
+        <v>13</v>
+      </c>
+      <c r="D865" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E865" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F865" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G865" t="s">
+        <v>429</v>
+      </c>
+      <c r="H865" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I865" t="s">
+        <v>19</v>
+      </c>
+      <c r="J865">
+        <v>1</v>
+      </c>
+      <c r="K865">
+        <v>260000</v>
+      </c>
+      <c r="L865">
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="866" spans="1:12">
+      <c r="A866">
+        <v>863</v>
+      </c>
+      <c r="B866">
+        <v>626402</v>
+      </c>
+      <c r="C866" t="s">
+        <v>13</v>
+      </c>
+      <c r="D866" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E866" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F866" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G866" t="s">
+        <v>429</v>
+      </c>
+      <c r="H866" t="s">
+        <v>671</v>
+      </c>
+      <c r="I866" t="s">
+        <v>19</v>
+      </c>
+      <c r="J866">
+        <v>1</v>
+      </c>
+      <c r="K866">
+        <v>340000</v>
+      </c>
+      <c r="L866">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="867" spans="1:12">
+      <c r="A867">
+        <v>864</v>
+      </c>
+      <c r="B867">
+        <v>626402</v>
+      </c>
+      <c r="C867" t="s">
+        <v>13</v>
+      </c>
+      <c r="D867" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E867" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F867" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G867" t="s">
+        <v>429</v>
+      </c>
+      <c r="H867" t="s">
+        <v>1012</v>
+      </c>
+      <c r="I867" t="s">
+        <v>19</v>
+      </c>
+      <c r="J867">
+        <v>1</v>
+      </c>
+      <c r="K867">
+        <v>340000</v>
+      </c>
+      <c r="L867">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="868" spans="1:12">
+      <c r="A868">
+        <v>865</v>
+      </c>
+      <c r="B868">
+        <v>626402</v>
+      </c>
+      <c r="C868" t="s">
+        <v>13</v>
+      </c>
+      <c r="D868" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E868" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F868" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G868" t="s">
+        <v>429</v>
+      </c>
+      <c r="H868" t="s">
+        <v>1199</v>
+      </c>
+      <c r="I868" t="s">
+        <v>19</v>
+      </c>
+      <c r="J868">
+        <v>1</v>
+      </c>
+      <c r="K868">
+        <v>890000</v>
+      </c>
+      <c r="L868">
+        <v>890000</v>
+      </c>
+    </row>
+    <row r="869" spans="1:12">
+      <c r="A869">
+        <v>866</v>
+      </c>
+      <c r="B869">
+        <v>626402</v>
+      </c>
+      <c r="C869" t="s">
+        <v>13</v>
+      </c>
+      <c r="D869" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E869" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F869" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G869" t="s">
+        <v>429</v>
+      </c>
+      <c r="H869" t="s">
+        <v>1200</v>
+      </c>
+      <c r="I869" t="s">
+        <v>19</v>
+      </c>
+      <c r="J869">
+        <v>1</v>
+      </c>
+      <c r="K869">
+        <v>850000</v>
+      </c>
+      <c r="L869">
+        <v>850000</v>
+      </c>
+    </row>
+    <row r="870" spans="1:12">
+      <c r="A870">
+        <v>867</v>
+      </c>
+      <c r="B870">
+        <v>626402</v>
+      </c>
+      <c r="C870" t="s">
+        <v>13</v>
+      </c>
+      <c r="D870" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E870" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F870" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G870" t="s">
+        <v>429</v>
+      </c>
+      <c r="H870" t="s">
+        <v>312</v>
+      </c>
+      <c r="I870" t="s">
+        <v>19</v>
+      </c>
+      <c r="J870">
+        <v>1</v>
+      </c>
+      <c r="K870">
+        <v>340000</v>
+      </c>
+      <c r="L870">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="871" spans="1:12">
+      <c r="A871">
+        <v>868</v>
+      </c>
+      <c r="B871">
+        <v>626402</v>
+      </c>
+      <c r="C871" t="s">
+        <v>13</v>
+      </c>
+      <c r="D871" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E871" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F871" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G871" t="s">
+        <v>429</v>
+      </c>
+      <c r="H871" t="s">
+        <v>388</v>
+      </c>
+      <c r="I871" t="s">
+        <v>19</v>
+      </c>
+      <c r="J871">
+        <v>1</v>
+      </c>
+      <c r="K871">
+        <v>680000</v>
+      </c>
+      <c r="L871">
+        <v>680000</v>
+      </c>
+    </row>
+    <row r="872" spans="1:12">
+      <c r="A872">
+        <v>869</v>
+      </c>
+      <c r="B872">
+        <v>626402</v>
+      </c>
+      <c r="C872" t="s">
+        <v>13</v>
+      </c>
+      <c r="D872" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E872" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F872" t="s">
+        <v>1202</v>
+      </c>
+      <c r="G872" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H872" t="s">
+        <v>284</v>
+      </c>
+      <c r="I872" t="s">
+        <v>19</v>
+      </c>
+      <c r="J872">
+        <v>1</v>
+      </c>
+      <c r="K872">
+        <v>9616780</v>
+      </c>
+      <c r="L872">
+        <v>9616780</v>
+      </c>
+    </row>
+    <row r="873" spans="1:12">
+      <c r="A873">
+        <v>870</v>
+      </c>
+      <c r="B873">
+        <v>626402</v>
+      </c>
+      <c r="C873" t="s">
+        <v>13</v>
+      </c>
+      <c r="D873" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E873" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F873" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G873" t="s">
+        <v>1206</v>
+      </c>
+      <c r="H873" t="s">
+        <v>284</v>
+      </c>
+      <c r="I873" t="s">
+        <v>19</v>
+      </c>
+      <c r="J873">
+        <v>1</v>
+      </c>
+      <c r="K873">
+        <v>1556500</v>
+      </c>
+      <c r="L873">
+        <v>1556500</v>
+      </c>
+    </row>
+    <row r="874" spans="1:12">
+      <c r="A874">
+        <v>871</v>
+      </c>
+      <c r="B874">
+        <v>626402</v>
+      </c>
+      <c r="C874" t="s">
+        <v>13</v>
+      </c>
+      <c r="D874" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E874" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F874" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G874" t="s">
+        <v>1209</v>
+      </c>
+      <c r="H874" t="s">
+        <v>272</v>
+      </c>
+      <c r="I874" t="s">
+        <v>19</v>
+      </c>
+      <c r="J874">
+        <v>1</v>
+      </c>
+      <c r="K874">
+        <v>910131</v>
+      </c>
+      <c r="L874">
+        <v>910131</v>
+      </c>
+    </row>
+    <row r="875" spans="1:12">
+      <c r="A875">
+        <v>872</v>
+      </c>
+      <c r="B875">
+        <v>626402</v>
+      </c>
+      <c r="C875" t="s">
+        <v>13</v>
+      </c>
+      <c r="D875" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E875" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F875" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G875" t="s">
+        <v>1212</v>
+      </c>
+      <c r="H875" t="s">
+        <v>272</v>
+      </c>
+      <c r="I875" t="s">
+        <v>19</v>
+      </c>
+      <c r="J875">
+        <v>1</v>
+      </c>
+      <c r="K875">
+        <v>661000</v>
+      </c>
+      <c r="L875">
+        <v>661000</v>
+      </c>
+    </row>
+    <row r="876" spans="1:12">
+      <c r="A876">
+        <v>873</v>
+      </c>
+      <c r="B876">
+        <v>626402</v>
+      </c>
+      <c r="C876" t="s">
+        <v>13</v>
+      </c>
+      <c r="D876" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E876" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F876" t="s">
+        <v>1214</v>
+      </c>
+      <c r="G876" t="s">
+        <v>1215</v>
+      </c>
+      <c r="H876" t="s">
+        <v>275</v>
+      </c>
+      <c r="I876" t="s">
+        <v>19</v>
+      </c>
+      <c r="J876">
+        <v>1</v>
+      </c>
+      <c r="K876">
+        <v>930000</v>
+      </c>
+      <c r="L876">
+        <v>930000</v>
+      </c>
+    </row>
+    <row r="877" spans="1:12">
+      <c r="A877">
+        <v>874</v>
+      </c>
+      <c r="B877">
+        <v>626402</v>
+      </c>
+      <c r="C877" t="s">
+        <v>13</v>
+      </c>
+      <c r="D877" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E877" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F877" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G877" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H877" t="s">
+        <v>275</v>
+      </c>
+      <c r="I877" t="s">
+        <v>19</v>
+      </c>
+      <c r="J877">
+        <v>1</v>
+      </c>
+      <c r="K877">
+        <v>2060500</v>
+      </c>
+      <c r="L877">
+        <v>2060500</v>
+      </c>
+    </row>
+    <row r="878" spans="1:12">
+      <c r="A878">
+        <v>875</v>
+      </c>
+      <c r="B878">
+        <v>626402</v>
+      </c>
+      <c r="C878" t="s">
+        <v>13</v>
+      </c>
+      <c r="D878" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E878" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F878" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G878" t="s">
+        <v>1221</v>
+      </c>
+      <c r="H878" t="s">
+        <v>275</v>
+      </c>
+      <c r="I878" t="s">
+        <v>19</v>
+      </c>
+      <c r="J878">
+        <v>1</v>
+      </c>
+      <c r="K878">
+        <v>580000</v>
+      </c>
+      <c r="L878">
+        <v>580000</v>
+      </c>
+    </row>
+    <row r="879" spans="1:12">
+      <c r="A879">
+        <v>876</v>
+      </c>
+      <c r="B879">
+        <v>626402</v>
+      </c>
+      <c r="C879" t="s">
+        <v>13</v>
+      </c>
+      <c r="D879" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E879" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F879" t="s">
+        <v>1223</v>
+      </c>
+      <c r="G879" t="s">
+        <v>1224</v>
+      </c>
+      <c r="H879" t="s">
+        <v>704</v>
+      </c>
+      <c r="I879" t="s">
+        <v>19</v>
+      </c>
+      <c r="J879">
+        <v>1</v>
+      </c>
+      <c r="K879">
+        <v>7430266</v>
+      </c>
+      <c r="L879">
+        <v>7430266</v>
+      </c>
+    </row>
+    <row r="880" spans="1:12">
+      <c r="A880">
+        <v>877</v>
+      </c>
+      <c r="B880">
+        <v>626402</v>
+      </c>
+      <c r="C880" t="s">
+        <v>13</v>
+      </c>
+      <c r="D880" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E880" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F880" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G880" t="s">
+        <v>1227</v>
+      </c>
+      <c r="H880" t="s">
+        <v>192</v>
+      </c>
+      <c r="I880" t="s">
+        <v>19</v>
+      </c>
+      <c r="J880">
+        <v>1</v>
+      </c>
+      <c r="K880">
+        <v>11133749</v>
+      </c>
+      <c r="L880">
+        <v>11133749</v>
+      </c>
+    </row>
+    <row r="881" spans="1:12">
+      <c r="A881">
+        <v>878</v>
+      </c>
+      <c r="B881">
+        <v>626402</v>
+      </c>
+      <c r="C881" t="s">
+        <v>13</v>
+      </c>
+      <c r="D881" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E881" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F881" t="s">
+        <v>1229</v>
+      </c>
+      <c r="G881" t="s">
+        <v>1230</v>
+      </c>
+      <c r="H881" t="s">
+        <v>703</v>
+      </c>
+      <c r="I881" t="s">
+        <v>19</v>
+      </c>
+      <c r="J881">
+        <v>1</v>
+      </c>
+      <c r="K881">
+        <v>3426080</v>
+      </c>
+      <c r="L881">
+        <v>3426080</v>
+      </c>
+    </row>
+    <row r="882" spans="1:12">
+      <c r="A882">
+        <v>879</v>
+      </c>
+      <c r="B882">
+        <v>626402</v>
+      </c>
+      <c r="C882" t="s">
+        <v>13</v>
+      </c>
+      <c r="D882" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E882" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F882" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G882" t="s">
+        <v>1233</v>
+      </c>
+      <c r="H882" t="s">
+        <v>414</v>
+      </c>
+      <c r="I882" t="s">
+        <v>19</v>
+      </c>
+      <c r="J882">
+        <v>1</v>
+      </c>
+      <c r="K882">
+        <v>222851484</v>
+      </c>
+      <c r="L882">
+        <v>222851484</v>
+      </c>
+    </row>
+    <row r="883" spans="1:12">
+      <c r="A883">
+        <v>880</v>
+      </c>
+      <c r="B883">
+        <v>626402</v>
+      </c>
+      <c r="C883" t="s">
+        <v>13</v>
+      </c>
+      <c r="D883" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E883" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F883" t="s">
+        <v>1235</v>
+      </c>
+      <c r="G883" t="s">
+        <v>1236</v>
+      </c>
+      <c r="H883" t="s">
+        <v>724</v>
+      </c>
+      <c r="I883" t="s">
+        <v>19</v>
+      </c>
+      <c r="J883">
+        <v>1</v>
+      </c>
+      <c r="K883">
+        <v>1544810</v>
+      </c>
+      <c r="L883">
+        <v>1544810</v>
+      </c>
+    </row>
+    <row r="884" spans="1:12">
+      <c r="A884">
+        <v>881</v>
+      </c>
+      <c r="B884">
+        <v>626402</v>
+      </c>
+      <c r="C884" t="s">
+        <v>13</v>
+      </c>
+      <c r="D884" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E884" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F884" t="s">
+        <v>1238</v>
+      </c>
+      <c r="G884" t="s">
+        <v>1239</v>
+      </c>
+      <c r="H884" t="s">
+        <v>1240</v>
+      </c>
+      <c r="I884" t="s">
+        <v>19</v>
+      </c>
+      <c r="J884">
+        <v>1</v>
+      </c>
+      <c r="K884">
+        <v>103750000</v>
+      </c>
+      <c r="L884">
+        <v>103750000</v>
+      </c>
+    </row>
+    <row r="885" spans="1:12">
+      <c r="A885">
+        <v>882</v>
+      </c>
+      <c r="B885">
+        <v>626402</v>
+      </c>
+      <c r="C885" t="s">
+        <v>13</v>
+      </c>
+      <c r="D885" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E885" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F885" t="s">
+        <v>1242</v>
+      </c>
+      <c r="G885" t="s">
+        <v>1243</v>
+      </c>
+      <c r="H885" t="s">
+        <v>732</v>
+      </c>
+      <c r="I885" t="s">
+        <v>19</v>
+      </c>
+      <c r="J885">
+        <v>1</v>
+      </c>
+      <c r="K885">
+        <v>8947677</v>
+      </c>
+      <c r="L885">
+        <v>8947677</v>
+      </c>
+    </row>
+    <row r="886" spans="1:12">
+      <c r="A886">
+        <v>883</v>
+      </c>
+      <c r="B886">
+        <v>626402</v>
+      </c>
+      <c r="C886" t="s">
+        <v>13</v>
+      </c>
+      <c r="D886" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E886" t="s">
+        <v>1244</v>
+      </c>
+      <c r="F886" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G886" t="s">
+        <v>1246</v>
+      </c>
+      <c r="H886" t="s">
+        <v>732</v>
+      </c>
+      <c r="I886" t="s">
+        <v>19</v>
+      </c>
+      <c r="J886">
+        <v>1</v>
+      </c>
+      <c r="K886">
+        <v>9935251</v>
+      </c>
+      <c r="L886">
+        <v>9935251</v>
+      </c>
+    </row>
+    <row r="887" spans="1:12">
+      <c r="A887">
+        <v>884</v>
+      </c>
+      <c r="B887">
+        <v>626402</v>
+      </c>
+      <c r="C887" t="s">
+        <v>13</v>
+      </c>
+      <c r="D887" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E887" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F887" t="s">
+        <v>1249</v>
+      </c>
+      <c r="G887" t="s">
+        <v>1250</v>
+      </c>
+      <c r="H887" t="s">
+        <v>363</v>
+      </c>
+      <c r="I887" t="s">
+        <v>19</v>
+      </c>
+      <c r="J887">
+        <v>1</v>
+      </c>
+      <c r="K887">
+        <v>6052227</v>
+      </c>
+      <c r="L887">
+        <v>6052227</v>
+      </c>
+    </row>
+    <row r="888" spans="1:12">
+      <c r="A888">
+        <v>885</v>
+      </c>
+      <c r="B888">
+        <v>626402</v>
+      </c>
+      <c r="C888" t="s">
+        <v>13</v>
+      </c>
+      <c r="D888" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E888" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F888" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G888" t="s">
+        <v>1253</v>
+      </c>
+      <c r="H888" t="s">
+        <v>363</v>
+      </c>
+      <c r="I888" t="s">
+        <v>19</v>
+      </c>
+      <c r="J888">
+        <v>1</v>
+      </c>
+      <c r="K888">
+        <v>7091500</v>
+      </c>
+      <c r="L888">
+        <v>7091500</v>
+      </c>
+    </row>
+    <row r="889" spans="1:12">
+      <c r="A889">
+        <v>886</v>
+      </c>
+      <c r="B889">
+        <v>626402</v>
+      </c>
+      <c r="C889" t="s">
+        <v>13</v>
+      </c>
+      <c r="D889" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E889" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F889" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G889" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H889" t="s">
+        <v>18</v>
+      </c>
+      <c r="I889" t="s">
+        <v>19</v>
+      </c>
+      <c r="J889">
+        <v>1</v>
+      </c>
+      <c r="K889">
+        <v>38825000</v>
+      </c>
+      <c r="L889">
+        <v>38825000</v>
+      </c>
+    </row>
+    <row r="890" spans="1:12">
+      <c r="A890">
+        <v>887</v>
+      </c>
+      <c r="B890">
+        <v>626402</v>
+      </c>
+      <c r="C890" t="s">
+        <v>13</v>
+      </c>
+      <c r="D890" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E890" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F890" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G890" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H890" t="s">
+        <v>20</v>
+      </c>
+      <c r="I890" t="s">
+        <v>19</v>
+      </c>
+      <c r="J890">
+        <v>1</v>
+      </c>
+      <c r="K890">
+        <v>3946</v>
+      </c>
+      <c r="L890">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="891" spans="1:12">
+      <c r="A891">
+        <v>888</v>
+      </c>
+      <c r="B891">
+        <v>626402</v>
+      </c>
+      <c r="C891" t="s">
+        <v>13</v>
+      </c>
+      <c r="D891" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E891" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F891" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G891" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H891" t="s">
+        <v>21</v>
+      </c>
+      <c r="I891" t="s">
+        <v>19</v>
+      </c>
+      <c r="J891">
+        <v>1</v>
+      </c>
+      <c r="K891">
+        <v>2349900</v>
+      </c>
+      <c r="L891">
+        <v>2349900</v>
+      </c>
+    </row>
+    <row r="892" spans="1:12">
+      <c r="A892">
+        <v>889</v>
+      </c>
+      <c r="B892">
+        <v>626402</v>
+      </c>
+      <c r="C892" t="s">
+        <v>13</v>
+      </c>
+      <c r="D892" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E892" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F892" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G892" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H892" t="s">
+        <v>22</v>
+      </c>
+      <c r="I892" t="s">
+        <v>19</v>
+      </c>
+      <c r="J892">
+        <v>1</v>
+      </c>
+      <c r="K892">
+        <v>840300</v>
+      </c>
+      <c r="L892">
+        <v>840300</v>
+      </c>
+    </row>
+    <row r="893" spans="1:12">
+      <c r="A893">
+        <v>890</v>
+      </c>
+      <c r="B893">
+        <v>626402</v>
+      </c>
+      <c r="C893" t="s">
+        <v>13</v>
+      </c>
+      <c r="D893" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E893" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F893" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G893" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H893" t="s">
+        <v>24</v>
+      </c>
+      <c r="I893" t="s">
+        <v>19</v>
+      </c>
+      <c r="J893">
+        <v>1</v>
+      </c>
+      <c r="K893">
+        <v>793498</v>
+      </c>
+      <c r="L893">
+        <v>793498</v>
+      </c>
+    </row>
+    <row r="894" spans="1:12">
+      <c r="A894">
+        <v>891</v>
+      </c>
+      <c r="B894">
+        <v>626402</v>
+      </c>
+      <c r="C894" t="s">
+        <v>13</v>
+      </c>
+      <c r="D894" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E894" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F894" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G894" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H894" t="s">
+        <v>18</v>
+      </c>
+      <c r="I894" t="s">
+        <v>19</v>
+      </c>
+      <c r="J894">
+        <v>1</v>
+      </c>
+      <c r="K894">
+        <v>671000</v>
+      </c>
+      <c r="L894">
+        <v>671000</v>
+      </c>
+    </row>
+    <row r="895" spans="1:12">
+      <c r="A895">
+        <v>892</v>
+      </c>
+      <c r="B895">
+        <v>626402</v>
+      </c>
+      <c r="C895" t="s">
+        <v>13</v>
+      </c>
+      <c r="D895" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E895" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F895" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G895" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H895" t="s">
+        <v>20</v>
+      </c>
+      <c r="I895" t="s">
+        <v>19</v>
+      </c>
+      <c r="J895">
+        <v>1</v>
+      </c>
+      <c r="K895">
+        <v>80</v>
+      </c>
+      <c r="L895">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="896" spans="1:12">
+      <c r="A896">
+        <v>893</v>
+      </c>
+      <c r="B896">
+        <v>626402</v>
+      </c>
+      <c r="C896" t="s">
+        <v>13</v>
+      </c>
+      <c r="D896" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E896" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F896" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G896" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H896" t="s">
+        <v>24</v>
+      </c>
+      <c r="I896" t="s">
+        <v>19</v>
+      </c>
+      <c r="J896">
+        <v>1</v>
+      </c>
+      <c r="K896">
+        <v>21667</v>
+      </c>
+      <c r="L896">
+        <v>21667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>